<commit_message>
added more data to end to end tests
</commit_message>
<xml_diff>
--- a/src/main/java/testData/ExcelFiles/E2E_Test_Data.xlsx
+++ b/src/main/java/testData/ExcelFiles/E2E_Test_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awhitten/IdeaProjects/Iceberg/src/main/java/testData/ExcelFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198B8362-4B7E-5346-8DD9-F8693F6131FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB332EB0-2F10-DB43-9814-5B24EAAB6505}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -229,7 +229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3581" uniqueCount="2905">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3579" uniqueCount="2903">
   <si>
     <t>Andorra</t>
   </si>
@@ -8895,9 +8895,6 @@
     <t>Tax Residency</t>
   </si>
   <si>
-    <t>DOB</t>
-  </si>
-  <si>
     <t>Residential Address</t>
   </si>
   <si>
@@ -8931,9 +8928,6 @@
     <t>Glaze Limited</t>
   </si>
   <si>
-    <t>31/09/1980</t>
-  </si>
-  <si>
     <t>YC394073D</t>
   </si>
   <si>
@@ -8949,7 +8943,7 @@
     <t>SS184804C</t>
   </si>
   <si>
-    <t>gift</t>
+    <t>Gift</t>
   </si>
 </sst>
 </file>
@@ -9097,7 +9091,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyFill="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -9160,12 +9154,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -9176,7 +9165,7 @@
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="9">
     <dxf>
       <font>
         <b val="0"/>
@@ -9221,9 +9210,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -9287,18 +9273,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{66A17FAD-981D-5B41-BBFC-5C46DB8223C2}" name="Table1" displayName="Table1" ref="A1:S6" totalsRowShown="0" headerRowDxfId="9" dataCellStyle="Normal">
-  <autoFilter ref="A1:S6" xr:uid="{9A576A1F-B3A3-1C4F-9DF6-F0570148ED85}"/>
-  <tableColumns count="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{66A17FAD-981D-5B41-BBFC-5C46DB8223C2}" name="Table1" displayName="Table1" ref="A1:R6" totalsRowShown="0" headerRowDxfId="8" dataCellStyle="Normal">
+  <autoFilter ref="A1:R6" xr:uid="{9A576A1F-B3A3-1C4F-9DF6-F0570148ED85}"/>
+  <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{7E9515AE-9F6E-A348-A7A8-E37FA4478783}" name="Scenario Type" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{F14DEEDD-F13E-3F47-8933-0ECB1C396173}" name="Mobile" dataDxfId="8" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{F14DEEDD-F13E-3F47-8933-0ECB1C396173}" name="Mobile" dataDxfId="7" dataCellStyle="Normal"/>
     <tableColumn id="3" xr3:uid="{204D9E2E-D519-7848-9A7E-6A1A14191AD0}" name="Email" dataCellStyle="Normal"/>
     <tableColumn id="4" xr3:uid="{653C44EE-BD43-3445-9EF9-4EF402DE6340}" name="Company" dataCellStyle="Normal"/>
     <tableColumn id="5" xr3:uid="{31B973B6-778E-AC40-9446-6BD4B99672FA}" name="Trading Name" dataCellStyle="Normal"/>
-    <tableColumn id="6" xr3:uid="{20CA079A-69FE-9F4B-B9F2-518AA4C1DF26}" name="Tax Residency" dataDxfId="7" dataCellStyle="Normal"/>
-    <tableColumn id="7" xr3:uid="{4B589A57-EFE3-AF4A-83A8-B31CFD30816A}" name="UTR" dataDxfId="6" dataCellStyle="Normal"/>
+    <tableColumn id="6" xr3:uid="{20CA079A-69FE-9F4B-B9F2-518AA4C1DF26}" name="Tax Residency" dataDxfId="6" dataCellStyle="Normal"/>
+    <tableColumn id="7" xr3:uid="{4B589A57-EFE3-AF4A-83A8-B31CFD30816A}" name="UTR" dataDxfId="5" dataCellStyle="Normal"/>
     <tableColumn id="8" xr3:uid="{6F1043C0-A74B-8A42-9223-7D931F19C3C4}" name="Previous Name" dataCellStyle="Normal"/>
-    <tableColumn id="9" xr3:uid="{9721BC23-DF5B-7544-8CC4-ACCF84D49EC6}" name="DOB" dataDxfId="5" dataCellStyle="Normal"/>
     <tableColumn id="10" xr3:uid="{88E6A19D-2B70-D541-911D-47BDE2B42406}" name="Residential Address" dataCellStyle="Normal"/>
     <tableColumn id="11" xr3:uid="{8654657B-C7CF-0640-AB7D-FA5E1C1EEBA2}" name="Nat Insurance Number" dataCellStyle="Normal"/>
     <tableColumn id="12" xr3:uid="{AF7A645F-938B-4647-BAA4-BB8F8BBC530F}" name="ID Number" dataDxfId="4" dataCellStyle="Normal"/>
@@ -20870,10 +20855,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{826EF1C6-3923-2840-ABB7-1988F417BDA7}">
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -20886,20 +20871,19 @@
     <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.6640625" style="30" customWidth="1"/>
     <col min="8" max="8" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5" style="44" customWidth="1"/>
-    <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.1640625" style="28" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19" customWidth="1"/>
-    <col min="15" max="15" width="22.6640625" style="28" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.1640625" style="28" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19" customWidth="1"/>
+    <col min="14" max="14" width="22.6640625" style="28" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="43" customFormat="1" ht="17">
+    <row r="1" spans="1:18" s="43" customFormat="1" ht="17">
       <c r="A1" s="39" t="s">
         <v>1827</v>
       </c>
@@ -20924,25 +20908,25 @@
       <c r="H1" s="39" t="s">
         <v>249</v>
       </c>
-      <c r="I1" s="46" t="s">
+      <c r="I1" s="42" t="s">
         <v>2886</v>
       </c>
-      <c r="J1" s="42" t="s">
+      <c r="J1" s="39" t="s">
         <v>2887</v>
       </c>
-      <c r="K1" s="39" t="s">
+      <c r="K1" s="40" t="s">
         <v>2888</v>
       </c>
-      <c r="L1" s="40" t="s">
+      <c r="L1" s="44" t="s">
         <v>2889</v>
       </c>
-      <c r="M1" s="45" t="s">
+      <c r="M1" s="39" t="s">
         <v>2890</v>
       </c>
-      <c r="N1" s="39" t="s">
+      <c r="N1" s="44" t="s">
         <v>2891</v>
       </c>
-      <c r="O1" s="45" t="s">
+      <c r="O1" s="39" t="s">
         <v>2892</v>
       </c>
       <c r="P1" s="39" t="s">
@@ -20954,11 +20938,8 @@
       <c r="R1" s="39" t="s">
         <v>2895</v>
       </c>
-      <c r="S1" s="39" t="s">
-        <v>2896</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19">
+    </row>
+    <row r="2" spans="1:18">
       <c r="B2" s="18" t="s">
         <v>2604</v>
       </c>
@@ -20966,7 +20947,7 @@
         <v>245</v>
       </c>
       <c r="D2" t="s">
-        <v>2897</v>
+        <v>2896</v>
       </c>
       <c r="E2" t="s">
         <v>1148</v>
@@ -20980,41 +20961,38 @@
       <c r="H2" t="s">
         <v>1034</v>
       </c>
-      <c r="I2" s="44">
-        <v>27892</v>
+      <c r="I2" t="s">
+        <v>247</v>
       </c>
       <c r="J2" t="s">
-        <v>247</v>
-      </c>
-      <c r="K2" t="s">
-        <v>2899</v>
-      </c>
-      <c r="L2" s="18">
+        <v>2897</v>
+      </c>
+      <c r="K2" s="18">
         <v>8780321437</v>
       </c>
-      <c r="M2" s="30">
+      <c r="L2" s="30">
         <v>10000</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="O2" s="30">
+      <c r="N2" s="30">
         <v>400</v>
       </c>
-      <c r="P2">
+      <c r="O2">
         <v>40000</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>718</v>
       </c>
-      <c r="R2" s="15">
+      <c r="Q2" s="15">
         <v>4000</v>
       </c>
-      <c r="S2" s="15" t="s">
-        <v>2904</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19">
+      <c r="R2" s="15" t="s">
+        <v>2902</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="B3" s="18" t="s">
         <v>2605</v>
       </c>
@@ -21022,7 +21000,7 @@
         <v>251</v>
       </c>
       <c r="D3" t="s">
-        <v>2897</v>
+        <v>2896</v>
       </c>
       <c r="E3" t="s">
         <v>1149</v>
@@ -21036,41 +21014,38 @@
       <c r="H3" t="s">
         <v>1020</v>
       </c>
-      <c r="I3" s="44">
-        <v>33451</v>
+      <c r="I3" t="s">
+        <v>490</v>
       </c>
       <c r="J3" t="s">
-        <v>490</v>
-      </c>
-      <c r="K3" t="s">
-        <v>2900</v>
-      </c>
-      <c r="L3" s="18">
+        <v>2898</v>
+      </c>
+      <c r="K3" s="18">
         <v>7164427402</v>
       </c>
-      <c r="M3" s="30">
+      <c r="L3" s="30">
         <v>100</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="O3" s="30">
+      <c r="N3" s="30">
         <v>56488</v>
       </c>
-      <c r="P3">
+      <c r="O3">
         <v>200000</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>1143</v>
       </c>
-      <c r="R3" s="15">
+      <c r="Q3" s="15">
         <v>435554</v>
       </c>
-      <c r="S3" s="15" t="s">
-        <v>2904</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19">
+      <c r="R3" s="15" t="s">
+        <v>2902</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="B4" s="18" t="s">
         <v>2880</v>
       </c>
@@ -21078,7 +21053,7 @@
         <v>252</v>
       </c>
       <c r="D4" t="s">
-        <v>2897</v>
+        <v>2896</v>
       </c>
       <c r="E4" t="s">
         <v>1150</v>
@@ -21092,41 +21067,38 @@
       <c r="H4" t="s">
         <v>988</v>
       </c>
-      <c r="I4" s="44">
-        <v>23309</v>
+      <c r="I4" t="s">
+        <v>491</v>
       </c>
       <c r="J4" t="s">
-        <v>491</v>
-      </c>
-      <c r="K4" t="s">
-        <v>2901</v>
-      </c>
-      <c r="L4" s="18">
+        <v>2899</v>
+      </c>
+      <c r="K4" s="18">
         <v>723868212</v>
       </c>
-      <c r="M4" s="30">
+      <c r="L4" s="30">
         <v>23567</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="O4" s="30">
+      <c r="N4" s="30">
         <v>290000</v>
       </c>
-      <c r="P4">
+      <c r="O4">
         <v>564434</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>1144</v>
       </c>
-      <c r="R4" s="15">
+      <c r="Q4" s="15">
         <v>12000</v>
       </c>
-      <c r="S4" s="15" t="s">
-        <v>2904</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19">
+      <c r="R4" s="15" t="s">
+        <v>2902</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
       <c r="B5" s="18" t="s">
         <v>2632</v>
       </c>
@@ -21134,7 +21106,7 @@
         <v>2309</v>
       </c>
       <c r="D5" t="s">
-        <v>2897</v>
+        <v>2896</v>
       </c>
       <c r="E5" t="s">
         <v>1152</v>
@@ -21148,41 +21120,38 @@
       <c r="H5" t="s">
         <v>2633</v>
       </c>
-      <c r="I5" s="44">
-        <v>31120</v>
+      <c r="I5" t="s">
+        <v>2634</v>
       </c>
       <c r="J5" t="s">
-        <v>2634</v>
-      </c>
-      <c r="K5" t="s">
+        <v>2900</v>
+      </c>
+      <c r="K5" s="45" t="s">
+        <v>2644</v>
+      </c>
+      <c r="L5" s="30">
+        <v>1</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N5" s="30">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="Q5" s="15">
+        <v>1</v>
+      </c>
+      <c r="R5" s="15" t="s">
         <v>2902</v>
       </c>
-      <c r="L5" s="48" t="s">
-        <v>2644</v>
-      </c>
-      <c r="M5" s="30">
-        <v>1</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="O5" s="30">
-        <v>1</v>
-      </c>
-      <c r="P5">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>720</v>
-      </c>
-      <c r="R5" s="15">
-        <v>1</v>
-      </c>
-      <c r="S5" s="15" t="s">
-        <v>2904</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19">
+    </row>
+    <row r="6" spans="1:18">
       <c r="B6" s="18" t="s">
         <v>2638</v>
       </c>
@@ -21190,7 +21159,7 @@
         <v>2637</v>
       </c>
       <c r="D6" t="s">
-        <v>2897</v>
+        <v>2896</v>
       </c>
       <c r="E6" t="s">
         <v>1134</v>
@@ -21204,38 +21173,35 @@
       <c r="H6" t="s">
         <v>1087</v>
       </c>
-      <c r="I6" s="47" t="s">
-        <v>2898</v>
+      <c r="I6" t="s">
+        <v>492</v>
       </c>
       <c r="J6" t="s">
-        <v>492</v>
-      </c>
-      <c r="K6" t="s">
-        <v>2903</v>
-      </c>
-      <c r="L6" s="18">
+        <v>2901</v>
+      </c>
+      <c r="K6" s="18">
         <v>2768421731</v>
       </c>
-      <c r="M6" s="30">
+      <c r="L6" s="30">
         <v>10000000</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="M6" s="2" t="s">
         <v>40</v>
+      </c>
+      <c r="N6" s="30">
+        <v>10000000</v>
       </c>
       <c r="O6" s="30">
         <v>10000000</v>
       </c>
-      <c r="P6" s="30">
+      <c r="P6" s="1" t="s">
+        <v>721</v>
+      </c>
+      <c r="Q6" s="30">
         <v>10000000</v>
       </c>
-      <c r="Q6" s="1" t="s">
-        <v>721</v>
-      </c>
-      <c r="R6" s="30">
-        <v>10000000</v>
-      </c>
-      <c r="S6" s="15" t="s">
-        <v>2904</v>
+      <c r="R6" s="15" t="s">
+        <v>2902</v>
       </c>
     </row>
   </sheetData>
@@ -21364,7 +21330,7 @@
     <row r="1" spans="1:11">
       <c r="A1" s="6" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,9999999)&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>TV7665922W</v>
+        <v>GK7402730W</v>
       </c>
       <c r="B1" t="s">
         <v>1522</v>
@@ -21376,7 +21342,7 @@
     <row r="2" spans="1:11">
       <c r="A2" s="6" t="str">
         <f ca="1">7&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,9999999)&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>7K3101516S</v>
+        <v>7U6432459V</v>
       </c>
       <c r="B2" t="s">
         <v>1523</v>
@@ -21386,21 +21352,21 @@
       </c>
       <c r="I2" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,999999)&amp;CHAR(RANDBETWEEN(65,90))&amp;(RANDBETWEEN(1,99))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>VYQNK11203H99BP</v>
+        <v>GALHG997823U62SK</v>
       </c>
       <c r="J2" s="28" t="str">
         <f t="shared" ref="J2" ca="1" si="0">RIGHT(I2, LEN(I2)-1)</f>
-        <v>YQNK11203H99BP</v>
+        <v>ALHG997823U62SK</v>
       </c>
       <c r="K2" s="14" t="str">
         <f ca="1">"07"&amp;J2</f>
-        <v>07YQNK11203H99BP</v>
+        <v>07ALHG997823U62SK</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="6" t="str">
         <f t="shared" ref="A3:A65" ca="1" si="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,9999999)&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>UF2533785V</v>
+        <v>QZ9330601M</v>
       </c>
       <c r="B3" t="s">
         <v>1524</v>
@@ -21410,13 +21376,13 @@
       </c>
       <c r="I3" t="str">
         <f t="shared" ref="I3:I66" ca="1" si="2">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,999999)&amp;CHAR(RANDBETWEEN(65,90))&amp;(RANDBETWEEN(1,99))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>BZSPN464768P77PA</v>
+        <v>YJZPI871463T45DX</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>QG6279058O</v>
+        <v>PK9917511J</v>
       </c>
       <c r="B4" t="s">
         <v>1525</v>
@@ -21426,13 +21392,13 @@
       </c>
       <c r="I4" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>TKZAC264584G56XG</v>
+        <v>CJBHZ473042L97CU</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>XW8944605O</v>
+        <v>DH5879808J</v>
       </c>
       <c r="B5" t="s">
         <v>1526</v>
@@ -21442,13 +21408,13 @@
       </c>
       <c r="I5" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>WSCNK867156U68JW</v>
+        <v>PUUHG703979U54UA</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>ZM8307547B</v>
+        <v>VN28632X</v>
       </c>
       <c r="B6" t="s">
         <v>1527</v>
@@ -21458,13 +21424,13 @@
       </c>
       <c r="I6" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>JQUYM666141I75NA</v>
+        <v>VGBLY941464L43CE</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>PP4857669A</v>
+        <v>KK2984910G</v>
       </c>
       <c r="B7" t="s">
         <v>1528</v>
@@ -21474,13 +21440,13 @@
       </c>
       <c r="I7" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>SVCAY782156L99IT</v>
+        <v>RQQBS90654I2FY</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>MR4514456Y</v>
+        <v>CI2390684E</v>
       </c>
       <c r="B8" t="s">
         <v>1529</v>
@@ -21490,13 +21456,13 @@
       </c>
       <c r="I8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>IJCZU449224N45WQ</v>
+        <v>NJWUH941885Q85FO</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>CS1869042G</v>
+        <v>EY4363671D</v>
       </c>
       <c r="B9" t="s">
         <v>1530</v>
@@ -21506,13 +21472,13 @@
       </c>
       <c r="I9" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>BJZHL953537N12UL</v>
+        <v>MLJGY993828B65ZO</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>AH3735364Z</v>
+        <v>YW7147604K</v>
       </c>
       <c r="B10" t="s">
         <v>1531</v>
@@ -21522,13 +21488,13 @@
       </c>
       <c r="I10" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>XVNUF7628F23FD</v>
+        <v>MAIFZ167810D91WK</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LA4212099O</v>
+        <v>MC3656992W</v>
       </c>
       <c r="B11" t="s">
         <v>1532</v>
@@ -21538,13 +21504,13 @@
       </c>
       <c r="I11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>JVKQV450843X26PG</v>
+        <v>YLVKB30950M8XU</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>JX864281N</v>
+        <v>IW7408411X</v>
       </c>
       <c r="B12" t="s">
         <v>1533</v>
@@ -21554,13 +21520,13 @@
       </c>
       <c r="I12" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CKRYX654161M52EM</v>
+        <v>DVECK539122R88ZD</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NN7874565X</v>
+        <v>NY6798926A</v>
       </c>
       <c r="B13" t="s">
         <v>1534</v>
@@ -21570,13 +21536,13 @@
       </c>
       <c r="I13" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>VGDQI943359Q73GD</v>
+        <v>BDBZI56633X58WT</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NC620226F</v>
+        <v>SM3265202I</v>
       </c>
       <c r="B14" t="s">
         <v>1535</v>
@@ -21586,13 +21552,13 @@
       </c>
       <c r="I14" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>TWWFL786438W22WV</v>
+        <v>WWBID475774K98LP</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>DY6919584F</v>
+        <v>VB5178898E</v>
       </c>
       <c r="B15" t="s">
         <v>1536</v>
@@ -21602,13 +21568,13 @@
       </c>
       <c r="I15" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>AHXON544832G32TR</v>
+        <v>ZMOEK833855K42GD</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>AV2382963T</v>
+        <v>OQ5804775Z</v>
       </c>
       <c r="B16" t="s">
         <v>1537</v>
@@ -21618,13 +21584,13 @@
       </c>
       <c r="I16" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>OWESA19366P41NJ</v>
+        <v>PJQQX723839J78XR</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UR6900927B</v>
+        <v>JF3649740Q</v>
       </c>
       <c r="B17" t="s">
         <v>1538</v>
@@ -21634,13 +21600,13 @@
       </c>
       <c r="I17" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>EHOXP452777F2IN</v>
+        <v>EMJIE968440F45YE</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>CW2150816R</v>
+        <v>TS451487X</v>
       </c>
       <c r="B18" t="s">
         <v>1539</v>
@@ -21650,13 +21616,13 @@
       </c>
       <c r="I18" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>TIKAN562249N97CX</v>
+        <v>OZTJH996757U88OC</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>HK5187584T</v>
+        <v>RM5177643J</v>
       </c>
       <c r="B19" t="s">
         <v>1540</v>
@@ -21666,13 +21632,13 @@
       </c>
       <c r="I19" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>HIUMX7579M76WN</v>
+        <v>YMOIS11546H18TX</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>TW9137332O</v>
+        <v>QE6998093I</v>
       </c>
       <c r="B20" t="s">
         <v>1541</v>
@@ -21682,13 +21648,13 @@
       </c>
       <c r="I20" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>MWDNN101702V44TT</v>
+        <v>XNENE640338N22PX</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>GB9306411L</v>
+        <v>YT6288565B</v>
       </c>
       <c r="B21" t="s">
         <v>1542</v>
@@ -21698,13 +21664,13 @@
       </c>
       <c r="I21" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>MCPNA622483M15AG</v>
+        <v>XHACT538297W18PG</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>OC9893893O</v>
+        <v>KO2343712O</v>
       </c>
       <c r="B22" t="s">
         <v>1543</v>
@@ -21714,13 +21680,13 @@
       </c>
       <c r="I22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>VQDJV704932Y20LT</v>
+        <v>OAHSY565822F32XG</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>TB753947K</v>
+        <v>KV3987634R</v>
       </c>
       <c r="B23" t="s">
         <v>1544</v>
@@ -21730,13 +21696,13 @@
       </c>
       <c r="I23" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KLZKC810865G71GT</v>
+        <v>VVSBO886456K39DZ</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NO4130515H</v>
+        <v>BY7295099E</v>
       </c>
       <c r="B24" t="s">
         <v>1545</v>
@@ -21746,13 +21712,13 @@
       </c>
       <c r="I24" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>ZDLVO685085Z49MT</v>
+        <v>KIQIX861527I1SO</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>DR362951X</v>
+        <v>MX7157284S</v>
       </c>
       <c r="B25" t="s">
         <v>1546</v>
@@ -21762,13 +21728,13 @@
       </c>
       <c r="I25" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>LJEMY270947P61LU</v>
+        <v>OIPLS312599X8DW</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>MC7652872D</v>
+        <v>JJ5047404H</v>
       </c>
       <c r="B26" t="s">
         <v>1547</v>
@@ -21778,13 +21744,13 @@
       </c>
       <c r="I26" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>ITNBV644034T26SP</v>
+        <v>LKNIG924428N96OW</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UJ1507751O</v>
+        <v>MK2163944X</v>
       </c>
       <c r="B27" t="s">
         <v>1548</v>
@@ -21794,13 +21760,13 @@
       </c>
       <c r="I27" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>YBNSA861473K15LU</v>
+        <v>TFBJG332448O56BE</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>DJ437162B</v>
+        <v>ZO9275218X</v>
       </c>
       <c r="B28" t="s">
         <v>1549</v>
@@ -21810,13 +21776,13 @@
       </c>
       <c r="I28" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>IQUVU477713B38NO</v>
+        <v>BGWXI518062P61NB</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>MA3509887D</v>
+        <v>KD8264652O</v>
       </c>
       <c r="B29" t="s">
         <v>1550</v>
@@ -21826,13 +21792,13 @@
       </c>
       <c r="I29" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>ZTYJE142103J10XC</v>
+        <v>EKXBH904649A91PI</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>OK8265838S</v>
+        <v>AJ8612651Y</v>
       </c>
       <c r="B30" t="s">
         <v>1551</v>
@@ -21842,13 +21808,13 @@
       </c>
       <c r="I30" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>MLGGZ617866G64PQ</v>
+        <v>QOAXR497558C43AK</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>WB9791713F</v>
+        <v>HL7524326L</v>
       </c>
       <c r="B31" t="s">
         <v>1552</v>
@@ -21858,13 +21824,13 @@
       </c>
       <c r="I31" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>BVSVN834383N70UT</v>
+        <v>UWQIY922937P33XM</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>CX1653947D</v>
+        <v>LX5023242I</v>
       </c>
       <c r="B32" t="s">
         <v>1553</v>
@@ -21874,13 +21840,13 @@
       </c>
       <c r="I32" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>WVYGN912128E27GI</v>
+        <v>NUIOE466474N55KW</v>
       </c>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>ZV6386453E</v>
+        <v>RA9215130R</v>
       </c>
       <c r="B33" t="s">
         <v>1554</v>
@@ -21890,13 +21856,13 @@
       </c>
       <c r="I33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>VTUNO503953D9ML</v>
+        <v>DZCUZ510086Y57AH</v>
       </c>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>MR5200927Y</v>
+        <v>NX9448852G</v>
       </c>
       <c r="B34" t="s">
         <v>1555</v>
@@ -21906,13 +21872,13 @@
       </c>
       <c r="I34" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>GWMCQ681663Y34NT</v>
+        <v>PBHSF198333V41RY</v>
       </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LU5493349P</v>
+        <v>BE9241628R</v>
       </c>
       <c r="B35" t="s">
         <v>1556</v>
@@ -21922,13 +21888,13 @@
       </c>
       <c r="I35" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>HMXNW859330U73LZ</v>
+        <v>APAEN749383J85XA</v>
       </c>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>XI9800038A</v>
+        <v>GK3488072X</v>
       </c>
       <c r="B36" t="s">
         <v>1557</v>
@@ -21938,13 +21904,13 @@
       </c>
       <c r="I36" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>FUROF545613C18AE</v>
+        <v>RHBEY287582L87PV</v>
       </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>DU1799609E</v>
+        <v>WE944582M</v>
       </c>
       <c r="B37" t="s">
         <v>1558</v>
@@ -21954,13 +21920,13 @@
       </c>
       <c r="I37" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>XRJWT991320C5ZT</v>
+        <v>GJFAC660641X98GA</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>VU3335567C</v>
+        <v>VV6706922A</v>
       </c>
       <c r="B38" t="s">
         <v>1559</v>
@@ -21970,13 +21936,13 @@
       </c>
       <c r="I38" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>BZITO915768V16UU</v>
+        <v>WEOIS827866H75SH</v>
       </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>VA2398990T</v>
+        <v>HA5136636C</v>
       </c>
       <c r="B39" t="s">
         <v>1560</v>
@@ -21986,13 +21952,13 @@
       </c>
       <c r="I39" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>RDEFP755125F10GA</v>
+        <v>CRYOO247791K39XH</v>
       </c>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>VW9503188B</v>
+        <v>MQ4289094X</v>
       </c>
       <c r="B40" t="s">
         <v>1561</v>
@@ -22002,13 +21968,13 @@
       </c>
       <c r="I40" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>BHMEG695047N46NT</v>
+        <v>HTIJH116068M18MF</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>VB9213431R</v>
+        <v>GE7065154E</v>
       </c>
       <c r="B41" t="s">
         <v>1562</v>
@@ -22018,13 +21984,13 @@
       </c>
       <c r="I41" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NIYUO452450P75FF</v>
+        <v>TCWSU192424S8GJ</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>PV1737273V</v>
+        <v>VM2571043T</v>
       </c>
       <c r="B42" t="s">
         <v>1563</v>
@@ -22034,13 +22000,13 @@
       </c>
       <c r="I42" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NEGYM1870T74SH</v>
+        <v>WOTIX590389H70EL</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>KR7481577E</v>
+        <v>ZQ6650199H</v>
       </c>
       <c r="B43" t="s">
         <v>1564</v>
@@ -22050,13 +22016,13 @@
       </c>
       <c r="I43" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CXFZU337280Y3UF</v>
+        <v>BGLXJ869530O27VG</v>
       </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>IT8582806D</v>
+        <v>FH2592815Z</v>
       </c>
       <c r="B44" t="s">
         <v>1565</v>
@@ -22066,13 +22032,13 @@
       </c>
       <c r="I44" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>PFSUZ906303Q54LS</v>
+        <v>PSALU493775Q23SP</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>EW1914428T</v>
+        <v>ZZ8836434U</v>
       </c>
       <c r="B45" t="s">
         <v>1566</v>
@@ -22082,13 +22048,13 @@
       </c>
       <c r="I45" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>AAHDA57091H97WI</v>
+        <v>HZYPD594142T89VB</v>
       </c>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>GH1524616U</v>
+        <v>JC9078853H</v>
       </c>
       <c r="B46" t="s">
         <v>1567</v>
@@ -22098,13 +22064,13 @@
       </c>
       <c r="I46" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>XBEFR408664C19PO</v>
+        <v>YXWAE350864U92CD</v>
       </c>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>YB6852606D</v>
+        <v>WP5513612J</v>
       </c>
       <c r="B47" t="s">
         <v>1568</v>
@@ -22114,13 +22080,13 @@
       </c>
       <c r="I47" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>ALISQ54786N70OJ</v>
+        <v>UFUGM359751G32ZN</v>
       </c>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UZ1334481N</v>
+        <v>EZ1948318D</v>
       </c>
       <c r="B48" t="s">
         <v>1569</v>
@@ -22130,13 +22096,13 @@
       </c>
       <c r="I48" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KPOMZ938670O28ZK</v>
+        <v>UZTLK641981X15MS</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>WG6158242W</v>
+        <v>CY4614912B</v>
       </c>
       <c r="B49" t="s">
         <v>1570</v>
@@ -22146,13 +22112,13 @@
       </c>
       <c r="I49" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>UMDYM151106D51BH</v>
+        <v>HXXOO360396V76QR</v>
       </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>YI4087248I</v>
+        <v>UJ8847625J</v>
       </c>
       <c r="B50" t="s">
         <v>1571</v>
@@ -22162,13 +22128,13 @@
       </c>
       <c r="I50" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>SJUCQ402905S76UB</v>
+        <v>EKSPN328182A12DV</v>
       </c>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LC6791680R</v>
+        <v>ZH7791032A</v>
       </c>
       <c r="B51" t="s">
         <v>1572</v>
@@ -22178,13 +22144,13 @@
       </c>
       <c r="I51" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>VUXNK548987A80EU</v>
+        <v>HSBAC330635P88PS</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>PI6040581U</v>
+        <v>MA6784384U</v>
       </c>
       <c r="B52" t="s">
         <v>1573</v>
@@ -22194,13 +22160,13 @@
       </c>
       <c r="I52" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>OZJJC423482W20IJ</v>
+        <v>PYUPC192393G76PI</v>
       </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LL6433206R</v>
+        <v>AJ3605760Y</v>
       </c>
       <c r="B53" t="s">
         <v>1574</v>
@@ -22210,13 +22176,13 @@
       </c>
       <c r="I53" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>HPGUR699523G98QG</v>
+        <v>GRUIW433259Z14RU</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UX6794401J</v>
+        <v>FS7576437K</v>
       </c>
       <c r="B54" t="s">
         <v>1575</v>
@@ -22226,13 +22192,13 @@
       </c>
       <c r="I54" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>DREQP743503E47MU</v>
+        <v>RPPZZ407464S20JB</v>
       </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>IS7967714Y</v>
+        <v>KZ709999M</v>
       </c>
       <c r="B55" t="s">
         <v>1576</v>
@@ -22242,13 +22208,13 @@
       </c>
       <c r="I55" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>UNQEL213420M95ZT</v>
+        <v>KSIHM986529X44ZD</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>GD7584987W</v>
+        <v>SD5864345L</v>
       </c>
       <c r="B56" t="s">
         <v>1577</v>
@@ -22258,13 +22224,13 @@
       </c>
       <c r="I56" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>VNDIG882886K29YD</v>
+        <v>KTJVK310551A56WP</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>HM4977169P</v>
+        <v>SH8169687P</v>
       </c>
       <c r="B57" t="s">
         <v>1578</v>
@@ -22274,13 +22240,13 @@
       </c>
       <c r="I57" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>ZXXCL78961F22KG</v>
+        <v>RQXGS224716Q27LY</v>
       </c>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>SB7034991N</v>
+        <v>HZ1931944H</v>
       </c>
       <c r="B58" t="s">
         <v>1579</v>
@@ -22290,13 +22256,13 @@
       </c>
       <c r="I58" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>FEHFI92937C60LP</v>
+        <v>UIKDP244422P80KT</v>
       </c>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>VG8819056X</v>
+        <v>BB8748967R</v>
       </c>
       <c r="B59" t="s">
         <v>1580</v>
@@ -22306,13 +22272,13 @@
       </c>
       <c r="I59" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>LUBAM469466X87TF</v>
+        <v>SMVQW526356I35SM</v>
       </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>PU8434443M</v>
+        <v>QG5387601I</v>
       </c>
       <c r="B60" t="s">
         <v>1581</v>
@@ -22322,13 +22288,13 @@
       </c>
       <c r="I60" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>HDQGJ117375K34RV</v>
+        <v>LIPDX541266Y58DS</v>
       </c>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>SU3402706Y</v>
+        <v>OH7456682S</v>
       </c>
       <c r="B61" t="s">
         <v>1582</v>
@@ -22338,13 +22304,13 @@
       </c>
       <c r="I61" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>XBMXH969558D19LR</v>
+        <v>XLVNR473981B87TI</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UA1797965O</v>
+        <v>PG4501625K</v>
       </c>
       <c r="B62" t="s">
         <v>1583</v>
@@ -22354,13 +22320,13 @@
       </c>
       <c r="I62" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>ISGWW321663B88QN</v>
+        <v>DCILC177644J65MN</v>
       </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>HL5357154I</v>
+        <v>XD4739960F</v>
       </c>
       <c r="B63" t="s">
         <v>1584</v>
@@ -22370,13 +22336,13 @@
       </c>
       <c r="I63" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>TONNB419524H79VB</v>
+        <v>BPUYS154879U74GD</v>
       </c>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>JP7626268T</v>
+        <v>UE5297000L</v>
       </c>
       <c r="B64" t="s">
         <v>1585</v>
@@ -22386,13 +22352,13 @@
       </c>
       <c r="I64" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>MKWNN289721D67XZ</v>
+        <v>OLFFF85338F71RX</v>
       </c>
     </row>
     <row r="65" spans="1:9">
       <c r="A65" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>CP1159069P</v>
+        <v>DZ1384997W</v>
       </c>
       <c r="B65" t="s">
         <v>1586</v>
@@ -22402,13 +22368,13 @@
       </c>
       <c r="I65" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>ECOEU587441P20JJ</v>
+        <v>BCQEL746241B54XG</v>
       </c>
     </row>
     <row r="66" spans="1:9">
       <c r="A66" s="6" t="str">
         <f t="shared" ref="A66:A129" ca="1" si="3">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,9999999)&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>OF1219631C</v>
+        <v>XZ4287722N</v>
       </c>
       <c r="B66" t="s">
         <v>1587</v>
@@ -22418,13 +22384,13 @@
       </c>
       <c r="I66" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KPIZD856732U22WF</v>
+        <v>KIOWE417294T90PO</v>
       </c>
     </row>
     <row r="67" spans="1:9">
       <c r="A67" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>TN9121967E</v>
+        <v>UL4619708L</v>
       </c>
       <c r="B67" t="s">
         <v>1588</v>
@@ -22434,13 +22400,13 @@
       </c>
       <c r="I67" t="str">
         <f t="shared" ref="I67:I130" ca="1" si="4">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,999999)&amp;CHAR(RANDBETWEEN(65,90))&amp;(RANDBETWEEN(1,99))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>RBJIW757214D34WN</v>
+        <v>NKSSK323802X23NB</v>
       </c>
     </row>
     <row r="68" spans="1:9">
       <c r="A68" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>EU2420918V</v>
+        <v>QX5767432T</v>
       </c>
       <c r="B68" t="s">
         <v>1589</v>
@@ -22450,13 +22416,13 @@
       </c>
       <c r="I68" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>MMAJH932271Q36PY</v>
+        <v>ATDRJ978028P8SI</v>
       </c>
     </row>
     <row r="69" spans="1:9">
       <c r="A69" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>KU104062K</v>
+        <v>RI5474709K</v>
       </c>
       <c r="B69" t="s">
         <v>1590</v>
@@ -22466,13 +22432,13 @@
       </c>
       <c r="I69" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>WZWLQ938881M68BJ</v>
+        <v>BNNNN930633V91HE</v>
       </c>
     </row>
     <row r="70" spans="1:9">
       <c r="A70" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>OI9406854U</v>
+        <v>AH2569776S</v>
       </c>
       <c r="B70" t="s">
         <v>1591</v>
@@ -22482,13 +22448,13 @@
       </c>
       <c r="I70" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>SHDKM802803A87SK</v>
+        <v>ASIOK433282D8YT</v>
       </c>
     </row>
     <row r="71" spans="1:9">
       <c r="A71" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>QY9253318Z</v>
+        <v>EH9480006Y</v>
       </c>
       <c r="B71" t="s">
         <v>1592</v>
@@ -22498,13 +22464,13 @@
       </c>
       <c r="I71" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>BYUWC83147K96HJ</v>
+        <v>ZKOEN331485E20HZ</v>
       </c>
     </row>
     <row r="72" spans="1:9">
       <c r="A72" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>BY5202359T</v>
+        <v>JT667103N</v>
       </c>
       <c r="B72" t="s">
         <v>1593</v>
@@ -22514,13 +22480,13 @@
       </c>
       <c r="I72" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>CDYUD392677D61UT</v>
+        <v>FJNCG349388E74MJ</v>
       </c>
     </row>
     <row r="73" spans="1:9">
       <c r="A73" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>PV7733739Q</v>
+        <v>JM1280292J</v>
       </c>
       <c r="B73" t="s">
         <v>1594</v>
@@ -22530,13 +22496,13 @@
       </c>
       <c r="I73" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>ZWAZI604466D13WX</v>
+        <v>QJABH142945F18XA</v>
       </c>
     </row>
     <row r="74" spans="1:9">
       <c r="A74" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>TU6848999U</v>
+        <v>SM8576515T</v>
       </c>
       <c r="B74" t="s">
         <v>1595</v>
@@ -22546,13 +22512,13 @@
       </c>
       <c r="I74" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>YMAEY379670R9DN</v>
+        <v>XPEVG780030W76FP</v>
       </c>
     </row>
     <row r="75" spans="1:9">
       <c r="A75" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UJ1870987B</v>
+        <v>BI7406434J</v>
       </c>
       <c r="B75" t="s">
         <v>1596</v>
@@ -22562,13 +22528,13 @@
       </c>
       <c r="I75" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>ZJBRU580826T89CD</v>
+        <v>IGPDG184006J81CB</v>
       </c>
     </row>
     <row r="76" spans="1:9">
       <c r="A76" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>ZC6778428K</v>
+        <v>EG8617475P</v>
       </c>
       <c r="B76" t="s">
         <v>1597</v>
@@ -22578,13 +22544,13 @@
       </c>
       <c r="I76" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>NOBBJ278695V42CJ</v>
+        <v>XKSAM581734V84WV</v>
       </c>
     </row>
     <row r="77" spans="1:9">
       <c r="A77" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>RR3392340J</v>
+        <v>OT2522628K</v>
       </c>
       <c r="B77" t="s">
         <v>1598</v>
@@ -22594,13 +22560,13 @@
       </c>
       <c r="I77" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>LNQRC35941A81VM</v>
+        <v>SEKAH715838I87FA</v>
       </c>
     </row>
     <row r="78" spans="1:9">
       <c r="A78" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>OL1842742E</v>
+        <v>HG9774684C</v>
       </c>
       <c r="B78" t="s">
         <v>1599</v>
@@ -22610,13 +22576,13 @@
       </c>
       <c r="I78" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>ZRXHF674172R44LI</v>
+        <v>SFDCJ917779F52XY</v>
       </c>
     </row>
     <row r="79" spans="1:9">
       <c r="A79" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>EF6663296D</v>
+        <v>RB8720299M</v>
       </c>
       <c r="B79" t="s">
         <v>1600</v>
@@ -22626,13 +22592,13 @@
       </c>
       <c r="I79" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>ZDSGH854337C22JL</v>
+        <v>LKLWE364256O15WS</v>
       </c>
     </row>
     <row r="80" spans="1:9">
       <c r="A80" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>RR7868120S</v>
+        <v>RX5203455M</v>
       </c>
       <c r="B80" t="s">
         <v>1601</v>
@@ -22642,13 +22608,13 @@
       </c>
       <c r="I80" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>EWZHE522553I55DQ</v>
+        <v>EEXSW559885T62US</v>
       </c>
     </row>
     <row r="81" spans="1:9">
       <c r="A81" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>AD4135701L</v>
+        <v>SW8133516O</v>
       </c>
       <c r="B81" t="s">
         <v>1602</v>
@@ -22658,13 +22624,13 @@
       </c>
       <c r="I81" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>YSZGC876311H99OJ</v>
+        <v>JAMGC885678E36TH</v>
       </c>
     </row>
     <row r="82" spans="1:9">
       <c r="A82" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>BB2183764C</v>
+        <v>AD1749544Q</v>
       </c>
       <c r="B82" t="s">
         <v>1603</v>
@@ -22674,13 +22640,13 @@
       </c>
       <c r="I82" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>SYWUH501927O86HE</v>
+        <v>TNXWK326500I48NG</v>
       </c>
     </row>
     <row r="83" spans="1:9">
       <c r="A83" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>AL8298502Q</v>
+        <v>HZ8092699C</v>
       </c>
       <c r="B83" t="s">
         <v>1604</v>
@@ -22690,13 +22656,13 @@
       </c>
       <c r="I83" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>NEOHB686056E88CR</v>
+        <v>RHZCU462975I68AZ</v>
       </c>
     </row>
     <row r="84" spans="1:9">
       <c r="A84" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>LO1393684F</v>
+        <v>XJ186576N</v>
       </c>
       <c r="B84" t="s">
         <v>1605</v>
@@ -22706,13 +22672,13 @@
       </c>
       <c r="I84" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>BDYWG840637V16IX</v>
+        <v>UDAOU267171C85FA</v>
       </c>
     </row>
     <row r="85" spans="1:9">
       <c r="A85" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>KL9240811H</v>
+        <v>PU5289716V</v>
       </c>
       <c r="B85" t="s">
         <v>1606</v>
@@ -22722,13 +22688,13 @@
       </c>
       <c r="I85" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>ZYCSO770723D2QZ</v>
+        <v>UIZKX68147E20VK</v>
       </c>
     </row>
     <row r="86" spans="1:9">
       <c r="A86" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>OL9409020S</v>
+        <v>CP6133655M</v>
       </c>
       <c r="B86" t="s">
         <v>1607</v>
@@ -22738,13 +22704,13 @@
       </c>
       <c r="I86" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>IIDVC610346T78QS</v>
+        <v>YEHNJ804611Z66XI</v>
       </c>
     </row>
     <row r="87" spans="1:9">
       <c r="A87" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>FC7391869S</v>
+        <v>EW2579092F</v>
       </c>
       <c r="B87" t="s">
         <v>1608</v>
@@ -22754,13 +22720,13 @@
       </c>
       <c r="I87" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>QJZYW649361X48BW</v>
+        <v>MJNMW79878A79AJ</v>
       </c>
     </row>
     <row r="88" spans="1:9">
       <c r="A88" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UG4249343K</v>
+        <v>LF8318461Z</v>
       </c>
       <c r="B88" t="s">
         <v>1609</v>
@@ -22770,13 +22736,13 @@
       </c>
       <c r="I88" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>YBMFB6977E43SB</v>
+        <v>YVPBA606806G44DA</v>
       </c>
     </row>
     <row r="89" spans="1:9">
       <c r="A89" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>EE9071757P</v>
+        <v>YZ98673I</v>
       </c>
       <c r="B89" t="s">
         <v>1610</v>
@@ -22786,13 +22752,13 @@
       </c>
       <c r="I89" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>TPMQB534563K64CL</v>
+        <v>YKDWU618821F7ZR</v>
       </c>
     </row>
     <row r="90" spans="1:9">
       <c r="A90" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>CH7018371Q</v>
+        <v>DQ9924579M</v>
       </c>
       <c r="B90" t="s">
         <v>1611</v>
@@ -22802,13 +22768,13 @@
       </c>
       <c r="I90" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>WKNBI545319U72LZ</v>
+        <v>OZGSA98255W43SU</v>
       </c>
     </row>
     <row r="91" spans="1:9">
       <c r="A91" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>AE5839222W</v>
+        <v>SC3428636V</v>
       </c>
       <c r="B91" t="s">
         <v>1612</v>
@@ -22818,13 +22784,13 @@
       </c>
       <c r="I91" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>RFBZB274991O60GU</v>
+        <v>BAUGI839793Z29GN</v>
       </c>
     </row>
     <row r="92" spans="1:9">
       <c r="A92" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>PV8032849F</v>
+        <v>UQ4666086I</v>
       </c>
       <c r="B92" t="s">
         <v>1613</v>
@@ -22834,13 +22800,13 @@
       </c>
       <c r="I92" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>WYSHB917842V45FX</v>
+        <v>DTGGS419416W13KM</v>
       </c>
     </row>
     <row r="93" spans="1:9">
       <c r="A93" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>AH8794956N</v>
+        <v>BI5677220N</v>
       </c>
       <c r="B93" t="s">
         <v>1614</v>
@@ -22850,13 +22816,13 @@
       </c>
       <c r="I93" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>RJUID529201F68VS</v>
+        <v>YKINV41800K42KQ</v>
       </c>
     </row>
     <row r="94" spans="1:9">
       <c r="A94" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>FO5676112B</v>
+        <v>EK4090469M</v>
       </c>
       <c r="B94" t="s">
         <v>1615</v>
@@ -22866,13 +22832,13 @@
       </c>
       <c r="I94" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>RIFTY840534Z17CM</v>
+        <v>RCZLE189907R70GK</v>
       </c>
     </row>
     <row r="95" spans="1:9">
       <c r="A95" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>VM9886149S</v>
+        <v>IE7964435L</v>
       </c>
       <c r="B95" t="s">
         <v>1616</v>
@@ -22882,13 +22848,13 @@
       </c>
       <c r="I95" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>THIDH199059K72NY</v>
+        <v>ZJYLO47668O38QP</v>
       </c>
     </row>
     <row r="96" spans="1:9">
       <c r="A96" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>BX7447923M</v>
+        <v>HS8706419I</v>
       </c>
       <c r="B96" t="s">
         <v>1617</v>
@@ -22898,13 +22864,13 @@
       </c>
       <c r="I96" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>ZLCLK493628J91AQ</v>
+        <v>FNYWL755985B48GO</v>
       </c>
     </row>
     <row r="97" spans="1:9">
       <c r="A97" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>ME5818754M</v>
+        <v>GM485426X</v>
       </c>
       <c r="B97" t="s">
         <v>1618</v>
@@ -22914,13 +22880,13 @@
       </c>
       <c r="I97" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>CVRJS654643F93IN</v>
+        <v>BODFK647763E26QF</v>
       </c>
     </row>
     <row r="98" spans="1:9">
       <c r="A98" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>VM8152455R</v>
+        <v>JR6780242T</v>
       </c>
       <c r="B98" t="s">
         <v>1619</v>
@@ -22930,13 +22896,13 @@
       </c>
       <c r="I98" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>IQKNY606015Z47GI</v>
+        <v>EOEJG511144U28IN</v>
       </c>
     </row>
     <row r="99" spans="1:9">
       <c r="A99" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>TM600623P</v>
+        <v>IW9339829T</v>
       </c>
       <c r="B99" t="s">
         <v>1620</v>
@@ -22946,13 +22912,13 @@
       </c>
       <c r="I99" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>GAPOB447938M8WM</v>
+        <v>BTTYB337882J7WD</v>
       </c>
     </row>
     <row r="100" spans="1:9">
       <c r="A100" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>GE1529254Z</v>
+        <v>HB9065578K</v>
       </c>
       <c r="B100" t="s">
         <v>1621</v>
@@ -22962,13 +22928,13 @@
       </c>
       <c r="I100" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>GGGYF317042C42BT</v>
+        <v>VRWZQ965534S10QN</v>
       </c>
     </row>
     <row r="101" spans="1:9">
       <c r="A101" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>JL6666081K</v>
+        <v>DY1104571I</v>
       </c>
       <c r="B101" t="s">
         <v>1622</v>
@@ -22978,13 +22944,13 @@
       </c>
       <c r="I101" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>XQIMK270428Y3ND</v>
+        <v>GZGPX880757E3WE</v>
       </c>
     </row>
     <row r="102" spans="1:9">
       <c r="A102" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>TL3912849M</v>
+        <v>QA1955427I</v>
       </c>
       <c r="B102" t="s">
         <v>1623</v>
@@ -22994,13 +22960,13 @@
       </c>
       <c r="I102" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>VWEUS724642R24KR</v>
+        <v>JYKEK359992Y11AB</v>
       </c>
     </row>
     <row r="103" spans="1:9">
       <c r="A103" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UW6650342O</v>
+        <v>UO6037072S</v>
       </c>
       <c r="B103" t="s">
         <v>1624</v>
@@ -23010,13 +22976,13 @@
       </c>
       <c r="I103" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>CKXGI404124U90CY</v>
+        <v>KJVYQ830527U34ON</v>
       </c>
     </row>
     <row r="104" spans="1:9">
       <c r="A104" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>KY292046F</v>
+        <v>GU7696587R</v>
       </c>
       <c r="B104" t="s">
         <v>1625</v>
@@ -23026,13 +22992,13 @@
       </c>
       <c r="I104" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>SGQAF949683R73VS</v>
+        <v>XVCFH632502G56UD</v>
       </c>
     </row>
     <row r="105" spans="1:9">
       <c r="A105" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>SR2011213X</v>
+        <v>VW3504231C</v>
       </c>
       <c r="B105" t="s">
         <v>1626</v>
@@ -23042,13 +23008,13 @@
       </c>
       <c r="I105" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>VWLHS370090I66RA</v>
+        <v>FZNAJ195873V8NZ</v>
       </c>
     </row>
     <row r="106" spans="1:9">
       <c r="A106" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>LE6949894A</v>
+        <v>AU1413606F</v>
       </c>
       <c r="B106" t="s">
         <v>1627</v>
@@ -23058,13 +23024,13 @@
       </c>
       <c r="I106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>DZNOL532385Y71WI</v>
+        <v>HSRUV486098T47RC</v>
       </c>
     </row>
     <row r="107" spans="1:9">
       <c r="A107" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>CG1277300Z</v>
+        <v>NE178347U</v>
       </c>
       <c r="B107" t="s">
         <v>1628</v>
@@ -23074,13 +23040,13 @@
       </c>
       <c r="I107" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>IFCFJ339975V91DD</v>
+        <v>QKATG106263Y23XG</v>
       </c>
     </row>
     <row r="108" spans="1:9">
       <c r="A108" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>RC3721820A</v>
+        <v>MH5822034R</v>
       </c>
       <c r="B108" t="s">
         <v>1629</v>
@@ -23090,13 +23056,13 @@
       </c>
       <c r="I108" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>VDOCH208242Z17SU</v>
+        <v>IWDIC677810P96CF</v>
       </c>
     </row>
     <row r="109" spans="1:9">
       <c r="A109" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>FN2249823Y</v>
+        <v>AF5879893H</v>
       </c>
       <c r="B109" t="s">
         <v>1630</v>
@@ -23106,13 +23072,13 @@
       </c>
       <c r="I109" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>FCZNK305596E27HV</v>
+        <v>FIAQW988403A79GY</v>
       </c>
     </row>
     <row r="110" spans="1:9">
       <c r="A110" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>PK3937274M</v>
+        <v>LA9519281J</v>
       </c>
       <c r="B110" t="s">
         <v>1631</v>
@@ -23122,13 +23088,13 @@
       </c>
       <c r="I110" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>BJHWE543626U39JJ</v>
+        <v>WOXXO992257G11PA</v>
       </c>
     </row>
     <row r="111" spans="1:9">
       <c r="A111" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>KU8936706A</v>
+        <v>HC6104155M</v>
       </c>
       <c r="B111" t="s">
         <v>1632</v>
@@ -23138,13 +23104,13 @@
       </c>
       <c r="I111" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>FBUBN282761J96TG</v>
+        <v>DZUKF495188X29NM</v>
       </c>
     </row>
     <row r="112" spans="1:9">
       <c r="A112" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>WD3979093M</v>
+        <v>MQ6165629F</v>
       </c>
       <c r="B112" t="s">
         <v>1633</v>
@@ -23154,13 +23120,13 @@
       </c>
       <c r="I112" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>PJOLF764402S77UE</v>
+        <v>TVZJG452371L19PN</v>
       </c>
     </row>
     <row r="113" spans="1:9">
       <c r="A113" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>MY2937537B</v>
+        <v>MP657963M</v>
       </c>
       <c r="B113" t="s">
         <v>1634</v>
@@ -23170,13 +23136,13 @@
       </c>
       <c r="I113" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>RWVOD701649Z53WT</v>
+        <v>EQOZH905598H77AU</v>
       </c>
     </row>
     <row r="114" spans="1:9">
       <c r="A114" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>JT3964899O</v>
+        <v>PN9862455M</v>
       </c>
       <c r="B114" t="s">
         <v>1635</v>
@@ -23186,13 +23152,13 @@
       </c>
       <c r="I114" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>SUZET351700R64JJ</v>
+        <v>YOQYG586930R2YQ</v>
       </c>
     </row>
     <row r="115" spans="1:9">
       <c r="A115" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>OJ7291655M</v>
+        <v>JZ3388884N</v>
       </c>
       <c r="B115" t="s">
         <v>1636</v>
@@ -23202,13 +23168,13 @@
       </c>
       <c r="I115" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>NFONF576625T99QD</v>
+        <v>ABXKA790875I62SO</v>
       </c>
     </row>
     <row r="116" spans="1:9">
       <c r="A116" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>DV6684667G</v>
+        <v>TM3545372Z</v>
       </c>
       <c r="B116" t="s">
         <v>1637</v>
@@ -23218,13 +23184,13 @@
       </c>
       <c r="I116" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>BEOCU514770R67RK</v>
+        <v>FIVMH516113R22DU</v>
       </c>
     </row>
     <row r="117" spans="1:9">
       <c r="A117" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>BE7059240E</v>
+        <v>WR3008210W</v>
       </c>
       <c r="B117" t="s">
         <v>1638</v>
@@ -23234,13 +23200,13 @@
       </c>
       <c r="I117" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>HMKMR967276O60RG</v>
+        <v>OCLEM860001I8CV</v>
       </c>
     </row>
     <row r="118" spans="1:9">
       <c r="A118" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>DG6743238T</v>
+        <v>KH9164513J</v>
       </c>
       <c r="B118" t="s">
         <v>1639</v>
@@ -23250,13 +23216,13 @@
       </c>
       <c r="I118" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>QRYEH605997S94AJ</v>
+        <v>JKWCN985360W3HZ</v>
       </c>
     </row>
     <row r="119" spans="1:9">
       <c r="A119" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>IP760617M</v>
+        <v>PY4894183B</v>
       </c>
       <c r="B119" t="s">
         <v>1640</v>
@@ -23266,13 +23232,13 @@
       </c>
       <c r="I119" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>ZQVYJ258626E90US</v>
+        <v>MPQUM685597X2NM</v>
       </c>
     </row>
     <row r="120" spans="1:9">
       <c r="A120" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>IE8979985O</v>
+        <v>DD8405887G</v>
       </c>
       <c r="B120" t="s">
         <v>1641</v>
@@ -23282,13 +23248,13 @@
       </c>
       <c r="I120" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>SRHAC183737J83CV</v>
+        <v>BAVHM869881C26RJ</v>
       </c>
     </row>
     <row r="121" spans="1:9">
       <c r="A121" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>SA4861024W</v>
+        <v>UL5335504M</v>
       </c>
       <c r="B121" t="s">
         <v>1642</v>
@@ -23298,13 +23264,13 @@
       </c>
       <c r="I121" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>SQJTB862542X65ZV</v>
+        <v>OIELD656629N90IF</v>
       </c>
     </row>
     <row r="122" spans="1:9">
       <c r="A122" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>ZS7930137Y</v>
+        <v>XB5588941S</v>
       </c>
       <c r="B122" t="s">
         <v>1643</v>
@@ -23314,13 +23280,13 @@
       </c>
       <c r="I122" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>IXKMM491914Q41RD</v>
+        <v>ALJAL651060D54DN</v>
       </c>
     </row>
     <row r="123" spans="1:9">
       <c r="A123" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>EN6686537Y</v>
+        <v>BG4885921E</v>
       </c>
       <c r="B123" t="s">
         <v>1644</v>
@@ -23330,13 +23296,13 @@
       </c>
       <c r="I123" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>DTYDR571879B95GG</v>
+        <v>MKKQJ419665O97QM</v>
       </c>
     </row>
     <row r="124" spans="1:9">
       <c r="A124" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UY6826419L</v>
+        <v>HN2191352E</v>
       </c>
       <c r="B124" t="s">
         <v>1645</v>
@@ -23346,13 +23312,13 @@
       </c>
       <c r="I124" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>JJETO789699X71WV</v>
+        <v>JXAXT414104M39LB</v>
       </c>
     </row>
     <row r="125" spans="1:9">
       <c r="A125" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>ZL8948740T</v>
+        <v>LB9424796J</v>
       </c>
       <c r="B125" t="s">
         <v>1646</v>
@@ -23362,13 +23328,13 @@
       </c>
       <c r="I125" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>TKTQE795675G38ZF</v>
+        <v>SISXM188568T98XL</v>
       </c>
     </row>
     <row r="126" spans="1:9">
       <c r="A126" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>WY4286682L</v>
+        <v>LP556850O</v>
       </c>
       <c r="B126" t="s">
         <v>1647</v>
@@ -23378,13 +23344,13 @@
       </c>
       <c r="I126" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>HUPJE192409U48JE</v>
+        <v>BHAIZ218648W43NY</v>
       </c>
     </row>
     <row r="127" spans="1:9">
       <c r="A127" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>HY4659014M</v>
+        <v>XB9722277D</v>
       </c>
       <c r="B127" t="s">
         <v>1648</v>
@@ -23394,13 +23360,13 @@
       </c>
       <c r="I127" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>KMBHA446723C23XB</v>
+        <v>NTVSK278667S60FF</v>
       </c>
     </row>
     <row r="128" spans="1:9">
       <c r="A128" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>XO8516249B</v>
+        <v>OZ7091514K</v>
       </c>
       <c r="B128" t="s">
         <v>1649</v>
@@ -23410,13 +23376,13 @@
       </c>
       <c r="I128" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>MDSRM970005J12WJ</v>
+        <v>RRMVN886534W61RQ</v>
       </c>
     </row>
     <row r="129" spans="1:9">
       <c r="A129" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>FK4538347H</v>
+        <v>KY8943243Y</v>
       </c>
       <c r="B129" t="s">
         <v>1650</v>
@@ -23426,13 +23392,13 @@
       </c>
       <c r="I129" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>LEDFS700615Q82IN</v>
+        <v>PUCMS109231S32CK</v>
       </c>
     </row>
     <row r="130" spans="1:9">
       <c r="A130" s="6" t="str">
         <f t="shared" ref="A130:A193" ca="1" si="5">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,9999999)&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>VT5100736Y</v>
+        <v>PX4279905C</v>
       </c>
       <c r="B130" t="s">
         <v>1651</v>
@@ -23442,13 +23408,13 @@
       </c>
       <c r="I130" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>DOGXD273766U94YU</v>
+        <v>QBDGP671763I50DN</v>
       </c>
     </row>
     <row r="131" spans="1:9">
       <c r="A131" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>KU7452062N</v>
+        <v>WA6720138F</v>
       </c>
       <c r="B131" t="s">
         <v>1652</v>
@@ -23458,13 +23424,13 @@
       </c>
       <c r="I131" t="str">
         <f t="shared" ref="I131:I194" ca="1" si="6">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,999999)&amp;CHAR(RANDBETWEEN(65,90))&amp;(RANDBETWEEN(1,99))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>FLZZT524479F18TR</v>
+        <v>EQZAQ24314P84ZE</v>
       </c>
     </row>
     <row r="132" spans="1:9">
       <c r="A132" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>GU6147391C</v>
+        <v>SZ7043986P</v>
       </c>
       <c r="B132" t="s">
         <v>1653</v>
@@ -23474,13 +23440,13 @@
       </c>
       <c r="I132" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>CPOAE211633K25KO</v>
+        <v>UTMTD665697E18NU</v>
       </c>
     </row>
     <row r="133" spans="1:9">
       <c r="A133" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>SE2130757S</v>
+        <v>RT1493870I</v>
       </c>
       <c r="B133" t="s">
         <v>1654</v>
@@ -23490,13 +23456,13 @@
       </c>
       <c r="I133" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>GNRMP825820Q32GW</v>
+        <v>DIXRQ509750S73SO</v>
       </c>
     </row>
     <row r="134" spans="1:9">
       <c r="A134" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>LT7504384H</v>
+        <v>IG5546245T</v>
       </c>
       <c r="B134" t="s">
         <v>1655</v>
@@ -23506,13 +23472,13 @@
       </c>
       <c r="I134" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>SMIOS707060K40PZ</v>
+        <v>IJVWP487629Q34VR</v>
       </c>
     </row>
     <row r="135" spans="1:9">
       <c r="A135" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>QH1742064K</v>
+        <v>EP2812346N</v>
       </c>
       <c r="B135" t="s">
         <v>1656</v>
@@ -23522,13 +23488,13 @@
       </c>
       <c r="I135" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>HTWNV602299W43FC</v>
+        <v>DGOVJ450606J91UW</v>
       </c>
     </row>
     <row r="136" spans="1:9">
       <c r="A136" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>TC6877185R</v>
+        <v>BW9458994C</v>
       </c>
       <c r="B136" t="s">
         <v>1657</v>
@@ -23538,13 +23504,13 @@
       </c>
       <c r="I136" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>TATPH279046D93JP</v>
+        <v>BSVEO166775O43JQ</v>
       </c>
     </row>
     <row r="137" spans="1:9">
       <c r="A137" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>NT7381015R</v>
+        <v>DO4391298O</v>
       </c>
       <c r="B137" t="s">
         <v>1658</v>
@@ -23554,13 +23520,13 @@
       </c>
       <c r="I137" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>GDGVD785171U59QR</v>
+        <v>LZNHE484259X52CT</v>
       </c>
     </row>
     <row r="138" spans="1:9">
       <c r="A138" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>XE2097643X</v>
+        <v>KM3414336P</v>
       </c>
       <c r="B138" t="s">
         <v>1659</v>
@@ -23570,13 +23536,13 @@
       </c>
       <c r="I138" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>ODROJ15074E20FO</v>
+        <v>LIFWK242687V69OZ</v>
       </c>
     </row>
     <row r="139" spans="1:9">
       <c r="A139" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>FB7337426I</v>
+        <v>JS1356750G</v>
       </c>
       <c r="B139" t="s">
         <v>1660</v>
@@ -23586,13 +23552,13 @@
       </c>
       <c r="I139" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>DNRGD713847G70TS</v>
+        <v>OMKWT623510J98FU</v>
       </c>
     </row>
     <row r="140" spans="1:9">
       <c r="A140" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>SX1228682J</v>
+        <v>XN6707120O</v>
       </c>
       <c r="B140" t="s">
         <v>1661</v>
@@ -23602,13 +23568,13 @@
       </c>
       <c r="I140" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>FKWLN460529W26QO</v>
+        <v>BUHNV44100P49RS</v>
       </c>
     </row>
     <row r="141" spans="1:9">
       <c r="A141" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>SI2178513T</v>
+        <v>KM5465641I</v>
       </c>
       <c r="B141" t="s">
         <v>1662</v>
@@ -23618,13 +23584,13 @@
       </c>
       <c r="I141" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>WZJUV266160W95CT</v>
+        <v>QFKQA143424R65YG</v>
       </c>
     </row>
     <row r="142" spans="1:9">
       <c r="A142" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>QT5170543J</v>
+        <v>XY4950615Y</v>
       </c>
       <c r="B142" t="s">
         <v>1663</v>
@@ -23634,13 +23600,13 @@
       </c>
       <c r="I142" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>CMNKF555611R29VJ</v>
+        <v>EINKT117179C53HQ</v>
       </c>
     </row>
     <row r="143" spans="1:9">
       <c r="A143" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>FW9678178Z</v>
+        <v>WD4106456Q</v>
       </c>
       <c r="B143" t="s">
         <v>1664</v>
@@ -23650,13 +23616,13 @@
       </c>
       <c r="I143" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>OSKSW664427G80BA</v>
+        <v>EEGAW615407Y36VP</v>
       </c>
     </row>
     <row r="144" spans="1:9">
       <c r="A144" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>EX4321561X</v>
+        <v>NP2007112T</v>
       </c>
       <c r="B144" t="s">
         <v>1665</v>
@@ -23666,13 +23632,13 @@
       </c>
       <c r="I144" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>MOCRW118895R71GX</v>
+        <v>FJVCJ667375T73HM</v>
       </c>
     </row>
     <row r="145" spans="1:12">
       <c r="A145" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>ZF5879337Y</v>
+        <v>MA7603782J</v>
       </c>
       <c r="B145" t="s">
         <v>1666</v>
@@ -23682,13 +23648,13 @@
       </c>
       <c r="I145" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>SKUAH379604B68OS</v>
+        <v>BVPIG372442Q88QO</v>
       </c>
     </row>
     <row r="146" spans="1:12">
       <c r="A146" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>JG7021515W</v>
+        <v>ZQ196392G</v>
       </c>
       <c r="B146" t="s">
         <v>1667</v>
@@ -23698,13 +23664,13 @@
       </c>
       <c r="I146" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>ESJBK307593Y65DC</v>
+        <v>PVIAV140902L34PT</v>
       </c>
     </row>
     <row r="147" spans="1:12">
       <c r="A147" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>OH1726297X</v>
+        <v>YB2646878D</v>
       </c>
       <c r="B147" t="s">
         <v>1668</v>
@@ -23714,13 +23680,13 @@
       </c>
       <c r="I147" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>UROLA454196M84LB</v>
+        <v>MZCED676785C46TO</v>
       </c>
     </row>
     <row r="148" spans="1:12">
       <c r="A148" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>GU5052419B</v>
+        <v>HE8205234Z</v>
       </c>
       <c r="B148" t="s">
         <v>1669</v>
@@ -23730,13 +23696,13 @@
       </c>
       <c r="I148" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>ECRAO730281W87SU</v>
+        <v>TAODI742191M35HT</v>
       </c>
     </row>
     <row r="149" spans="1:12">
       <c r="A149" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>PO1054033T</v>
+        <v>UG8660067A</v>
       </c>
       <c r="B149" t="s">
         <v>1670</v>
@@ -23746,13 +23712,13 @@
       </c>
       <c r="I149" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>KBWZJ149981I27BX</v>
+        <v>UIBAM779042N4XN</v>
       </c>
     </row>
     <row r="150" spans="1:12">
       <c r="A150" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>KA281608D</v>
+        <v>AL9437517W</v>
       </c>
       <c r="B150" t="s">
         <v>1671</v>
@@ -23762,13 +23728,13 @@
       </c>
       <c r="I150" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LLPDR13994P33RO</v>
+        <v>PUANF670216Y4IX</v>
       </c>
     </row>
     <row r="151" spans="1:12">
       <c r="A151" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>NZ2197765P</v>
+        <v>NA3563557O</v>
       </c>
       <c r="B151" t="s">
         <v>1672</v>
@@ -23778,13 +23744,13 @@
       </c>
       <c r="I151" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>ZKTWF397129C88WH</v>
+        <v>ADABB169390N64TC</v>
       </c>
     </row>
     <row r="152" spans="1:12">
       <c r="A152" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>GQ6534251A</v>
+        <v>EJ492604Q</v>
       </c>
       <c r="B152" t="s">
         <v>1673</v>
@@ -23794,7 +23760,7 @@
       </c>
       <c r="I152" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>QFUXP728821I27LF</v>
+        <v>AKOYZ784659W59LE</v>
       </c>
       <c r="K152" s="28" t="e">
         <f t="shared" ref="K152" si="7">RIGHT(J152, LEN(J152)-1)</f>
@@ -23808,7 +23774,7 @@
     <row r="153" spans="1:12">
       <c r="A153" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>LE7587168X</v>
+        <v>AU7896054T</v>
       </c>
       <c r="B153" t="s">
         <v>1674</v>
@@ -23818,13 +23784,13 @@
       </c>
       <c r="I153" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>VFRIM724728N67VV</v>
+        <v>FTMZO343218Y51XR</v>
       </c>
     </row>
     <row r="154" spans="1:12">
       <c r="A154" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>KA6640260U</v>
+        <v>JG5229649Z</v>
       </c>
       <c r="B154" t="s">
         <v>1675</v>
@@ -23834,13 +23800,13 @@
       </c>
       <c r="I154" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>KEKTQ845884H39LT</v>
+        <v>AVTCA238389D93ZL</v>
       </c>
     </row>
     <row r="155" spans="1:12">
       <c r="A155" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>GG8188397S</v>
+        <v>YL4838986X</v>
       </c>
       <c r="B155" t="s">
         <v>1676</v>
@@ -23850,13 +23816,13 @@
       </c>
       <c r="I155" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>PHAUP858115V9IY</v>
+        <v>OOCJP300984F21NY</v>
       </c>
     </row>
     <row r="156" spans="1:12">
       <c r="A156" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>UA9228806I</v>
+        <v>HT4767986A</v>
       </c>
       <c r="B156" t="s">
         <v>1677</v>
@@ -23866,13 +23832,13 @@
       </c>
       <c r="I156" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>HWNQJ992607N33FD</v>
+        <v>SYKCB769708W80RE</v>
       </c>
     </row>
     <row r="157" spans="1:12">
       <c r="A157" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>SK2426015P</v>
+        <v>ZT7695979K</v>
       </c>
       <c r="B157" t="s">
         <v>1678</v>
@@ -23882,13 +23848,13 @@
       </c>
       <c r="I157" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>BYJCX790235X81IE</v>
+        <v>RVFOH453266P63LE</v>
       </c>
     </row>
     <row r="158" spans="1:12">
       <c r="A158" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>DG6861347Y</v>
+        <v>MP9352819T</v>
       </c>
       <c r="B158" t="s">
         <v>1679</v>
@@ -23898,13 +23864,13 @@
       </c>
       <c r="I158" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>QRLII626980Y27NK</v>
+        <v>VOKPR320670G72AX</v>
       </c>
     </row>
     <row r="159" spans="1:12">
       <c r="A159" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>YF8006872C</v>
+        <v>IX5187804P</v>
       </c>
       <c r="B159" t="s">
         <v>1680</v>
@@ -23914,13 +23880,13 @@
       </c>
       <c r="I159" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>PTZKS14378N70XQ</v>
+        <v>TZAGJ69725F7RY</v>
       </c>
     </row>
     <row r="160" spans="1:12">
       <c r="A160" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>JG2921530D</v>
+        <v>XP8062041B</v>
       </c>
       <c r="B160" t="s">
         <v>1681</v>
@@ -23930,13 +23896,13 @@
       </c>
       <c r="I160" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>KFMPD513675H38MD</v>
+        <v>FCDNZ84606L9BU</v>
       </c>
     </row>
     <row r="161" spans="1:9">
       <c r="A161" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>QB574635Z</v>
+        <v>MB9104859W</v>
       </c>
       <c r="B161" t="s">
         <v>1682</v>
@@ -23946,13 +23912,13 @@
       </c>
       <c r="I161" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LTBUH741894A43UU</v>
+        <v>UOWQL491953W50MN</v>
       </c>
     </row>
     <row r="162" spans="1:9">
       <c r="A162" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>DO2468270T</v>
+        <v>BO2696130A</v>
       </c>
       <c r="B162" t="s">
         <v>1683</v>
@@ -23962,13 +23928,13 @@
       </c>
       <c r="I162" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>DPBFN454794G6PK</v>
+        <v>YBYYS806913Q69VS</v>
       </c>
     </row>
     <row r="163" spans="1:9">
       <c r="A163" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>YK4832997J</v>
+        <v>TB5901046M</v>
       </c>
       <c r="B163" t="s">
         <v>1684</v>
@@ -23978,13 +23944,13 @@
       </c>
       <c r="I163" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>KXEAH570408W95MU</v>
+        <v>DOLMI840788X96JS</v>
       </c>
     </row>
     <row r="164" spans="1:9">
       <c r="A164" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>IY926611R</v>
+        <v>XC4671270V</v>
       </c>
       <c r="B164" t="s">
         <v>1685</v>
@@ -23994,13 +23960,13 @@
       </c>
       <c r="I164" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>ALOFB888496Z12LA</v>
+        <v>YPNXW210840Z5QR</v>
       </c>
     </row>
     <row r="165" spans="1:9">
       <c r="A165" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>SO6637031S</v>
+        <v>OJ8329827B</v>
       </c>
       <c r="B165" t="s">
         <v>1686</v>
@@ -24010,13 +23976,13 @@
       </c>
       <c r="I165" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>VMEPR694847T86HT</v>
+        <v>ONNID157855Z1ZS</v>
       </c>
     </row>
     <row r="166" spans="1:9">
       <c r="A166" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>JB4645956L</v>
+        <v>EK4167683J</v>
       </c>
       <c r="B166" t="s">
         <v>1687</v>
@@ -24026,13 +23992,13 @@
       </c>
       <c r="I166" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>DPLYZ343598T94RA</v>
+        <v>BDHZV493124C19XJ</v>
       </c>
     </row>
     <row r="167" spans="1:9">
       <c r="A167" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>XV7823250O</v>
+        <v>ND9239111J</v>
       </c>
       <c r="B167" t="s">
         <v>1688</v>
@@ -24042,13 +24008,13 @@
       </c>
       <c r="I167" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>OILVB150106K12AC</v>
+        <v>UWPES91334W97KO</v>
       </c>
     </row>
     <row r="168" spans="1:9">
       <c r="A168" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>EI4039659K</v>
+        <v>UU4436591E</v>
       </c>
       <c r="B168" t="s">
         <v>1689</v>
@@ -24058,13 +24024,13 @@
       </c>
       <c r="I168" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>JOLEZ754483A9ZC</v>
+        <v>AHQUF754988V12XQ</v>
       </c>
     </row>
     <row r="169" spans="1:9">
       <c r="A169" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>AW9669369H</v>
+        <v>KL1279904B</v>
       </c>
       <c r="B169" t="s">
         <v>1690</v>
@@ -24074,13 +24040,13 @@
       </c>
       <c r="I169" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>XEBZX558529N37CY</v>
+        <v>NAQGH492909A2AU</v>
       </c>
     </row>
     <row r="170" spans="1:9">
       <c r="A170" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>ZK3593353L</v>
+        <v>TP493783L</v>
       </c>
       <c r="B170" t="s">
         <v>1691</v>
@@ -24090,13 +24056,13 @@
       </c>
       <c r="I170" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>HZANV960102A57FL</v>
+        <v>VQNPL55622B70RP</v>
       </c>
     </row>
     <row r="171" spans="1:9">
       <c r="A171" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>LG480816Q</v>
+        <v>LQ5757428Q</v>
       </c>
       <c r="B171" t="s">
         <v>1692</v>
@@ -24106,13 +24072,13 @@
       </c>
       <c r="I171" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>WCIHS421862V85UU</v>
+        <v>JOZGY918859G32AK</v>
       </c>
     </row>
     <row r="172" spans="1:9">
       <c r="A172" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>FD1853566H</v>
+        <v>ZO4073157W</v>
       </c>
       <c r="B172" t="s">
         <v>1693</v>
@@ -24122,13 +24088,13 @@
       </c>
       <c r="I172" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>NRQOJ748797G89XK</v>
+        <v>ILIYM496712A62JD</v>
       </c>
     </row>
     <row r="173" spans="1:9">
       <c r="A173" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>XC8012378C</v>
+        <v>WR713696G</v>
       </c>
       <c r="B173" t="s">
         <v>1694</v>
@@ -24138,13 +24104,13 @@
       </c>
       <c r="I173" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>FVNRG642771U7FY</v>
+        <v>KRAXX587618O89BH</v>
       </c>
     </row>
     <row r="174" spans="1:9">
       <c r="A174" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>JT143612I</v>
+        <v>UI689544A</v>
       </c>
       <c r="B174" t="s">
         <v>1695</v>
@@ -24154,13 +24120,13 @@
       </c>
       <c r="I174" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>YOUDO108600A31DR</v>
+        <v>RSUJZ784993V72PM</v>
       </c>
     </row>
     <row r="175" spans="1:9">
       <c r="A175" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>VN3071405Q</v>
+        <v>QH4836182Z</v>
       </c>
       <c r="B175" t="s">
         <v>1696</v>
@@ -24170,13 +24136,13 @@
       </c>
       <c r="I175" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>ZYDHU272086A80SI</v>
+        <v>NFCHU429339E75MB</v>
       </c>
     </row>
     <row r="176" spans="1:9">
       <c r="A176" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>PJ6086340L</v>
+        <v>PG4713107T</v>
       </c>
       <c r="B176" t="s">
         <v>1697</v>
@@ -24186,13 +24152,13 @@
       </c>
       <c r="I176" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>OJJZP86167G24OI</v>
+        <v>HRFXH946942H25DT</v>
       </c>
     </row>
     <row r="177" spans="1:9">
       <c r="A177" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>ZH8177000O</v>
+        <v>NI2642514I</v>
       </c>
       <c r="B177" t="s">
         <v>1698</v>
@@ -24202,13 +24168,13 @@
       </c>
       <c r="I177" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>JOMKY745474X44RW</v>
+        <v>HHKWU501837B77UW</v>
       </c>
     </row>
     <row r="178" spans="1:9">
       <c r="A178" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>TF9772910X</v>
+        <v>XV2455915O</v>
       </c>
       <c r="B178" t="s">
         <v>1699</v>
@@ -24218,13 +24184,13 @@
       </c>
       <c r="I178" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>UEZKC650204O83PQ</v>
+        <v>GOZSW709180P95FL</v>
       </c>
     </row>
     <row r="179" spans="1:9">
       <c r="A179" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>RW9971484F</v>
+        <v>CJ1395260P</v>
       </c>
       <c r="B179" t="s">
         <v>1700</v>
@@ -24234,13 +24200,13 @@
       </c>
       <c r="I179" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>SNHWI212527N75DT</v>
+        <v>KHPYV570911J21AZ</v>
       </c>
     </row>
     <row r="180" spans="1:9">
       <c r="A180" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>OL7828272D</v>
+        <v>BW6008534N</v>
       </c>
       <c r="B180" t="s">
         <v>1701</v>
@@ -24250,13 +24216,13 @@
       </c>
       <c r="I180" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>PRDNC525838I89TE</v>
+        <v>OPXTD192363B32YO</v>
       </c>
     </row>
     <row r="181" spans="1:9">
       <c r="A181" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>XY8724629P</v>
+        <v>WM1814816T</v>
       </c>
       <c r="B181" t="s">
         <v>1702</v>
@@ -24266,13 +24232,13 @@
       </c>
       <c r="I181" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>NSHVM605946Q93CM</v>
+        <v>XODWD542439N99KQ</v>
       </c>
     </row>
     <row r="182" spans="1:9">
       <c r="A182" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>RB5742891D</v>
+        <v>VS1115884F</v>
       </c>
       <c r="B182" t="s">
         <v>1703</v>
@@ -24282,13 +24248,13 @@
       </c>
       <c r="I182" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>XDSWV751823Y46KM</v>
+        <v>EKCAS707269U68QC</v>
       </c>
     </row>
     <row r="183" spans="1:9">
       <c r="A183" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>PA2857425F</v>
+        <v>ZH780709S</v>
       </c>
       <c r="B183" t="s">
         <v>1704</v>
@@ -24298,13 +24264,13 @@
       </c>
       <c r="I183" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>RELXI155983X20GA</v>
+        <v>DXFFD580648C83DX</v>
       </c>
     </row>
     <row r="184" spans="1:9">
       <c r="A184" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>XT2998876U</v>
+        <v>CF613050G</v>
       </c>
       <c r="B184" t="s">
         <v>1705</v>
@@ -24314,13 +24280,13 @@
       </c>
       <c r="I184" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>AYHYC325936Z37IP</v>
+        <v>HOQWK120291Y40AP</v>
       </c>
     </row>
     <row r="185" spans="1:9">
       <c r="A185" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>PU5692285M</v>
+        <v>HH6375884D</v>
       </c>
       <c r="B185" t="s">
         <v>1706</v>
@@ -24330,13 +24296,13 @@
       </c>
       <c r="I185" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>VHXTN93222K88JU</v>
+        <v>PEBYM193561P81IC</v>
       </c>
     </row>
     <row r="186" spans="1:9">
       <c r="A186" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>OC1567301P</v>
+        <v>PI4681849U</v>
       </c>
       <c r="B186" t="s">
         <v>1707</v>
@@ -24346,13 +24312,13 @@
       </c>
       <c r="I186" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>HPTOU177500E7RS</v>
+        <v>AVNOI313458F26BC</v>
       </c>
     </row>
     <row r="187" spans="1:9">
       <c r="A187" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>PI6961098R</v>
+        <v>RO4584987W</v>
       </c>
       <c r="B187" t="s">
         <v>1708</v>
@@ -24362,13 +24328,13 @@
       </c>
       <c r="I187" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>ZSUEU198515D85DB</v>
+        <v>JQNQU488470Z62IV</v>
       </c>
     </row>
     <row r="188" spans="1:9">
       <c r="A188" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>JK8624994D</v>
+        <v>ZU79709Y</v>
       </c>
       <c r="B188" t="s">
         <v>1709</v>
@@ -24378,13 +24344,13 @@
       </c>
       <c r="I188" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>NYOZD37620U31BD</v>
+        <v>DZCUN401343A28GS</v>
       </c>
     </row>
     <row r="189" spans="1:9">
       <c r="A189" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>DX223197H</v>
+        <v>ZT419096I</v>
       </c>
       <c r="B189" t="s">
         <v>1710</v>
@@ -24394,13 +24360,13 @@
       </c>
       <c r="I189" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>MDQTI456673Z12LX</v>
+        <v>FYVFS114629T53ED</v>
       </c>
     </row>
     <row r="190" spans="1:9">
       <c r="A190" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>DH5430760B</v>
+        <v>FK1746497V</v>
       </c>
       <c r="B190" t="s">
         <v>1711</v>
@@ -24410,13 +24376,13 @@
       </c>
       <c r="I190" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LRLKW542100M53YV</v>
+        <v>YAYNC207094G9II</v>
       </c>
     </row>
     <row r="191" spans="1:9">
       <c r="A191" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>UG72164Z</v>
+        <v>EE8775595D</v>
       </c>
       <c r="B191" t="s">
         <v>1712</v>
@@ -24426,13 +24392,13 @@
       </c>
       <c r="I191" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>SYVCK434108Q26ZA</v>
+        <v>SMEFS104151Q30OK</v>
       </c>
     </row>
     <row r="192" spans="1:9">
       <c r="A192" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>SM8935581J</v>
+        <v>BM3879450O</v>
       </c>
       <c r="B192" t="s">
         <v>1713</v>
@@ -24442,13 +24408,13 @@
       </c>
       <c r="I192" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>MPJCG847097Z44KN</v>
+        <v>RGAZY898608L31CC</v>
       </c>
     </row>
     <row r="193" spans="1:9">
       <c r="A193" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>QX633721G</v>
+        <v>RV4205767C</v>
       </c>
       <c r="B193" t="s">
         <v>1714</v>
@@ -24458,13 +24424,13 @@
       </c>
       <c r="I193" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>DISHP593768C36IL</v>
+        <v>TGAPO318329X75HM</v>
       </c>
     </row>
     <row r="194" spans="1:9">
       <c r="A194" s="6" t="str">
         <f t="shared" ref="A194:A257" ca="1" si="8">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,9999999)&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>EL5605723J</v>
+        <v>PY1230303P</v>
       </c>
       <c r="B194" t="s">
         <v>1715</v>
@@ -24474,13 +24440,13 @@
       </c>
       <c r="I194" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>RYVBJ240399B47PR</v>
+        <v>KHYYM562354F31PL</v>
       </c>
     </row>
     <row r="195" spans="1:9">
       <c r="A195" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>NP3036966G</v>
+        <v>XD9952411L</v>
       </c>
       <c r="B195" t="s">
         <v>1716</v>
@@ -24490,13 +24456,13 @@
       </c>
       <c r="I195" t="str">
         <f t="shared" ref="I195:I250" ca="1" si="9">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,999999)&amp;CHAR(RANDBETWEEN(65,90))&amp;(RANDBETWEEN(1,99))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>GRALI342452D25JP</v>
+        <v>WREFG681156C55FJ</v>
       </c>
     </row>
     <row r="196" spans="1:9">
       <c r="A196" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>XW8895589E</v>
+        <v>XE7466007M</v>
       </c>
       <c r="B196" t="s">
         <v>1717</v>
@@ -24506,13 +24472,13 @@
       </c>
       <c r="I196" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>XEMRW703973M80NK</v>
+        <v>QWQZU1453B79WZ</v>
       </c>
     </row>
     <row r="197" spans="1:9">
       <c r="A197" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>XV9626488P</v>
+        <v>XZ770849O</v>
       </c>
       <c r="B197" t="s">
         <v>1718</v>
@@ -24522,13 +24488,13 @@
       </c>
       <c r="I197" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>BJYXO599890K6ME</v>
+        <v>GAJAA771120V75FA</v>
       </c>
     </row>
     <row r="198" spans="1:9">
       <c r="A198" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>VK4134228S</v>
+        <v>GK61431J</v>
       </c>
       <c r="B198" t="s">
         <v>1719</v>
@@ -24538,13 +24504,13 @@
       </c>
       <c r="I198" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>SACAV981885P71AT</v>
+        <v>BOXCN641060A52QN</v>
       </c>
     </row>
     <row r="199" spans="1:9">
       <c r="A199" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>FC4198300S</v>
+        <v>NN696642S</v>
       </c>
       <c r="B199" t="s">
         <v>1720</v>
@@ -24554,13 +24520,13 @@
       </c>
       <c r="I199" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>XDCMZ358713W69VQ</v>
+        <v>QKJPX703479N55UR</v>
       </c>
     </row>
     <row r="200" spans="1:9">
       <c r="A200" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>OR2357238I</v>
+        <v>NG6015262A</v>
       </c>
       <c r="B200" t="s">
         <v>1721</v>
@@ -24570,13 +24536,13 @@
       </c>
       <c r="I200" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>IJUQY366801M51ZZ</v>
+        <v>NVWKH551715Y29OQ</v>
       </c>
     </row>
     <row r="201" spans="1:9">
       <c r="A201" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>GP4874619E</v>
+        <v>MO5304162J</v>
       </c>
       <c r="B201" t="s">
         <v>1722</v>
@@ -24586,13 +24552,13 @@
       </c>
       <c r="I201" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>JXAQH331273O74LU</v>
+        <v>RWRRU308256Y85GR</v>
       </c>
     </row>
     <row r="202" spans="1:9">
       <c r="A202" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>PN2202509T</v>
+        <v>EG3373491V</v>
       </c>
       <c r="B202" t="s">
         <v>1723</v>
@@ -24602,13 +24568,13 @@
       </c>
       <c r="I202" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>SUGAW206345M73OX</v>
+        <v>LSXIH887534R83AG</v>
       </c>
     </row>
     <row r="203" spans="1:9">
       <c r="A203" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>EU16273W</v>
+        <v>JB1338876C</v>
       </c>
       <c r="B203" t="s">
         <v>1724</v>
@@ -24618,13 +24584,13 @@
       </c>
       <c r="I203" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>EBVIH485609J62UV</v>
+        <v>KDYXA962842F62QK</v>
       </c>
     </row>
     <row r="204" spans="1:9">
       <c r="A204" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>SJ1646490S</v>
+        <v>WE9181899F</v>
       </c>
       <c r="B204" t="s">
         <v>1725</v>
@@ -24634,13 +24600,13 @@
       </c>
       <c r="I204" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>ARDSB382607K58RU</v>
+        <v>QIFKQ170354R53SH</v>
       </c>
     </row>
     <row r="205" spans="1:9">
       <c r="A205" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>UR2865454O</v>
+        <v>TU4787968G</v>
       </c>
       <c r="B205" t="s">
         <v>1726</v>
@@ -24650,13 +24616,13 @@
       </c>
       <c r="I205" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>GYFTD599046S72KX</v>
+        <v>LNBNC35281A25OY</v>
       </c>
     </row>
     <row r="206" spans="1:9">
       <c r="A206" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>VK8934461P</v>
+        <v>XV8858365B</v>
       </c>
       <c r="B206" t="s">
         <v>1727</v>
@@ -24666,13 +24632,13 @@
       </c>
       <c r="I206" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>KZQHM256736H9BZ</v>
+        <v>OVYHD56820I19QO</v>
       </c>
     </row>
     <row r="207" spans="1:9">
       <c r="A207" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>WY4385066Q</v>
+        <v>BK992348P</v>
       </c>
       <c r="B207" t="s">
         <v>1728</v>
@@ -24682,13 +24648,13 @@
       </c>
       <c r="I207" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>TDIHW34548Q76YP</v>
+        <v>YIKGA477544J24KP</v>
       </c>
     </row>
     <row r="208" spans="1:9">
       <c r="A208" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>OB6745129M</v>
+        <v>YK2981823S</v>
       </c>
       <c r="B208" t="s">
         <v>1729</v>
@@ -24698,13 +24664,13 @@
       </c>
       <c r="I208" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>UIPBU276693G65CE</v>
+        <v>RVXLH922169J13MD</v>
       </c>
     </row>
     <row r="209" spans="1:9">
       <c r="A209" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>XN8293628I</v>
+        <v>YX580031T</v>
       </c>
       <c r="B209" t="s">
         <v>1730</v>
@@ -24714,13 +24680,13 @@
       </c>
       <c r="I209" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>RKSOI906327I71XQ</v>
+        <v>LHSPY134452G63VB</v>
       </c>
     </row>
     <row r="210" spans="1:9">
       <c r="A210" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>QA1190573I</v>
+        <v>QA4654653U</v>
       </c>
       <c r="B210" t="s">
         <v>1731</v>
@@ -24730,13 +24696,13 @@
       </c>
       <c r="I210" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>DIOIJ454606W7FO</v>
+        <v>AEIIW641122Q20PE</v>
       </c>
     </row>
     <row r="211" spans="1:9">
       <c r="A211" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>NS6043529Q</v>
+        <v>OD1263757R</v>
       </c>
       <c r="B211" t="s">
         <v>1732</v>
@@ -24746,13 +24712,13 @@
       </c>
       <c r="I211" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>GKJGP19846Z79EV</v>
+        <v>YYRRJ359418N36BU</v>
       </c>
     </row>
     <row r="212" spans="1:9">
       <c r="A212" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>QX7879326W</v>
+        <v>PC6226232Q</v>
       </c>
       <c r="B212" t="s">
         <v>1733</v>
@@ -24762,13 +24728,13 @@
       </c>
       <c r="I212" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>VIYFP890722J48DA</v>
+        <v>UFSQL950738B12IJ</v>
       </c>
     </row>
     <row r="213" spans="1:9">
       <c r="A213" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>GJ8645469O</v>
+        <v>AB8732296Z</v>
       </c>
       <c r="B213" t="s">
         <v>1734</v>
@@ -24778,13 +24744,13 @@
       </c>
       <c r="I213" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>AFIYQ118308B54VV</v>
+        <v>BRWSZ402181W66MF</v>
       </c>
     </row>
     <row r="214" spans="1:9">
       <c r="A214" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>SJ3594933Q</v>
+        <v>FV3140107C</v>
       </c>
       <c r="B214" t="s">
         <v>1735</v>
@@ -24794,13 +24760,13 @@
       </c>
       <c r="I214" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>BWUZV246972F76JZ</v>
+        <v>TGVNI567479K82BQ</v>
       </c>
     </row>
     <row r="215" spans="1:9">
       <c r="A215" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>KK3624789N</v>
+        <v>VA7374479F</v>
       </c>
       <c r="B215" t="s">
         <v>1736</v>
@@ -24810,13 +24776,13 @@
       </c>
       <c r="I215" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>IFYSL335504C2HO</v>
+        <v>BCRDJ170118G58VK</v>
       </c>
     </row>
     <row r="216" spans="1:9">
       <c r="A216" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>TE7584633E</v>
+        <v>ZS1587097M</v>
       </c>
       <c r="B216" t="s">
         <v>1737</v>
@@ -24826,13 +24792,13 @@
       </c>
       <c r="I216" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>AHSXZ721326W78ZS</v>
+        <v>LKLBM825755F86KF</v>
       </c>
     </row>
     <row r="217" spans="1:9">
       <c r="A217" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>LY5493205A</v>
+        <v>WP6987253V</v>
       </c>
       <c r="B217" t="s">
         <v>1738</v>
@@ -24842,13 +24808,13 @@
       </c>
       <c r="I217" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>MXHPS191800G44SX</v>
+        <v>HEXSF164792N76OQ</v>
       </c>
     </row>
     <row r="218" spans="1:9">
       <c r="A218" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>PU2801977L</v>
+        <v>VW7243766V</v>
       </c>
       <c r="B218" t="s">
         <v>1739</v>
@@ -24858,13 +24824,13 @@
       </c>
       <c r="I218" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>SJLUA917793E73QI</v>
+        <v>JCNRW33645G72QO</v>
       </c>
     </row>
     <row r="219" spans="1:9">
       <c r="A219" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>DO9590219U</v>
+        <v>RF9885292J</v>
       </c>
       <c r="B219" t="s">
         <v>1740</v>
@@ -24874,13 +24840,13 @@
       </c>
       <c r="I219" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>XCSQA501417R87SN</v>
+        <v>SRGNC787523C54VY</v>
       </c>
     </row>
     <row r="220" spans="1:9">
       <c r="A220" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>YD8312326X</v>
+        <v>GR4836648E</v>
       </c>
       <c r="B220" t="s">
         <v>1741</v>
@@ -24890,13 +24856,13 @@
       </c>
       <c r="I220" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>XPSOC63974I18ZM</v>
+        <v>MHRKR173515V37AY</v>
       </c>
     </row>
     <row r="221" spans="1:9">
       <c r="A221" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>RQ8182323I</v>
+        <v>MA2734767Y</v>
       </c>
       <c r="B221" t="s">
         <v>1742</v>
@@ -24906,13 +24872,13 @@
       </c>
       <c r="I221" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>QWZMG214504K89NH</v>
+        <v>QPLSN77837C69NX</v>
       </c>
     </row>
     <row r="222" spans="1:9">
       <c r="A222" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>MP4818050G</v>
+        <v>TK7354588F</v>
       </c>
       <c r="B222" t="s">
         <v>1743</v>
@@ -24922,13 +24888,13 @@
       </c>
       <c r="I222" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>RZMUY888398I65YO</v>
+        <v>WYZMP889995G24FV</v>
       </c>
     </row>
     <row r="223" spans="1:9">
       <c r="A223" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>HX7774205U</v>
+        <v>GQ7580790F</v>
       </c>
       <c r="B223" t="s">
         <v>1744</v>
@@ -24938,13 +24904,13 @@
       </c>
       <c r="I223" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>LILFV508809N10UF</v>
+        <v>RDAKL804224Z82LO</v>
       </c>
     </row>
     <row r="224" spans="1:9">
       <c r="A224" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>CI3421357A</v>
+        <v>CI208418C</v>
       </c>
       <c r="B224" t="s">
         <v>1745</v>
@@ -24954,13 +24920,13 @@
       </c>
       <c r="I224" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>CLMCG178200C17IA</v>
+        <v>PZHZA728230V41HS</v>
       </c>
     </row>
     <row r="225" spans="1:9">
       <c r="A225" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>FS5226681C</v>
+        <v>MH4040869P</v>
       </c>
       <c r="B225" t="s">
         <v>1746</v>
@@ -24970,13 +24936,13 @@
       </c>
       <c r="I225" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>EHRZL737647R37VO</v>
+        <v>ONKXN599525O28BD</v>
       </c>
     </row>
     <row r="226" spans="1:9">
       <c r="A226" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>RY7101673A</v>
+        <v>ZG8456071Q</v>
       </c>
       <c r="B226" t="s">
         <v>1747</v>
@@ -24986,13 +24952,13 @@
       </c>
       <c r="I226" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>RUIHH1014T97UX</v>
+        <v>TQNWL234010L73ZK</v>
       </c>
     </row>
     <row r="227" spans="1:9">
       <c r="A227" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>VS5659107J</v>
+        <v>KS3576960E</v>
       </c>
       <c r="B227" t="s">
         <v>1748</v>
@@ -25002,13 +24968,13 @@
       </c>
       <c r="I227" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>UIZCS528246Z76PZ</v>
+        <v>RKOMT380767L70CM</v>
       </c>
     </row>
     <row r="228" spans="1:9">
       <c r="A228" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>KD9193072V</v>
+        <v>QH8238951J</v>
       </c>
       <c r="B228" t="s">
         <v>1749</v>
@@ -25018,13 +24984,13 @@
       </c>
       <c r="I228" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>VHPXZ339065U31GB</v>
+        <v>UAQMP817939S73MT</v>
       </c>
     </row>
     <row r="229" spans="1:9">
       <c r="A229" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>XR7755256Z</v>
+        <v>BQ9178751M</v>
       </c>
       <c r="B229" t="s">
         <v>1750</v>
@@ -25034,13 +25000,13 @@
       </c>
       <c r="I229" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>SCKIB570033E21XR</v>
+        <v>MEIAM523539O51OA</v>
       </c>
     </row>
     <row r="230" spans="1:9">
       <c r="A230" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>OS2929141P</v>
+        <v>XF8052942X</v>
       </c>
       <c r="B230" t="s">
         <v>1751</v>
@@ -25050,13 +25016,13 @@
       </c>
       <c r="I230" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>CLSJZ838411J86HZ</v>
+        <v>NKHHJ850315N38PX</v>
       </c>
     </row>
     <row r="231" spans="1:9">
       <c r="A231" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>SQ7490293N</v>
+        <v>EA7671235K</v>
       </c>
       <c r="B231" t="s">
         <v>1752</v>
@@ -25066,13 +25032,13 @@
       </c>
       <c r="I231" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>PMDDJ549297Z85FS</v>
+        <v>EPPZL747614L74JJ</v>
       </c>
     </row>
     <row r="232" spans="1:9">
       <c r="A232" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>YA2547221D</v>
+        <v>QP7834614J</v>
       </c>
       <c r="B232" t="s">
         <v>1753</v>
@@ -25082,13 +25048,13 @@
       </c>
       <c r="I232" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>IQBIE467888U30IY</v>
+        <v>ANLHX595747K12SO</v>
       </c>
     </row>
     <row r="233" spans="1:9">
       <c r="A233" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>XZ8869368E</v>
+        <v>XZ8271467G</v>
       </c>
       <c r="B233" t="s">
         <v>1754</v>
@@ -25098,13 +25064,13 @@
       </c>
       <c r="I233" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>XVYAQ638943C80TK</v>
+        <v>IEBMZ317555P64YN</v>
       </c>
     </row>
     <row r="234" spans="1:9">
       <c r="A234" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>MG4634084A</v>
+        <v>RO406825D</v>
       </c>
       <c r="B234" t="s">
         <v>1755</v>
@@ -25114,13 +25080,13 @@
       </c>
       <c r="I234" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>AHXUM933538E84FC</v>
+        <v>SYBOZ908111Y62CM</v>
       </c>
     </row>
     <row r="235" spans="1:9">
       <c r="A235" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>RS7184163R</v>
+        <v>IP4351992R</v>
       </c>
       <c r="B235" t="s">
         <v>1756</v>
@@ -25130,13 +25096,13 @@
       </c>
       <c r="I235" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>JWVON339713A57MP</v>
+        <v>ZOFKU283507U21XI</v>
       </c>
     </row>
     <row r="236" spans="1:9">
       <c r="A236" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>BL6823916K</v>
+        <v>PQ1941902Q</v>
       </c>
       <c r="B236" t="s">
         <v>1757</v>
@@ -25146,13 +25112,13 @@
       </c>
       <c r="I236" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>EWORH382966F39QZ</v>
+        <v>BEHGI171446C18KD</v>
       </c>
     </row>
     <row r="237" spans="1:9">
       <c r="A237" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>YC4312585S</v>
+        <v>AC4616277M</v>
       </c>
       <c r="B237" t="s">
         <v>1758</v>
@@ -25162,13 +25128,13 @@
       </c>
       <c r="I237" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>UYDJF779332E98VB</v>
+        <v>AJHRB425360U34BC</v>
       </c>
     </row>
     <row r="238" spans="1:9">
       <c r="A238" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>GJ7119485W</v>
+        <v>CO4835690N</v>
       </c>
       <c r="B238" t="s">
         <v>1759</v>
@@ -25178,13 +25144,13 @@
       </c>
       <c r="I238" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>QROHG921369S70GZ</v>
+        <v>XJPUF787300Z99RE</v>
       </c>
     </row>
     <row r="239" spans="1:9">
       <c r="A239" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>BX7840909T</v>
+        <v>VE8884782W</v>
       </c>
       <c r="B239" t="s">
         <v>1760</v>
@@ -25194,13 +25160,13 @@
       </c>
       <c r="I239" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>PVTNL706039O48GL</v>
+        <v>HWMLR32689T63SX</v>
       </c>
     </row>
     <row r="240" spans="1:9">
       <c r="A240" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>EV3985781I</v>
+        <v>OX3729586J</v>
       </c>
       <c r="B240" t="s">
         <v>1761</v>
@@ -25210,13 +25176,13 @@
       </c>
       <c r="I240" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>ARGKK224627L78RD</v>
+        <v>ESTOF551813P23CO</v>
       </c>
     </row>
     <row r="241" spans="1:9">
       <c r="A241" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>YY1654092I</v>
+        <v>CV1860550K</v>
       </c>
       <c r="B241" t="s">
         <v>1762</v>
@@ -25226,13 +25192,13 @@
       </c>
       <c r="I241" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>WHAOV173178F75IX</v>
+        <v>QKPTR986174L83PV</v>
       </c>
     </row>
     <row r="242" spans="1:9">
       <c r="A242" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>ER1351186P</v>
+        <v>FN3956851C</v>
       </c>
       <c r="B242" t="s">
         <v>1763</v>
@@ -25242,13 +25208,13 @@
       </c>
       <c r="I242" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>JCELB858318C22FH</v>
+        <v>VZLNM195078D89ES</v>
       </c>
     </row>
     <row r="243" spans="1:9">
       <c r="A243" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>ZA7395182R</v>
+        <v>VC6853714Z</v>
       </c>
       <c r="B243" t="s">
         <v>1764</v>
@@ -25258,104 +25224,104 @@
       </c>
       <c r="I243" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>PAZWZ898755U17CS</v>
+        <v>VOAVZ74711K73KK</v>
       </c>
     </row>
     <row r="244" spans="1:9">
       <c r="A244" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>UW4234103U</v>
+        <v>UE8151192Y</v>
       </c>
       <c r="B244" t="s">
         <v>1765</v>
       </c>
       <c r="I244" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>ARESW754727I56VO</v>
+        <v>INFCF587594K21ER</v>
       </c>
     </row>
     <row r="245" spans="1:9">
       <c r="A245" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>FJ8550535Y</v>
+        <v>MQ5470219W</v>
       </c>
       <c r="B245" t="s">
         <v>1766</v>
       </c>
       <c r="I245" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>QSZOT921117V87FV</v>
+        <v>YSRUF671904K87KM</v>
       </c>
     </row>
     <row r="246" spans="1:9">
       <c r="A246" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>PM3989512U</v>
+        <v>AP7921413S</v>
       </c>
       <c r="B246" t="s">
         <v>1767</v>
       </c>
       <c r="I246" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>JEJTQ11390A44RH</v>
+        <v>QRJOO972424E70HH</v>
       </c>
     </row>
     <row r="247" spans="1:9">
       <c r="A247" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>VG4352199B</v>
+        <v>CM6851382T</v>
       </c>
       <c r="B247" t="s">
         <v>1768</v>
       </c>
       <c r="I247" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>ZZREQ38781O89PC</v>
+        <v>SPJIC780968A91UU</v>
       </c>
     </row>
     <row r="248" spans="1:9">
       <c r="A248" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>IB7964911H</v>
+        <v>GE1114159W</v>
       </c>
       <c r="B248" t="s">
         <v>1769</v>
       </c>
       <c r="I248" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>NIQJZ453028K70KF</v>
+        <v>ZWWYL237712R42JA</v>
       </c>
     </row>
     <row r="249" spans="1:9">
       <c r="A249" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>NG7429678Z</v>
+        <v>PA6603862J</v>
       </c>
       <c r="B249" t="s">
         <v>1770</v>
       </c>
       <c r="I249" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>ENERO387774Z21PK</v>
+        <v>EKXNR486550Q47VT</v>
       </c>
     </row>
     <row r="250" spans="1:9">
       <c r="A250" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>BG7726494Y</v>
+        <v>RR3559673X</v>
       </c>
       <c r="B250" t="s">
         <v>1771</v>
       </c>
       <c r="I250" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>QWCUK785600H96EB</v>
+        <v>CQMKL124167Y3ID</v>
       </c>
     </row>
     <row r="251" spans="1:9">
       <c r="A251" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>IK1790935Y</v>
+        <v>KT4703321W</v>
       </c>
       <c r="B251" t="s">
         <v>1772</v>
@@ -25364,7 +25330,7 @@
     <row r="252" spans="1:9">
       <c r="A252" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>LZ7715694D</v>
+        <v>NE9104649F</v>
       </c>
       <c r="B252" t="s">
         <v>1773</v>
@@ -25373,7 +25339,7 @@
     <row r="253" spans="1:9">
       <c r="A253" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>ZB7361054M</v>
+        <v>OX3407406S</v>
       </c>
       <c r="B253" t="s">
         <v>1774</v>
@@ -25382,7 +25348,7 @@
     <row r="254" spans="1:9">
       <c r="A254" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>UI4105483Y</v>
+        <v>FK1532265Y</v>
       </c>
       <c r="B254" t="s">
         <v>1775</v>
@@ -25391,7 +25357,7 @@
     <row r="255" spans="1:9">
       <c r="A255" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>VH4195132B</v>
+        <v>EL8850245K</v>
       </c>
       <c r="B255" t="s">
         <v>1776</v>
@@ -25400,7 +25366,7 @@
     <row r="256" spans="1:9">
       <c r="A256" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>XT1113105T</v>
+        <v>RZ8733681X</v>
       </c>
       <c r="B256" t="s">
         <v>1777</v>
@@ -25409,7 +25375,7 @@
     <row r="257" spans="1:2">
       <c r="A257" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>HQ8972545O</v>
+        <v>HP7961366D</v>
       </c>
       <c r="B257" t="s">
         <v>1778</v>
@@ -25418,7 +25384,7 @@
     <row r="258" spans="1:2">
       <c r="A258" s="6" t="str">
         <f t="shared" ref="A258:A300" ca="1" si="10">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,9999999)&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>AV5888970N</v>
+        <v>KY3398598D</v>
       </c>
       <c r="B258" t="s">
         <v>1779</v>
@@ -25427,7 +25393,7 @@
     <row r="259" spans="1:2">
       <c r="A259" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>QO2273767V</v>
+        <v>OX5931141I</v>
       </c>
       <c r="B259" t="s">
         <v>1780</v>
@@ -25436,7 +25402,7 @@
     <row r="260" spans="1:2">
       <c r="A260" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>MR145069Z</v>
+        <v>UN1157364O</v>
       </c>
       <c r="B260" t="s">
         <v>1781</v>
@@ -25445,7 +25411,7 @@
     <row r="261" spans="1:2">
       <c r="A261" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>ZY1113066E</v>
+        <v>FN862101C</v>
       </c>
       <c r="B261" t="s">
         <v>1782</v>
@@ -25454,7 +25420,7 @@
     <row r="262" spans="1:2">
       <c r="A262" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>TP3704944I</v>
+        <v>CY6822677L</v>
       </c>
       <c r="B262" t="s">
         <v>1783</v>
@@ -25463,7 +25429,7 @@
     <row r="263" spans="1:2">
       <c r="A263" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>MJ4858840I</v>
+        <v>KU3263034Z</v>
       </c>
       <c r="B263" t="s">
         <v>1784</v>
@@ -25472,7 +25438,7 @@
     <row r="264" spans="1:2">
       <c r="A264" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>TA797659G</v>
+        <v>SV7371876Q</v>
       </c>
       <c r="B264" t="s">
         <v>1785</v>
@@ -25481,7 +25447,7 @@
     <row r="265" spans="1:2">
       <c r="A265" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>ES8940582U</v>
+        <v>RO9456509K</v>
       </c>
       <c r="B265" t="s">
         <v>1786</v>
@@ -25490,7 +25456,7 @@
     <row r="266" spans="1:2">
       <c r="A266" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>GU1281311T</v>
+        <v>HO8460840V</v>
       </c>
       <c r="B266" t="s">
         <v>1787</v>
@@ -25499,7 +25465,7 @@
     <row r="267" spans="1:2">
       <c r="A267" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>HN2151960O</v>
+        <v>WZ4540635C</v>
       </c>
       <c r="B267" t="s">
         <v>1788</v>
@@ -25508,7 +25474,7 @@
     <row r="268" spans="1:2">
       <c r="A268" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>QK3332500Q</v>
+        <v>SC4692581V</v>
       </c>
       <c r="B268" t="s">
         <v>1789</v>
@@ -25517,7 +25483,7 @@
     <row r="269" spans="1:2">
       <c r="A269" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>NA224577Y</v>
+        <v>US7598496P</v>
       </c>
       <c r="B269" t="s">
         <v>1790</v>
@@ -25526,7 +25492,7 @@
     <row r="270" spans="1:2">
       <c r="A270" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>SX747452M</v>
+        <v>ZW9767158Z</v>
       </c>
       <c r="B270" t="s">
         <v>1791</v>
@@ -25535,7 +25501,7 @@
     <row r="271" spans="1:2">
       <c r="A271" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>AI7891098T</v>
+        <v>MS1717833S</v>
       </c>
       <c r="B271" t="s">
         <v>1792</v>
@@ -25544,7 +25510,7 @@
     <row r="272" spans="1:2">
       <c r="A272" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>KV7387392Y</v>
+        <v>KI4606833I</v>
       </c>
       <c r="B272" t="s">
         <v>1793</v>
@@ -25553,7 +25519,7 @@
     <row r="273" spans="1:2">
       <c r="A273" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>WO1221979N</v>
+        <v>XZ3571329W</v>
       </c>
       <c r="B273" t="s">
         <v>1794</v>
@@ -25562,7 +25528,7 @@
     <row r="274" spans="1:2">
       <c r="A274" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>YE7479020R</v>
+        <v>US7154560C</v>
       </c>
       <c r="B274" t="s">
         <v>1795</v>
@@ -25571,7 +25537,7 @@
     <row r="275" spans="1:2">
       <c r="A275" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>FN5051840W</v>
+        <v>UC1523289X</v>
       </c>
       <c r="B275" t="s">
         <v>1796</v>
@@ -25580,7 +25546,7 @@
     <row r="276" spans="1:2">
       <c r="A276" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>ND9018009Q</v>
+        <v>AW1843541S</v>
       </c>
       <c r="B276" t="s">
         <v>1797</v>
@@ -25589,7 +25555,7 @@
     <row r="277" spans="1:2">
       <c r="A277" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>FL6497646U</v>
+        <v>GV6680567S</v>
       </c>
       <c r="B277" t="s">
         <v>1798</v>
@@ -25598,7 +25564,7 @@
     <row r="278" spans="1:2">
       <c r="A278" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>AP9704064I</v>
+        <v>RE9331966T</v>
       </c>
       <c r="B278" t="s">
         <v>1799</v>
@@ -25607,7 +25573,7 @@
     <row r="279" spans="1:2">
       <c r="A279" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>VZ4295177O</v>
+        <v>ZI3458363O</v>
       </c>
       <c r="B279" t="s">
         <v>1800</v>
@@ -25616,7 +25582,7 @@
     <row r="280" spans="1:2">
       <c r="A280" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>SZ9632679K</v>
+        <v>AQ8499917M</v>
       </c>
       <c r="B280" t="s">
         <v>1801</v>
@@ -25625,7 +25591,7 @@
     <row r="281" spans="1:2">
       <c r="A281" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>LZ6996451P</v>
+        <v>SY6523205R</v>
       </c>
       <c r="B281" t="s">
         <v>1802</v>
@@ -25634,7 +25600,7 @@
     <row r="282" spans="1:2">
       <c r="A282" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>WG6786831A</v>
+        <v>SU8909373Z</v>
       </c>
       <c r="B282" t="s">
         <v>1803</v>
@@ -25643,7 +25609,7 @@
     <row r="283" spans="1:2">
       <c r="A283" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>HM31212O</v>
+        <v>ER7912473A</v>
       </c>
       <c r="B283" t="s">
         <v>1804</v>
@@ -25652,7 +25618,7 @@
     <row r="284" spans="1:2">
       <c r="A284" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>YO9492597E</v>
+        <v>WT8505778T</v>
       </c>
       <c r="B284" t="s">
         <v>1805</v>
@@ -25661,7 +25627,7 @@
     <row r="285" spans="1:2">
       <c r="A285" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>JU3946583L</v>
+        <v>WK7830083A</v>
       </c>
       <c r="B285" t="s">
         <v>1806</v>
@@ -25670,7 +25636,7 @@
     <row r="286" spans="1:2">
       <c r="A286" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>VT100299O</v>
+        <v>JR4357618F</v>
       </c>
       <c r="B286" t="s">
         <v>1807</v>
@@ -25679,7 +25645,7 @@
     <row r="287" spans="1:2">
       <c r="A287" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>TD2743520B</v>
+        <v>OG4780401P</v>
       </c>
       <c r="B287" t="s">
         <v>1808</v>
@@ -25688,7 +25654,7 @@
     <row r="288" spans="1:2">
       <c r="A288" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>OP2827575O</v>
+        <v>RB5571412P</v>
       </c>
       <c r="B288" t="s">
         <v>1809</v>
@@ -25697,7 +25663,7 @@
     <row r="289" spans="1:2">
       <c r="A289" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>CB4922202I</v>
+        <v>GS4710249J</v>
       </c>
       <c r="B289" t="s">
         <v>1810</v>
@@ -25706,7 +25672,7 @@
     <row r="290" spans="1:2">
       <c r="A290" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>AA3231426B</v>
+        <v>YZ4351071K</v>
       </c>
       <c r="B290" t="s">
         <v>1811</v>
@@ -25715,7 +25681,7 @@
     <row r="291" spans="1:2">
       <c r="A291" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>RT4400004Y</v>
+        <v>MN344085Z</v>
       </c>
       <c r="B291" t="s">
         <v>1812</v>
@@ -25724,7 +25690,7 @@
     <row r="292" spans="1:2">
       <c r="A292" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>CE7803063T</v>
+        <v>UD8218177A</v>
       </c>
       <c r="B292" t="s">
         <v>1813</v>
@@ -25733,7 +25699,7 @@
     <row r="293" spans="1:2">
       <c r="A293" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>SS3672843U</v>
+        <v>PE1906379J</v>
       </c>
       <c r="B293" t="s">
         <v>1814</v>
@@ -25742,7 +25708,7 @@
     <row r="294" spans="1:2">
       <c r="A294" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>TI2599839M</v>
+        <v>QF3511095V</v>
       </c>
       <c r="B294" t="s">
         <v>1815</v>
@@ -25751,7 +25717,7 @@
     <row r="295" spans="1:2">
       <c r="A295" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>WD3912374E</v>
+        <v>BP4939869W</v>
       </c>
       <c r="B295" t="s">
         <v>1816</v>
@@ -25760,7 +25726,7 @@
     <row r="296" spans="1:2">
       <c r="A296" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>SR9803527V</v>
+        <v>QP7868822A</v>
       </c>
       <c r="B296" t="s">
         <v>1817</v>
@@ -25769,7 +25735,7 @@
     <row r="297" spans="1:2">
       <c r="A297" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>AT502480Q</v>
+        <v>XH2728511V</v>
       </c>
       <c r="B297" t="s">
         <v>1818</v>
@@ -25778,7 +25744,7 @@
     <row r="298" spans="1:2">
       <c r="A298" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>VP9632436M</v>
+        <v>TF4087966K</v>
       </c>
       <c r="B298" t="s">
         <v>1819</v>
@@ -25787,7 +25753,7 @@
     <row r="299" spans="1:2">
       <c r="A299" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>QI7636253Y</v>
+        <v>IW2110306Z</v>
       </c>
       <c r="B299" t="s">
         <v>1820</v>
@@ -25796,7 +25762,7 @@
     <row r="300" spans="1:2">
       <c r="A300" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>SJ6240214Q</v>
+        <v>NN4196764C</v>
       </c>
       <c r="B300" t="s">
         <v>1821</v>

</xml_diff>

<commit_message>
added tests for CUICE2037
</commit_message>
<xml_diff>
--- a/src/main/java/testData/ExcelFiles/E2E_Test_Data.xlsx
+++ b/src/main/java/testData/ExcelFiles/E2E_Test_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awhitten/IdeaProjects/Iceberg/src/main/java/testData/ExcelFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DD7330-C6FF-AB4E-8407-73FB4A9E084E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D32F3EC-FAC4-E64E-9E82-7F1C28343E49}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -263,7 +263,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3681" uniqueCount="2921">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3687" uniqueCount="2927">
   <si>
     <t>Andorra</t>
   </si>
@@ -9032,6 +9032,24 @@
   </si>
   <si>
     <t>Timeout</t>
+  </si>
+  <si>
+    <t>4532507073978721</t>
+  </si>
+  <si>
+    <t>4485641780472590</t>
+  </si>
+  <si>
+    <t>4539099375715228</t>
+  </si>
+  <si>
+    <t>4929170705471788</t>
+  </si>
+  <si>
+    <t>4916102956301054</t>
+  </si>
+  <si>
+    <t>4539940654914463</t>
   </si>
 </sst>
 </file>
@@ -9179,7 +9197,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyFill="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -9246,6 +9264,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -9255,7 +9274,7 @@
   </cellStyles>
   <dxfs count="19">
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <font>
@@ -21450,7 +21469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F9F5B7-248C-D14D-81F7-32D073538DE9}">
   <dimension ref="A1:W6"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
@@ -21911,20 +21930,20 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="20.5" customWidth="1"/>
-    <col min="2" max="2" width="22.5" style="28" customWidth="1"/>
+    <col min="2" max="2" width="22.5" style="30" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>2914</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="30" t="s">
         <v>2915</v>
       </c>
     </row>
@@ -21932,48 +21951,48 @@
       <c r="A2" t="s">
         <v>2916</v>
       </c>
-      <c r="B2" s="30">
-        <v>4532507073978720</v>
+      <c r="B2" s="46" t="s">
+        <v>2921</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>2917</v>
       </c>
-      <c r="B3" s="30">
-        <v>4539099375715220</v>
+      <c r="B3" s="46" t="s">
+        <v>2923</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>2918</v>
       </c>
-      <c r="B4" s="30">
-        <v>4929170705471780</v>
+      <c r="B4" s="46" t="s">
+        <v>2924</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>2919</v>
       </c>
-      <c r="B5" s="30">
-        <v>4485641780472590</v>
+      <c r="B5" s="46" t="s">
+        <v>2922</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>2919</v>
       </c>
-      <c r="B6" s="30">
-        <v>4916102956301050</v>
+      <c r="B6" s="46" t="s">
+        <v>2925</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>2920</v>
       </c>
-      <c r="B7" s="30">
-        <v>4539940654914460</v>
+      <c r="B7" s="46" t="s">
+        <v>2926</v>
       </c>
     </row>
   </sheetData>
@@ -22095,7 +22114,7 @@
     <row r="1" spans="1:11">
       <c r="A1" s="6" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,9999999)&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>AB3598670B</v>
+        <v>GE8738818I</v>
       </c>
       <c r="B1" t="s">
         <v>1522</v>
@@ -22107,7 +22126,7 @@
     <row r="2" spans="1:11">
       <c r="A2" s="6" t="str">
         <f ca="1">7&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,9999999)&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>7G6509823Y</v>
+        <v>7S9806060K</v>
       </c>
       <c r="B2" t="s">
         <v>1523</v>
@@ -22117,21 +22136,21 @@
       </c>
       <c r="I2" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,999999)&amp;CHAR(RANDBETWEEN(65,90))&amp;(RANDBETWEEN(1,99))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>BFXHV423731A63WU</v>
+        <v>FVSSJ555782H15ET</v>
       </c>
       <c r="J2" s="28" t="str">
         <f t="shared" ref="J2" ca="1" si="0">RIGHT(I2, LEN(I2)-1)</f>
-        <v>FXHV423731A63WU</v>
+        <v>VSSJ555782H15ET</v>
       </c>
       <c r="K2" s="14" t="str">
         <f ca="1">"07"&amp;J2</f>
-        <v>07FXHV423731A63WU</v>
+        <v>07VSSJ555782H15ET</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="6" t="str">
         <f t="shared" ref="A3:A65" ca="1" si="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,9999999)&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>RT9014438S</v>
+        <v>DA4304176J</v>
       </c>
       <c r="B3" t="s">
         <v>1524</v>
@@ -22141,13 +22160,13 @@
       </c>
       <c r="I3" t="str">
         <f t="shared" ref="I3:I66" ca="1" si="2">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,999999)&amp;CHAR(RANDBETWEEN(65,90))&amp;(RANDBETWEEN(1,99))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>ITZXW782869U11HR</v>
+        <v>KRYSZ899271O25WO</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>FR1473349B</v>
+        <v>RL3692992M</v>
       </c>
       <c r="B4" t="s">
         <v>1525</v>
@@ -22157,13 +22176,13 @@
       </c>
       <c r="I4" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>SRTOU741595C47GJ</v>
+        <v>FCXIE663382I60VF</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>EK957727Z</v>
+        <v>DU8333321O</v>
       </c>
       <c r="B5" t="s">
         <v>1526</v>
@@ -22173,13 +22192,13 @@
       </c>
       <c r="I5" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>LJIIV912078E2MK</v>
+        <v>CWQPE401669R59MY</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>HU6334785V</v>
+        <v>JN3595407A</v>
       </c>
       <c r="B6" t="s">
         <v>1527</v>
@@ -22189,13 +22208,13 @@
       </c>
       <c r="I6" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>DKYNK767349R63AP</v>
+        <v>HNNMM299709Z75QP</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>BF1842607D</v>
+        <v>DS6038077A</v>
       </c>
       <c r="B7" t="s">
         <v>1528</v>
@@ -22205,13 +22224,13 @@
       </c>
       <c r="I7" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>OZDLB362252F66JQ</v>
+        <v>KVYPL521500Z23GV</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>GI1188247T</v>
+        <v>EQ4681413T</v>
       </c>
       <c r="B8" t="s">
         <v>1529</v>
@@ -22221,13 +22240,13 @@
       </c>
       <c r="I8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>PXBRB963155P4AR</v>
+        <v>TSQPD267505U25KE</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>RN631370P</v>
+        <v>PE8026084V</v>
       </c>
       <c r="B9" t="s">
         <v>1530</v>
@@ -22237,13 +22256,13 @@
       </c>
       <c r="I9" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>LNPEJ522407M75FA</v>
+        <v>QHHFW849819G73SK</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>TF7111255N</v>
+        <v>UJ6346553Q</v>
       </c>
       <c r="B10" t="s">
         <v>1531</v>
@@ -22253,13 +22272,13 @@
       </c>
       <c r="I10" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>BCEBM885377G13NV</v>
+        <v>VMLWT400161V3QU</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>RB2273593S</v>
+        <v>FR9742762V</v>
       </c>
       <c r="B11" t="s">
         <v>1532</v>
@@ -22269,13 +22288,13 @@
       </c>
       <c r="I11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NWRVM419400B53MS</v>
+        <v>HDJLS423278E75BF</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>GJ7780082U</v>
+        <v>OO1973927S</v>
       </c>
       <c r="B12" t="s">
         <v>1533</v>
@@ -22285,13 +22304,13 @@
       </c>
       <c r="I12" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>JRUHS836972B97TY</v>
+        <v>FGXXX546840B94EB</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>YU2903988H</v>
+        <v>AM7627974T</v>
       </c>
       <c r="B13" t="s">
         <v>1534</v>
@@ -22301,13 +22320,13 @@
       </c>
       <c r="I13" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>AMRST467739L47WL</v>
+        <v>QAIJZ741113V23AS</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>JN8096360O</v>
+        <v>ZN2509346F</v>
       </c>
       <c r="B14" t="s">
         <v>1535</v>
@@ -22317,13 +22336,13 @@
       </c>
       <c r="I14" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>URHFH233567P97VT</v>
+        <v>UUQVH573718N24JZ</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>DZ9019667P</v>
+        <v>MS285860P</v>
       </c>
       <c r="B15" t="s">
         <v>1536</v>
@@ -22333,13 +22352,13 @@
       </c>
       <c r="I15" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>BHNEY292408J12RE</v>
+        <v>BDQZO140075N9EA</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>SJ2229640A</v>
+        <v>PK3464015Q</v>
       </c>
       <c r="B16" t="s">
         <v>1537</v>
@@ -22349,13 +22368,13 @@
       </c>
       <c r="I16" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CUEEH516593S10QJ</v>
+        <v>WITPE166526Y19WW</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>AM3678173N</v>
+        <v>MZ5360747K</v>
       </c>
       <c r="B17" t="s">
         <v>1538</v>
@@ -22365,13 +22384,13 @@
       </c>
       <c r="I17" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>VWRCF31307V9YK</v>
+        <v>QJVDE311067C61YH</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NA716399P</v>
+        <v>DS6589469D</v>
       </c>
       <c r="B18" t="s">
         <v>1539</v>
@@ -22381,13 +22400,13 @@
       </c>
       <c r="I18" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>SRWWN190815K46JP</v>
+        <v>EYIWG86832G17ML</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>TT7416825D</v>
+        <v>DS2066725W</v>
       </c>
       <c r="B19" t="s">
         <v>1540</v>
@@ -22397,13 +22416,13 @@
       </c>
       <c r="I19" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>GYEUM97870X72NL</v>
+        <v>IDPCU308422C29IC</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>WM5225748L</v>
+        <v>BZ6050621J</v>
       </c>
       <c r="B20" t="s">
         <v>1541</v>
@@ -22413,13 +22432,13 @@
       </c>
       <c r="I20" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>GQEKG407643B47FN</v>
+        <v>VFNVK483671U51HR</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>ZI8377422Y</v>
+        <v>FY9930767H</v>
       </c>
       <c r="B21" t="s">
         <v>1542</v>
@@ -22429,13 +22448,13 @@
       </c>
       <c r="I21" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CLWJS680243D68TW</v>
+        <v>CTXXT235608I5CR</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>IF9095438I</v>
+        <v>DA7984769B</v>
       </c>
       <c r="B22" t="s">
         <v>1543</v>
@@ -22445,13 +22464,13 @@
       </c>
       <c r="I22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>BMMYM149523L34KZ</v>
+        <v>WFJIS49961R36SD</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>SC2559513B</v>
+        <v>MZ1167152C</v>
       </c>
       <c r="B23" t="s">
         <v>1544</v>
@@ -22461,13 +22480,13 @@
       </c>
       <c r="I23" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>WINGD553012C93TV</v>
+        <v>RKRAY897774D93ED</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>TP6466743T</v>
+        <v>RV6367878Q</v>
       </c>
       <c r="B24" t="s">
         <v>1545</v>
@@ -22477,13 +22496,13 @@
       </c>
       <c r="I24" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>WIKEQ610173I2ER</v>
+        <v>LUQLC743025Z74AG</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>HJ752514Q</v>
+        <v>TD4397729U</v>
       </c>
       <c r="B25" t="s">
         <v>1546</v>
@@ -22493,13 +22512,13 @@
       </c>
       <c r="I25" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>MRDJD419509H97LE</v>
+        <v>HSCWC121357C28MC</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>BO9528760L</v>
+        <v>FO2189346F</v>
       </c>
       <c r="B26" t="s">
         <v>1547</v>
@@ -22509,13 +22528,13 @@
       </c>
       <c r="I26" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>QZLNR610623J70KW</v>
+        <v>TLLPW659117F30TC</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UQ7329929A</v>
+        <v>WT8095498G</v>
       </c>
       <c r="B27" t="s">
         <v>1548</v>
@@ -22525,13 +22544,13 @@
       </c>
       <c r="I27" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>LGUOF48629Q27WZ</v>
+        <v>YJWAD236217Q5HL</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>KM7084582A</v>
+        <v>TU9442855M</v>
       </c>
       <c r="B28" t="s">
         <v>1549</v>
@@ -22541,13 +22560,13 @@
       </c>
       <c r="I28" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>SLBEM957967K40UE</v>
+        <v>CSOVT343465C43AD</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>EE9452695T</v>
+        <v>CA5404397W</v>
       </c>
       <c r="B29" t="s">
         <v>1550</v>
@@ -22557,13 +22576,13 @@
       </c>
       <c r="I29" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>MRMXR466637E90AO</v>
+        <v>VNGAN424275G75YG</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>AK2953288D</v>
+        <v>GO8812679U</v>
       </c>
       <c r="B30" t="s">
         <v>1551</v>
@@ -22573,13 +22592,13 @@
       </c>
       <c r="I30" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>FNSQP134056E37ZK</v>
+        <v>DWNNW426546N39GT</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>WN7224090U</v>
+        <v>KY4751165Q</v>
       </c>
       <c r="B31" t="s">
         <v>1552</v>
@@ -22589,13 +22608,13 @@
       </c>
       <c r="I31" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>SMHJB361090R85FQ</v>
+        <v>SSISQ5058R39LV</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>AE5652429D</v>
+        <v>PT3462173B</v>
       </c>
       <c r="B32" t="s">
         <v>1553</v>
@@ -22605,13 +22624,13 @@
       </c>
       <c r="I32" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>JIVGZ639243P29NN</v>
+        <v>ZHOZE560353L14KP</v>
       </c>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>ET7707455L</v>
+        <v>AV748217A</v>
       </c>
       <c r="B33" t="s">
         <v>1554</v>
@@ -22621,13 +22640,13 @@
       </c>
       <c r="I33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>MOWJS278341J74VA</v>
+        <v>YVKWP490506C80XN</v>
       </c>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>OL5339815K</v>
+        <v>UB9078949H</v>
       </c>
       <c r="B34" t="s">
         <v>1555</v>
@@ -22637,13 +22656,13 @@
       </c>
       <c r="I34" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>FUHYM546698S15FA</v>
+        <v>TJMLY180361A48IZ</v>
       </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>CE8523483A</v>
+        <v>DV5274031C</v>
       </c>
       <c r="B35" t="s">
         <v>1556</v>
@@ -22653,13 +22672,13 @@
       </c>
       <c r="I35" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>SHUPN955204E22PS</v>
+        <v>QVRVQ620329S92JT</v>
       </c>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>VY7624756E</v>
+        <v>YO1474767H</v>
       </c>
       <c r="B36" t="s">
         <v>1557</v>
@@ -22669,13 +22688,13 @@
       </c>
       <c r="I36" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CUPTA620916T15NR</v>
+        <v>BBJXW924248E96LV</v>
       </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UA1897544C</v>
+        <v>WY1824881R</v>
       </c>
       <c r="B37" t="s">
         <v>1558</v>
@@ -22685,13 +22704,13 @@
       </c>
       <c r="I37" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>OSFQA957867P68DW</v>
+        <v>OTGXM807574U57SB</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>MM5735803Z</v>
+        <v>RF8971443R</v>
       </c>
       <c r="B38" t="s">
         <v>1559</v>
@@ -22701,13 +22720,13 @@
       </c>
       <c r="I38" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>QFGAB377534O33XO</v>
+        <v>MXJGZ572760F43FN</v>
       </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>XX8845658X</v>
+        <v>VW5870110O</v>
       </c>
       <c r="B39" t="s">
         <v>1560</v>
@@ -22717,13 +22736,13 @@
       </c>
       <c r="I39" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CJRAA725831O26JL</v>
+        <v>CZPFY970199G3NB</v>
       </c>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>MJ9246883H</v>
+        <v>HS4624253I</v>
       </c>
       <c r="B40" t="s">
         <v>1561</v>
@@ -22733,13 +22752,13 @@
       </c>
       <c r="I40" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>JAXHE527816A23XD</v>
+        <v>RLIDA21141P4UL</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>BB5431499E</v>
+        <v>KQ7183154C</v>
       </c>
       <c r="B41" t="s">
         <v>1562</v>
@@ -22749,13 +22768,13 @@
       </c>
       <c r="I41" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NVABQ846455Z18AJ</v>
+        <v>YPCJT88257B59HO</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>JL3460485X</v>
+        <v>XG4109783J</v>
       </c>
       <c r="B42" t="s">
         <v>1563</v>
@@ -22765,13 +22784,13 @@
       </c>
       <c r="I42" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>IPTOC53411M41NF</v>
+        <v>GFLJB932020M25EF</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>SL6797624D</v>
+        <v>KP258707H</v>
       </c>
       <c r="B43" t="s">
         <v>1564</v>
@@ -22781,13 +22800,13 @@
       </c>
       <c r="I43" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>YECDJ836234C51EX</v>
+        <v>ATAKQ907701D98HZ</v>
       </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>TU7140186P</v>
+        <v>QY7227832G</v>
       </c>
       <c r="B44" t="s">
         <v>1565</v>
@@ -22797,13 +22816,13 @@
       </c>
       <c r="I44" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>LFXQB323657C99OA</v>
+        <v>AJAAP420926Y31XI</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>JK774022P</v>
+        <v>CG8950995S</v>
       </c>
       <c r="B45" t="s">
         <v>1566</v>
@@ -22813,13 +22832,13 @@
       </c>
       <c r="I45" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>JGIDJ793819C8FV</v>
+        <v>TPVZX916054A94YR</v>
       </c>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>AL5751819O</v>
+        <v>NG2510648W</v>
       </c>
       <c r="B46" t="s">
         <v>1567</v>
@@ -22829,13 +22848,13 @@
       </c>
       <c r="I46" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>DNPLL392081P70US</v>
+        <v>DZIJU27376P70YN</v>
       </c>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>IU3335505R</v>
+        <v>OO9896779D</v>
       </c>
       <c r="B47" t="s">
         <v>1568</v>
@@ -22845,13 +22864,13 @@
       </c>
       <c r="I47" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>JQOQV580987R7PH</v>
+        <v>YVWIQ307999T60FB</v>
       </c>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NM3238843T</v>
+        <v>IC1057284K</v>
       </c>
       <c r="B48" t="s">
         <v>1569</v>
@@ -22861,13 +22880,13 @@
       </c>
       <c r="I48" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>SFREE586998X26YB</v>
+        <v>DATZQ327281G82DR</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LH5926835S</v>
+        <v>PA3695094N</v>
       </c>
       <c r="B49" t="s">
         <v>1570</v>
@@ -22877,13 +22896,13 @@
       </c>
       <c r="I49" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>RNRGU801547Y11KJ</v>
+        <v>KTQHZ140133M93QM</v>
       </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>JQ5992601U</v>
+        <v>UQ7403731G</v>
       </c>
       <c r="B50" t="s">
         <v>1571</v>
@@ -22893,13 +22912,13 @@
       </c>
       <c r="I50" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>VRPIK515748L34FM</v>
+        <v>XZRKP173825Q6AQ</v>
       </c>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LQ9733155T</v>
+        <v>UE2541396W</v>
       </c>
       <c r="B51" t="s">
         <v>1572</v>
@@ -22909,13 +22928,13 @@
       </c>
       <c r="I51" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>UIBVF616684Y67OI</v>
+        <v>XJNRC200895O31WD</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>GR8854352Q</v>
+        <v>AD7900362H</v>
       </c>
       <c r="B52" t="s">
         <v>1573</v>
@@ -22925,13 +22944,13 @@
       </c>
       <c r="I52" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>XFLBU903704R1TQ</v>
+        <v>SGIUV368536T67FY</v>
       </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>ND6479163A</v>
+        <v>PW5067173D</v>
       </c>
       <c r="B53" t="s">
         <v>1574</v>
@@ -22941,13 +22960,13 @@
       </c>
       <c r="I53" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>OVFVQ806383K52AW</v>
+        <v>SYLPP827214D8HW</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UQ2100426Y</v>
+        <v>LL6935662F</v>
       </c>
       <c r="B54" t="s">
         <v>1575</v>
@@ -22957,13 +22976,13 @@
       </c>
       <c r="I54" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CBYOO980449G82IF</v>
+        <v>JPYQT836358V96NO</v>
       </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>ED7774218Z</v>
+        <v>TV2210165V</v>
       </c>
       <c r="B55" t="s">
         <v>1576</v>
@@ -22973,13 +22992,13 @@
       </c>
       <c r="I55" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>JPCPQ904774W46WR</v>
+        <v>WLJSA980288E21OR</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UF5864304Q</v>
+        <v>AK1607462F</v>
       </c>
       <c r="B56" t="s">
         <v>1577</v>
@@ -22989,13 +23008,13 @@
       </c>
       <c r="I56" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>INFEU727272S40YT</v>
+        <v>NFOTK725322H75ZY</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>TY7634671Y</v>
+        <v>XF5659122U</v>
       </c>
       <c r="B57" t="s">
         <v>1578</v>
@@ -23005,13 +23024,13 @@
       </c>
       <c r="I57" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>UJDAW797706V41AU</v>
+        <v>YWZBQ779835V21ML</v>
       </c>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>MD7261864L</v>
+        <v>TB5832512G</v>
       </c>
       <c r="B58" t="s">
         <v>1579</v>
@@ -23021,13 +23040,13 @@
       </c>
       <c r="I58" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>ZJNNJ835774J5NH</v>
+        <v>XUWBH158422N13KN</v>
       </c>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>EY3691743L</v>
+        <v>UL9073232Y</v>
       </c>
       <c r="B59" t="s">
         <v>1580</v>
@@ -23037,13 +23056,13 @@
       </c>
       <c r="I59" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>RWSLG545251Q64TD</v>
+        <v>TCHUR177497H6EC</v>
       </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>ZG7333059Q</v>
+        <v>UA8041102W</v>
       </c>
       <c r="B60" t="s">
         <v>1581</v>
@@ -23053,13 +23072,13 @@
       </c>
       <c r="I60" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>SWRFV933222H96WD</v>
+        <v>OIYKL684256M31BZ</v>
       </c>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>WR2729994M</v>
+        <v>OI2111963O</v>
       </c>
       <c r="B61" t="s">
         <v>1582</v>
@@ -23069,13 +23088,13 @@
       </c>
       <c r="I61" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>GVIQB480398S60NX</v>
+        <v>IBQXV279382J40TI</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>ZA5596760Y</v>
+        <v>DH9457180R</v>
       </c>
       <c r="B62" t="s">
         <v>1583</v>
@@ -23085,13 +23104,13 @@
       </c>
       <c r="I62" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>WTAGY885406M12FH</v>
+        <v>UVGPE825414T54DT</v>
       </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>TA5802213M</v>
+        <v>KX3778623N</v>
       </c>
       <c r="B63" t="s">
         <v>1584</v>
@@ -23101,13 +23120,13 @@
       </c>
       <c r="I63" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>JDNGC977310I81QP</v>
+        <v>GDYHL266485I40DX</v>
       </c>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>TC1028544K</v>
+        <v>GC1614231R</v>
       </c>
       <c r="B64" t="s">
         <v>1585</v>
@@ -23117,13 +23136,13 @@
       </c>
       <c r="I64" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>ZPVFQ950291F20FK</v>
+        <v>WZHZV832194Y31YX</v>
       </c>
     </row>
     <row r="65" spans="1:9">
       <c r="A65" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>VG9882146K</v>
+        <v>CN801035V</v>
       </c>
       <c r="B65" t="s">
         <v>1586</v>
@@ -23133,13 +23152,13 @@
       </c>
       <c r="I65" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>YVVFW605406W18JR</v>
+        <v>XRICP459975D60DI</v>
       </c>
     </row>
     <row r="66" spans="1:9">
       <c r="A66" s="6" t="str">
         <f t="shared" ref="A66:A129" ca="1" si="3">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,9999999)&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>NY1409835V</v>
+        <v>ZM6058726H</v>
       </c>
       <c r="B66" t="s">
         <v>1587</v>
@@ -23149,13 +23168,13 @@
       </c>
       <c r="I66" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CYWMX864158W93IP</v>
+        <v>EBTGH937344B8OH</v>
       </c>
     </row>
     <row r="67" spans="1:9">
       <c r="A67" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>XY5829415A</v>
+        <v>PE2288016U</v>
       </c>
       <c r="B67" t="s">
         <v>1588</v>
@@ -23165,13 +23184,13 @@
       </c>
       <c r="I67" t="str">
         <f t="shared" ref="I67:I130" ca="1" si="4">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,999999)&amp;CHAR(RANDBETWEEN(65,90))&amp;(RANDBETWEEN(1,99))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>ACYHP469799Q24QL</v>
+        <v>TKAOC332965N33PA</v>
       </c>
     </row>
     <row r="68" spans="1:9">
       <c r="A68" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>VI135431M</v>
+        <v>PB4527600V</v>
       </c>
       <c r="B68" t="s">
         <v>1589</v>
@@ -23181,13 +23200,13 @@
       </c>
       <c r="I68" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>FZRKU570888S34GW</v>
+        <v>XORUD241811Y13JV</v>
       </c>
     </row>
     <row r="69" spans="1:9">
       <c r="A69" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>BK5843042G</v>
+        <v>HX7312911R</v>
       </c>
       <c r="B69" t="s">
         <v>1590</v>
@@ -23197,13 +23216,13 @@
       </c>
       <c r="I69" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>LHXDI128486D26CB</v>
+        <v>NBLSC909220J55RY</v>
       </c>
     </row>
     <row r="70" spans="1:9">
       <c r="A70" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>XA6244729I</v>
+        <v>PT6351447X</v>
       </c>
       <c r="B70" t="s">
         <v>1591</v>
@@ -23213,13 +23232,13 @@
       </c>
       <c r="I70" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>YONNI979534F89MT</v>
+        <v>OMZTE997150P58MZ</v>
       </c>
     </row>
     <row r="71" spans="1:9">
       <c r="A71" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>HB7414501D</v>
+        <v>QA2096072O</v>
       </c>
       <c r="B71" t="s">
         <v>1592</v>
@@ -23229,13 +23248,13 @@
       </c>
       <c r="I71" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>MLRDL338722V77PH</v>
+        <v>RXYFE807193O88MH</v>
       </c>
     </row>
     <row r="72" spans="1:9">
       <c r="A72" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>RB5182593F</v>
+        <v>UT503091E</v>
       </c>
       <c r="B72" t="s">
         <v>1593</v>
@@ -23245,13 +23264,13 @@
       </c>
       <c r="I72" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>KXEQT490164A82UQ</v>
+        <v>ACEQB937469I63PP</v>
       </c>
     </row>
     <row r="73" spans="1:9">
       <c r="A73" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>WK4184974G</v>
+        <v>JJ2048015Y</v>
       </c>
       <c r="B73" t="s">
         <v>1594</v>
@@ -23261,13 +23280,13 @@
       </c>
       <c r="I73" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>YZVPQ585190S39DC</v>
+        <v>KRUAJ973913F28KB</v>
       </c>
     </row>
     <row r="74" spans="1:9">
       <c r="A74" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>SP7723634J</v>
+        <v>NZ9448336L</v>
       </c>
       <c r="B74" t="s">
         <v>1595</v>
@@ -23277,13 +23296,13 @@
       </c>
       <c r="I74" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>VGCVP156372R60KF</v>
+        <v>EQDFA213544N31GJ</v>
       </c>
     </row>
     <row r="75" spans="1:9">
       <c r="A75" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>PK9275830M</v>
+        <v>BT7712427L</v>
       </c>
       <c r="B75" t="s">
         <v>1596</v>
@@ -23293,13 +23312,13 @@
       </c>
       <c r="I75" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>UOWGD162236J36QH</v>
+        <v>KZYBL616166A91DL</v>
       </c>
     </row>
     <row r="76" spans="1:9">
       <c r="A76" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>QO39967H</v>
+        <v>TQ1373896P</v>
       </c>
       <c r="B76" t="s">
         <v>1597</v>
@@ -23309,13 +23328,13 @@
       </c>
       <c r="I76" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>JVZXA606152P89OM</v>
+        <v>LFDYD815794T54JO</v>
       </c>
     </row>
     <row r="77" spans="1:9">
       <c r="A77" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>CK2674577I</v>
+        <v>HD3089506P</v>
       </c>
       <c r="B77" t="s">
         <v>1598</v>
@@ -23325,13 +23344,13 @@
       </c>
       <c r="I77" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>KAFNT62832B92JT</v>
+        <v>MXOAN891109O87JN</v>
       </c>
     </row>
     <row r="78" spans="1:9">
       <c r="A78" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>CK1047630Y</v>
+        <v>CJ9473767J</v>
       </c>
       <c r="B78" t="s">
         <v>1599</v>
@@ -23341,13 +23360,13 @@
       </c>
       <c r="I78" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>CHYJI677548W14CN</v>
+        <v>IVGJE988929V17HG</v>
       </c>
     </row>
     <row r="79" spans="1:9">
       <c r="A79" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>PQ6052265A</v>
+        <v>VD1064366J</v>
       </c>
       <c r="B79" t="s">
         <v>1600</v>
@@ -23357,13 +23376,13 @@
       </c>
       <c r="I79" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>IIOQD504517V18MZ</v>
+        <v>WMNIL684950U31KO</v>
       </c>
     </row>
     <row r="80" spans="1:9">
       <c r="A80" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>BK5515648T</v>
+        <v>WT6665250E</v>
       </c>
       <c r="B80" t="s">
         <v>1601</v>
@@ -23373,13 +23392,13 @@
       </c>
       <c r="I80" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>LUGNP251581X43BC</v>
+        <v>VFSFP693937T43MR</v>
       </c>
     </row>
     <row r="81" spans="1:9">
       <c r="A81" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>HI5639858O</v>
+        <v>WW2116527L</v>
       </c>
       <c r="B81" t="s">
         <v>1602</v>
@@ -23389,13 +23408,13 @@
       </c>
       <c r="I81" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>PPFGE894268P37IO</v>
+        <v>XFXXQ3725K51VI</v>
       </c>
     </row>
     <row r="82" spans="1:9">
       <c r="A82" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>LW5265528P</v>
+        <v>ES3196394G</v>
       </c>
       <c r="B82" t="s">
         <v>1603</v>
@@ -23405,13 +23424,13 @@
       </c>
       <c r="I82" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>EZVRJ585877B30IR</v>
+        <v>TCQFD379412W99LL</v>
       </c>
     </row>
     <row r="83" spans="1:9">
       <c r="A83" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>NO4048047R</v>
+        <v>CK4361444P</v>
       </c>
       <c r="B83" t="s">
         <v>1604</v>
@@ -23421,13 +23440,13 @@
       </c>
       <c r="I83" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>EOMNJ991344P13OP</v>
+        <v>TLIUT689253D99SM</v>
       </c>
     </row>
     <row r="84" spans="1:9">
       <c r="A84" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>RY8145448K</v>
+        <v>PL8274198Z</v>
       </c>
       <c r="B84" t="s">
         <v>1605</v>
@@ -23437,13 +23456,13 @@
       </c>
       <c r="I84" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>DGYXP350588G60IY</v>
+        <v>AAJLT180993J31ND</v>
       </c>
     </row>
     <row r="85" spans="1:9">
       <c r="A85" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>LD362635C</v>
+        <v>ED3850384Q</v>
       </c>
       <c r="B85" t="s">
         <v>1606</v>
@@ -23453,13 +23472,13 @@
       </c>
       <c r="I85" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>NOOHJ816332M28PA</v>
+        <v>QEOXB958560U81PU</v>
       </c>
     </row>
     <row r="86" spans="1:9">
       <c r="A86" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>AP9368058L</v>
+        <v>EC933825D</v>
       </c>
       <c r="B86" t="s">
         <v>1607</v>
@@ -23469,13 +23488,13 @@
       </c>
       <c r="I86" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>JUCYF1343M69GR</v>
+        <v>NHFCK387541E51ZR</v>
       </c>
     </row>
     <row r="87" spans="1:9">
       <c r="A87" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>OI5068889I</v>
+        <v>OE1657988G</v>
       </c>
       <c r="B87" t="s">
         <v>1608</v>
@@ -23485,13 +23504,13 @@
       </c>
       <c r="I87" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>ZSMEH650182U24RJ</v>
+        <v>SZUQT14346Q54OI</v>
       </c>
     </row>
     <row r="88" spans="1:9">
       <c r="A88" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>VD1038245S</v>
+        <v>KG2466555R</v>
       </c>
       <c r="B88" t="s">
         <v>1609</v>
@@ -23501,13 +23520,13 @@
       </c>
       <c r="I88" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>LNXQR418980G17NT</v>
+        <v>UUIUW521038Y82MQ</v>
       </c>
     </row>
     <row r="89" spans="1:9">
       <c r="A89" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>MG7241958B</v>
+        <v>QJ3483783Z</v>
       </c>
       <c r="B89" t="s">
         <v>1610</v>
@@ -23517,13 +23536,13 @@
       </c>
       <c r="I89" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>YEGTC905467W10FX</v>
+        <v>KDDAP239760N26VS</v>
       </c>
     </row>
     <row r="90" spans="1:9">
       <c r="A90" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>GU4207029E</v>
+        <v>OP7166219S</v>
       </c>
       <c r="B90" t="s">
         <v>1611</v>
@@ -23533,13 +23552,13 @@
       </c>
       <c r="I90" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>AMOYE507850M76QU</v>
+        <v>YSGHC377068R44XC</v>
       </c>
     </row>
     <row r="91" spans="1:9">
       <c r="A91" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>FD5718082Z</v>
+        <v>BR5576327I</v>
       </c>
       <c r="B91" t="s">
         <v>1612</v>
@@ -23549,13 +23568,13 @@
       </c>
       <c r="I91" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>XSIQG155848C38HR</v>
+        <v>NLYDQ138089V53HK</v>
       </c>
     </row>
     <row r="92" spans="1:9">
       <c r="A92" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>DD2834817X</v>
+        <v>HJ5247975K</v>
       </c>
       <c r="B92" t="s">
         <v>1613</v>
@@ -23565,13 +23584,13 @@
       </c>
       <c r="I92" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>GCKPP465158R8PM</v>
+        <v>GHIAK912880V88QP</v>
       </c>
     </row>
     <row r="93" spans="1:9">
       <c r="A93" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>MH2157844O</v>
+        <v>EL1365628F</v>
       </c>
       <c r="B93" t="s">
         <v>1614</v>
@@ -23581,13 +23600,13 @@
       </c>
       <c r="I93" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>FHQJW232185U37GV</v>
+        <v>NCVIV281171V11ZV</v>
       </c>
     </row>
     <row r="94" spans="1:9">
       <c r="A94" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>DO6484225J</v>
+        <v>TM6739124V</v>
       </c>
       <c r="B94" t="s">
         <v>1615</v>
@@ -23597,13 +23616,13 @@
       </c>
       <c r="I94" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>IKGVX370172F72MZ</v>
+        <v>OBDRX597659R89QW</v>
       </c>
     </row>
     <row r="95" spans="1:9">
       <c r="A95" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>OS2710654G</v>
+        <v>NO3961568U</v>
       </c>
       <c r="B95" t="s">
         <v>1616</v>
@@ -23613,13 +23632,13 @@
       </c>
       <c r="I95" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>FORWN4217G82WQ</v>
+        <v>EPYWM29002Q38QW</v>
       </c>
     </row>
     <row r="96" spans="1:9">
       <c r="A96" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>CG6381857B</v>
+        <v>WJ2253720B</v>
       </c>
       <c r="B96" t="s">
         <v>1617</v>
@@ -23629,13 +23648,13 @@
       </c>
       <c r="I96" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>JAKNX156030M92XD</v>
+        <v>OUXDC506584C23LU</v>
       </c>
     </row>
     <row r="97" spans="1:9">
       <c r="A97" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>RH7525132L</v>
+        <v>CW3133428T</v>
       </c>
       <c r="B97" t="s">
         <v>1618</v>
@@ -23645,13 +23664,13 @@
       </c>
       <c r="I97" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>XCSSR381887L15WG</v>
+        <v>KHDDG366065H16HB</v>
       </c>
     </row>
     <row r="98" spans="1:9">
       <c r="A98" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>EP4572634F</v>
+        <v>NW2482391L</v>
       </c>
       <c r="B98" t="s">
         <v>1619</v>
@@ -23661,13 +23680,13 @@
       </c>
       <c r="I98" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>SJBIX252047U91RS</v>
+        <v>TBDYB828992S1SO</v>
       </c>
     </row>
     <row r="99" spans="1:9">
       <c r="A99" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>YO5575627C</v>
+        <v>UT7511480S</v>
       </c>
       <c r="B99" t="s">
         <v>1620</v>
@@ -23677,13 +23696,13 @@
       </c>
       <c r="I99" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>YVCNO937772C56WN</v>
+        <v>SWXIL482782H42KL</v>
       </c>
     </row>
     <row r="100" spans="1:9">
       <c r="A100" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>CY6368958G</v>
+        <v>MJ4535359W</v>
       </c>
       <c r="B100" t="s">
         <v>1621</v>
@@ -23693,13 +23712,13 @@
       </c>
       <c r="I100" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>EFGZG853678L5PY</v>
+        <v>OZLBN498563X58SS</v>
       </c>
     </row>
     <row r="101" spans="1:9">
       <c r="A101" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>RT5083906H</v>
+        <v>XE4919888I</v>
       </c>
       <c r="B101" t="s">
         <v>1622</v>
@@ -23709,13 +23728,13 @@
       </c>
       <c r="I101" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>YUYVJ92552Z95EM</v>
+        <v>XYIVI737431C80GV</v>
       </c>
     </row>
     <row r="102" spans="1:9">
       <c r="A102" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UI1688112M</v>
+        <v>PH8743968O</v>
       </c>
       <c r="B102" t="s">
         <v>1623</v>
@@ -23725,13 +23744,13 @@
       </c>
       <c r="I102" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>SESKV159186N84ZY</v>
+        <v>ZXNUW755092F90TF</v>
       </c>
     </row>
     <row r="103" spans="1:9">
       <c r="A103" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>KF1440391Z</v>
+        <v>UZ9038451F</v>
       </c>
       <c r="B103" t="s">
         <v>1624</v>
@@ -23741,13 +23760,13 @@
       </c>
       <c r="I103" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>QBPHE23081U56NZ</v>
+        <v>GUQYU964253P34GD</v>
       </c>
     </row>
     <row r="104" spans="1:9">
       <c r="A104" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>GA7219804O</v>
+        <v>UF5885440W</v>
       </c>
       <c r="B104" t="s">
         <v>1625</v>
@@ -23757,13 +23776,13 @@
       </c>
       <c r="I104" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>PDJVS128814I6SD</v>
+        <v>WMIZJ265277P35WD</v>
       </c>
     </row>
     <row r="105" spans="1:9">
       <c r="A105" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UU8421789O</v>
+        <v>IW5251638M</v>
       </c>
       <c r="B105" t="s">
         <v>1626</v>
@@ -23773,13 +23792,13 @@
       </c>
       <c r="I105" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>UBTVF612765S67FL</v>
+        <v>PBIHS12201Z71MD</v>
       </c>
     </row>
     <row r="106" spans="1:9">
       <c r="A106" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>QR1781668U</v>
+        <v>RO2628537T</v>
       </c>
       <c r="B106" t="s">
         <v>1627</v>
@@ -23789,13 +23808,13 @@
       </c>
       <c r="I106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>UIKDJ930450Q22YB</v>
+        <v>NKXGM59202A60HG</v>
       </c>
     </row>
     <row r="107" spans="1:9">
       <c r="A107" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>LB5842341M</v>
+        <v>QU8647351T</v>
       </c>
       <c r="B107" t="s">
         <v>1628</v>
@@ -23805,13 +23824,13 @@
       </c>
       <c r="I107" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>CIHRC703136K70FP</v>
+        <v>FXCAK262799D17PW</v>
       </c>
     </row>
     <row r="108" spans="1:9">
       <c r="A108" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>EG4308465G</v>
+        <v>ZA2868902S</v>
       </c>
       <c r="B108" t="s">
         <v>1629</v>
@@ -23821,13 +23840,13 @@
       </c>
       <c r="I108" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>XSOJL419495A36LT</v>
+        <v>RARUY6477S47RM</v>
       </c>
     </row>
     <row r="109" spans="1:9">
       <c r="A109" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>WL7366657K</v>
+        <v>EY628135N</v>
       </c>
       <c r="B109" t="s">
         <v>1630</v>
@@ -23837,13 +23856,13 @@
       </c>
       <c r="I109" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>SROOM803590Q25SQ</v>
+        <v>YMNPK552829Z3UU</v>
       </c>
     </row>
     <row r="110" spans="1:9">
       <c r="A110" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>NS5256593C</v>
+        <v>YY4904058U</v>
       </c>
       <c r="B110" t="s">
         <v>1631</v>
@@ -23853,13 +23872,13 @@
       </c>
       <c r="I110" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>MLUGQ782262N18OK</v>
+        <v>VRZTH102336O94ON</v>
       </c>
     </row>
     <row r="111" spans="1:9">
       <c r="A111" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UX4866110U</v>
+        <v>VF7990217K</v>
       </c>
       <c r="B111" t="s">
         <v>1632</v>
@@ -23869,13 +23888,13 @@
       </c>
       <c r="I111" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>IFZFC424154R19FX</v>
+        <v>ZDBGB891727Z60OX</v>
       </c>
     </row>
     <row r="112" spans="1:9">
       <c r="A112" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>BM5554563J</v>
+        <v>BV9757594P</v>
       </c>
       <c r="B112" t="s">
         <v>1633</v>
@@ -23885,13 +23904,13 @@
       </c>
       <c r="I112" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>BHRQP24665M56FM</v>
+        <v>MVARN800905N91OZ</v>
       </c>
     </row>
     <row r="113" spans="1:9">
       <c r="A113" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>FU101691D</v>
+        <v>HJ7786415Q</v>
       </c>
       <c r="B113" t="s">
         <v>1634</v>
@@ -23901,13 +23920,13 @@
       </c>
       <c r="I113" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>CRYRP552819K69AU</v>
+        <v>VRELE830942S98NQ</v>
       </c>
     </row>
     <row r="114" spans="1:9">
       <c r="A114" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>KN9749847L</v>
+        <v>AE8626955H</v>
       </c>
       <c r="B114" t="s">
         <v>1635</v>
@@ -23917,13 +23936,13 @@
       </c>
       <c r="I114" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>UMSYM111307A81DJ</v>
+        <v>KAXAH233741D5XV</v>
       </c>
     </row>
     <row r="115" spans="1:9">
       <c r="A115" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>VX2362269F</v>
+        <v>NB5373637Y</v>
       </c>
       <c r="B115" t="s">
         <v>1636</v>
@@ -23933,13 +23952,13 @@
       </c>
       <c r="I115" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>DIOZS654166I61UA</v>
+        <v>FJGJF148585J23YC</v>
       </c>
     </row>
     <row r="116" spans="1:9">
       <c r="A116" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>BI963112U</v>
+        <v>OI48325U</v>
       </c>
       <c r="B116" t="s">
         <v>1637</v>
@@ -23949,13 +23968,13 @@
       </c>
       <c r="I116" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>WVPYN430028O66PH</v>
+        <v>NTWSF260750J98KJ</v>
       </c>
     </row>
     <row r="117" spans="1:9">
       <c r="A117" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>FO4769281D</v>
+        <v>HP6359375G</v>
       </c>
       <c r="B117" t="s">
         <v>1638</v>
@@ -23965,13 +23984,13 @@
       </c>
       <c r="I117" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>QXAYG911728O99TL</v>
+        <v>ZIBAW59428R99YT</v>
       </c>
     </row>
     <row r="118" spans="1:9">
       <c r="A118" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>WX6857332V</v>
+        <v>CG1440786Z</v>
       </c>
       <c r="B118" t="s">
         <v>1639</v>
@@ -23981,13 +24000,13 @@
       </c>
       <c r="I118" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>XSUFJ80290Y4MW</v>
+        <v>LVYVH325333R24TZ</v>
       </c>
     </row>
     <row r="119" spans="1:9">
       <c r="A119" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>ZF8995279K</v>
+        <v>VU4990279F</v>
       </c>
       <c r="B119" t="s">
         <v>1640</v>
@@ -23997,13 +24016,13 @@
       </c>
       <c r="I119" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>ZRVPT647624P10TK</v>
+        <v>POTFM751334N43GH</v>
       </c>
     </row>
     <row r="120" spans="1:9">
       <c r="A120" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>ZH9274374E</v>
+        <v>IT4153582Q</v>
       </c>
       <c r="B120" t="s">
         <v>1641</v>
@@ -24013,13 +24032,13 @@
       </c>
       <c r="I120" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>YORTE720703P73ZT</v>
+        <v>IQBAT326074U89TQ</v>
       </c>
     </row>
     <row r="121" spans="1:9">
       <c r="A121" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>ZF8753755V</v>
+        <v>VD6724908O</v>
       </c>
       <c r="B121" t="s">
         <v>1642</v>
@@ -24029,13 +24048,13 @@
       </c>
       <c r="I121" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>OOGSB682480J20RO</v>
+        <v>VBJZK929232Y65JY</v>
       </c>
     </row>
     <row r="122" spans="1:9">
       <c r="A122" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>CX3839418E</v>
+        <v>OT5809224G</v>
       </c>
       <c r="B122" t="s">
         <v>1643</v>
@@ -24045,13 +24064,13 @@
       </c>
       <c r="I122" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>BZYDE439614R15FE</v>
+        <v>LVIYG545916P31QK</v>
       </c>
     </row>
     <row r="123" spans="1:9">
       <c r="A123" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>OZ9888030Y</v>
+        <v>AN5187211U</v>
       </c>
       <c r="B123" t="s">
         <v>1644</v>
@@ -24061,13 +24080,13 @@
       </c>
       <c r="I123" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>EFYHD222026P72PV</v>
+        <v>YXPXN596172R70AK</v>
       </c>
     </row>
     <row r="124" spans="1:9">
       <c r="A124" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>SO4324669V</v>
+        <v>BX7541172A</v>
       </c>
       <c r="B124" t="s">
         <v>1645</v>
@@ -24077,13 +24096,13 @@
       </c>
       <c r="I124" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>ZBRYK176423C47QR</v>
+        <v>EIYPM33382D98AU</v>
       </c>
     </row>
     <row r="125" spans="1:9">
       <c r="A125" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>IY3610320L</v>
+        <v>YO4483103B</v>
       </c>
       <c r="B125" t="s">
         <v>1646</v>
@@ -24093,13 +24112,13 @@
       </c>
       <c r="I125" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>NHNCK443412F90GW</v>
+        <v>KRSMI307931W59JK</v>
       </c>
     </row>
     <row r="126" spans="1:9">
       <c r="A126" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>QS9731275C</v>
+        <v>IB7740800W</v>
       </c>
       <c r="B126" t="s">
         <v>1647</v>
@@ -24109,13 +24128,13 @@
       </c>
       <c r="I126" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>YZHIU692671P31WD</v>
+        <v>HNTNS622830C15YO</v>
       </c>
     </row>
     <row r="127" spans="1:9">
       <c r="A127" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>LR5443023R</v>
+        <v>KB4136510Q</v>
       </c>
       <c r="B127" t="s">
         <v>1648</v>
@@ -24125,13 +24144,13 @@
       </c>
       <c r="I127" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>TBFYC922456E12HV</v>
+        <v>YAXOD271545B40KI</v>
       </c>
     </row>
     <row r="128" spans="1:9">
       <c r="A128" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>OW1253372B</v>
+        <v>UD1899872L</v>
       </c>
       <c r="B128" t="s">
         <v>1649</v>
@@ -24141,13 +24160,13 @@
       </c>
       <c r="I128" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>KKFQU610134L27DQ</v>
+        <v>NHTYS237251R82WZ</v>
       </c>
     </row>
     <row r="129" spans="1:9">
       <c r="A129" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>QL1502589O</v>
+        <v>GC3091085S</v>
       </c>
       <c r="B129" t="s">
         <v>1650</v>
@@ -24157,13 +24176,13 @@
       </c>
       <c r="I129" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>JMUON707505R9MS</v>
+        <v>ZESMO387159Z40CY</v>
       </c>
     </row>
     <row r="130" spans="1:9">
       <c r="A130" s="6" t="str">
         <f t="shared" ref="A130:A193" ca="1" si="5">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,9999999)&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>ZF9948026F</v>
+        <v>RE5211339T</v>
       </c>
       <c r="B130" t="s">
         <v>1651</v>
@@ -24173,13 +24192,13 @@
       </c>
       <c r="I130" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>GMBOX567049N24AB</v>
+        <v>TRGDR385338E58GD</v>
       </c>
     </row>
     <row r="131" spans="1:9">
       <c r="A131" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>VB5431459U</v>
+        <v>OJ8516873B</v>
       </c>
       <c r="B131" t="s">
         <v>1652</v>
@@ -24189,13 +24208,13 @@
       </c>
       <c r="I131" t="str">
         <f t="shared" ref="I131:I194" ca="1" si="6">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,999999)&amp;CHAR(RANDBETWEEN(65,90))&amp;(RANDBETWEEN(1,99))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>WRUWF923891L58GU</v>
+        <v>UIIXY154202O18TI</v>
       </c>
     </row>
     <row r="132" spans="1:9">
       <c r="A132" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>UQ2967739T</v>
+        <v>TC85668E</v>
       </c>
       <c r="B132" t="s">
         <v>1653</v>
@@ -24205,13 +24224,13 @@
       </c>
       <c r="I132" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>SYKQS495413W26TV</v>
+        <v>BJTZU153801Z1AM</v>
       </c>
     </row>
     <row r="133" spans="1:9">
       <c r="A133" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>BW3410640I</v>
+        <v>OG7002544K</v>
       </c>
       <c r="B133" t="s">
         <v>1654</v>
@@ -24221,13 +24240,13 @@
       </c>
       <c r="I133" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>CJXKQ489357N36PH</v>
+        <v>XLIKZ599756Y73BO</v>
       </c>
     </row>
     <row r="134" spans="1:9">
       <c r="A134" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>SZ4865787U</v>
+        <v>LL300333M</v>
       </c>
       <c r="B134" t="s">
         <v>1655</v>
@@ -24237,13 +24256,13 @@
       </c>
       <c r="I134" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>USHWF190988P19OW</v>
+        <v>NDMTG313150U98YJ</v>
       </c>
     </row>
     <row r="135" spans="1:9">
       <c r="A135" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>QL5312372B</v>
+        <v>OJ3259483Q</v>
       </c>
       <c r="B135" t="s">
         <v>1656</v>
@@ -24253,13 +24272,13 @@
       </c>
       <c r="I135" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>YOETU496087F60TN</v>
+        <v>AZVFV20492R33KH</v>
       </c>
     </row>
     <row r="136" spans="1:9">
       <c r="A136" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>GF7948560J</v>
+        <v>RG6714268O</v>
       </c>
       <c r="B136" t="s">
         <v>1657</v>
@@ -24269,13 +24288,13 @@
       </c>
       <c r="I136" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>TNRMA323184W97DK</v>
+        <v>GSQEG244619P98PP</v>
       </c>
     </row>
     <row r="137" spans="1:9">
       <c r="A137" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>QW9073640G</v>
+        <v>ON8440972B</v>
       </c>
       <c r="B137" t="s">
         <v>1658</v>
@@ -24285,13 +24304,13 @@
       </c>
       <c r="I137" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>DLUYD535099I26IC</v>
+        <v>LYVZM814780D97TQ</v>
       </c>
     </row>
     <row r="138" spans="1:9">
       <c r="A138" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>OF8527148I</v>
+        <v>VQ9809663G</v>
       </c>
       <c r="B138" t="s">
         <v>1659</v>
@@ -24301,13 +24320,13 @@
       </c>
       <c r="I138" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>JETOY336541X11DM</v>
+        <v>EAUXT190967M31ZB</v>
       </c>
     </row>
     <row r="139" spans="1:9">
       <c r="A139" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>KR5588135Y</v>
+        <v>ZT2361255T</v>
       </c>
       <c r="B139" t="s">
         <v>1660</v>
@@ -24317,13 +24336,13 @@
       </c>
       <c r="I139" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>AXVMR94504L17WI</v>
+        <v>CTMVY152525N50ZN</v>
       </c>
     </row>
     <row r="140" spans="1:9">
       <c r="A140" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>GI9071030D</v>
+        <v>SB8648009I</v>
       </c>
       <c r="B140" t="s">
         <v>1661</v>
@@ -24333,13 +24352,13 @@
       </c>
       <c r="I140" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>MDHDV271731Q79JN</v>
+        <v>RDJLC569049B77ZD</v>
       </c>
     </row>
     <row r="141" spans="1:9">
       <c r="A141" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>FM7272717Q</v>
+        <v>ZK2352316O</v>
       </c>
       <c r="B141" t="s">
         <v>1662</v>
@@ -24349,13 +24368,13 @@
       </c>
       <c r="I141" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>MSQHW259773V11WX</v>
+        <v>ZAFFN77363Q29MX</v>
       </c>
     </row>
     <row r="142" spans="1:9">
       <c r="A142" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>ZH2341533O</v>
+        <v>NH4455940Z</v>
       </c>
       <c r="B142" t="s">
         <v>1663</v>
@@ -24365,13 +24384,13 @@
       </c>
       <c r="I142" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>AGFGM459272P20PU</v>
+        <v>SXROL312832H79TN</v>
       </c>
     </row>
     <row r="143" spans="1:9">
       <c r="A143" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>RX4090232O</v>
+        <v>HD6309510B</v>
       </c>
       <c r="B143" t="s">
         <v>1664</v>
@@ -24381,13 +24400,13 @@
       </c>
       <c r="I143" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>ETHPN892782B92FR</v>
+        <v>JFKFY630662S87RX</v>
       </c>
     </row>
     <row r="144" spans="1:9">
       <c r="A144" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>UC9676432K</v>
+        <v>ZC2829374A</v>
       </c>
       <c r="B144" t="s">
         <v>1665</v>
@@ -24397,13 +24416,13 @@
       </c>
       <c r="I144" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>MZQXM775548E11HQ</v>
+        <v>ZXXYI73458U24RV</v>
       </c>
     </row>
     <row r="145" spans="1:12">
       <c r="A145" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>PN8602952T</v>
+        <v>EB7217877U</v>
       </c>
       <c r="B145" t="s">
         <v>1666</v>
@@ -24413,13 +24432,13 @@
       </c>
       <c r="I145" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>ZDSMB734185M83YF</v>
+        <v>VDYJF748139A9EH</v>
       </c>
     </row>
     <row r="146" spans="1:12">
       <c r="A146" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>PI741589T</v>
+        <v>NS2628688L</v>
       </c>
       <c r="B146" t="s">
         <v>1667</v>
@@ -24429,13 +24448,13 @@
       </c>
       <c r="I146" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>RSIYK229965G71GY</v>
+        <v>TFTEM406931N25NA</v>
       </c>
     </row>
     <row r="147" spans="1:12">
       <c r="A147" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>BJ8566749J</v>
+        <v>RF2576786I</v>
       </c>
       <c r="B147" t="s">
         <v>1668</v>
@@ -24445,13 +24464,13 @@
       </c>
       <c r="I147" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>XLRXE531499I60FB</v>
+        <v>BRMXY415236I34ZD</v>
       </c>
     </row>
     <row r="148" spans="1:12">
       <c r="A148" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>US4539777J</v>
+        <v>KW7122192D</v>
       </c>
       <c r="B148" t="s">
         <v>1669</v>
@@ -24461,13 +24480,13 @@
       </c>
       <c r="I148" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>NZXZG570337W44AZ</v>
+        <v>PXPLN620519J75PI</v>
       </c>
     </row>
     <row r="149" spans="1:12">
       <c r="A149" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>NL8215590D</v>
+        <v>QB9585165F</v>
       </c>
       <c r="B149" t="s">
         <v>1670</v>
@@ -24477,13 +24496,13 @@
       </c>
       <c r="I149" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>DWYEC613959G97UH</v>
+        <v>PLAPQ800229R81VP</v>
       </c>
     </row>
     <row r="150" spans="1:12">
       <c r="A150" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>BD643668C</v>
+        <v>CS5777346Z</v>
       </c>
       <c r="B150" t="s">
         <v>1671</v>
@@ -24493,13 +24512,13 @@
       </c>
       <c r="I150" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>OJLMQ395808U90NO</v>
+        <v>YXNHN214841V38JV</v>
       </c>
     </row>
     <row r="151" spans="1:12">
       <c r="A151" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>QQ96630Q</v>
+        <v>BU9072565W</v>
       </c>
       <c r="B151" t="s">
         <v>1672</v>
@@ -24509,13 +24528,13 @@
       </c>
       <c r="I151" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>ZKWYV449720Z27CW</v>
+        <v>YVNIN131256Z25SM</v>
       </c>
     </row>
     <row r="152" spans="1:12">
       <c r="A152" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>GM3651289I</v>
+        <v>ST5749492D</v>
       </c>
       <c r="B152" t="s">
         <v>1673</v>
@@ -24525,7 +24544,7 @@
       </c>
       <c r="I152" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>DIWVJ583399P93QS</v>
+        <v>QFHGC721673A26IV</v>
       </c>
       <c r="K152" s="28" t="e">
         <f t="shared" ref="K152" si="7">RIGHT(J152, LEN(J152)-1)</f>
@@ -24539,7 +24558,7 @@
     <row r="153" spans="1:12">
       <c r="A153" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>GJ8749128S</v>
+        <v>NR3505639K</v>
       </c>
       <c r="B153" t="s">
         <v>1674</v>
@@ -24549,13 +24568,13 @@
       </c>
       <c r="I153" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>ELKWX801627N36XR</v>
+        <v>QQBFV355926V50NV</v>
       </c>
     </row>
     <row r="154" spans="1:12">
       <c r="A154" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>GY5264136C</v>
+        <v>NP4209069U</v>
       </c>
       <c r="B154" t="s">
         <v>1675</v>
@@ -24565,13 +24584,13 @@
       </c>
       <c r="I154" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>HZINC838514Y10XP</v>
+        <v>QMFUJ702626Q15AJ</v>
       </c>
     </row>
     <row r="155" spans="1:12">
       <c r="A155" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>BV1839017B</v>
+        <v>QM1088819M</v>
       </c>
       <c r="B155" t="s">
         <v>1676</v>
@@ -24581,13 +24600,13 @@
       </c>
       <c r="I155" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>VXUTC529511H66YI</v>
+        <v>SVMGR100440U50PU</v>
       </c>
     </row>
     <row r="156" spans="1:12">
       <c r="A156" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>JR5019634D</v>
+        <v>QN5871547U</v>
       </c>
       <c r="B156" t="s">
         <v>1677</v>
@@ -24597,13 +24616,13 @@
       </c>
       <c r="I156" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>PFWVC821853G65IA</v>
+        <v>LLDJC325444Q25OJ</v>
       </c>
     </row>
     <row r="157" spans="1:12">
       <c r="A157" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>TD5913682C</v>
+        <v>UK7666136I</v>
       </c>
       <c r="B157" t="s">
         <v>1678</v>
@@ -24613,13 +24632,13 @@
       </c>
       <c r="I157" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>HQAYM48805V36ZI</v>
+        <v>KHUKC793379T49TL</v>
       </c>
     </row>
     <row r="158" spans="1:12">
       <c r="A158" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>IP17591L</v>
+        <v>XP7363449M</v>
       </c>
       <c r="B158" t="s">
         <v>1679</v>
@@ -24629,13 +24648,13 @@
       </c>
       <c r="I158" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>FENTP826611B40XB</v>
+        <v>PPEPL771250R82CT</v>
       </c>
     </row>
     <row r="159" spans="1:12">
       <c r="A159" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>GB7529484Y</v>
+        <v>DF3894386N</v>
       </c>
       <c r="B159" t="s">
         <v>1680</v>
@@ -24645,13 +24664,13 @@
       </c>
       <c r="I159" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>UEORU114971O99OJ</v>
+        <v>DVFEF924046P42YZ</v>
       </c>
     </row>
     <row r="160" spans="1:12">
       <c r="A160" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>UU6567567H</v>
+        <v>NG7570539E</v>
       </c>
       <c r="B160" t="s">
         <v>1681</v>
@@ -24661,13 +24680,13 @@
       </c>
       <c r="I160" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>MQFIQ187405U81LK</v>
+        <v>KLWWF639866M37FC</v>
       </c>
     </row>
     <row r="161" spans="1:9">
       <c r="A161" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>FP867510R</v>
+        <v>VA6281791K</v>
       </c>
       <c r="B161" t="s">
         <v>1682</v>
@@ -24677,13 +24696,13 @@
       </c>
       <c r="I161" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>QBOTM297306T45AL</v>
+        <v>GAISI620256U83VG</v>
       </c>
     </row>
     <row r="162" spans="1:9">
       <c r="A162" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>WN5597997V</v>
+        <v>AB3260599Q</v>
       </c>
       <c r="B162" t="s">
         <v>1683</v>
@@ -24693,13 +24712,13 @@
       </c>
       <c r="I162" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>WMQPK458290S9LL</v>
+        <v>MKQNT116153O45RK</v>
       </c>
     </row>
     <row r="163" spans="1:9">
       <c r="A163" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>WC4806063H</v>
+        <v>BG1806400N</v>
       </c>
       <c r="B163" t="s">
         <v>1684</v>
@@ -24709,13 +24728,13 @@
       </c>
       <c r="I163" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>YMJOH734583Y89MT</v>
+        <v>RCKJR844506C1CT</v>
       </c>
     </row>
     <row r="164" spans="1:9">
       <c r="A164" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>NP2027691H</v>
+        <v>EW3148458K</v>
       </c>
       <c r="B164" t="s">
         <v>1685</v>
@@ -24725,13 +24744,13 @@
       </c>
       <c r="I164" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>FCVOT929506E55TS</v>
+        <v>KDFFU762091K4MF</v>
       </c>
     </row>
     <row r="165" spans="1:9">
       <c r="A165" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>KI7267102K</v>
+        <v>TF3466957P</v>
       </c>
       <c r="B165" t="s">
         <v>1686</v>
@@ -24741,13 +24760,13 @@
       </c>
       <c r="I165" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>XVVWF86327G74MD</v>
+        <v>HGIZD585068E75QJ</v>
       </c>
     </row>
     <row r="166" spans="1:9">
       <c r="A166" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>YE3081937L</v>
+        <v>WY6790906W</v>
       </c>
       <c r="B166" t="s">
         <v>1687</v>
@@ -24757,13 +24776,13 @@
       </c>
       <c r="I166" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>HVWZI485316O43VC</v>
+        <v>JUJZW847872H47CI</v>
       </c>
     </row>
     <row r="167" spans="1:9">
       <c r="A167" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>HS9058900N</v>
+        <v>TU8963345K</v>
       </c>
       <c r="B167" t="s">
         <v>1688</v>
@@ -24773,13 +24792,13 @@
       </c>
       <c r="I167" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LPKCI625912I21RC</v>
+        <v>SICSZ267893V30XN</v>
       </c>
     </row>
     <row r="168" spans="1:9">
       <c r="A168" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>IV5641458D</v>
+        <v>DA5435647E</v>
       </c>
       <c r="B168" t="s">
         <v>1689</v>
@@ -24789,13 +24808,13 @@
       </c>
       <c r="I168" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>NDRPB226146C83GH</v>
+        <v>ITPYH487257A84XJ</v>
       </c>
     </row>
     <row r="169" spans="1:9">
       <c r="A169" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>KD8701450T</v>
+        <v>HN558071Y</v>
       </c>
       <c r="B169" t="s">
         <v>1690</v>
@@ -24805,13 +24824,13 @@
       </c>
       <c r="I169" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>AHZWD877347X32HJ</v>
+        <v>HPUWL396333K73QI</v>
       </c>
     </row>
     <row r="170" spans="1:9">
       <c r="A170" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>KP7520478S</v>
+        <v>RF386400H</v>
       </c>
       <c r="B170" t="s">
         <v>1691</v>
@@ -24821,13 +24840,13 @@
       </c>
       <c r="I170" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>FRHFX259312H40GH</v>
+        <v>VSGRF768942Z97NS</v>
       </c>
     </row>
     <row r="171" spans="1:9">
       <c r="A171" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>CG4642111O</v>
+        <v>HS7022790V</v>
       </c>
       <c r="B171" t="s">
         <v>1692</v>
@@ -24837,13 +24856,13 @@
       </c>
       <c r="I171" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>YNGBH343700L97GY</v>
+        <v>CURYX188914R34UA</v>
       </c>
     </row>
     <row r="172" spans="1:9">
       <c r="A172" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>EZ528625W</v>
+        <v>JD488024W</v>
       </c>
       <c r="B172" t="s">
         <v>1693</v>
@@ -24853,13 +24872,13 @@
       </c>
       <c r="I172" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>GFKEC282635L81VB</v>
+        <v>AEQZM815109Z30UR</v>
       </c>
     </row>
     <row r="173" spans="1:9">
       <c r="A173" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>SK6075122A</v>
+        <v>PR5251998A</v>
       </c>
       <c r="B173" t="s">
         <v>1694</v>
@@ -24869,13 +24888,13 @@
       </c>
       <c r="I173" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>UMDME63877J76WY</v>
+        <v>FAGRO223989X54KC</v>
       </c>
     </row>
     <row r="174" spans="1:9">
       <c r="A174" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>EI4276975S</v>
+        <v>DY8928123K</v>
       </c>
       <c r="B174" t="s">
         <v>1695</v>
@@ -24885,13 +24904,13 @@
       </c>
       <c r="I174" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>SLMLM882397Z98CE</v>
+        <v>KRYZO112700Z91HX</v>
       </c>
     </row>
     <row r="175" spans="1:9">
       <c r="A175" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>EW5291129X</v>
+        <v>XP7336068M</v>
       </c>
       <c r="B175" t="s">
         <v>1696</v>
@@ -24901,13 +24920,13 @@
       </c>
       <c r="I175" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>SAIUU952185F98OA</v>
+        <v>JTPNM133590B75CG</v>
       </c>
     </row>
     <row r="176" spans="1:9">
       <c r="A176" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>XH6603872Y</v>
+        <v>FI2351734V</v>
       </c>
       <c r="B176" t="s">
         <v>1697</v>
@@ -24917,13 +24936,13 @@
       </c>
       <c r="I176" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>FAFMC860720J81EU</v>
+        <v>LEHXN919534I13JY</v>
       </c>
     </row>
     <row r="177" spans="1:9">
       <c r="A177" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>KD7693324A</v>
+        <v>TG2777816R</v>
       </c>
       <c r="B177" t="s">
         <v>1698</v>
@@ -24933,13 +24952,13 @@
       </c>
       <c r="I177" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>JRUWD638361D20EP</v>
+        <v>KGOJF205776V99VZ</v>
       </c>
     </row>
     <row r="178" spans="1:9">
       <c r="A178" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>KT2423654B</v>
+        <v>VP769913S</v>
       </c>
       <c r="B178" t="s">
         <v>1699</v>
@@ -24949,13 +24968,13 @@
       </c>
       <c r="I178" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>NYZJC304061F46NE</v>
+        <v>IUNRO213253X79VW</v>
       </c>
     </row>
     <row r="179" spans="1:9">
       <c r="A179" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>CB6968875L</v>
+        <v>JV3310067C</v>
       </c>
       <c r="B179" t="s">
         <v>1700</v>
@@ -24965,13 +24984,13 @@
       </c>
       <c r="I179" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>TENMT591834Y62CP</v>
+        <v>ZEVFQ312041J94TW</v>
       </c>
     </row>
     <row r="180" spans="1:9">
       <c r="A180" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>ZF5217027Z</v>
+        <v>UF1360958D</v>
       </c>
       <c r="B180" t="s">
         <v>1701</v>
@@ -24981,13 +25000,13 @@
       </c>
       <c r="I180" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>GIVBW136250N81ZU</v>
+        <v>WEXBL700222Z93RK</v>
       </c>
     </row>
     <row r="181" spans="1:9">
       <c r="A181" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>JL7939502Q</v>
+        <v>JS4796112H</v>
       </c>
       <c r="B181" t="s">
         <v>1702</v>
@@ -24997,13 +25016,13 @@
       </c>
       <c r="I181" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>YNANP977421W49TF</v>
+        <v>XQFLH444823C52GA</v>
       </c>
     </row>
     <row r="182" spans="1:9">
       <c r="A182" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>WY7755622J</v>
+        <v>FM6026637U</v>
       </c>
       <c r="B182" t="s">
         <v>1703</v>
@@ -25013,13 +25032,13 @@
       </c>
       <c r="I182" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>KNWOM495627Z93QF</v>
+        <v>IIDAQ975405V70FE</v>
       </c>
     </row>
     <row r="183" spans="1:9">
       <c r="A183" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>CP8506291Q</v>
+        <v>TK8023544G</v>
       </c>
       <c r="B183" t="s">
         <v>1704</v>
@@ -25029,13 +25048,13 @@
       </c>
       <c r="I183" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>HFEOK188798T1HT</v>
+        <v>HIUXT518067R54XA</v>
       </c>
     </row>
     <row r="184" spans="1:9">
       <c r="A184" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>SB4378913A</v>
+        <v>WG6462625N</v>
       </c>
       <c r="B184" t="s">
         <v>1705</v>
@@ -25045,13 +25064,13 @@
       </c>
       <c r="I184" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>OPAUH212035G77DX</v>
+        <v>OLXOR226719J69OK</v>
       </c>
     </row>
     <row r="185" spans="1:9">
       <c r="A185" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>TO9936734M</v>
+        <v>EL5764135B</v>
       </c>
       <c r="B185" t="s">
         <v>1706</v>
@@ -25061,13 +25080,13 @@
       </c>
       <c r="I185" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>OCUAD654068Q47RS</v>
+        <v>MHOBC240600M30FH</v>
       </c>
     </row>
     <row r="186" spans="1:9">
       <c r="A186" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>VF2598593Y</v>
+        <v>ID5985595N</v>
       </c>
       <c r="B186" t="s">
         <v>1707</v>
@@ -25077,13 +25096,13 @@
       </c>
       <c r="I186" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>YYUOY25344Q25EO</v>
+        <v>BBLPB563491X32GT</v>
       </c>
     </row>
     <row r="187" spans="1:9">
       <c r="A187" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>XJ3975103E</v>
+        <v>TX2672261T</v>
       </c>
       <c r="B187" t="s">
         <v>1708</v>
@@ -25093,13 +25112,13 @@
       </c>
       <c r="I187" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>FNMMG683613K5DC</v>
+        <v>XVSOJ167291Y48LS</v>
       </c>
     </row>
     <row r="188" spans="1:9">
       <c r="A188" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>HZ4834824Z</v>
+        <v>WT6764789X</v>
       </c>
       <c r="B188" t="s">
         <v>1709</v>
@@ -25109,13 +25128,13 @@
       </c>
       <c r="I188" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>FFVNN721260O59VH</v>
+        <v>JGBHJ349842U36DW</v>
       </c>
     </row>
     <row r="189" spans="1:9">
       <c r="A189" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>GT7010912O</v>
+        <v>OG2189282K</v>
       </c>
       <c r="B189" t="s">
         <v>1710</v>
@@ -25125,13 +25144,13 @@
       </c>
       <c r="I189" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>TFOZD230437R12ZL</v>
+        <v>KBIVG807150M34NR</v>
       </c>
     </row>
     <row r="190" spans="1:9">
       <c r="A190" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>AX7717462D</v>
+        <v>ZZ3730437Z</v>
       </c>
       <c r="B190" t="s">
         <v>1711</v>
@@ -25141,13 +25160,13 @@
       </c>
       <c r="I190" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>JYKZH852368V82AM</v>
+        <v>ZGPEV784679K8NH</v>
       </c>
     </row>
     <row r="191" spans="1:9">
       <c r="A191" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>BE8992342X</v>
+        <v>MT5690784S</v>
       </c>
       <c r="B191" t="s">
         <v>1712</v>
@@ -25157,13 +25176,13 @@
       </c>
       <c r="I191" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>KVVHE613100M35WF</v>
+        <v>QKQAZ965913N76RQ</v>
       </c>
     </row>
     <row r="192" spans="1:9">
       <c r="A192" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>PM6526926T</v>
+        <v>GO7921095O</v>
       </c>
       <c r="B192" t="s">
         <v>1713</v>
@@ -25173,13 +25192,13 @@
       </c>
       <c r="I192" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>PGKSF325500O71NC</v>
+        <v>VZPDY260983O60QZ</v>
       </c>
     </row>
     <row r="193" spans="1:9">
       <c r="A193" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>XA8385654Z</v>
+        <v>JI675964C</v>
       </c>
       <c r="B193" t="s">
         <v>1714</v>
@@ -25189,13 +25208,13 @@
       </c>
       <c r="I193" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>FHORV102782J35AC</v>
+        <v>RZBJJ810148P90YX</v>
       </c>
     </row>
     <row r="194" spans="1:9">
       <c r="A194" s="6" t="str">
         <f t="shared" ref="A194:A257" ca="1" si="8">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,9999999)&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>HO4445890P</v>
+        <v>LB6548833C</v>
       </c>
       <c r="B194" t="s">
         <v>1715</v>
@@ -25205,13 +25224,13 @@
       </c>
       <c r="I194" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>MIQKY992541L14LC</v>
+        <v>QRUDM639459G15HJ</v>
       </c>
     </row>
     <row r="195" spans="1:9">
       <c r="A195" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>CW773147R</v>
+        <v>WU5474482V</v>
       </c>
       <c r="B195" t="s">
         <v>1716</v>
@@ -25221,13 +25240,13 @@
       </c>
       <c r="I195" t="str">
         <f t="shared" ref="I195:I250" ca="1" si="9">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,999999)&amp;CHAR(RANDBETWEEN(65,90))&amp;(RANDBETWEEN(1,99))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>YCNMK697016A72NC</v>
+        <v>VNDFY974121U90AZ</v>
       </c>
     </row>
     <row r="196" spans="1:9">
       <c r="A196" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>HZ6578949L</v>
+        <v>CV2300714X</v>
       </c>
       <c r="B196" t="s">
         <v>1717</v>
@@ -25237,13 +25256,13 @@
       </c>
       <c r="I196" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>SWOGF55955X45LD</v>
+        <v>JHFTI713183J56BX</v>
       </c>
     </row>
     <row r="197" spans="1:9">
       <c r="A197" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>HO703427Z</v>
+        <v>PP4338753I</v>
       </c>
       <c r="B197" t="s">
         <v>1718</v>
@@ -25253,13 +25272,13 @@
       </c>
       <c r="I197" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>YBAWY928085W5FH</v>
+        <v>TPNVI752797F33LT</v>
       </c>
     </row>
     <row r="198" spans="1:9">
       <c r="A198" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>LF3143143Q</v>
+        <v>TW7379971J</v>
       </c>
       <c r="B198" t="s">
         <v>1719</v>
@@ -25269,13 +25288,13 @@
       </c>
       <c r="I198" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>MSJSZ698344U10GO</v>
+        <v>LSSUF401814V10VG</v>
       </c>
     </row>
     <row r="199" spans="1:9">
       <c r="A199" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>VZ5831544T</v>
+        <v>HD9239142U</v>
       </c>
       <c r="B199" t="s">
         <v>1720</v>
@@ -25285,13 +25304,13 @@
       </c>
       <c r="I199" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>KNNRD846880O47OX</v>
+        <v>MJADA24865U43GW</v>
       </c>
     </row>
     <row r="200" spans="1:9">
       <c r="A200" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>WR4772263Q</v>
+        <v>DH6878645Y</v>
       </c>
       <c r="B200" t="s">
         <v>1721</v>
@@ -25301,13 +25320,13 @@
       </c>
       <c r="I200" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>ATNAL97721Y7IC</v>
+        <v>QWNAV621791W31YN</v>
       </c>
     </row>
     <row r="201" spans="1:9">
       <c r="A201" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>RR1058797M</v>
+        <v>DZ8592449C</v>
       </c>
       <c r="B201" t="s">
         <v>1722</v>
@@ -25317,13 +25336,13 @@
       </c>
       <c r="I201" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>IZJTH90672V55XE</v>
+        <v>IQMHF962636H73PY</v>
       </c>
     </row>
     <row r="202" spans="1:9">
       <c r="A202" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>XZ7924831B</v>
+        <v>GS4856420A</v>
       </c>
       <c r="B202" t="s">
         <v>1723</v>
@@ -25333,13 +25352,13 @@
       </c>
       <c r="I202" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>LLIUA790438B69MP</v>
+        <v>PGUDH755285M73AW</v>
       </c>
     </row>
     <row r="203" spans="1:9">
       <c r="A203" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>IJ1627740I</v>
+        <v>LG4584410Z</v>
       </c>
       <c r="B203" t="s">
         <v>1724</v>
@@ -25349,13 +25368,13 @@
       </c>
       <c r="I203" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>DYKUG509597H61WZ</v>
+        <v>PSJGX564647R98HR</v>
       </c>
     </row>
     <row r="204" spans="1:9">
       <c r="A204" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>SU7737169Q</v>
+        <v>ZL8919493V</v>
       </c>
       <c r="B204" t="s">
         <v>1725</v>
@@ -25365,13 +25384,13 @@
       </c>
       <c r="I204" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>NIPEI266632B67RE</v>
+        <v>ZPQLG109003R67RW</v>
       </c>
     </row>
     <row r="205" spans="1:9">
       <c r="A205" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>UU7132474X</v>
+        <v>YO8795646P</v>
       </c>
       <c r="B205" t="s">
         <v>1726</v>
@@ -25381,13 +25400,13 @@
       </c>
       <c r="I205" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>DFQJI309862U49JY</v>
+        <v>ZFYRA18680T41CE</v>
       </c>
     </row>
     <row r="206" spans="1:9">
       <c r="A206" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>XH9822952M</v>
+        <v>LK8492683V</v>
       </c>
       <c r="B206" t="s">
         <v>1727</v>
@@ -25397,13 +25416,13 @@
       </c>
       <c r="I206" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>AFFQZ562526H77KI</v>
+        <v>DKKSW490951Z71XX</v>
       </c>
     </row>
     <row r="207" spans="1:9">
       <c r="A207" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>NJ3809350J</v>
+        <v>QP2129000T</v>
       </c>
       <c r="B207" t="s">
         <v>1728</v>
@@ -25413,13 +25432,13 @@
       </c>
       <c r="I207" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>KCTPD172453K79DD</v>
+        <v>CLCCV800092T52FU</v>
       </c>
     </row>
     <row r="208" spans="1:9">
       <c r="A208" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>DO2827295Q</v>
+        <v>IS4761504W</v>
       </c>
       <c r="B208" t="s">
         <v>1729</v>
@@ -25429,13 +25448,13 @@
       </c>
       <c r="I208" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>KYYYC35788L40BI</v>
+        <v>TEMCG286913S77DT</v>
       </c>
     </row>
     <row r="209" spans="1:9">
       <c r="A209" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>GB9798325T</v>
+        <v>WP6722396P</v>
       </c>
       <c r="B209" t="s">
         <v>1730</v>
@@ -25445,13 +25464,13 @@
       </c>
       <c r="I209" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>MWTLR998292G95VU</v>
+        <v>OQGNH323233V45HA</v>
       </c>
     </row>
     <row r="210" spans="1:9">
       <c r="A210" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>DN8024750Q</v>
+        <v>UV127404O</v>
       </c>
       <c r="B210" t="s">
         <v>1731</v>
@@ -25461,13 +25480,13 @@
       </c>
       <c r="I210" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>MGXDB688982H48BH</v>
+        <v>BGTWW159419K92TS</v>
       </c>
     </row>
     <row r="211" spans="1:9">
       <c r="A211" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>WB5412902V</v>
+        <v>KE4115900W</v>
       </c>
       <c r="B211" t="s">
         <v>1732</v>
@@ -25477,13 +25496,13 @@
       </c>
       <c r="I211" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>YYYLA595882M72YX</v>
+        <v>JRKKU895225V18ZR</v>
       </c>
     </row>
     <row r="212" spans="1:9">
       <c r="A212" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>NE2701321P</v>
+        <v>BR3703723Z</v>
       </c>
       <c r="B212" t="s">
         <v>1733</v>
@@ -25493,13 +25512,13 @@
       </c>
       <c r="I212" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>IGPTY102734F48XJ</v>
+        <v>EVSHS370013T80OL</v>
       </c>
     </row>
     <row r="213" spans="1:9">
       <c r="A213" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>RX853282J</v>
+        <v>QV9721884E</v>
       </c>
       <c r="B213" t="s">
         <v>1734</v>
@@ -25509,13 +25528,13 @@
       </c>
       <c r="I213" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>LAGGQ974357B60KR</v>
+        <v>NZUBM969314P47DV</v>
       </c>
     </row>
     <row r="214" spans="1:9">
       <c r="A214" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>HA4131844A</v>
+        <v>IL8914911V</v>
       </c>
       <c r="B214" t="s">
         <v>1735</v>
@@ -25525,13 +25544,13 @@
       </c>
       <c r="I214" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>HQUHM436535R57RC</v>
+        <v>QSFFB192555H47OO</v>
       </c>
     </row>
     <row r="215" spans="1:9">
       <c r="A215" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>VL1596562I</v>
+        <v>ST2657382H</v>
       </c>
       <c r="B215" t="s">
         <v>1736</v>
@@ -25541,13 +25560,13 @@
       </c>
       <c r="I215" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>UUENA730360X13BS</v>
+        <v>VVIGH330863C32DU</v>
       </c>
     </row>
     <row r="216" spans="1:9">
       <c r="A216" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>JL6067191H</v>
+        <v>BR1662312V</v>
       </c>
       <c r="B216" t="s">
         <v>1737</v>
@@ -25557,13 +25576,13 @@
       </c>
       <c r="I216" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>YZRCU321302A8GL</v>
+        <v>DFLEF321931F22SR</v>
       </c>
     </row>
     <row r="217" spans="1:9">
       <c r="A217" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>ZR2936517A</v>
+        <v>LF2257306F</v>
       </c>
       <c r="B217" t="s">
         <v>1738</v>
@@ -25573,13 +25592,13 @@
       </c>
       <c r="I217" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>POUSL633990J80WQ</v>
+        <v>NSBBA995409P50RA</v>
       </c>
     </row>
     <row r="218" spans="1:9">
       <c r="A218" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>OB6459125W</v>
+        <v>OF3462454N</v>
       </c>
       <c r="B218" t="s">
         <v>1739</v>
@@ -25589,13 +25608,13 @@
       </c>
       <c r="I218" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>ZVSFW563853X38HC</v>
+        <v>PVUCI698739J87SJ</v>
       </c>
     </row>
     <row r="219" spans="1:9">
       <c r="A219" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>LL3634182S</v>
+        <v>FC5085028R</v>
       </c>
       <c r="B219" t="s">
         <v>1740</v>
@@ -25605,13 +25624,13 @@
       </c>
       <c r="I219" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>PXPJP497840O23DC</v>
+        <v>HGSYI501684V29DE</v>
       </c>
     </row>
     <row r="220" spans="1:9">
       <c r="A220" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>YJ8350513G</v>
+        <v>GE5956493T</v>
       </c>
       <c r="B220" t="s">
         <v>1741</v>
@@ -25621,13 +25640,13 @@
       </c>
       <c r="I220" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>INMFU923074Y98BA</v>
+        <v>MVNGN437248O94KQ</v>
       </c>
     </row>
     <row r="221" spans="1:9">
       <c r="A221" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>ZQ1649784E</v>
+        <v>KE4001431I</v>
       </c>
       <c r="B221" t="s">
         <v>1742</v>
@@ -25637,13 +25656,13 @@
       </c>
       <c r="I221" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>SDNKT238775Y63EF</v>
+        <v>WYQNK748171N45IO</v>
       </c>
     </row>
     <row r="222" spans="1:9">
       <c r="A222" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>QV1741963X</v>
+        <v>PF6098079P</v>
       </c>
       <c r="B222" t="s">
         <v>1743</v>
@@ -25653,13 +25672,13 @@
       </c>
       <c r="I222" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>XHNDI583492X57TL</v>
+        <v>QFJRL882181A91KN</v>
       </c>
     </row>
     <row r="223" spans="1:9">
       <c r="A223" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>ER4396171K</v>
+        <v>IR2408726F</v>
       </c>
       <c r="B223" t="s">
         <v>1744</v>
@@ -25669,13 +25688,13 @@
       </c>
       <c r="I223" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>YYOOY235713C72HQ</v>
+        <v>MOITD817968Y83MV</v>
       </c>
     </row>
     <row r="224" spans="1:9">
       <c r="A224" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>IS2850750I</v>
+        <v>VD1807576H</v>
       </c>
       <c r="B224" t="s">
         <v>1745</v>
@@ -25685,13 +25704,13 @@
       </c>
       <c r="I224" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>KARKD139317J58TI</v>
+        <v>POYHV169445O21VJ</v>
       </c>
     </row>
     <row r="225" spans="1:9">
       <c r="A225" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>LR1011792H</v>
+        <v>YQ6971893V</v>
       </c>
       <c r="B225" t="s">
         <v>1746</v>
@@ -25701,13 +25720,13 @@
       </c>
       <c r="I225" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>KIUQV595223I26SI</v>
+        <v>WVAXY583348B18RD</v>
       </c>
     </row>
     <row r="226" spans="1:9">
       <c r="A226" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>JK8870146K</v>
+        <v>EF2350080S</v>
       </c>
       <c r="B226" t="s">
         <v>1747</v>
@@ -25717,13 +25736,13 @@
       </c>
       <c r="I226" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>QVWXD250057Y96UA</v>
+        <v>SKSIG328256S63AW</v>
       </c>
     </row>
     <row r="227" spans="1:9">
       <c r="A227" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>KJ1743164A</v>
+        <v>JV9514110H</v>
       </c>
       <c r="B227" t="s">
         <v>1748</v>
@@ -25733,13 +25752,13 @@
       </c>
       <c r="I227" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>MYTGP244458G67FN</v>
+        <v>LYDNM491967B56CK</v>
       </c>
     </row>
     <row r="228" spans="1:9">
       <c r="A228" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>TS5002020K</v>
+        <v>WU1697879N</v>
       </c>
       <c r="B228" t="s">
         <v>1749</v>
@@ -25749,13 +25768,13 @@
       </c>
       <c r="I228" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>SVXFN722883A18RH</v>
+        <v>KAWDG349960C51AS</v>
       </c>
     </row>
     <row r="229" spans="1:9">
       <c r="A229" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>NG4940567V</v>
+        <v>WO3622202Q</v>
       </c>
       <c r="B229" t="s">
         <v>1750</v>
@@ -25765,13 +25784,13 @@
       </c>
       <c r="I229" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>ZWUUI674960Y33RW</v>
+        <v>QRUUI324139U18SN</v>
       </c>
     </row>
     <row r="230" spans="1:9">
       <c r="A230" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>XY4788246B</v>
+        <v>OX373610F</v>
       </c>
       <c r="B230" t="s">
         <v>1751</v>
@@ -25781,13 +25800,13 @@
       </c>
       <c r="I230" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>VSOGQ810360D35IQ</v>
+        <v>PRTDF340837W76XE</v>
       </c>
     </row>
     <row r="231" spans="1:9">
       <c r="A231" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>LN8157472Z</v>
+        <v>RF6568136O</v>
       </c>
       <c r="B231" t="s">
         <v>1752</v>
@@ -25797,13 +25816,13 @@
       </c>
       <c r="I231" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>IYCDW438435Q86FA</v>
+        <v>XJFHA99057C79WW</v>
       </c>
     </row>
     <row r="232" spans="1:9">
       <c r="A232" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>YC4210294L</v>
+        <v>QV7012179G</v>
       </c>
       <c r="B232" t="s">
         <v>1753</v>
@@ -25813,13 +25832,13 @@
       </c>
       <c r="I232" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>OHXWT559774Z60XD</v>
+        <v>FLWSG755553R29PQ</v>
       </c>
     </row>
     <row r="233" spans="1:9">
       <c r="A233" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>ZZ6390252T</v>
+        <v>YW5873064R</v>
       </c>
       <c r="B233" t="s">
         <v>1754</v>
@@ -25829,13 +25848,13 @@
       </c>
       <c r="I233" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>GQJAQ942415S56KR</v>
+        <v>DWBMB430532H79LO</v>
       </c>
     </row>
     <row r="234" spans="1:9">
       <c r="A234" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>VH379878B</v>
+        <v>FM8063548C</v>
       </c>
       <c r="B234" t="s">
         <v>1755</v>
@@ -25845,13 +25864,13 @@
       </c>
       <c r="I234" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>TUKZY909871S16ZV</v>
+        <v>VTRKJ991336B65HS</v>
       </c>
     </row>
     <row r="235" spans="1:9">
       <c r="A235" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>SQ6719038U</v>
+        <v>MA5054252J</v>
       </c>
       <c r="B235" t="s">
         <v>1756</v>
@@ -25861,13 +25880,13 @@
       </c>
       <c r="I235" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>MGRBP946778P91HX</v>
+        <v>XDBIU662999H95EP</v>
       </c>
     </row>
     <row r="236" spans="1:9">
       <c r="A236" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>QE4524252N</v>
+        <v>JE6026279M</v>
       </c>
       <c r="B236" t="s">
         <v>1757</v>
@@ -25877,13 +25896,13 @@
       </c>
       <c r="I236" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>FMHRF132535D41FO</v>
+        <v>JLXOD521726Q76NW</v>
       </c>
     </row>
     <row r="237" spans="1:9">
       <c r="A237" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>IW3555808S</v>
+        <v>AC1337881G</v>
       </c>
       <c r="B237" t="s">
         <v>1758</v>
@@ -25893,13 +25912,13 @@
       </c>
       <c r="I237" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>CWIEI940482T89PU</v>
+        <v>MJIFM399950E84FO</v>
       </c>
     </row>
     <row r="238" spans="1:9">
       <c r="A238" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>ZV8191370Z</v>
+        <v>OR3431608H</v>
       </c>
       <c r="B238" t="s">
         <v>1759</v>
@@ -25909,13 +25928,13 @@
       </c>
       <c r="I238" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>FGUNM82926R36TT</v>
+        <v>UKXVF869517F72RE</v>
       </c>
     </row>
     <row r="239" spans="1:9">
       <c r="A239" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>XJ2250136A</v>
+        <v>IC7036540S</v>
       </c>
       <c r="B239" t="s">
         <v>1760</v>
@@ -25925,13 +25944,13 @@
       </c>
       <c r="I239" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>TJESG728577J40IM</v>
+        <v>YZXPR976397Y53LJ</v>
       </c>
     </row>
     <row r="240" spans="1:9">
       <c r="A240" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>LP2551658L</v>
+        <v>ML2848836Z</v>
       </c>
       <c r="B240" t="s">
         <v>1761</v>
@@ -25941,13 +25960,13 @@
       </c>
       <c r="I240" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>LTPDH46420D40TZ</v>
+        <v>WJQYJ565330E27PD</v>
       </c>
     </row>
     <row r="241" spans="1:9">
       <c r="A241" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>DY6591844E</v>
+        <v>UK4874335O</v>
       </c>
       <c r="B241" t="s">
         <v>1762</v>
@@ -25957,13 +25976,13 @@
       </c>
       <c r="I241" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>MCDOG58216V15SE</v>
+        <v>IZBQS497659B52GJ</v>
       </c>
     </row>
     <row r="242" spans="1:9">
       <c r="A242" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>RN9389836G</v>
+        <v>AZ2988561P</v>
       </c>
       <c r="B242" t="s">
         <v>1763</v>
@@ -25973,13 +25992,13 @@
       </c>
       <c r="I242" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>ZKNMR463282U95IW</v>
+        <v>RHXUX223455X27FJ</v>
       </c>
     </row>
     <row r="243" spans="1:9">
       <c r="A243" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>YB2646758C</v>
+        <v>NZ2525330I</v>
       </c>
       <c r="B243" t="s">
         <v>1764</v>
@@ -25989,104 +26008,104 @@
       </c>
       <c r="I243" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>HCORK367913T44BV</v>
+        <v>KEGOW372061X91PF</v>
       </c>
     </row>
     <row r="244" spans="1:9">
       <c r="A244" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>IE7715819Z</v>
+        <v>TH7903508S</v>
       </c>
       <c r="B244" t="s">
         <v>1765</v>
       </c>
       <c r="I244" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>GEDPW739061V27TY</v>
+        <v>ZRPQN48641R29ZW</v>
       </c>
     </row>
     <row r="245" spans="1:9">
       <c r="A245" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>OA1106524U</v>
+        <v>FJ867040I</v>
       </c>
       <c r="B245" t="s">
         <v>1766</v>
       </c>
       <c r="I245" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>DLEXH62595K60RC</v>
+        <v>JZDVZ816744R56KH</v>
       </c>
     </row>
     <row r="246" spans="1:9">
       <c r="A246" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>NV6451079O</v>
+        <v>TT7278913E</v>
       </c>
       <c r="B246" t="s">
         <v>1767</v>
       </c>
       <c r="I246" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>HWRCQ318349H55HH</v>
+        <v>GAVFH45750T7EQ</v>
       </c>
     </row>
     <row r="247" spans="1:9">
       <c r="A247" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>HP4587520M</v>
+        <v>SU5068409C</v>
       </c>
       <c r="B247" t="s">
         <v>1768</v>
       </c>
       <c r="I247" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>OEXMA986164T37ZR</v>
+        <v>JFZMM371349U90MU</v>
       </c>
     </row>
     <row r="248" spans="1:9">
       <c r="A248" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>DH8755589H</v>
+        <v>PX5789314M</v>
       </c>
       <c r="B248" t="s">
         <v>1769</v>
       </c>
       <c r="I248" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>RAZPR489312X10TE</v>
+        <v>LXQWZ738949U3AO</v>
       </c>
     </row>
     <row r="249" spans="1:9">
       <c r="A249" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>GC2591098E</v>
+        <v>ZE47798Z</v>
       </c>
       <c r="B249" t="s">
         <v>1770</v>
       </c>
       <c r="I249" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>QDGUA981168F23IX</v>
+        <v>YVRAZ570197U70GI</v>
       </c>
     </row>
     <row r="250" spans="1:9">
       <c r="A250" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>HW7234119M</v>
+        <v>XA5837262C</v>
       </c>
       <c r="B250" t="s">
         <v>1771</v>
       </c>
       <c r="I250" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>FKZLS379945H1GS</v>
+        <v>URZMB995167U31DF</v>
       </c>
     </row>
     <row r="251" spans="1:9">
       <c r="A251" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>UM7201504V</v>
+        <v>KW8530749E</v>
       </c>
       <c r="B251" t="s">
         <v>1772</v>
@@ -26095,7 +26114,7 @@
     <row r="252" spans="1:9">
       <c r="A252" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>JY6431537Z</v>
+        <v>MA1529933D</v>
       </c>
       <c r="B252" t="s">
         <v>1773</v>
@@ -26104,7 +26123,7 @@
     <row r="253" spans="1:9">
       <c r="A253" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>EP8949677T</v>
+        <v>DV2385447S</v>
       </c>
       <c r="B253" t="s">
         <v>1774</v>
@@ -26113,7 +26132,7 @@
     <row r="254" spans="1:9">
       <c r="A254" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>CS8718991A</v>
+        <v>AZ1339278N</v>
       </c>
       <c r="B254" t="s">
         <v>1775</v>
@@ -26122,7 +26141,7 @@
     <row r="255" spans="1:9">
       <c r="A255" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>NE2903539V</v>
+        <v>FO3875174P</v>
       </c>
       <c r="B255" t="s">
         <v>1776</v>
@@ -26131,7 +26150,7 @@
     <row r="256" spans="1:9">
       <c r="A256" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>PG5610022B</v>
+        <v>EF6375086O</v>
       </c>
       <c r="B256" t="s">
         <v>1777</v>
@@ -26140,7 +26159,7 @@
     <row r="257" spans="1:2">
       <c r="A257" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>TX4570957V</v>
+        <v>KJ6184491Z</v>
       </c>
       <c r="B257" t="s">
         <v>1778</v>
@@ -26149,7 +26168,7 @@
     <row r="258" spans="1:2">
       <c r="A258" s="6" t="str">
         <f t="shared" ref="A258:A300" ca="1" si="10">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,9999999)&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>BP6796286R</v>
+        <v>XV1270855M</v>
       </c>
       <c r="B258" t="s">
         <v>1779</v>
@@ -26158,7 +26177,7 @@
     <row r="259" spans="1:2">
       <c r="A259" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>DT7687134B</v>
+        <v>NK6055469Q</v>
       </c>
       <c r="B259" t="s">
         <v>1780</v>
@@ -26167,7 +26186,7 @@
     <row r="260" spans="1:2">
       <c r="A260" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>OR7920272K</v>
+        <v>GZ1440516H</v>
       </c>
       <c r="B260" t="s">
         <v>1781</v>
@@ -26176,7 +26195,7 @@
     <row r="261" spans="1:2">
       <c r="A261" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>EG4330898M</v>
+        <v>IN9642015Q</v>
       </c>
       <c r="B261" t="s">
         <v>1782</v>
@@ -26185,7 +26204,7 @@
     <row r="262" spans="1:2">
       <c r="A262" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>FG1467139G</v>
+        <v>JI1198607S</v>
       </c>
       <c r="B262" t="s">
         <v>1783</v>
@@ -26194,7 +26213,7 @@
     <row r="263" spans="1:2">
       <c r="A263" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>VW5236457W</v>
+        <v>JL8408708Y</v>
       </c>
       <c r="B263" t="s">
         <v>1784</v>
@@ -26203,7 +26222,7 @@
     <row r="264" spans="1:2">
       <c r="A264" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>RT2754558Q</v>
+        <v>EX1914855I</v>
       </c>
       <c r="B264" t="s">
         <v>1785</v>
@@ -26212,7 +26231,7 @@
     <row r="265" spans="1:2">
       <c r="A265" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>WA9867864F</v>
+        <v>QH4190625R</v>
       </c>
       <c r="B265" t="s">
         <v>1786</v>
@@ -26221,7 +26240,7 @@
     <row r="266" spans="1:2">
       <c r="A266" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>CU9600035W</v>
+        <v>ZP2351479X</v>
       </c>
       <c r="B266" t="s">
         <v>1787</v>
@@ -26230,7 +26249,7 @@
     <row r="267" spans="1:2">
       <c r="A267" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>SF245533L</v>
+        <v>IS6427366K</v>
       </c>
       <c r="B267" t="s">
         <v>1788</v>
@@ -26239,7 +26258,7 @@
     <row r="268" spans="1:2">
       <c r="A268" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>QW7140965A</v>
+        <v>OT7277583S</v>
       </c>
       <c r="B268" t="s">
         <v>1789</v>
@@ -26248,7 +26267,7 @@
     <row r="269" spans="1:2">
       <c r="A269" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>MQ3263561A</v>
+        <v>SQ6482260U</v>
       </c>
       <c r="B269" t="s">
         <v>1790</v>
@@ -26257,7 +26276,7 @@
     <row r="270" spans="1:2">
       <c r="A270" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>LW8293877L</v>
+        <v>NO2514320O</v>
       </c>
       <c r="B270" t="s">
         <v>1791</v>
@@ -26266,7 +26285,7 @@
     <row r="271" spans="1:2">
       <c r="A271" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>XH6129033S</v>
+        <v>DZ6933245P</v>
       </c>
       <c r="B271" t="s">
         <v>1792</v>
@@ -26275,7 +26294,7 @@
     <row r="272" spans="1:2">
       <c r="A272" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>FD8337078T</v>
+        <v>RO67527F</v>
       </c>
       <c r="B272" t="s">
         <v>1793</v>
@@ -26284,7 +26303,7 @@
     <row r="273" spans="1:2">
       <c r="A273" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>HM649546N</v>
+        <v>PT4663688N</v>
       </c>
       <c r="B273" t="s">
         <v>1794</v>
@@ -26293,7 +26312,7 @@
     <row r="274" spans="1:2">
       <c r="A274" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>CE9711036K</v>
+        <v>VL1067462G</v>
       </c>
       <c r="B274" t="s">
         <v>1795</v>
@@ -26302,7 +26321,7 @@
     <row r="275" spans="1:2">
       <c r="A275" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>WG5867017Z</v>
+        <v>ZR2927538R</v>
       </c>
       <c r="B275" t="s">
         <v>1796</v>
@@ -26311,7 +26330,7 @@
     <row r="276" spans="1:2">
       <c r="A276" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>FL895941K</v>
+        <v>KF2771909V</v>
       </c>
       <c r="B276" t="s">
         <v>1797</v>
@@ -26320,7 +26339,7 @@
     <row r="277" spans="1:2">
       <c r="A277" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>BI559497K</v>
+        <v>XF4693666C</v>
       </c>
       <c r="B277" t="s">
         <v>1798</v>
@@ -26329,7 +26348,7 @@
     <row r="278" spans="1:2">
       <c r="A278" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>KL2402368O</v>
+        <v>AB1150461Y</v>
       </c>
       <c r="B278" t="s">
         <v>1799</v>
@@ -26338,7 +26357,7 @@
     <row r="279" spans="1:2">
       <c r="A279" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>JZ5195411C</v>
+        <v>VX3837793O</v>
       </c>
       <c r="B279" t="s">
         <v>1800</v>
@@ -26347,7 +26366,7 @@
     <row r="280" spans="1:2">
       <c r="A280" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>UH3424720Z</v>
+        <v>RA2777999D</v>
       </c>
       <c r="B280" t="s">
         <v>1801</v>
@@ -26356,7 +26375,7 @@
     <row r="281" spans="1:2">
       <c r="A281" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>YR8404086M</v>
+        <v>HY4165334B</v>
       </c>
       <c r="B281" t="s">
         <v>1802</v>
@@ -26365,7 +26384,7 @@
     <row r="282" spans="1:2">
       <c r="A282" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>XX4054725J</v>
+        <v>CO8008888N</v>
       </c>
       <c r="B282" t="s">
         <v>1803</v>
@@ -26374,7 +26393,7 @@
     <row r="283" spans="1:2">
       <c r="A283" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>OF4655109L</v>
+        <v>LE3190235V</v>
       </c>
       <c r="B283" t="s">
         <v>1804</v>
@@ -26383,7 +26402,7 @@
     <row r="284" spans="1:2">
       <c r="A284" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>SS6080241O</v>
+        <v>BJ928468D</v>
       </c>
       <c r="B284" t="s">
         <v>1805</v>
@@ -26392,7 +26411,7 @@
     <row r="285" spans="1:2">
       <c r="A285" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>DC1233757W</v>
+        <v>KB1873526W</v>
       </c>
       <c r="B285" t="s">
         <v>1806</v>
@@ -26401,7 +26420,7 @@
     <row r="286" spans="1:2">
       <c r="A286" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>SX1115991D</v>
+        <v>HK4367475G</v>
       </c>
       <c r="B286" t="s">
         <v>1807</v>
@@ -26410,7 +26429,7 @@
     <row r="287" spans="1:2">
       <c r="A287" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>LT7931659X</v>
+        <v>NJ662681H</v>
       </c>
       <c r="B287" t="s">
         <v>1808</v>
@@ -26419,7 +26438,7 @@
     <row r="288" spans="1:2">
       <c r="A288" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>EE4717459O</v>
+        <v>TM5610774F</v>
       </c>
       <c r="B288" t="s">
         <v>1809</v>
@@ -26428,7 +26447,7 @@
     <row r="289" spans="1:2">
       <c r="A289" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>ZE2445814Y</v>
+        <v>FJ7211214Z</v>
       </c>
       <c r="B289" t="s">
         <v>1810</v>
@@ -26437,7 +26456,7 @@
     <row r="290" spans="1:2">
       <c r="A290" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>XD7791909J</v>
+        <v>AE4827568J</v>
       </c>
       <c r="B290" t="s">
         <v>1811</v>
@@ -26446,7 +26465,7 @@
     <row r="291" spans="1:2">
       <c r="A291" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>OT9781931E</v>
+        <v>IC7234369U</v>
       </c>
       <c r="B291" t="s">
         <v>1812</v>
@@ -26455,7 +26474,7 @@
     <row r="292" spans="1:2">
       <c r="A292" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>RS5247166G</v>
+        <v>SG3948312L</v>
       </c>
       <c r="B292" t="s">
         <v>1813</v>
@@ -26464,7 +26483,7 @@
     <row r="293" spans="1:2">
       <c r="A293" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>MW7644810L</v>
+        <v>YN8009080P</v>
       </c>
       <c r="B293" t="s">
         <v>1814</v>
@@ -26473,7 +26492,7 @@
     <row r="294" spans="1:2">
       <c r="A294" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>WW3689185C</v>
+        <v>ZP923821Q</v>
       </c>
       <c r="B294" t="s">
         <v>1815</v>
@@ -26482,7 +26501,7 @@
     <row r="295" spans="1:2">
       <c r="A295" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>XK2611651C</v>
+        <v>IF1494705K</v>
       </c>
       <c r="B295" t="s">
         <v>1816</v>
@@ -26491,7 +26510,7 @@
     <row r="296" spans="1:2">
       <c r="A296" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>FM5561304U</v>
+        <v>OK1394405T</v>
       </c>
       <c r="B296" t="s">
         <v>1817</v>
@@ -26500,7 +26519,7 @@
     <row r="297" spans="1:2">
       <c r="A297" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>VQ6240841U</v>
+        <v>JI859690O</v>
       </c>
       <c r="B297" t="s">
         <v>1818</v>
@@ -26509,7 +26528,7 @@
     <row r="298" spans="1:2">
       <c r="A298" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>YK8950920X</v>
+        <v>FS881731S</v>
       </c>
       <c r="B298" t="s">
         <v>1819</v>
@@ -26518,7 +26537,7 @@
     <row r="299" spans="1:2">
       <c r="A299" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>AE3988417W</v>
+        <v>GE8288986Y</v>
       </c>
       <c r="B299" t="s">
         <v>1820</v>
@@ -26527,7 +26546,7 @@
     <row r="300" spans="1:2">
       <c r="A300" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>SD1371960N</v>
+        <v>XQ361732X</v>
       </c>
       <c r="B300" t="s">
         <v>1821</v>

</xml_diff>

<commit_message>
making changes to git ignore
</commit_message>
<xml_diff>
--- a/src/main/java/testData/ExcelFiles/E2E_Test_Data.xlsx
+++ b/src/main/java/testData/ExcelFiles/E2E_Test_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awhitten/IdeaProjects/Iceberg/src/main/java/testData/ExcelFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D32F3EC-FAC4-E64E-9E82-7F1C28343E49}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A251E713-8BBF-5D4D-A5E2-E3D529BD3EB1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21930,7 +21930,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A12" sqref="A12:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -22114,7 +22114,7 @@
     <row r="1" spans="1:11">
       <c r="A1" s="6" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,9999999)&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>GE8738818I</v>
+        <v>FH9784718V</v>
       </c>
       <c r="B1" t="s">
         <v>1522</v>
@@ -22126,7 +22126,7 @@
     <row r="2" spans="1:11">
       <c r="A2" s="6" t="str">
         <f ca="1">7&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,9999999)&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>7S9806060K</v>
+        <v>7L9095710K</v>
       </c>
       <c r="B2" t="s">
         <v>1523</v>
@@ -22136,21 +22136,21 @@
       </c>
       <c r="I2" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,999999)&amp;CHAR(RANDBETWEEN(65,90))&amp;(RANDBETWEEN(1,99))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>FVSSJ555782H15ET</v>
+        <v>DUGFL881365Z1AQ</v>
       </c>
       <c r="J2" s="28" t="str">
         <f t="shared" ref="J2" ca="1" si="0">RIGHT(I2, LEN(I2)-1)</f>
-        <v>VSSJ555782H15ET</v>
+        <v>UGFL881365Z1AQ</v>
       </c>
       <c r="K2" s="14" t="str">
         <f ca="1">"07"&amp;J2</f>
-        <v>07VSSJ555782H15ET</v>
+        <v>07UGFL881365Z1AQ</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="6" t="str">
         <f t="shared" ref="A3:A65" ca="1" si="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,9999999)&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>DA4304176J</v>
+        <v>KT6737876B</v>
       </c>
       <c r="B3" t="s">
         <v>1524</v>
@@ -22160,13 +22160,13 @@
       </c>
       <c r="I3" t="str">
         <f t="shared" ref="I3:I66" ca="1" si="2">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,999999)&amp;CHAR(RANDBETWEEN(65,90))&amp;(RANDBETWEEN(1,99))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>KRYSZ899271O25WO</v>
+        <v>HZJEA340726Q66LZ</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>RL3692992M</v>
+        <v>SR9284059D</v>
       </c>
       <c r="B4" t="s">
         <v>1525</v>
@@ -22176,13 +22176,13 @@
       </c>
       <c r="I4" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>FCXIE663382I60VF</v>
+        <v>AMOPU612111L7BF</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>DU8333321O</v>
+        <v>BE4236254K</v>
       </c>
       <c r="B5" t="s">
         <v>1526</v>
@@ -22192,13 +22192,13 @@
       </c>
       <c r="I5" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CWQPE401669R59MY</v>
+        <v>EQVOP31272O60WW</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>JN3595407A</v>
+        <v>UX9745161G</v>
       </c>
       <c r="B6" t="s">
         <v>1527</v>
@@ -22208,13 +22208,13 @@
       </c>
       <c r="I6" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>HNNMM299709Z75QP</v>
+        <v>FISBF145317Z13IY</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>DS6038077A</v>
+        <v>DO3175556W</v>
       </c>
       <c r="B7" t="s">
         <v>1528</v>
@@ -22224,13 +22224,13 @@
       </c>
       <c r="I7" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KVYPL521500Z23GV</v>
+        <v>TEWWJ4540G92AE</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>EQ4681413T</v>
+        <v>JG718415O</v>
       </c>
       <c r="B8" t="s">
         <v>1529</v>
@@ -22240,13 +22240,13 @@
       </c>
       <c r="I8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>TSQPD267505U25KE</v>
+        <v>SBZPL236858E81NM</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>PE8026084V</v>
+        <v>KV8038176N</v>
       </c>
       <c r="B9" t="s">
         <v>1530</v>
@@ -22256,13 +22256,13 @@
       </c>
       <c r="I9" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>QHHFW849819G73SK</v>
+        <v>PMAYH637046B90WF</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UJ6346553Q</v>
+        <v>GL5180630R</v>
       </c>
       <c r="B10" t="s">
         <v>1531</v>
@@ -22272,13 +22272,13 @@
       </c>
       <c r="I10" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>VMLWT400161V3QU</v>
+        <v>NASTX492899U54MK</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>FR9742762V</v>
+        <v>ZN5250572S</v>
       </c>
       <c r="B11" t="s">
         <v>1532</v>
@@ -22288,13 +22288,13 @@
       </c>
       <c r="I11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>HDJLS423278E75BF</v>
+        <v>TTHKZ316752K89QO</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>OO1973927S</v>
+        <v>LO8516891W</v>
       </c>
       <c r="B12" t="s">
         <v>1533</v>
@@ -22304,13 +22304,13 @@
       </c>
       <c r="I12" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>FGXXX546840B94EB</v>
+        <v>PERPU572528B25GY</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>AM7627974T</v>
+        <v>VB1644112S</v>
       </c>
       <c r="B13" t="s">
         <v>1534</v>
@@ -22320,13 +22320,13 @@
       </c>
       <c r="I13" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>QAIJZ741113V23AS</v>
+        <v>KBPUV247510A92HW</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>ZN2509346F</v>
+        <v>MC9700420D</v>
       </c>
       <c r="B14" t="s">
         <v>1535</v>
@@ -22336,13 +22336,13 @@
       </c>
       <c r="I14" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>UUQVH573718N24JZ</v>
+        <v>LYZOQ684378K37UH</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>MS285860P</v>
+        <v>BK6938816T</v>
       </c>
       <c r="B15" t="s">
         <v>1536</v>
@@ -22352,13 +22352,13 @@
       </c>
       <c r="I15" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>BDQZO140075N9EA</v>
+        <v>LOETU833045D32ZC</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>PK3464015Q</v>
+        <v>WW3963241U</v>
       </c>
       <c r="B16" t="s">
         <v>1537</v>
@@ -22368,13 +22368,13 @@
       </c>
       <c r="I16" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>WITPE166526Y19WW</v>
+        <v>VGZQM794697R57FJ</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>MZ5360747K</v>
+        <v>UH8305943L</v>
       </c>
       <c r="B17" t="s">
         <v>1538</v>
@@ -22384,13 +22384,13 @@
       </c>
       <c r="I17" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>QJVDE311067C61YH</v>
+        <v>NMCVO989333Y16ZE</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>DS6589469D</v>
+        <v>JZ3564619I</v>
       </c>
       <c r="B18" t="s">
         <v>1539</v>
@@ -22400,13 +22400,13 @@
       </c>
       <c r="I18" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>EYIWG86832G17ML</v>
+        <v>JOPZA241193A92EY</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>DS2066725W</v>
+        <v>SA2317527O</v>
       </c>
       <c r="B19" t="s">
         <v>1540</v>
@@ -22416,13 +22416,13 @@
       </c>
       <c r="I19" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>IDPCU308422C29IC</v>
+        <v>TPBOK288906Z78OR</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>BZ6050621J</v>
+        <v>NL7435085X</v>
       </c>
       <c r="B20" t="s">
         <v>1541</v>
@@ -22432,13 +22432,13 @@
       </c>
       <c r="I20" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>VFNVK483671U51HR</v>
+        <v>XVDFG604303G95YK</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>FY9930767H</v>
+        <v>LW5486997V</v>
       </c>
       <c r="B21" t="s">
         <v>1542</v>
@@ -22448,13 +22448,13 @@
       </c>
       <c r="I21" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CTXXT235608I5CR</v>
+        <v>VBLZG289834R74VG</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>DA7984769B</v>
+        <v>IA9020729X</v>
       </c>
       <c r="B22" t="s">
         <v>1543</v>
@@ -22464,13 +22464,13 @@
       </c>
       <c r="I22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>WFJIS49961R36SD</v>
+        <v>DWZOG96248U45UU</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>MZ1167152C</v>
+        <v>QO7855099S</v>
       </c>
       <c r="B23" t="s">
         <v>1544</v>
@@ -22480,13 +22480,13 @@
       </c>
       <c r="I23" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>RKRAY897774D93ED</v>
+        <v>VKLZB99865T3BQ</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>RV6367878Q</v>
+        <v>BL916499A</v>
       </c>
       <c r="B24" t="s">
         <v>1545</v>
@@ -22496,13 +22496,13 @@
       </c>
       <c r="I24" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>LUQLC743025Z74AG</v>
+        <v>WRRBV473463M89JM</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>TD4397729U</v>
+        <v>LK6275349F</v>
       </c>
       <c r="B25" t="s">
         <v>1546</v>
@@ -22512,13 +22512,13 @@
       </c>
       <c r="I25" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>HSCWC121357C28MC</v>
+        <v>GVGZD796036I1EM</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>FO2189346F</v>
+        <v>WB9145383L</v>
       </c>
       <c r="B26" t="s">
         <v>1547</v>
@@ -22528,13 +22528,13 @@
       </c>
       <c r="I26" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>TLLPW659117F30TC</v>
+        <v>LPMUR956821D68YG</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>WT8095498G</v>
+        <v>SP8754410V</v>
       </c>
       <c r="B27" t="s">
         <v>1548</v>
@@ -22544,13 +22544,13 @@
       </c>
       <c r="I27" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>YJWAD236217Q5HL</v>
+        <v>WCEKL825480K45NL</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>TU9442855M</v>
+        <v>PN1035287N</v>
       </c>
       <c r="B28" t="s">
         <v>1549</v>
@@ -22560,13 +22560,13 @@
       </c>
       <c r="I28" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CSOVT343465C43AD</v>
+        <v>RJTOT928119G26IO</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>CA5404397W</v>
+        <v>UU6473790M</v>
       </c>
       <c r="B29" t="s">
         <v>1550</v>
@@ -22576,13 +22576,13 @@
       </c>
       <c r="I29" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>VNGAN424275G75YG</v>
+        <v>RKOLA592952V55WS</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>GO8812679U</v>
+        <v>GI347679C</v>
       </c>
       <c r="B30" t="s">
         <v>1551</v>
@@ -22592,13 +22592,13 @@
       </c>
       <c r="I30" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>DWNNW426546N39GT</v>
+        <v>GEFJH42252B52HK</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>KY4751165Q</v>
+        <v>HU7972672F</v>
       </c>
       <c r="B31" t="s">
         <v>1552</v>
@@ -22608,13 +22608,13 @@
       </c>
       <c r="I31" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>SSISQ5058R39LV</v>
+        <v>DINIJ103821X42ZO</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>PT3462173B</v>
+        <v>JQ7675329S</v>
       </c>
       <c r="B32" t="s">
         <v>1553</v>
@@ -22624,13 +22624,13 @@
       </c>
       <c r="I32" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>ZHOZE560353L14KP</v>
+        <v>AAQIS377762D18LB</v>
       </c>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>AV748217A</v>
+        <v>OS8441908T</v>
       </c>
       <c r="B33" t="s">
         <v>1554</v>
@@ -22640,13 +22640,13 @@
       </c>
       <c r="I33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>YVKWP490506C80XN</v>
+        <v>WPVAU656980Q71BT</v>
       </c>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UB9078949H</v>
+        <v>GK6625680N</v>
       </c>
       <c r="B34" t="s">
         <v>1555</v>
@@ -22656,13 +22656,13 @@
       </c>
       <c r="I34" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>TJMLY180361A48IZ</v>
+        <v>FDQIV450242J34JN</v>
       </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>DV5274031C</v>
+        <v>NN7251166I</v>
       </c>
       <c r="B35" t="s">
         <v>1556</v>
@@ -22672,13 +22672,13 @@
       </c>
       <c r="I35" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>QVRVQ620329S92JT</v>
+        <v>FKWBB38906I74WB</v>
       </c>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>YO1474767H</v>
+        <v>DR8885642B</v>
       </c>
       <c r="B36" t="s">
         <v>1557</v>
@@ -22688,13 +22688,13 @@
       </c>
       <c r="I36" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>BBJXW924248E96LV</v>
+        <v>HBQHY786855S56LX</v>
       </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>WY1824881R</v>
+        <v>FJ2319359F</v>
       </c>
       <c r="B37" t="s">
         <v>1558</v>
@@ -22704,13 +22704,13 @@
       </c>
       <c r="I37" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>OTGXM807574U57SB</v>
+        <v>YHLAQ267236I45AN</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>RF8971443R</v>
+        <v>AE4054702P</v>
       </c>
       <c r="B38" t="s">
         <v>1559</v>
@@ -22720,13 +22720,13 @@
       </c>
       <c r="I38" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>MXJGZ572760F43FN</v>
+        <v>QVSOE973827Z98QB</v>
       </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>VW5870110O</v>
+        <v>GO9084401F</v>
       </c>
       <c r="B39" t="s">
         <v>1560</v>
@@ -22736,13 +22736,13 @@
       </c>
       <c r="I39" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>CZPFY970199G3NB</v>
+        <v>KIBLD812549W74CJ</v>
       </c>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>HS4624253I</v>
+        <v>WO9403554U</v>
       </c>
       <c r="B40" t="s">
         <v>1561</v>
@@ -22752,13 +22752,13 @@
       </c>
       <c r="I40" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>RLIDA21141P4UL</v>
+        <v>QYCBR745069O24GX</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>KQ7183154C</v>
+        <v>FB2060487L</v>
       </c>
       <c r="B41" t="s">
         <v>1562</v>
@@ -22768,13 +22768,13 @@
       </c>
       <c r="I41" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>YPCJT88257B59HO</v>
+        <v>ZMMIQ494122O47CR</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>XG4109783J</v>
+        <v>XV6817367B</v>
       </c>
       <c r="B42" t="s">
         <v>1563</v>
@@ -22784,13 +22784,13 @@
       </c>
       <c r="I42" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>GFLJB932020M25EF</v>
+        <v>LCEOD515723L34LN</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>KP258707H</v>
+        <v>LT2588220H</v>
       </c>
       <c r="B43" t="s">
         <v>1564</v>
@@ -22800,13 +22800,13 @@
       </c>
       <c r="I43" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>ATAKQ907701D98HZ</v>
+        <v>IXYAD276998W79JH</v>
       </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>QY7227832G</v>
+        <v>ND8133576C</v>
       </c>
       <c r="B44" t="s">
         <v>1565</v>
@@ -22816,13 +22816,13 @@
       </c>
       <c r="I44" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>AJAAP420926Y31XI</v>
+        <v>NWPYA629338C97OB</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>CG8950995S</v>
+        <v>MY4767916M</v>
       </c>
       <c r="B45" t="s">
         <v>1566</v>
@@ -22832,13 +22832,13 @@
       </c>
       <c r="I45" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>TPVZX916054A94YR</v>
+        <v>XCOIG767295A19GO</v>
       </c>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NG2510648W</v>
+        <v>AV8952823R</v>
       </c>
       <c r="B46" t="s">
         <v>1567</v>
@@ -22848,13 +22848,13 @@
       </c>
       <c r="I46" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>DZIJU27376P70YN</v>
+        <v>RDWVG871311U43DE</v>
       </c>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>OO9896779D</v>
+        <v>DW9987955B</v>
       </c>
       <c r="B47" t="s">
         <v>1568</v>
@@ -22864,13 +22864,13 @@
       </c>
       <c r="I47" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>YVWIQ307999T60FB</v>
+        <v>AQLCH993790C23DI</v>
       </c>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>IC1057284K</v>
+        <v>UM121904G</v>
       </c>
       <c r="B48" t="s">
         <v>1569</v>
@@ -22880,13 +22880,13 @@
       </c>
       <c r="I48" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>DATZQ327281G82DR</v>
+        <v>SVJCX712112B48IO</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>PA3695094N</v>
+        <v>ZQ1863548E</v>
       </c>
       <c r="B49" t="s">
         <v>1570</v>
@@ -22896,13 +22896,13 @@
       </c>
       <c r="I49" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KTQHZ140133M93QM</v>
+        <v>TSDXU275815S11UO</v>
       </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UQ7403731G</v>
+        <v>IU973039R</v>
       </c>
       <c r="B50" t="s">
         <v>1571</v>
@@ -22912,13 +22912,13 @@
       </c>
       <c r="I50" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>XZRKP173825Q6AQ</v>
+        <v>DUIPS798296G47QY</v>
       </c>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UE2541396W</v>
+        <v>VH833982D</v>
       </c>
       <c r="B51" t="s">
         <v>1572</v>
@@ -22928,13 +22928,13 @@
       </c>
       <c r="I51" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>XJNRC200895O31WD</v>
+        <v>QTVAM903340C13AM</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>AD7900362H</v>
+        <v>FU71821R</v>
       </c>
       <c r="B52" t="s">
         <v>1573</v>
@@ -22944,13 +22944,13 @@
       </c>
       <c r="I52" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>SGIUV368536T67FY</v>
+        <v>QZQFD561259U60WY</v>
       </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>PW5067173D</v>
+        <v>TD6809504T</v>
       </c>
       <c r="B53" t="s">
         <v>1574</v>
@@ -22960,13 +22960,13 @@
       </c>
       <c r="I53" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>SYLPP827214D8HW</v>
+        <v>MWFWF904691W52BR</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LL6935662F</v>
+        <v>WD9101527P</v>
       </c>
       <c r="B54" t="s">
         <v>1575</v>
@@ -22976,13 +22976,13 @@
       </c>
       <c r="I54" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>JPYQT836358V96NO</v>
+        <v>KJZCZ207729N25EH</v>
       </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>TV2210165V</v>
+        <v>JZ5959427A</v>
       </c>
       <c r="B55" t="s">
         <v>1576</v>
@@ -22992,13 +22992,13 @@
       </c>
       <c r="I55" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>WLJSA980288E21OR</v>
+        <v>UEWRA767550X13WO</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>AK1607462F</v>
+        <v>BF3380967R</v>
       </c>
       <c r="B56" t="s">
         <v>1577</v>
@@ -23008,13 +23008,13 @@
       </c>
       <c r="I56" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NFOTK725322H75ZY</v>
+        <v>MDEJD626454V68FH</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>XF5659122U</v>
+        <v>ZH3336539I</v>
       </c>
       <c r="B57" t="s">
         <v>1578</v>
@@ -23024,13 +23024,13 @@
       </c>
       <c r="I57" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>YWZBQ779835V21ML</v>
+        <v>THGBA144951M31QW</v>
       </c>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>TB5832512G</v>
+        <v>TV8937249O</v>
       </c>
       <c r="B58" t="s">
         <v>1579</v>
@@ -23040,13 +23040,13 @@
       </c>
       <c r="I58" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>XUWBH158422N13KN</v>
+        <v>NQTKV583398L43WZ</v>
       </c>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UL9073232Y</v>
+        <v>KE2197084E</v>
       </c>
       <c r="B59" t="s">
         <v>1580</v>
@@ -23056,13 +23056,13 @@
       </c>
       <c r="I59" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>TCHUR177497H6EC</v>
+        <v>NDBGX19278F88HS</v>
       </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UA8041102W</v>
+        <v>SX2383951A</v>
       </c>
       <c r="B60" t="s">
         <v>1581</v>
@@ -23072,13 +23072,13 @@
       </c>
       <c r="I60" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>OIYKL684256M31BZ</v>
+        <v>FSXFX332521S54JD</v>
       </c>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>OI2111963O</v>
+        <v>SP1369639X</v>
       </c>
       <c r="B61" t="s">
         <v>1582</v>
@@ -23088,13 +23088,13 @@
       </c>
       <c r="I61" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>IBQXV279382J40TI</v>
+        <v>HESAW938306H89LS</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>DH9457180R</v>
+        <v>UR2521718A</v>
       </c>
       <c r="B62" t="s">
         <v>1583</v>
@@ -23104,13 +23104,13 @@
       </c>
       <c r="I62" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>UVGPE825414T54DT</v>
+        <v>ZTIVT199499R65VP</v>
       </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>KX3778623N</v>
+        <v>HT1733975N</v>
       </c>
       <c r="B63" t="s">
         <v>1584</v>
@@ -23120,13 +23120,13 @@
       </c>
       <c r="I63" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>GDYHL266485I40DX</v>
+        <v>KKHSW176745W14HD</v>
       </c>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>GC1614231R</v>
+        <v>DK9328262D</v>
       </c>
       <c r="B64" t="s">
         <v>1585</v>
@@ -23136,13 +23136,13 @@
       </c>
       <c r="I64" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>WZHZV832194Y31YX</v>
+        <v>WKDNP27436Z90RR</v>
       </c>
     </row>
     <row r="65" spans="1:9">
       <c r="A65" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>CN801035V</v>
+        <v>XL6125226S</v>
       </c>
       <c r="B65" t="s">
         <v>1586</v>
@@ -23152,13 +23152,13 @@
       </c>
       <c r="I65" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>XRICP459975D60DI</v>
+        <v>HPKBX422544W3AB</v>
       </c>
     </row>
     <row r="66" spans="1:9">
       <c r="A66" s="6" t="str">
         <f t="shared" ref="A66:A129" ca="1" si="3">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,9999999)&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>ZM6058726H</v>
+        <v>FU805558B</v>
       </c>
       <c r="B66" t="s">
         <v>1587</v>
@@ -23168,13 +23168,13 @@
       </c>
       <c r="I66" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>EBTGH937344B8OH</v>
+        <v>FNDOE629890P67BL</v>
       </c>
     </row>
     <row r="67" spans="1:9">
       <c r="A67" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>PE2288016U</v>
+        <v>XW4206449U</v>
       </c>
       <c r="B67" t="s">
         <v>1588</v>
@@ -23184,13 +23184,13 @@
       </c>
       <c r="I67" t="str">
         <f t="shared" ref="I67:I130" ca="1" si="4">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,999999)&amp;CHAR(RANDBETWEEN(65,90))&amp;(RANDBETWEEN(1,99))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>TKAOC332965N33PA</v>
+        <v>UKZRF234658V41MQ</v>
       </c>
     </row>
     <row r="68" spans="1:9">
       <c r="A68" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>PB4527600V</v>
+        <v>HJ3467969J</v>
       </c>
       <c r="B68" t="s">
         <v>1589</v>
@@ -23200,13 +23200,13 @@
       </c>
       <c r="I68" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>XORUD241811Y13JV</v>
+        <v>QNEOB471894R84VX</v>
       </c>
     </row>
     <row r="69" spans="1:9">
       <c r="A69" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>HX7312911R</v>
+        <v>RI3481869V</v>
       </c>
       <c r="B69" t="s">
         <v>1590</v>
@@ -23216,13 +23216,13 @@
       </c>
       <c r="I69" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>NBLSC909220J55RY</v>
+        <v>BKJQZ591542W43HL</v>
       </c>
     </row>
     <row r="70" spans="1:9">
       <c r="A70" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>PT6351447X</v>
+        <v>BH9004029W</v>
       </c>
       <c r="B70" t="s">
         <v>1591</v>
@@ -23232,13 +23232,13 @@
       </c>
       <c r="I70" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>OMZTE997150P58MZ</v>
+        <v>ZGEPA113299W41GN</v>
       </c>
     </row>
     <row r="71" spans="1:9">
       <c r="A71" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>QA2096072O</v>
+        <v>CT9876362U</v>
       </c>
       <c r="B71" t="s">
         <v>1592</v>
@@ -23248,13 +23248,13 @@
       </c>
       <c r="I71" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>RXYFE807193O88MH</v>
+        <v>YWRCY182239J12IZ</v>
       </c>
     </row>
     <row r="72" spans="1:9">
       <c r="A72" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UT503091E</v>
+        <v>TU1690633R</v>
       </c>
       <c r="B72" t="s">
         <v>1593</v>
@@ -23264,13 +23264,13 @@
       </c>
       <c r="I72" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>ACEQB937469I63PP</v>
+        <v>QCEML663428E3FP</v>
       </c>
     </row>
     <row r="73" spans="1:9">
       <c r="A73" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>JJ2048015Y</v>
+        <v>ZK3199302F</v>
       </c>
       <c r="B73" t="s">
         <v>1594</v>
@@ -23280,13 +23280,13 @@
       </c>
       <c r="I73" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>KRUAJ973913F28KB</v>
+        <v>PGZOT461698O73FT</v>
       </c>
     </row>
     <row r="74" spans="1:9">
       <c r="A74" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>NZ9448336L</v>
+        <v>GU5751557P</v>
       </c>
       <c r="B74" t="s">
         <v>1595</v>
@@ -23296,13 +23296,13 @@
       </c>
       <c r="I74" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>EQDFA213544N31GJ</v>
+        <v>DWZPF673223D31HJ</v>
       </c>
     </row>
     <row r="75" spans="1:9">
       <c r="A75" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>BT7712427L</v>
+        <v>HO7522228C</v>
       </c>
       <c r="B75" t="s">
         <v>1596</v>
@@ -23312,13 +23312,13 @@
       </c>
       <c r="I75" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>KZYBL616166A91DL</v>
+        <v>YZRJP850573T50PW</v>
       </c>
     </row>
     <row r="76" spans="1:9">
       <c r="A76" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>TQ1373896P</v>
+        <v>YR4265141E</v>
       </c>
       <c r="B76" t="s">
         <v>1597</v>
@@ -23328,13 +23328,13 @@
       </c>
       <c r="I76" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>LFDYD815794T54JO</v>
+        <v>RDHKU168419T82UU</v>
       </c>
     </row>
     <row r="77" spans="1:9">
       <c r="A77" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>HD3089506P</v>
+        <v>AY127720C</v>
       </c>
       <c r="B77" t="s">
         <v>1598</v>
@@ -23344,13 +23344,13 @@
       </c>
       <c r="I77" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>MXOAN891109O87JN</v>
+        <v>NZUPE835398N24ER</v>
       </c>
     </row>
     <row r="78" spans="1:9">
       <c r="A78" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>CJ9473767J</v>
+        <v>UE9741631T</v>
       </c>
       <c r="B78" t="s">
         <v>1599</v>
@@ -23360,13 +23360,13 @@
       </c>
       <c r="I78" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>IVGJE988929V17HG</v>
+        <v>BKUXW135421R92RA</v>
       </c>
     </row>
     <row r="79" spans="1:9">
       <c r="A79" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>VD1064366J</v>
+        <v>DX3537023W</v>
       </c>
       <c r="B79" t="s">
         <v>1600</v>
@@ -23376,13 +23376,13 @@
       </c>
       <c r="I79" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>WMNIL684950U31KO</v>
+        <v>BTOAM276459R37CS</v>
       </c>
     </row>
     <row r="80" spans="1:9">
       <c r="A80" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>WT6665250E</v>
+        <v>VG4968A</v>
       </c>
       <c r="B80" t="s">
         <v>1601</v>
@@ -23392,13 +23392,13 @@
       </c>
       <c r="I80" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>VFSFP693937T43MR</v>
+        <v>RQLGJ901528U67LX</v>
       </c>
     </row>
     <row r="81" spans="1:9">
       <c r="A81" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>WW2116527L</v>
+        <v>WF4095871L</v>
       </c>
       <c r="B81" t="s">
         <v>1602</v>
@@ -23408,13 +23408,13 @@
       </c>
       <c r="I81" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>XFXXQ3725K51VI</v>
+        <v>LZRBE575077Q15BO</v>
       </c>
     </row>
     <row r="82" spans="1:9">
       <c r="A82" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>ES3196394G</v>
+        <v>UW6062704G</v>
       </c>
       <c r="B82" t="s">
         <v>1603</v>
@@ -23424,13 +23424,13 @@
       </c>
       <c r="I82" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>TCQFD379412W99LL</v>
+        <v>PQYTS408390B94TR</v>
       </c>
     </row>
     <row r="83" spans="1:9">
       <c r="A83" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>CK4361444P</v>
+        <v>KY3047445K</v>
       </c>
       <c r="B83" t="s">
         <v>1604</v>
@@ -23440,13 +23440,13 @@
       </c>
       <c r="I83" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>TLIUT689253D99SM</v>
+        <v>YMUZG827153Z84WR</v>
       </c>
     </row>
     <row r="84" spans="1:9">
       <c r="A84" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>PL8274198Z</v>
+        <v>TZ4296337Z</v>
       </c>
       <c r="B84" t="s">
         <v>1605</v>
@@ -23456,13 +23456,13 @@
       </c>
       <c r="I84" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>AAJLT180993J31ND</v>
+        <v>HISLD662310C2EH</v>
       </c>
     </row>
     <row r="85" spans="1:9">
       <c r="A85" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>ED3850384Q</v>
+        <v>UX9419536X</v>
       </c>
       <c r="B85" t="s">
         <v>1606</v>
@@ -23472,13 +23472,13 @@
       </c>
       <c r="I85" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>QEOXB958560U81PU</v>
+        <v>IKZYW537173E63QX</v>
       </c>
     </row>
     <row r="86" spans="1:9">
       <c r="A86" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>EC933825D</v>
+        <v>QZ5532385T</v>
       </c>
       <c r="B86" t="s">
         <v>1607</v>
@@ -23488,13 +23488,13 @@
       </c>
       <c r="I86" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>NHFCK387541E51ZR</v>
+        <v>XKZOO956359M10IZ</v>
       </c>
     </row>
     <row r="87" spans="1:9">
       <c r="A87" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>OE1657988G</v>
+        <v>MH8808751N</v>
       </c>
       <c r="B87" t="s">
         <v>1608</v>
@@ -23504,13 +23504,13 @@
       </c>
       <c r="I87" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>SZUQT14346Q54OI</v>
+        <v>ZPRSK206396N22EQ</v>
       </c>
     </row>
     <row r="88" spans="1:9">
       <c r="A88" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>KG2466555R</v>
+        <v>UD1347269K</v>
       </c>
       <c r="B88" t="s">
         <v>1609</v>
@@ -23520,13 +23520,13 @@
       </c>
       <c r="I88" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>UUIUW521038Y82MQ</v>
+        <v>ZXSVE682768H66DU</v>
       </c>
     </row>
     <row r="89" spans="1:9">
       <c r="A89" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>QJ3483783Z</v>
+        <v>KH7201873K</v>
       </c>
       <c r="B89" t="s">
         <v>1610</v>
@@ -23536,13 +23536,13 @@
       </c>
       <c r="I89" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>KDDAP239760N26VS</v>
+        <v>YJFCS1868C5VS</v>
       </c>
     </row>
     <row r="90" spans="1:9">
       <c r="A90" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>OP7166219S</v>
+        <v>CX831816D</v>
       </c>
       <c r="B90" t="s">
         <v>1611</v>
@@ -23552,13 +23552,13 @@
       </c>
       <c r="I90" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>YSGHC377068R44XC</v>
+        <v>UITWN788729C96HC</v>
       </c>
     </row>
     <row r="91" spans="1:9">
       <c r="A91" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>BR5576327I</v>
+        <v>SX6381245U</v>
       </c>
       <c r="B91" t="s">
         <v>1612</v>
@@ -23568,13 +23568,13 @@
       </c>
       <c r="I91" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>NLYDQ138089V53HK</v>
+        <v>WMUMM717174C55EX</v>
       </c>
     </row>
     <row r="92" spans="1:9">
       <c r="A92" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>HJ5247975K</v>
+        <v>ZM2542034H</v>
       </c>
       <c r="B92" t="s">
         <v>1613</v>
@@ -23584,13 +23584,13 @@
       </c>
       <c r="I92" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>GHIAK912880V88QP</v>
+        <v>NTHGY340151M68YV</v>
       </c>
     </row>
     <row r="93" spans="1:9">
       <c r="A93" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>EL1365628F</v>
+        <v>GA2599836Z</v>
       </c>
       <c r="B93" t="s">
         <v>1614</v>
@@ -23600,13 +23600,13 @@
       </c>
       <c r="I93" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>NCVIV281171V11ZV</v>
+        <v>MYMLM980228I38WY</v>
       </c>
     </row>
     <row r="94" spans="1:9">
       <c r="A94" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>TM6739124V</v>
+        <v>WV7622694J</v>
       </c>
       <c r="B94" t="s">
         <v>1615</v>
@@ -23616,13 +23616,13 @@
       </c>
       <c r="I94" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>OBDRX597659R89QW</v>
+        <v>CIYID86726P87WL</v>
       </c>
     </row>
     <row r="95" spans="1:9">
       <c r="A95" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>NO3961568U</v>
+        <v>OC7432887O</v>
       </c>
       <c r="B95" t="s">
         <v>1616</v>
@@ -23632,13 +23632,13 @@
       </c>
       <c r="I95" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>EPYWM29002Q38QW</v>
+        <v>AVDUG143062D99WH</v>
       </c>
     </row>
     <row r="96" spans="1:9">
       <c r="A96" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>WJ2253720B</v>
+        <v>RQ7025519Z</v>
       </c>
       <c r="B96" t="s">
         <v>1617</v>
@@ -23648,13 +23648,13 @@
       </c>
       <c r="I96" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>OUXDC506584C23LU</v>
+        <v>PMLRF821255J78GD</v>
       </c>
     </row>
     <row r="97" spans="1:9">
       <c r="A97" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>CW3133428T</v>
+        <v>YI2427848P</v>
       </c>
       <c r="B97" t="s">
         <v>1618</v>
@@ -23664,13 +23664,13 @@
       </c>
       <c r="I97" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>KHDDG366065H16HB</v>
+        <v>WJTEK788307N3JK</v>
       </c>
     </row>
     <row r="98" spans="1:9">
       <c r="A98" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>NW2482391L</v>
+        <v>IR5092041N</v>
       </c>
       <c r="B98" t="s">
         <v>1619</v>
@@ -23680,13 +23680,13 @@
       </c>
       <c r="I98" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>TBDYB828992S1SO</v>
+        <v>SPDHR158368A64PK</v>
       </c>
     </row>
     <row r="99" spans="1:9">
       <c r="A99" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UT7511480S</v>
+        <v>RV8764704H</v>
       </c>
       <c r="B99" t="s">
         <v>1620</v>
@@ -23696,13 +23696,13 @@
       </c>
       <c r="I99" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>SWXIL482782H42KL</v>
+        <v>WYRQA276183Y24ML</v>
       </c>
     </row>
     <row r="100" spans="1:9">
       <c r="A100" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>MJ4535359W</v>
+        <v>LQ1869867E</v>
       </c>
       <c r="B100" t="s">
         <v>1621</v>
@@ -23712,13 +23712,13 @@
       </c>
       <c r="I100" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>OZLBN498563X58SS</v>
+        <v>UJPOU760687E94XT</v>
       </c>
     </row>
     <row r="101" spans="1:9">
       <c r="A101" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>XE4919888I</v>
+        <v>MS4295528M</v>
       </c>
       <c r="B101" t="s">
         <v>1622</v>
@@ -23728,13 +23728,13 @@
       </c>
       <c r="I101" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>XYIVI737431C80GV</v>
+        <v>QULGL129856P45US</v>
       </c>
     </row>
     <row r="102" spans="1:9">
       <c r="A102" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>PH8743968O</v>
+        <v>AL787582U</v>
       </c>
       <c r="B102" t="s">
         <v>1623</v>
@@ -23744,13 +23744,13 @@
       </c>
       <c r="I102" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>ZXNUW755092F90TF</v>
+        <v>WODTI347107D57FH</v>
       </c>
     </row>
     <row r="103" spans="1:9">
       <c r="A103" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UZ9038451F</v>
+        <v>LI4226178R</v>
       </c>
       <c r="B103" t="s">
         <v>1624</v>
@@ -23760,13 +23760,13 @@
       </c>
       <c r="I103" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>GUQYU964253P34GD</v>
+        <v>SHABA307114R2LH</v>
       </c>
     </row>
     <row r="104" spans="1:9">
       <c r="A104" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UF5885440W</v>
+        <v>CW605673O</v>
       </c>
       <c r="B104" t="s">
         <v>1625</v>
@@ -23776,13 +23776,13 @@
       </c>
       <c r="I104" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>WMIZJ265277P35WD</v>
+        <v>PZCQT811096X55EH</v>
       </c>
     </row>
     <row r="105" spans="1:9">
       <c r="A105" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>IW5251638M</v>
+        <v>LB9737913S</v>
       </c>
       <c r="B105" t="s">
         <v>1626</v>
@@ -23792,13 +23792,13 @@
       </c>
       <c r="I105" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>PBIHS12201Z71MD</v>
+        <v>LGPYW262291O67QE</v>
       </c>
     </row>
     <row r="106" spans="1:9">
       <c r="A106" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>RO2628537T</v>
+        <v>VJ61737U</v>
       </c>
       <c r="B106" t="s">
         <v>1627</v>
@@ -23808,13 +23808,13 @@
       </c>
       <c r="I106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>NKXGM59202A60HG</v>
+        <v>XLUSP356357G28MK</v>
       </c>
     </row>
     <row r="107" spans="1:9">
       <c r="A107" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>QU8647351T</v>
+        <v>ZP2994134X</v>
       </c>
       <c r="B107" t="s">
         <v>1628</v>
@@ -23824,13 +23824,13 @@
       </c>
       <c r="I107" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>FXCAK262799D17PW</v>
+        <v>UVLBE731473Y95PP</v>
       </c>
     </row>
     <row r="108" spans="1:9">
       <c r="A108" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>ZA2868902S</v>
+        <v>SQ4127323S</v>
       </c>
       <c r="B108" t="s">
         <v>1629</v>
@@ -23840,13 +23840,13 @@
       </c>
       <c r="I108" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>RARUY6477S47RM</v>
+        <v>DODVB660362V8HM</v>
       </c>
     </row>
     <row r="109" spans="1:9">
       <c r="A109" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>EY628135N</v>
+        <v>AJ1952942Z</v>
       </c>
       <c r="B109" t="s">
         <v>1630</v>
@@ -23856,13 +23856,13 @@
       </c>
       <c r="I109" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>YMNPK552829Z3UU</v>
+        <v>GTGPD130305I22EE</v>
       </c>
     </row>
     <row r="110" spans="1:9">
       <c r="A110" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>YY4904058U</v>
+        <v>BV1995546O</v>
       </c>
       <c r="B110" t="s">
         <v>1631</v>
@@ -23872,13 +23872,13 @@
       </c>
       <c r="I110" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>VRZTH102336O94ON</v>
+        <v>FCOWO806563A32GH</v>
       </c>
     </row>
     <row r="111" spans="1:9">
       <c r="A111" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>VF7990217K</v>
+        <v>TP573761D</v>
       </c>
       <c r="B111" t="s">
         <v>1632</v>
@@ -23888,13 +23888,13 @@
       </c>
       <c r="I111" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>ZDBGB891727Z60OX</v>
+        <v>KZZPD824788W53MO</v>
       </c>
     </row>
     <row r="112" spans="1:9">
       <c r="A112" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>BV9757594P</v>
+        <v>JN1117574D</v>
       </c>
       <c r="B112" t="s">
         <v>1633</v>
@@ -23904,13 +23904,13 @@
       </c>
       <c r="I112" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>MVARN800905N91OZ</v>
+        <v>WNUGL331074C23XE</v>
       </c>
     </row>
     <row r="113" spans="1:9">
       <c r="A113" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>HJ7786415Q</v>
+        <v>ME9174323G</v>
       </c>
       <c r="B113" t="s">
         <v>1634</v>
@@ -23920,13 +23920,13 @@
       </c>
       <c r="I113" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>VRELE830942S98NQ</v>
+        <v>WAYYD772454A64AC</v>
       </c>
     </row>
     <row r="114" spans="1:9">
       <c r="A114" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>AE8626955H</v>
+        <v>LY836035J</v>
       </c>
       <c r="B114" t="s">
         <v>1635</v>
@@ -23936,13 +23936,13 @@
       </c>
       <c r="I114" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>KAXAH233741D5XV</v>
+        <v>OJNKL720744S32LE</v>
       </c>
     </row>
     <row r="115" spans="1:9">
       <c r="A115" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>NB5373637Y</v>
+        <v>QR6462394N</v>
       </c>
       <c r="B115" t="s">
         <v>1636</v>
@@ -23952,13 +23952,13 @@
       </c>
       <c r="I115" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>FJGJF148585J23YC</v>
+        <v>OBREU373386F79RT</v>
       </c>
     </row>
     <row r="116" spans="1:9">
       <c r="A116" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>OI48325U</v>
+        <v>QE1718440K</v>
       </c>
       <c r="B116" t="s">
         <v>1637</v>
@@ -23968,13 +23968,13 @@
       </c>
       <c r="I116" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>NTWSF260750J98KJ</v>
+        <v>RTRXQ772218U26FI</v>
       </c>
     </row>
     <row r="117" spans="1:9">
       <c r="A117" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>HP6359375G</v>
+        <v>AH7080886C</v>
       </c>
       <c r="B117" t="s">
         <v>1638</v>
@@ -23984,13 +23984,13 @@
       </c>
       <c r="I117" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>ZIBAW59428R99YT</v>
+        <v>QGHJS480320W97BZ</v>
       </c>
     </row>
     <row r="118" spans="1:9">
       <c r="A118" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>CG1440786Z</v>
+        <v>IR8378486U</v>
       </c>
       <c r="B118" t="s">
         <v>1639</v>
@@ -24000,13 +24000,13 @@
       </c>
       <c r="I118" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>LVYVH325333R24TZ</v>
+        <v>NMNVE752692I51KG</v>
       </c>
     </row>
     <row r="119" spans="1:9">
       <c r="A119" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>VU4990279F</v>
+        <v>KO9743218Y</v>
       </c>
       <c r="B119" t="s">
         <v>1640</v>
@@ -24016,13 +24016,13 @@
       </c>
       <c r="I119" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>POTFM751334N43GH</v>
+        <v>MHBZM663694P84OJ</v>
       </c>
     </row>
     <row r="120" spans="1:9">
       <c r="A120" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>IT4153582Q</v>
+        <v>TP4568917H</v>
       </c>
       <c r="B120" t="s">
         <v>1641</v>
@@ -24032,13 +24032,13 @@
       </c>
       <c r="I120" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>IQBAT326074U89TQ</v>
+        <v>ODZII9489U40GV</v>
       </c>
     </row>
     <row r="121" spans="1:9">
       <c r="A121" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>VD6724908O</v>
+        <v>XX345810H</v>
       </c>
       <c r="B121" t="s">
         <v>1642</v>
@@ -24048,13 +24048,13 @@
       </c>
       <c r="I121" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>VBJZK929232Y65JY</v>
+        <v>WMIUI919525R44SH</v>
       </c>
     </row>
     <row r="122" spans="1:9">
       <c r="A122" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>OT5809224G</v>
+        <v>HO5385515F</v>
       </c>
       <c r="B122" t="s">
         <v>1643</v>
@@ -24064,13 +24064,13 @@
       </c>
       <c r="I122" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>LVIYG545916P31QK</v>
+        <v>TQLLO230548Z10HH</v>
       </c>
     </row>
     <row r="123" spans="1:9">
       <c r="A123" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>AN5187211U</v>
+        <v>YL429091Y</v>
       </c>
       <c r="B123" t="s">
         <v>1644</v>
@@ -24080,13 +24080,13 @@
       </c>
       <c r="I123" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>YXPXN596172R70AK</v>
+        <v>STXXO75123Q69DP</v>
       </c>
     </row>
     <row r="124" spans="1:9">
       <c r="A124" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>BX7541172A</v>
+        <v>OF6742848T</v>
       </c>
       <c r="B124" t="s">
         <v>1645</v>
@@ -24096,13 +24096,13 @@
       </c>
       <c r="I124" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>EIYPM33382D98AU</v>
+        <v>LOIDN523601E43CS</v>
       </c>
     </row>
     <row r="125" spans="1:9">
       <c r="A125" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>YO4483103B</v>
+        <v>AK5365056G</v>
       </c>
       <c r="B125" t="s">
         <v>1646</v>
@@ -24112,13 +24112,13 @@
       </c>
       <c r="I125" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>KRSMI307931W59JK</v>
+        <v>PUOIA422488T83ZQ</v>
       </c>
     </row>
     <row r="126" spans="1:9">
       <c r="A126" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>IB7740800W</v>
+        <v>FJ2290446X</v>
       </c>
       <c r="B126" t="s">
         <v>1647</v>
@@ -24128,13 +24128,13 @@
       </c>
       <c r="I126" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>HNTNS622830C15YO</v>
+        <v>VRMGI211670C80FL</v>
       </c>
     </row>
     <row r="127" spans="1:9">
       <c r="A127" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>KB4136510Q</v>
+        <v>UK4463996T</v>
       </c>
       <c r="B127" t="s">
         <v>1648</v>
@@ -24144,13 +24144,13 @@
       </c>
       <c r="I127" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>YAXOD271545B40KI</v>
+        <v>OKDNS103176Q75QL</v>
       </c>
     </row>
     <row r="128" spans="1:9">
       <c r="A128" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UD1899872L</v>
+        <v>HD4152463Y</v>
       </c>
       <c r="B128" t="s">
         <v>1649</v>
@@ -24160,13 +24160,13 @@
       </c>
       <c r="I128" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>NHTYS237251R82WZ</v>
+        <v>GFMZM311044N31IU</v>
       </c>
     </row>
     <row r="129" spans="1:9">
       <c r="A129" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>GC3091085S</v>
+        <v>BR2693664W</v>
       </c>
       <c r="B129" t="s">
         <v>1650</v>
@@ -24176,13 +24176,13 @@
       </c>
       <c r="I129" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>ZESMO387159Z40CY</v>
+        <v>JQPTR454532I14BX</v>
       </c>
     </row>
     <row r="130" spans="1:9">
       <c r="A130" s="6" t="str">
         <f t="shared" ref="A130:A193" ca="1" si="5">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,9999999)&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>RE5211339T</v>
+        <v>YJ1996120E</v>
       </c>
       <c r="B130" t="s">
         <v>1651</v>
@@ -24192,13 +24192,13 @@
       </c>
       <c r="I130" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>TRGDR385338E58GD</v>
+        <v>ZNTCJ846346O97XS</v>
       </c>
     </row>
     <row r="131" spans="1:9">
       <c r="A131" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>OJ8516873B</v>
+        <v>WC471801X</v>
       </c>
       <c r="B131" t="s">
         <v>1652</v>
@@ -24208,13 +24208,13 @@
       </c>
       <c r="I131" t="str">
         <f t="shared" ref="I131:I194" ca="1" si="6">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,999999)&amp;CHAR(RANDBETWEEN(65,90))&amp;(RANDBETWEEN(1,99))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>UIIXY154202O18TI</v>
+        <v>OTGGH217468E77ZW</v>
       </c>
     </row>
     <row r="132" spans="1:9">
       <c r="A132" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>TC85668E</v>
+        <v>GQ295815F</v>
       </c>
       <c r="B132" t="s">
         <v>1653</v>
@@ -24224,13 +24224,13 @@
       </c>
       <c r="I132" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>BJTZU153801Z1AM</v>
+        <v>PJYYW676223Z50UI</v>
       </c>
     </row>
     <row r="133" spans="1:9">
       <c r="A133" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>OG7002544K</v>
+        <v>FF1797825G</v>
       </c>
       <c r="B133" t="s">
         <v>1654</v>
@@ -24240,13 +24240,13 @@
       </c>
       <c r="I133" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>XLIKZ599756Y73BO</v>
+        <v>AWFJB334723L38JD</v>
       </c>
     </row>
     <row r="134" spans="1:9">
       <c r="A134" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>LL300333M</v>
+        <v>IG4913061V</v>
       </c>
       <c r="B134" t="s">
         <v>1655</v>
@@ -24256,13 +24256,13 @@
       </c>
       <c r="I134" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>NDMTG313150U98YJ</v>
+        <v>CCHRS967021D63RZ</v>
       </c>
     </row>
     <row r="135" spans="1:9">
       <c r="A135" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>OJ3259483Q</v>
+        <v>KE2022875I</v>
       </c>
       <c r="B135" t="s">
         <v>1656</v>
@@ -24272,13 +24272,13 @@
       </c>
       <c r="I135" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>AZVFV20492R33KH</v>
+        <v>UZMUP729509G64KR</v>
       </c>
     </row>
     <row r="136" spans="1:9">
       <c r="A136" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>RG6714268O</v>
+        <v>PK5976850L</v>
       </c>
       <c r="B136" t="s">
         <v>1657</v>
@@ -24288,13 +24288,13 @@
       </c>
       <c r="I136" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>GSQEG244619P98PP</v>
+        <v>RZZVS687157Y68UL</v>
       </c>
     </row>
     <row r="137" spans="1:9">
       <c r="A137" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>ON8440972B</v>
+        <v>EW401050F</v>
       </c>
       <c r="B137" t="s">
         <v>1658</v>
@@ -24304,13 +24304,13 @@
       </c>
       <c r="I137" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LYVZM814780D97TQ</v>
+        <v>IVUYI782058M91AI</v>
       </c>
     </row>
     <row r="138" spans="1:9">
       <c r="A138" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>VQ9809663G</v>
+        <v>LV6318762O</v>
       </c>
       <c r="B138" t="s">
         <v>1659</v>
@@ -24320,13 +24320,13 @@
       </c>
       <c r="I138" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>EAUXT190967M31ZB</v>
+        <v>TPFUR150575Z4PZ</v>
       </c>
     </row>
     <row r="139" spans="1:9">
       <c r="A139" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>ZT2361255T</v>
+        <v>VK4390449M</v>
       </c>
       <c r="B139" t="s">
         <v>1660</v>
@@ -24336,13 +24336,13 @@
       </c>
       <c r="I139" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>CTMVY152525N50ZN</v>
+        <v>CBSDA625606R50AL</v>
       </c>
     </row>
     <row r="140" spans="1:9">
       <c r="A140" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>SB8648009I</v>
+        <v>NW4754589T</v>
       </c>
       <c r="B140" t="s">
         <v>1661</v>
@@ -24352,13 +24352,13 @@
       </c>
       <c r="I140" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>RDJLC569049B77ZD</v>
+        <v>RPZAE892507N29PL</v>
       </c>
     </row>
     <row r="141" spans="1:9">
       <c r="A141" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>ZK2352316O</v>
+        <v>RO4815903Y</v>
       </c>
       <c r="B141" t="s">
         <v>1662</v>
@@ -24368,13 +24368,13 @@
       </c>
       <c r="I141" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>ZAFFN77363Q29MX</v>
+        <v>SUXOB97752M21BV</v>
       </c>
     </row>
     <row r="142" spans="1:9">
       <c r="A142" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>NH4455940Z</v>
+        <v>ST1845047U</v>
       </c>
       <c r="B142" t="s">
         <v>1663</v>
@@ -24384,13 +24384,13 @@
       </c>
       <c r="I142" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>SXROL312832H79TN</v>
+        <v>HBBWS142558P15TW</v>
       </c>
     </row>
     <row r="143" spans="1:9">
       <c r="A143" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>HD6309510B</v>
+        <v>GA5706771S</v>
       </c>
       <c r="B143" t="s">
         <v>1664</v>
@@ -24400,13 +24400,13 @@
       </c>
       <c r="I143" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>JFKFY630662S87RX</v>
+        <v>WVQKP373090W81TU</v>
       </c>
     </row>
     <row r="144" spans="1:9">
       <c r="A144" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>ZC2829374A</v>
+        <v>VF372942R</v>
       </c>
       <c r="B144" t="s">
         <v>1665</v>
@@ -24416,13 +24416,13 @@
       </c>
       <c r="I144" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>ZXXYI73458U24RV</v>
+        <v>BUTQT989119L3IB</v>
       </c>
     </row>
     <row r="145" spans="1:12">
       <c r="A145" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>EB7217877U</v>
+        <v>UB1036058W</v>
       </c>
       <c r="B145" t="s">
         <v>1666</v>
@@ -24432,13 +24432,13 @@
       </c>
       <c r="I145" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>VDYJF748139A9EH</v>
+        <v>SGWMA312536S30MU</v>
       </c>
     </row>
     <row r="146" spans="1:12">
       <c r="A146" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>NS2628688L</v>
+        <v>DW6762077Z</v>
       </c>
       <c r="B146" t="s">
         <v>1667</v>
@@ -24448,13 +24448,13 @@
       </c>
       <c r="I146" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>TFTEM406931N25NA</v>
+        <v>DWUWS438815L73TA</v>
       </c>
     </row>
     <row r="147" spans="1:12">
       <c r="A147" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>RF2576786I</v>
+        <v>AM4903020J</v>
       </c>
       <c r="B147" t="s">
         <v>1668</v>
@@ -24464,13 +24464,13 @@
       </c>
       <c r="I147" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>BRMXY415236I34ZD</v>
+        <v>QDDEO413444U23TY</v>
       </c>
     </row>
     <row r="148" spans="1:12">
       <c r="A148" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>KW7122192D</v>
+        <v>CH6742505B</v>
       </c>
       <c r="B148" t="s">
         <v>1669</v>
@@ -24480,13 +24480,13 @@
       </c>
       <c r="I148" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>PXPLN620519J75PI</v>
+        <v>NSBFZ947159X5GI</v>
       </c>
     </row>
     <row r="149" spans="1:12">
       <c r="A149" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>QB9585165F</v>
+        <v>KJ71344Z</v>
       </c>
       <c r="B149" t="s">
         <v>1670</v>
@@ -24496,13 +24496,13 @@
       </c>
       <c r="I149" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>PLAPQ800229R81VP</v>
+        <v>FRDFZ882051U56WR</v>
       </c>
     </row>
     <row r="150" spans="1:12">
       <c r="A150" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>CS5777346Z</v>
+        <v>MQ3256089R</v>
       </c>
       <c r="B150" t="s">
         <v>1671</v>
@@ -24512,13 +24512,13 @@
       </c>
       <c r="I150" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>YXNHN214841V38JV</v>
+        <v>UTQKW195567W67LX</v>
       </c>
     </row>
     <row r="151" spans="1:12">
       <c r="A151" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>BU9072565W</v>
+        <v>ML9909333B</v>
       </c>
       <c r="B151" t="s">
         <v>1672</v>
@@ -24528,13 +24528,13 @@
       </c>
       <c r="I151" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>YVNIN131256Z25SM</v>
+        <v>UEKEB166453V78JI</v>
       </c>
     </row>
     <row r="152" spans="1:12">
       <c r="A152" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>ST5749492D</v>
+        <v>DL4937517M</v>
       </c>
       <c r="B152" t="s">
         <v>1673</v>
@@ -24544,7 +24544,7 @@
       </c>
       <c r="I152" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>QFHGC721673A26IV</v>
+        <v>ZZQAX183130S41XA</v>
       </c>
       <c r="K152" s="28" t="e">
         <f t="shared" ref="K152" si="7">RIGHT(J152, LEN(J152)-1)</f>
@@ -24558,7 +24558,7 @@
     <row r="153" spans="1:12">
       <c r="A153" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>NR3505639K</v>
+        <v>MV7716475A</v>
       </c>
       <c r="B153" t="s">
         <v>1674</v>
@@ -24568,13 +24568,13 @@
       </c>
       <c r="I153" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>QQBFV355926V50NV</v>
+        <v>TPTYX337930A14WE</v>
       </c>
     </row>
     <row r="154" spans="1:12">
       <c r="A154" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>NP4209069U</v>
+        <v>CY849766P</v>
       </c>
       <c r="B154" t="s">
         <v>1675</v>
@@ -24584,13 +24584,13 @@
       </c>
       <c r="I154" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>QMFUJ702626Q15AJ</v>
+        <v>ALZLB272680V36ID</v>
       </c>
     </row>
     <row r="155" spans="1:12">
       <c r="A155" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>QM1088819M</v>
+        <v>JI6793157I</v>
       </c>
       <c r="B155" t="s">
         <v>1676</v>
@@ -24600,13 +24600,13 @@
       </c>
       <c r="I155" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>SVMGR100440U50PU</v>
+        <v>VRTDT325561O74ZN</v>
       </c>
     </row>
     <row r="156" spans="1:12">
       <c r="A156" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>QN5871547U</v>
+        <v>HN7755953S</v>
       </c>
       <c r="B156" t="s">
         <v>1677</v>
@@ -24616,13 +24616,13 @@
       </c>
       <c r="I156" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LLDJC325444Q25OJ</v>
+        <v>JTBZE472482Y40GF</v>
       </c>
     </row>
     <row r="157" spans="1:12">
       <c r="A157" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>UK7666136I</v>
+        <v>KR9143626I</v>
       </c>
       <c r="B157" t="s">
         <v>1678</v>
@@ -24632,13 +24632,13 @@
       </c>
       <c r="I157" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>KHUKC793379T49TL</v>
+        <v>LDPOR876654W65DX</v>
       </c>
     </row>
     <row r="158" spans="1:12">
       <c r="A158" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>XP7363449M</v>
+        <v>NC8411176B</v>
       </c>
       <c r="B158" t="s">
         <v>1679</v>
@@ -24648,13 +24648,13 @@
       </c>
       <c r="I158" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>PPEPL771250R82CT</v>
+        <v>ARGVB850248F72JY</v>
       </c>
     </row>
     <row r="159" spans="1:12">
       <c r="A159" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>DF3894386N</v>
+        <v>UX2864461J</v>
       </c>
       <c r="B159" t="s">
         <v>1680</v>
@@ -24664,13 +24664,13 @@
       </c>
       <c r="I159" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>DVFEF924046P42YZ</v>
+        <v>QMNDG709856R11DM</v>
       </c>
     </row>
     <row r="160" spans="1:12">
       <c r="A160" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>NG7570539E</v>
+        <v>YV9556978Z</v>
       </c>
       <c r="B160" t="s">
         <v>1681</v>
@@ -24680,13 +24680,13 @@
       </c>
       <c r="I160" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>KLWWF639866M37FC</v>
+        <v>QZSJB552915H73AS</v>
       </c>
     </row>
     <row r="161" spans="1:9">
       <c r="A161" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>VA6281791K</v>
+        <v>JZ3348191E</v>
       </c>
       <c r="B161" t="s">
         <v>1682</v>
@@ -24696,13 +24696,13 @@
       </c>
       <c r="I161" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>GAISI620256U83VG</v>
+        <v>KOIRT645720A34FW</v>
       </c>
     </row>
     <row r="162" spans="1:9">
       <c r="A162" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>AB3260599Q</v>
+        <v>YT4751442Q</v>
       </c>
       <c r="B162" t="s">
         <v>1683</v>
@@ -24712,13 +24712,13 @@
       </c>
       <c r="I162" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>MKQNT116153O45RK</v>
+        <v>VJHBJ877750C77JU</v>
       </c>
     </row>
     <row r="163" spans="1:9">
       <c r="A163" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>BG1806400N</v>
+        <v>QV9335353O</v>
       </c>
       <c r="B163" t="s">
         <v>1684</v>
@@ -24728,13 +24728,13 @@
       </c>
       <c r="I163" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>RCKJR844506C1CT</v>
+        <v>LSUQI742935R90JR</v>
       </c>
     </row>
     <row r="164" spans="1:9">
       <c r="A164" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>EW3148458K</v>
+        <v>YR39512K</v>
       </c>
       <c r="B164" t="s">
         <v>1685</v>
@@ -24744,13 +24744,13 @@
       </c>
       <c r="I164" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>KDFFU762091K4MF</v>
+        <v>JWVHV222624N35NB</v>
       </c>
     </row>
     <row r="165" spans="1:9">
       <c r="A165" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>TF3466957P</v>
+        <v>LH3928469I</v>
       </c>
       <c r="B165" t="s">
         <v>1686</v>
@@ -24760,13 +24760,13 @@
       </c>
       <c r="I165" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>HGIZD585068E75QJ</v>
+        <v>PRRVP596109W58QO</v>
       </c>
     </row>
     <row r="166" spans="1:9">
       <c r="A166" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>WY6790906W</v>
+        <v>IP475060J</v>
       </c>
       <c r="B166" t="s">
         <v>1687</v>
@@ -24776,13 +24776,13 @@
       </c>
       <c r="I166" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>JUJZW847872H47CI</v>
+        <v>KIXYP290761J59RY</v>
       </c>
     </row>
     <row r="167" spans="1:9">
       <c r="A167" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>TU8963345K</v>
+        <v>IZ7501512F</v>
       </c>
       <c r="B167" t="s">
         <v>1688</v>
@@ -24792,13 +24792,13 @@
       </c>
       <c r="I167" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>SICSZ267893V30XN</v>
+        <v>URTPR223090S30LY</v>
       </c>
     </row>
     <row r="168" spans="1:9">
       <c r="A168" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>DA5435647E</v>
+        <v>QT6831510X</v>
       </c>
       <c r="B168" t="s">
         <v>1689</v>
@@ -24808,13 +24808,13 @@
       </c>
       <c r="I168" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>ITPYH487257A84XJ</v>
+        <v>PIRMT281354A10UU</v>
       </c>
     </row>
     <row r="169" spans="1:9">
       <c r="A169" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>HN558071Y</v>
+        <v>SZ2020922W</v>
       </c>
       <c r="B169" t="s">
         <v>1690</v>
@@ -24824,13 +24824,13 @@
       </c>
       <c r="I169" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>HPUWL396333K73QI</v>
+        <v>YVCME782811O29HP</v>
       </c>
     </row>
     <row r="170" spans="1:9">
       <c r="A170" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>RF386400H</v>
+        <v>QB1257552O</v>
       </c>
       <c r="B170" t="s">
         <v>1691</v>
@@ -24840,13 +24840,13 @@
       </c>
       <c r="I170" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>VSGRF768942Z97NS</v>
+        <v>TVACX221157Y62AP</v>
       </c>
     </row>
     <row r="171" spans="1:9">
       <c r="A171" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>HS7022790V</v>
+        <v>LI2376345U</v>
       </c>
       <c r="B171" t="s">
         <v>1692</v>
@@ -24856,13 +24856,13 @@
       </c>
       <c r="I171" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>CURYX188914R34UA</v>
+        <v>PRNIB127583X13FN</v>
       </c>
     </row>
     <row r="172" spans="1:9">
       <c r="A172" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>JD488024W</v>
+        <v>OV9973914K</v>
       </c>
       <c r="B172" t="s">
         <v>1693</v>
@@ -24872,13 +24872,13 @@
       </c>
       <c r="I172" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>AEQZM815109Z30UR</v>
+        <v>WQCTA341782G87TP</v>
       </c>
     </row>
     <row r="173" spans="1:9">
       <c r="A173" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>PR5251998A</v>
+        <v>WT4298069S</v>
       </c>
       <c r="B173" t="s">
         <v>1694</v>
@@ -24888,13 +24888,13 @@
       </c>
       <c r="I173" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>FAGRO223989X54KC</v>
+        <v>WAHRC27648B71XZ</v>
       </c>
     </row>
     <row r="174" spans="1:9">
       <c r="A174" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>DY8928123K</v>
+        <v>VG6168320F</v>
       </c>
       <c r="B174" t="s">
         <v>1695</v>
@@ -24904,13 +24904,13 @@
       </c>
       <c r="I174" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>KRYZO112700Z91HX</v>
+        <v>JEWFS355043J62GU</v>
       </c>
     </row>
     <row r="175" spans="1:9">
       <c r="A175" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>XP7336068M</v>
+        <v>NK3432611O</v>
       </c>
       <c r="B175" t="s">
         <v>1696</v>
@@ -24920,13 +24920,13 @@
       </c>
       <c r="I175" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>JTPNM133590B75CG</v>
+        <v>MSETL933709J88QG</v>
       </c>
     </row>
     <row r="176" spans="1:9">
       <c r="A176" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>FI2351734V</v>
+        <v>EX1921839Q</v>
       </c>
       <c r="B176" t="s">
         <v>1697</v>
@@ -24936,13 +24936,13 @@
       </c>
       <c r="I176" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LEHXN919534I13JY</v>
+        <v>AQSVP213375T79XU</v>
       </c>
     </row>
     <row r="177" spans="1:9">
       <c r="A177" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>TG2777816R</v>
+        <v>GY2997642D</v>
       </c>
       <c r="B177" t="s">
         <v>1698</v>
@@ -24952,13 +24952,13 @@
       </c>
       <c r="I177" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>KGOJF205776V99VZ</v>
+        <v>ESCKD123625L71RR</v>
       </c>
     </row>
     <row r="178" spans="1:9">
       <c r="A178" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>VP769913S</v>
+        <v>BO4059730V</v>
       </c>
       <c r="B178" t="s">
         <v>1699</v>
@@ -24968,13 +24968,13 @@
       </c>
       <c r="I178" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>IUNRO213253X79VW</v>
+        <v>KPDOF471258X15ZZ</v>
       </c>
     </row>
     <row r="179" spans="1:9">
       <c r="A179" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>JV3310067C</v>
+        <v>DA906877G</v>
       </c>
       <c r="B179" t="s">
         <v>1700</v>
@@ -24984,13 +24984,13 @@
       </c>
       <c r="I179" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>ZEVFQ312041J94TW</v>
+        <v>QCSFQ441539W11HM</v>
       </c>
     </row>
     <row r="180" spans="1:9">
       <c r="A180" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>UF1360958D</v>
+        <v>FR1618941U</v>
       </c>
       <c r="B180" t="s">
         <v>1701</v>
@@ -25000,13 +25000,13 @@
       </c>
       <c r="I180" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>WEXBL700222Z93RK</v>
+        <v>PFYLV57644U90BY</v>
       </c>
     </row>
     <row r="181" spans="1:9">
       <c r="A181" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>JS4796112H</v>
+        <v>YB5431863P</v>
       </c>
       <c r="B181" t="s">
         <v>1702</v>
@@ -25016,13 +25016,13 @@
       </c>
       <c r="I181" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>XQFLH444823C52GA</v>
+        <v>BBAFQ706563F35AZ</v>
       </c>
     </row>
     <row r="182" spans="1:9">
       <c r="A182" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>FM6026637U</v>
+        <v>YQ7396946U</v>
       </c>
       <c r="B182" t="s">
         <v>1703</v>
@@ -25032,13 +25032,13 @@
       </c>
       <c r="I182" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>IIDAQ975405V70FE</v>
+        <v>HAHBO412881A89WF</v>
       </c>
     </row>
     <row r="183" spans="1:9">
       <c r="A183" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>TK8023544G</v>
+        <v>LR8297583Q</v>
       </c>
       <c r="B183" t="s">
         <v>1704</v>
@@ -25048,13 +25048,13 @@
       </c>
       <c r="I183" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>HIUXT518067R54XA</v>
+        <v>PMHBA108714B68MA</v>
       </c>
     </row>
     <row r="184" spans="1:9">
       <c r="A184" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>WG6462625N</v>
+        <v>SS8894115P</v>
       </c>
       <c r="B184" t="s">
         <v>1705</v>
@@ -25064,13 +25064,13 @@
       </c>
       <c r="I184" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>OLXOR226719J69OK</v>
+        <v>RYLOK58425T42NY</v>
       </c>
     </row>
     <row r="185" spans="1:9">
       <c r="A185" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>EL5764135B</v>
+        <v>PS7584831T</v>
       </c>
       <c r="B185" t="s">
         <v>1706</v>
@@ -25080,13 +25080,13 @@
       </c>
       <c r="I185" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>MHOBC240600M30FH</v>
+        <v>GCYDM980740M48VU</v>
       </c>
     </row>
     <row r="186" spans="1:9">
       <c r="A186" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>ID5985595N</v>
+        <v>BU22158M</v>
       </c>
       <c r="B186" t="s">
         <v>1707</v>
@@ -25096,13 +25096,13 @@
       </c>
       <c r="I186" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>BBLPB563491X32GT</v>
+        <v>KKAZA425070I29NI</v>
       </c>
     </row>
     <row r="187" spans="1:9">
       <c r="A187" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>TX2672261T</v>
+        <v>PC7618068K</v>
       </c>
       <c r="B187" t="s">
         <v>1708</v>
@@ -25112,13 +25112,13 @@
       </c>
       <c r="I187" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>XVSOJ167291Y48LS</v>
+        <v>ZHWQZ150488W19MO</v>
       </c>
     </row>
     <row r="188" spans="1:9">
       <c r="A188" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>WT6764789X</v>
+        <v>JN2989662I</v>
       </c>
       <c r="B188" t="s">
         <v>1709</v>
@@ -25128,13 +25128,13 @@
       </c>
       <c r="I188" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>JGBHJ349842U36DW</v>
+        <v>LBEOF201362W62DD</v>
       </c>
     </row>
     <row r="189" spans="1:9">
       <c r="A189" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>OG2189282K</v>
+        <v>HV6372500S</v>
       </c>
       <c r="B189" t="s">
         <v>1710</v>
@@ -25144,13 +25144,13 @@
       </c>
       <c r="I189" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>KBIVG807150M34NR</v>
+        <v>MCFMU66253M88TG</v>
       </c>
     </row>
     <row r="190" spans="1:9">
       <c r="A190" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>ZZ3730437Z</v>
+        <v>WG24901K</v>
       </c>
       <c r="B190" t="s">
         <v>1711</v>
@@ -25160,13 +25160,13 @@
       </c>
       <c r="I190" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>ZGPEV784679K8NH</v>
+        <v>MHCUJ688047M36CU</v>
       </c>
     </row>
     <row r="191" spans="1:9">
       <c r="A191" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>MT5690784S</v>
+        <v>GK7891302K</v>
       </c>
       <c r="B191" t="s">
         <v>1712</v>
@@ -25176,13 +25176,13 @@
       </c>
       <c r="I191" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>QKQAZ965913N76RQ</v>
+        <v>KNNHB211040G41SA</v>
       </c>
     </row>
     <row r="192" spans="1:9">
       <c r="A192" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>GO7921095O</v>
+        <v>ZQ6652586E</v>
       </c>
       <c r="B192" t="s">
         <v>1713</v>
@@ -25192,13 +25192,13 @@
       </c>
       <c r="I192" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>VZPDY260983O60QZ</v>
+        <v>PGXPG565079U56PB</v>
       </c>
     </row>
     <row r="193" spans="1:9">
       <c r="A193" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>JI675964C</v>
+        <v>HJ2029108V</v>
       </c>
       <c r="B193" t="s">
         <v>1714</v>
@@ -25208,13 +25208,13 @@
       </c>
       <c r="I193" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>RZBJJ810148P90YX</v>
+        <v>LRUML878771O27BX</v>
       </c>
     </row>
     <row r="194" spans="1:9">
       <c r="A194" s="6" t="str">
         <f t="shared" ref="A194:A257" ca="1" si="8">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,9999999)&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>LB6548833C</v>
+        <v>EP7552716D</v>
       </c>
       <c r="B194" t="s">
         <v>1715</v>
@@ -25224,13 +25224,13 @@
       </c>
       <c r="I194" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>QRUDM639459G15HJ</v>
+        <v>NQIMO26129J62YM</v>
       </c>
     </row>
     <row r="195" spans="1:9">
       <c r="A195" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>WU5474482V</v>
+        <v>UJ1973167Z</v>
       </c>
       <c r="B195" t="s">
         <v>1716</v>
@@ -25240,13 +25240,13 @@
       </c>
       <c r="I195" t="str">
         <f t="shared" ref="I195:I250" ca="1" si="9">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,999999)&amp;CHAR(RANDBETWEEN(65,90))&amp;(RANDBETWEEN(1,99))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>VNDFY974121U90AZ</v>
+        <v>TGVHJ885853H73UM</v>
       </c>
     </row>
     <row r="196" spans="1:9">
       <c r="A196" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>CV2300714X</v>
+        <v>EI4336711J</v>
       </c>
       <c r="B196" t="s">
         <v>1717</v>
@@ -25256,13 +25256,13 @@
       </c>
       <c r="I196" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>JHFTI713183J56BX</v>
+        <v>GGKKA905597H37VM</v>
       </c>
     </row>
     <row r="197" spans="1:9">
       <c r="A197" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>PP4338753I</v>
+        <v>KW4038349U</v>
       </c>
       <c r="B197" t="s">
         <v>1718</v>
@@ -25272,13 +25272,13 @@
       </c>
       <c r="I197" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>TPNVI752797F33LT</v>
+        <v>ISXQS59871H17XO</v>
       </c>
     </row>
     <row r="198" spans="1:9">
       <c r="A198" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>TW7379971J</v>
+        <v>MJ8229443F</v>
       </c>
       <c r="B198" t="s">
         <v>1719</v>
@@ -25288,13 +25288,13 @@
       </c>
       <c r="I198" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>LSSUF401814V10VG</v>
+        <v>XEWSZ653008M90WO</v>
       </c>
     </row>
     <row r="199" spans="1:9">
       <c r="A199" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>HD9239142U</v>
+        <v>AB9893787Q</v>
       </c>
       <c r="B199" t="s">
         <v>1720</v>
@@ -25304,13 +25304,13 @@
       </c>
       <c r="I199" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>MJADA24865U43GW</v>
+        <v>EETNJ89281S8DP</v>
       </c>
     </row>
     <row r="200" spans="1:9">
       <c r="A200" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>DH6878645Y</v>
+        <v>XR1908418U</v>
       </c>
       <c r="B200" t="s">
         <v>1721</v>
@@ -25320,13 +25320,13 @@
       </c>
       <c r="I200" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>QWNAV621791W31YN</v>
+        <v>FBECK254111Y95JI</v>
       </c>
     </row>
     <row r="201" spans="1:9">
       <c r="A201" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>DZ8592449C</v>
+        <v>QU8168893L</v>
       </c>
       <c r="B201" t="s">
         <v>1722</v>
@@ -25336,13 +25336,13 @@
       </c>
       <c r="I201" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>IQMHF962636H73PY</v>
+        <v>COVOO692771T95XM</v>
       </c>
     </row>
     <row r="202" spans="1:9">
       <c r="A202" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>GS4856420A</v>
+        <v>CZ1333171E</v>
       </c>
       <c r="B202" t="s">
         <v>1723</v>
@@ -25352,13 +25352,13 @@
       </c>
       <c r="I202" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>PGUDH755285M73AW</v>
+        <v>KLHBI775268G5JU</v>
       </c>
     </row>
     <row r="203" spans="1:9">
       <c r="A203" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>LG4584410Z</v>
+        <v>KF8155426J</v>
       </c>
       <c r="B203" t="s">
         <v>1724</v>
@@ -25368,13 +25368,13 @@
       </c>
       <c r="I203" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>PSJGX564647R98HR</v>
+        <v>SPREA494178F41HN</v>
       </c>
     </row>
     <row r="204" spans="1:9">
       <c r="A204" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>ZL8919493V</v>
+        <v>PD7402708D</v>
       </c>
       <c r="B204" t="s">
         <v>1725</v>
@@ -25384,13 +25384,13 @@
       </c>
       <c r="I204" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>ZPQLG109003R67RW</v>
+        <v>SKCUR96962P35QM</v>
       </c>
     </row>
     <row r="205" spans="1:9">
       <c r="A205" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>YO8795646P</v>
+        <v>MV2315284I</v>
       </c>
       <c r="B205" t="s">
         <v>1726</v>
@@ -25400,13 +25400,13 @@
       </c>
       <c r="I205" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>ZFYRA18680T41CE</v>
+        <v>QDAGR821028J66EM</v>
       </c>
     </row>
     <row r="206" spans="1:9">
       <c r="A206" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>LK8492683V</v>
+        <v>XP8858406H</v>
       </c>
       <c r="B206" t="s">
         <v>1727</v>
@@ -25416,13 +25416,13 @@
       </c>
       <c r="I206" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>DKKSW490951Z71XX</v>
+        <v>IJGSU461034J22RK</v>
       </c>
     </row>
     <row r="207" spans="1:9">
       <c r="A207" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>QP2129000T</v>
+        <v>MT7069206X</v>
       </c>
       <c r="B207" t="s">
         <v>1728</v>
@@ -25432,13 +25432,13 @@
       </c>
       <c r="I207" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>CLCCV800092T52FU</v>
+        <v>JBLVU225680J48IQ</v>
       </c>
     </row>
     <row r="208" spans="1:9">
       <c r="A208" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>IS4761504W</v>
+        <v>RI654128O</v>
       </c>
       <c r="B208" t="s">
         <v>1729</v>
@@ -25448,13 +25448,13 @@
       </c>
       <c r="I208" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>TEMCG286913S77DT</v>
+        <v>BPPTG613954W37RA</v>
       </c>
     </row>
     <row r="209" spans="1:9">
       <c r="A209" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>WP6722396P</v>
+        <v>EX6070930V</v>
       </c>
       <c r="B209" t="s">
         <v>1730</v>
@@ -25464,13 +25464,13 @@
       </c>
       <c r="I209" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>OQGNH323233V45HA</v>
+        <v>SJOME528911Z48RB</v>
       </c>
     </row>
     <row r="210" spans="1:9">
       <c r="A210" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>UV127404O</v>
+        <v>BH5669105W</v>
       </c>
       <c r="B210" t="s">
         <v>1731</v>
@@ -25480,13 +25480,13 @@
       </c>
       <c r="I210" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>BGTWW159419K92TS</v>
+        <v>HOVKJ862977Z92FQ</v>
       </c>
     </row>
     <row r="211" spans="1:9">
       <c r="A211" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>KE4115900W</v>
+        <v>NK5242121P</v>
       </c>
       <c r="B211" t="s">
         <v>1732</v>
@@ -25496,13 +25496,13 @@
       </c>
       <c r="I211" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>JRKKU895225V18ZR</v>
+        <v>MUNQO616191U60YF</v>
       </c>
     </row>
     <row r="212" spans="1:9">
       <c r="A212" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>BR3703723Z</v>
+        <v>AE2680486L</v>
       </c>
       <c r="B212" t="s">
         <v>1733</v>
@@ -25512,13 +25512,13 @@
       </c>
       <c r="I212" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>EVSHS370013T80OL</v>
+        <v>SBZOC25893G51WV</v>
       </c>
     </row>
     <row r="213" spans="1:9">
       <c r="A213" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>QV9721884E</v>
+        <v>UH2821158E</v>
       </c>
       <c r="B213" t="s">
         <v>1734</v>
@@ -25528,13 +25528,13 @@
       </c>
       <c r="I213" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>NZUBM969314P47DV</v>
+        <v>BGFXW441023Q50TH</v>
       </c>
     </row>
     <row r="214" spans="1:9">
       <c r="A214" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>IL8914911V</v>
+        <v>UC2574966D</v>
       </c>
       <c r="B214" t="s">
         <v>1735</v>
@@ -25544,13 +25544,13 @@
       </c>
       <c r="I214" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>QSFFB192555H47OO</v>
+        <v>NCIZX789337D24BL</v>
       </c>
     </row>
     <row r="215" spans="1:9">
       <c r="A215" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>ST2657382H</v>
+        <v>KY703476T</v>
       </c>
       <c r="B215" t="s">
         <v>1736</v>
@@ -25560,13 +25560,13 @@
       </c>
       <c r="I215" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>VVIGH330863C32DU</v>
+        <v>FRBKK756911B61EQ</v>
       </c>
     </row>
     <row r="216" spans="1:9">
       <c r="A216" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>BR1662312V</v>
+        <v>SW8778144W</v>
       </c>
       <c r="B216" t="s">
         <v>1737</v>
@@ -25576,13 +25576,13 @@
       </c>
       <c r="I216" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>DFLEF321931F22SR</v>
+        <v>RILZT909885M25HP</v>
       </c>
     </row>
     <row r="217" spans="1:9">
       <c r="A217" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>LF2257306F</v>
+        <v>KF1205512W</v>
       </c>
       <c r="B217" t="s">
         <v>1738</v>
@@ -25592,13 +25592,13 @@
       </c>
       <c r="I217" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>NSBBA995409P50RA</v>
+        <v>GRGAJ140723B44GF</v>
       </c>
     </row>
     <row r="218" spans="1:9">
       <c r="A218" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>OF3462454N</v>
+        <v>LU1031761P</v>
       </c>
       <c r="B218" t="s">
         <v>1739</v>
@@ -25608,13 +25608,13 @@
       </c>
       <c r="I218" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>PVUCI698739J87SJ</v>
+        <v>SMCIG989796R47PG</v>
       </c>
     </row>
     <row r="219" spans="1:9">
       <c r="A219" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>FC5085028R</v>
+        <v>IJ6770731G</v>
       </c>
       <c r="B219" t="s">
         <v>1740</v>
@@ -25624,13 +25624,13 @@
       </c>
       <c r="I219" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>HGSYI501684V29DE</v>
+        <v>DTFTB966697R51FL</v>
       </c>
     </row>
     <row r="220" spans="1:9">
       <c r="A220" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>GE5956493T</v>
+        <v>NR5342731V</v>
       </c>
       <c r="B220" t="s">
         <v>1741</v>
@@ -25640,13 +25640,13 @@
       </c>
       <c r="I220" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>MVNGN437248O94KQ</v>
+        <v>WYVSM604645N36JH</v>
       </c>
     </row>
     <row r="221" spans="1:9">
       <c r="A221" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>KE4001431I</v>
+        <v>OW2341668E</v>
       </c>
       <c r="B221" t="s">
         <v>1742</v>
@@ -25656,13 +25656,13 @@
       </c>
       <c r="I221" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>WYQNK748171N45IO</v>
+        <v>QPNHI273157O35PP</v>
       </c>
     </row>
     <row r="222" spans="1:9">
       <c r="A222" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>PF6098079P</v>
+        <v>JT1190786M</v>
       </c>
       <c r="B222" t="s">
         <v>1743</v>
@@ -25672,13 +25672,13 @@
       </c>
       <c r="I222" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>QFJRL882181A91KN</v>
+        <v>YEKKM483227X84ZL</v>
       </c>
     </row>
     <row r="223" spans="1:9">
       <c r="A223" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>IR2408726F</v>
+        <v>ZV5392790D</v>
       </c>
       <c r="B223" t="s">
         <v>1744</v>
@@ -25688,13 +25688,13 @@
       </c>
       <c r="I223" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>MOITD817968Y83MV</v>
+        <v>VSULT903695H38EI</v>
       </c>
     </row>
     <row r="224" spans="1:9">
       <c r="A224" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>VD1807576H</v>
+        <v>LV5734640D</v>
       </c>
       <c r="B224" t="s">
         <v>1745</v>
@@ -25704,13 +25704,13 @@
       </c>
       <c r="I224" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>POYHV169445O21VJ</v>
+        <v>HNWIC553082V85HX</v>
       </c>
     </row>
     <row r="225" spans="1:9">
       <c r="A225" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>YQ6971893V</v>
+        <v>QI5369840J</v>
       </c>
       <c r="B225" t="s">
         <v>1746</v>
@@ -25720,13 +25720,13 @@
       </c>
       <c r="I225" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>WVAXY583348B18RD</v>
+        <v>ZSWDQ991397G74QN</v>
       </c>
     </row>
     <row r="226" spans="1:9">
       <c r="A226" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>EF2350080S</v>
+        <v>PX4288531U</v>
       </c>
       <c r="B226" t="s">
         <v>1747</v>
@@ -25736,13 +25736,13 @@
       </c>
       <c r="I226" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>SKSIG328256S63AW</v>
+        <v>FLWGW66920X30GA</v>
       </c>
     </row>
     <row r="227" spans="1:9">
       <c r="A227" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>JV9514110H</v>
+        <v>IL6346578I</v>
       </c>
       <c r="B227" t="s">
         <v>1748</v>
@@ -25752,13 +25752,13 @@
       </c>
       <c r="I227" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>LYDNM491967B56CK</v>
+        <v>OOLWI498904I45TK</v>
       </c>
     </row>
     <row r="228" spans="1:9">
       <c r="A228" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>WU1697879N</v>
+        <v>JJ9733120F</v>
       </c>
       <c r="B228" t="s">
         <v>1749</v>
@@ -25768,13 +25768,13 @@
       </c>
       <c r="I228" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>KAWDG349960C51AS</v>
+        <v>UMWBU910780I67NX</v>
       </c>
     </row>
     <row r="229" spans="1:9">
       <c r="A229" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>WO3622202Q</v>
+        <v>GE9430770B</v>
       </c>
       <c r="B229" t="s">
         <v>1750</v>
@@ -25784,13 +25784,13 @@
       </c>
       <c r="I229" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>QRUUI324139U18SN</v>
+        <v>HUHGX754760K36XF</v>
       </c>
     </row>
     <row r="230" spans="1:9">
       <c r="A230" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>OX373610F</v>
+        <v>HT7760807K</v>
       </c>
       <c r="B230" t="s">
         <v>1751</v>
@@ -25800,13 +25800,13 @@
       </c>
       <c r="I230" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>PRTDF340837W76XE</v>
+        <v>DCNLQ965150T3KO</v>
       </c>
     </row>
     <row r="231" spans="1:9">
       <c r="A231" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>RF6568136O</v>
+        <v>NA9613223O</v>
       </c>
       <c r="B231" t="s">
         <v>1752</v>
@@ -25816,13 +25816,13 @@
       </c>
       <c r="I231" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>XJFHA99057C79WW</v>
+        <v>HXUYM700484O35GR</v>
       </c>
     </row>
     <row r="232" spans="1:9">
       <c r="A232" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>QV7012179G</v>
+        <v>WT7192130L</v>
       </c>
       <c r="B232" t="s">
         <v>1753</v>
@@ -25832,13 +25832,13 @@
       </c>
       <c r="I232" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>FLWSG755553R29PQ</v>
+        <v>WIDJI100141S91OC</v>
       </c>
     </row>
     <row r="233" spans="1:9">
       <c r="A233" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>YW5873064R</v>
+        <v>KN6201321G</v>
       </c>
       <c r="B233" t="s">
         <v>1754</v>
@@ -25848,13 +25848,13 @@
       </c>
       <c r="I233" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>DWBMB430532H79LO</v>
+        <v>PHBHK931033P69ZO</v>
       </c>
     </row>
     <row r="234" spans="1:9">
       <c r="A234" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>FM8063548C</v>
+        <v>VI4181059A</v>
       </c>
       <c r="B234" t="s">
         <v>1755</v>
@@ -25864,13 +25864,13 @@
       </c>
       <c r="I234" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>VTRKJ991336B65HS</v>
+        <v>CQIKT377697I81HD</v>
       </c>
     </row>
     <row r="235" spans="1:9">
       <c r="A235" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>MA5054252J</v>
+        <v>VP9719793Q</v>
       </c>
       <c r="B235" t="s">
         <v>1756</v>
@@ -25880,13 +25880,13 @@
       </c>
       <c r="I235" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>XDBIU662999H95EP</v>
+        <v>JTAPB310652V83WF</v>
       </c>
     </row>
     <row r="236" spans="1:9">
       <c r="A236" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>JE6026279M</v>
+        <v>XJ6322813K</v>
       </c>
       <c r="B236" t="s">
         <v>1757</v>
@@ -25896,13 +25896,13 @@
       </c>
       <c r="I236" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>JLXOD521726Q76NW</v>
+        <v>VIXQH494235I61CY</v>
       </c>
     </row>
     <row r="237" spans="1:9">
       <c r="A237" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>AC1337881G</v>
+        <v>HM8306987O</v>
       </c>
       <c r="B237" t="s">
         <v>1758</v>
@@ -25912,13 +25912,13 @@
       </c>
       <c r="I237" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>MJIFM399950E84FO</v>
+        <v>CQNHK922801W66YD</v>
       </c>
     </row>
     <row r="238" spans="1:9">
       <c r="A238" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>OR3431608H</v>
+        <v>ET7801797K</v>
       </c>
       <c r="B238" t="s">
         <v>1759</v>
@@ -25928,13 +25928,13 @@
       </c>
       <c r="I238" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>UKXVF869517F72RE</v>
+        <v>RYUEF654243G85OP</v>
       </c>
     </row>
     <row r="239" spans="1:9">
       <c r="A239" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>IC7036540S</v>
+        <v>RL9452606L</v>
       </c>
       <c r="B239" t="s">
         <v>1760</v>
@@ -25944,13 +25944,13 @@
       </c>
       <c r="I239" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>YZXPR976397Y53LJ</v>
+        <v>MTTIP822358Q40QJ</v>
       </c>
     </row>
     <row r="240" spans="1:9">
       <c r="A240" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>ML2848836Z</v>
+        <v>FO9729572F</v>
       </c>
       <c r="B240" t="s">
         <v>1761</v>
@@ -25960,13 +25960,13 @@
       </c>
       <c r="I240" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>WJQYJ565330E27PD</v>
+        <v>FUPXT705944N63GI</v>
       </c>
     </row>
     <row r="241" spans="1:9">
       <c r="A241" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>UK4874335O</v>
+        <v>ZX9530406O</v>
       </c>
       <c r="B241" t="s">
         <v>1762</v>
@@ -25976,13 +25976,13 @@
       </c>
       <c r="I241" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>IZBQS497659B52GJ</v>
+        <v>JUQYA984074B87IY</v>
       </c>
     </row>
     <row r="242" spans="1:9">
       <c r="A242" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>AZ2988561P</v>
+        <v>GH2543272B</v>
       </c>
       <c r="B242" t="s">
         <v>1763</v>
@@ -25992,13 +25992,13 @@
       </c>
       <c r="I242" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>RHXUX223455X27FJ</v>
+        <v>ATXRI349142D96UV</v>
       </c>
     </row>
     <row r="243" spans="1:9">
       <c r="A243" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>NZ2525330I</v>
+        <v>RE5159908O</v>
       </c>
       <c r="B243" t="s">
         <v>1764</v>
@@ -26008,104 +26008,104 @@
       </c>
       <c r="I243" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>KEGOW372061X91PF</v>
+        <v>MFFMZ787522X97EA</v>
       </c>
     </row>
     <row r="244" spans="1:9">
       <c r="A244" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>TH7903508S</v>
+        <v>BA8829094L</v>
       </c>
       <c r="B244" t="s">
         <v>1765</v>
       </c>
       <c r="I244" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>ZRPQN48641R29ZW</v>
+        <v>PLIYA745539Z36SL</v>
       </c>
     </row>
     <row r="245" spans="1:9">
       <c r="A245" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>FJ867040I</v>
+        <v>YB9527716A</v>
       </c>
       <c r="B245" t="s">
         <v>1766</v>
       </c>
       <c r="I245" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>JZDVZ816744R56KH</v>
+        <v>VGQKW307370X16YA</v>
       </c>
     </row>
     <row r="246" spans="1:9">
       <c r="A246" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>TT7278913E</v>
+        <v>SK8645580N</v>
       </c>
       <c r="B246" t="s">
         <v>1767</v>
       </c>
       <c r="I246" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>GAVFH45750T7EQ</v>
+        <v>PZQBE267421N30TA</v>
       </c>
     </row>
     <row r="247" spans="1:9">
       <c r="A247" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>SU5068409C</v>
+        <v>YL7268550D</v>
       </c>
       <c r="B247" t="s">
         <v>1768</v>
       </c>
       <c r="I247" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>JFZMM371349U90MU</v>
+        <v>CAHOH851344A6PD</v>
       </c>
     </row>
     <row r="248" spans="1:9">
       <c r="A248" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>PX5789314M</v>
+        <v>EP9334854F</v>
       </c>
       <c r="B248" t="s">
         <v>1769</v>
       </c>
       <c r="I248" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>LXQWZ738949U3AO</v>
+        <v>ALJRC269148L71VT</v>
       </c>
     </row>
     <row r="249" spans="1:9">
       <c r="A249" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>ZE47798Z</v>
+        <v>TA9504255R</v>
       </c>
       <c r="B249" t="s">
         <v>1770</v>
       </c>
       <c r="I249" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>YVRAZ570197U70GI</v>
+        <v>IRPDU673538Y71WS</v>
       </c>
     </row>
     <row r="250" spans="1:9">
       <c r="A250" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>XA5837262C</v>
+        <v>JG3331763W</v>
       </c>
       <c r="B250" t="s">
         <v>1771</v>
       </c>
       <c r="I250" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>URZMB995167U31DF</v>
+        <v>XHURA606180C19KY</v>
       </c>
     </row>
     <row r="251" spans="1:9">
       <c r="A251" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>KW8530749E</v>
+        <v>JH9683030R</v>
       </c>
       <c r="B251" t="s">
         <v>1772</v>
@@ -26114,7 +26114,7 @@
     <row r="252" spans="1:9">
       <c r="A252" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>MA1529933D</v>
+        <v>IP5032269J</v>
       </c>
       <c r="B252" t="s">
         <v>1773</v>
@@ -26123,7 +26123,7 @@
     <row r="253" spans="1:9">
       <c r="A253" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>DV2385447S</v>
+        <v>UN9134160B</v>
       </c>
       <c r="B253" t="s">
         <v>1774</v>
@@ -26132,7 +26132,7 @@
     <row r="254" spans="1:9">
       <c r="A254" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>AZ1339278N</v>
+        <v>WR5217109H</v>
       </c>
       <c r="B254" t="s">
         <v>1775</v>
@@ -26141,7 +26141,7 @@
     <row r="255" spans="1:9">
       <c r="A255" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>FO3875174P</v>
+        <v>GE4919812U</v>
       </c>
       <c r="B255" t="s">
         <v>1776</v>
@@ -26150,7 +26150,7 @@
     <row r="256" spans="1:9">
       <c r="A256" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>EF6375086O</v>
+        <v>SN550655A</v>
       </c>
       <c r="B256" t="s">
         <v>1777</v>
@@ -26159,7 +26159,7 @@
     <row r="257" spans="1:2">
       <c r="A257" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>KJ6184491Z</v>
+        <v>JG3719253S</v>
       </c>
       <c r="B257" t="s">
         <v>1778</v>
@@ -26168,7 +26168,7 @@
     <row r="258" spans="1:2">
       <c r="A258" s="6" t="str">
         <f t="shared" ref="A258:A300" ca="1" si="10">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,9999999)&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>XV1270855M</v>
+        <v>JC355010I</v>
       </c>
       <c r="B258" t="s">
         <v>1779</v>
@@ -26177,7 +26177,7 @@
     <row r="259" spans="1:2">
       <c r="A259" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>NK6055469Q</v>
+        <v>HO132417T</v>
       </c>
       <c r="B259" t="s">
         <v>1780</v>
@@ -26186,7 +26186,7 @@
     <row r="260" spans="1:2">
       <c r="A260" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>GZ1440516H</v>
+        <v>UN8541913N</v>
       </c>
       <c r="B260" t="s">
         <v>1781</v>
@@ -26195,7 +26195,7 @@
     <row r="261" spans="1:2">
       <c r="A261" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>IN9642015Q</v>
+        <v>UC893381W</v>
       </c>
       <c r="B261" t="s">
         <v>1782</v>
@@ -26204,7 +26204,7 @@
     <row r="262" spans="1:2">
       <c r="A262" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>JI1198607S</v>
+        <v>XP7168311C</v>
       </c>
       <c r="B262" t="s">
         <v>1783</v>
@@ -26213,7 +26213,7 @@
     <row r="263" spans="1:2">
       <c r="A263" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>JL8408708Y</v>
+        <v>SE3323080T</v>
       </c>
       <c r="B263" t="s">
         <v>1784</v>
@@ -26222,7 +26222,7 @@
     <row r="264" spans="1:2">
       <c r="A264" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>EX1914855I</v>
+        <v>NC2035111G</v>
       </c>
       <c r="B264" t="s">
         <v>1785</v>
@@ -26231,7 +26231,7 @@
     <row r="265" spans="1:2">
       <c r="A265" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>QH4190625R</v>
+        <v>NA893557E</v>
       </c>
       <c r="B265" t="s">
         <v>1786</v>
@@ -26240,7 +26240,7 @@
     <row r="266" spans="1:2">
       <c r="A266" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>ZP2351479X</v>
+        <v>WM3587023R</v>
       </c>
       <c r="B266" t="s">
         <v>1787</v>
@@ -26249,7 +26249,7 @@
     <row r="267" spans="1:2">
       <c r="A267" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>IS6427366K</v>
+        <v>QN4992779G</v>
       </c>
       <c r="B267" t="s">
         <v>1788</v>
@@ -26258,7 +26258,7 @@
     <row r="268" spans="1:2">
       <c r="A268" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>OT7277583S</v>
+        <v>AQ3732638H</v>
       </c>
       <c r="B268" t="s">
         <v>1789</v>
@@ -26267,7 +26267,7 @@
     <row r="269" spans="1:2">
       <c r="A269" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>SQ6482260U</v>
+        <v>YH3692895T</v>
       </c>
       <c r="B269" t="s">
         <v>1790</v>
@@ -26276,7 +26276,7 @@
     <row r="270" spans="1:2">
       <c r="A270" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>NO2514320O</v>
+        <v>BC8512083Y</v>
       </c>
       <c r="B270" t="s">
         <v>1791</v>
@@ -26285,7 +26285,7 @@
     <row r="271" spans="1:2">
       <c r="A271" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>DZ6933245P</v>
+        <v>QR7182884V</v>
       </c>
       <c r="B271" t="s">
         <v>1792</v>
@@ -26294,7 +26294,7 @@
     <row r="272" spans="1:2">
       <c r="A272" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>RO67527F</v>
+        <v>RG7051218C</v>
       </c>
       <c r="B272" t="s">
         <v>1793</v>
@@ -26303,7 +26303,7 @@
     <row r="273" spans="1:2">
       <c r="A273" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>PT4663688N</v>
+        <v>XL7451926Z</v>
       </c>
       <c r="B273" t="s">
         <v>1794</v>
@@ -26312,7 +26312,7 @@
     <row r="274" spans="1:2">
       <c r="A274" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>VL1067462G</v>
+        <v>KB4581908M</v>
       </c>
       <c r="B274" t="s">
         <v>1795</v>
@@ -26321,7 +26321,7 @@
     <row r="275" spans="1:2">
       <c r="A275" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>ZR2927538R</v>
+        <v>GH1200811J</v>
       </c>
       <c r="B275" t="s">
         <v>1796</v>
@@ -26330,7 +26330,7 @@
     <row r="276" spans="1:2">
       <c r="A276" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>KF2771909V</v>
+        <v>PD8340210S</v>
       </c>
       <c r="B276" t="s">
         <v>1797</v>
@@ -26339,7 +26339,7 @@
     <row r="277" spans="1:2">
       <c r="A277" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>XF4693666C</v>
+        <v>NQ221841S</v>
       </c>
       <c r="B277" t="s">
         <v>1798</v>
@@ -26348,7 +26348,7 @@
     <row r="278" spans="1:2">
       <c r="A278" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>AB1150461Y</v>
+        <v>TY7271317H</v>
       </c>
       <c r="B278" t="s">
         <v>1799</v>
@@ -26357,7 +26357,7 @@
     <row r="279" spans="1:2">
       <c r="A279" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>VX3837793O</v>
+        <v>US5246442S</v>
       </c>
       <c r="B279" t="s">
         <v>1800</v>
@@ -26366,7 +26366,7 @@
     <row r="280" spans="1:2">
       <c r="A280" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>RA2777999D</v>
+        <v>LU3804553H</v>
       </c>
       <c r="B280" t="s">
         <v>1801</v>
@@ -26375,7 +26375,7 @@
     <row r="281" spans="1:2">
       <c r="A281" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>HY4165334B</v>
+        <v>TE9077424V</v>
       </c>
       <c r="B281" t="s">
         <v>1802</v>
@@ -26384,7 +26384,7 @@
     <row r="282" spans="1:2">
       <c r="A282" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>CO8008888N</v>
+        <v>ZF6944213E</v>
       </c>
       <c r="B282" t="s">
         <v>1803</v>
@@ -26393,7 +26393,7 @@
     <row r="283" spans="1:2">
       <c r="A283" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>LE3190235V</v>
+        <v>VS4650423S</v>
       </c>
       <c r="B283" t="s">
         <v>1804</v>
@@ -26402,7 +26402,7 @@
     <row r="284" spans="1:2">
       <c r="A284" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>BJ928468D</v>
+        <v>XC9686143L</v>
       </c>
       <c r="B284" t="s">
         <v>1805</v>
@@ -26411,7 +26411,7 @@
     <row r="285" spans="1:2">
       <c r="A285" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>KB1873526W</v>
+        <v>FG4457432X</v>
       </c>
       <c r="B285" t="s">
         <v>1806</v>
@@ -26420,7 +26420,7 @@
     <row r="286" spans="1:2">
       <c r="A286" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>HK4367475G</v>
+        <v>YG2146221Q</v>
       </c>
       <c r="B286" t="s">
         <v>1807</v>
@@ -26429,7 +26429,7 @@
     <row r="287" spans="1:2">
       <c r="A287" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>NJ662681H</v>
+        <v>XT3482908S</v>
       </c>
       <c r="B287" t="s">
         <v>1808</v>
@@ -26438,7 +26438,7 @@
     <row r="288" spans="1:2">
       <c r="A288" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>TM5610774F</v>
+        <v>XV5608166G</v>
       </c>
       <c r="B288" t="s">
         <v>1809</v>
@@ -26447,7 +26447,7 @@
     <row r="289" spans="1:2">
       <c r="A289" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>FJ7211214Z</v>
+        <v>NS156311A</v>
       </c>
       <c r="B289" t="s">
         <v>1810</v>
@@ -26456,7 +26456,7 @@
     <row r="290" spans="1:2">
       <c r="A290" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>AE4827568J</v>
+        <v>AH5619178C</v>
       </c>
       <c r="B290" t="s">
         <v>1811</v>
@@ -26465,7 +26465,7 @@
     <row r="291" spans="1:2">
       <c r="A291" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>IC7234369U</v>
+        <v>CX8391109U</v>
       </c>
       <c r="B291" t="s">
         <v>1812</v>
@@ -26474,7 +26474,7 @@
     <row r="292" spans="1:2">
       <c r="A292" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>SG3948312L</v>
+        <v>WP6248009X</v>
       </c>
       <c r="B292" t="s">
         <v>1813</v>
@@ -26483,7 +26483,7 @@
     <row r="293" spans="1:2">
       <c r="A293" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>YN8009080P</v>
+        <v>TX5345499V</v>
       </c>
       <c r="B293" t="s">
         <v>1814</v>
@@ -26492,7 +26492,7 @@
     <row r="294" spans="1:2">
       <c r="A294" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>ZP923821Q</v>
+        <v>BY77834B</v>
       </c>
       <c r="B294" t="s">
         <v>1815</v>
@@ -26501,7 +26501,7 @@
     <row r="295" spans="1:2">
       <c r="A295" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>IF1494705K</v>
+        <v>HZ2737182L</v>
       </c>
       <c r="B295" t="s">
         <v>1816</v>
@@ -26510,7 +26510,7 @@
     <row r="296" spans="1:2">
       <c r="A296" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>OK1394405T</v>
+        <v>LY4531354X</v>
       </c>
       <c r="B296" t="s">
         <v>1817</v>
@@ -26519,7 +26519,7 @@
     <row r="297" spans="1:2">
       <c r="A297" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>JI859690O</v>
+        <v>HM1468722F</v>
       </c>
       <c r="B297" t="s">
         <v>1818</v>
@@ -26528,7 +26528,7 @@
     <row r="298" spans="1:2">
       <c r="A298" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>FS881731S</v>
+        <v>LC4804452A</v>
       </c>
       <c r="B298" t="s">
         <v>1819</v>
@@ -26537,7 +26537,7 @@
     <row r="299" spans="1:2">
       <c r="A299" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>GE8288986Y</v>
+        <v>VJ6411709P</v>
       </c>
       <c r="B299" t="s">
         <v>1820</v>
@@ -26546,7 +26546,7 @@
     <row r="300" spans="1:2">
       <c r="A300" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>XQ361732X</v>
+        <v>DM506571F</v>
       </c>
       <c r="B300" t="s">
         <v>1821</v>

</xml_diff>

<commit_message>
Added tests for 2076
</commit_message>
<xml_diff>
--- a/src/main/java/testData/ExcelFiles/E2E_Test_Data.xlsx
+++ b/src/main/java/testData/ExcelFiles/E2E_Test_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awhitten/IdeaProjects/Iceberg/src/main/java/testData/ExcelFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A251E713-8BBF-5D4D-A5E2-E3D529BD3EB1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4910D4-EAE2-7041-8958-8672FFD7A972}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21930,7 +21930,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:A13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -22114,7 +22114,7 @@
     <row r="1" spans="1:11">
       <c r="A1" s="6" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,9999999)&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>FH9784718V</v>
+        <v>QX4354024Y</v>
       </c>
       <c r="B1" t="s">
         <v>1522</v>
@@ -22126,7 +22126,7 @@
     <row r="2" spans="1:11">
       <c r="A2" s="6" t="str">
         <f ca="1">7&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,9999999)&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>7L9095710K</v>
+        <v>7Y9413316U</v>
       </c>
       <c r="B2" t="s">
         <v>1523</v>
@@ -22136,21 +22136,21 @@
       </c>
       <c r="I2" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,999999)&amp;CHAR(RANDBETWEEN(65,90))&amp;(RANDBETWEEN(1,99))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>DUGFL881365Z1AQ</v>
+        <v>FMKVH986156Q49VH</v>
       </c>
       <c r="J2" s="28" t="str">
         <f t="shared" ref="J2" ca="1" si="0">RIGHT(I2, LEN(I2)-1)</f>
-        <v>UGFL881365Z1AQ</v>
+        <v>MKVH986156Q49VH</v>
       </c>
       <c r="K2" s="14" t="str">
         <f ca="1">"07"&amp;J2</f>
-        <v>07UGFL881365Z1AQ</v>
+        <v>07MKVH986156Q49VH</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="6" t="str">
         <f t="shared" ref="A3:A65" ca="1" si="1">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,9999999)&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>KT6737876B</v>
+        <v>DQ7706216Z</v>
       </c>
       <c r="B3" t="s">
         <v>1524</v>
@@ -22160,13 +22160,13 @@
       </c>
       <c r="I3" t="str">
         <f t="shared" ref="I3:I66" ca="1" si="2">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,999999)&amp;CHAR(RANDBETWEEN(65,90))&amp;(RANDBETWEEN(1,99))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>HZJEA340726Q66LZ</v>
+        <v>LESUU910679B27SH</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>SR9284059D</v>
+        <v>LW9307207Q</v>
       </c>
       <c r="B4" t="s">
         <v>1525</v>
@@ -22176,13 +22176,13 @@
       </c>
       <c r="I4" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>AMOPU612111L7BF</v>
+        <v>RQOTX734007B52IK</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>BE4236254K</v>
+        <v>AX4257096N</v>
       </c>
       <c r="B5" t="s">
         <v>1526</v>
@@ -22192,13 +22192,13 @@
       </c>
       <c r="I5" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>EQVOP31272O60WW</v>
+        <v>MIJCM53948G73LZ</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UX9745161G</v>
+        <v>XP645857S</v>
       </c>
       <c r="B6" t="s">
         <v>1527</v>
@@ -22208,13 +22208,13 @@
       </c>
       <c r="I6" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>FISBF145317Z13IY</v>
+        <v>MBKJD744100M6UP</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>DO3175556W</v>
+        <v>ZK7779297K</v>
       </c>
       <c r="B7" t="s">
         <v>1528</v>
@@ -22224,13 +22224,13 @@
       </c>
       <c r="I7" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>TEWWJ4540G92AE</v>
+        <v>WUTWZ438191Q8CC</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>JG718415O</v>
+        <v>BB7213741G</v>
       </c>
       <c r="B8" t="s">
         <v>1529</v>
@@ -22240,13 +22240,13 @@
       </c>
       <c r="I8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>SBZPL236858E81NM</v>
+        <v>BEKJD600443N39UI</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>KV8038176N</v>
+        <v>TO9533924H</v>
       </c>
       <c r="B9" t="s">
         <v>1530</v>
@@ -22256,13 +22256,13 @@
       </c>
       <c r="I9" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>PMAYH637046B90WF</v>
+        <v>CWXQD806725O31ML</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>GL5180630R</v>
+        <v>RP7823332S</v>
       </c>
       <c r="B10" t="s">
         <v>1531</v>
@@ -22272,13 +22272,13 @@
       </c>
       <c r="I10" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NASTX492899U54MK</v>
+        <v>MPZET93147L2RK</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>ZN5250572S</v>
+        <v>YR5216203R</v>
       </c>
       <c r="B11" t="s">
         <v>1532</v>
@@ -22288,13 +22288,13 @@
       </c>
       <c r="I11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>TTHKZ316752K89QO</v>
+        <v>MQQMN167902S18NA</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LO8516891W</v>
+        <v>VZ7219168M</v>
       </c>
       <c r="B12" t="s">
         <v>1533</v>
@@ -22304,13 +22304,13 @@
       </c>
       <c r="I12" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>PERPU572528B25GY</v>
+        <v>UNHME433517I34DD</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>VB1644112S</v>
+        <v>GE9371742H</v>
       </c>
       <c r="B13" t="s">
         <v>1534</v>
@@ -22320,13 +22320,13 @@
       </c>
       <c r="I13" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KBPUV247510A92HW</v>
+        <v>ORANI413081Z94VT</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>MC9700420D</v>
+        <v>JW2529571S</v>
       </c>
       <c r="B14" t="s">
         <v>1535</v>
@@ -22336,13 +22336,13 @@
       </c>
       <c r="I14" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>LYZOQ684378K37UH</v>
+        <v>FSDLH461409H47UY</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>BK6938816T</v>
+        <v>GT57506Y</v>
       </c>
       <c r="B15" t="s">
         <v>1536</v>
@@ -22352,13 +22352,13 @@
       </c>
       <c r="I15" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>LOETU833045D32ZC</v>
+        <v>CBTIP339237Z18GJ</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>WW3963241U</v>
+        <v>JV2741133D</v>
       </c>
       <c r="B16" t="s">
         <v>1537</v>
@@ -22368,13 +22368,13 @@
       </c>
       <c r="I16" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>VGZQM794697R57FJ</v>
+        <v>OLEDA707562D23LF</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UH8305943L</v>
+        <v>RG6650020W</v>
       </c>
       <c r="B17" t="s">
         <v>1538</v>
@@ -22384,13 +22384,13 @@
       </c>
       <c r="I17" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NMCVO989333Y16ZE</v>
+        <v>AVKON684033S38TA</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>JZ3564619I</v>
+        <v>MG8124558W</v>
       </c>
       <c r="B18" t="s">
         <v>1539</v>
@@ -22400,13 +22400,13 @@
       </c>
       <c r="I18" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>JOPZA241193A92EY</v>
+        <v>NGVPV245775E5DC</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>SA2317527O</v>
+        <v>KB2609663W</v>
       </c>
       <c r="B19" t="s">
         <v>1540</v>
@@ -22416,13 +22416,13 @@
       </c>
       <c r="I19" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>TPBOK288906Z78OR</v>
+        <v>VHFPM597165I67PH</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NL7435085X</v>
+        <v>LN793422C</v>
       </c>
       <c r="B20" t="s">
         <v>1541</v>
@@ -22432,13 +22432,13 @@
       </c>
       <c r="I20" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>XVDFG604303G95YK</v>
+        <v>ORMXF84605N60KK</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LW5486997V</v>
+        <v>FK7572551A</v>
       </c>
       <c r="B21" t="s">
         <v>1542</v>
@@ -22448,13 +22448,13 @@
       </c>
       <c r="I21" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>VBLZG289834R74VG</v>
+        <v>CIBXA971855B2TX</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>IA9020729X</v>
+        <v>GU6628984M</v>
       </c>
       <c r="B22" t="s">
         <v>1543</v>
@@ -22464,13 +22464,13 @@
       </c>
       <c r="I22" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>DWZOG96248U45UU</v>
+        <v>DVGLI984711R24PB</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>QO7855099S</v>
+        <v>QJ560916T</v>
       </c>
       <c r="B23" t="s">
         <v>1544</v>
@@ -22480,13 +22480,13 @@
       </c>
       <c r="I23" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>VKLZB99865T3BQ</v>
+        <v>SDAGR500455I85BB</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>BL916499A</v>
+        <v>EI5900894Q</v>
       </c>
       <c r="B24" t="s">
         <v>1545</v>
@@ -22496,13 +22496,13 @@
       </c>
       <c r="I24" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>WRRBV473463M89JM</v>
+        <v>NVRJH970332K64FP</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LK6275349F</v>
+        <v>SH1737202I</v>
       </c>
       <c r="B25" t="s">
         <v>1546</v>
@@ -22512,13 +22512,13 @@
       </c>
       <c r="I25" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>GVGZD796036I1EM</v>
+        <v>TDIKT86401M65QF</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>WB9145383L</v>
+        <v>LM7898701B</v>
       </c>
       <c r="B26" t="s">
         <v>1547</v>
@@ -22528,13 +22528,13 @@
       </c>
       <c r="I26" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>LPMUR956821D68YG</v>
+        <v>EEBSA290506O11BV</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>SP8754410V</v>
+        <v>DE8543578F</v>
       </c>
       <c r="B27" t="s">
         <v>1548</v>
@@ -22544,13 +22544,13 @@
       </c>
       <c r="I27" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>WCEKL825480K45NL</v>
+        <v>LPRCX955893M67FM</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>PN1035287N</v>
+        <v>FR742052C</v>
       </c>
       <c r="B28" t="s">
         <v>1549</v>
@@ -22560,13 +22560,13 @@
       </c>
       <c r="I28" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>RJTOT928119G26IO</v>
+        <v>LLHNC438072D17TY</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UU6473790M</v>
+        <v>SW9988224M</v>
       </c>
       <c r="B29" t="s">
         <v>1550</v>
@@ -22576,13 +22576,13 @@
       </c>
       <c r="I29" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>RKOLA592952V55WS</v>
+        <v>OMLWJ592587U77YV</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>GI347679C</v>
+        <v>FY8957779G</v>
       </c>
       <c r="B30" t="s">
         <v>1551</v>
@@ -22592,13 +22592,13 @@
       </c>
       <c r="I30" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>GEFJH42252B52HK</v>
+        <v>UEIWP232508Q99HW</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>HU7972672F</v>
+        <v>QT5189661J</v>
       </c>
       <c r="B31" t="s">
         <v>1552</v>
@@ -22608,13 +22608,13 @@
       </c>
       <c r="I31" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>DINIJ103821X42ZO</v>
+        <v>JSZQZ149301A55EW</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>JQ7675329S</v>
+        <v>FP9174453P</v>
       </c>
       <c r="B32" t="s">
         <v>1553</v>
@@ -22624,13 +22624,13 @@
       </c>
       <c r="I32" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>AAQIS377762D18LB</v>
+        <v>ITJBL183373W82QC</v>
       </c>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>OS8441908T</v>
+        <v>EO3860888B</v>
       </c>
       <c r="B33" t="s">
         <v>1554</v>
@@ -22640,13 +22640,13 @@
       </c>
       <c r="I33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>WPVAU656980Q71BT</v>
+        <v>EGXMG262005Y75GQ</v>
       </c>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>GK6625680N</v>
+        <v>OS4685773X</v>
       </c>
       <c r="B34" t="s">
         <v>1555</v>
@@ -22656,13 +22656,13 @@
       </c>
       <c r="I34" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>FDQIV450242J34JN</v>
+        <v>ZVCIN698360M64GU</v>
       </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>NN7251166I</v>
+        <v>TT8252418I</v>
       </c>
       <c r="B35" t="s">
         <v>1556</v>
@@ -22672,13 +22672,13 @@
       </c>
       <c r="I35" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>FKWBB38906I74WB</v>
+        <v>BKSDV521943I77AU</v>
       </c>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>DR8885642B</v>
+        <v>AP4989483O</v>
       </c>
       <c r="B36" t="s">
         <v>1557</v>
@@ -22688,13 +22688,13 @@
       </c>
       <c r="I36" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>HBQHY786855S56LX</v>
+        <v>HZPLZ450694J26VV</v>
       </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>FJ2319359F</v>
+        <v>KZ7559123B</v>
       </c>
       <c r="B37" t="s">
         <v>1558</v>
@@ -22704,13 +22704,13 @@
       </c>
       <c r="I37" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>YHLAQ267236I45AN</v>
+        <v>DYBFE525031L57FF</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>AE4054702P</v>
+        <v>EO9276123V</v>
       </c>
       <c r="B38" t="s">
         <v>1559</v>
@@ -22720,13 +22720,13 @@
       </c>
       <c r="I38" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>QVSOE973827Z98QB</v>
+        <v>FSDCV918315Q67UM</v>
       </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>GO9084401F</v>
+        <v>OI2145999A</v>
       </c>
       <c r="B39" t="s">
         <v>1560</v>
@@ -22736,13 +22736,13 @@
       </c>
       <c r="I39" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KIBLD812549W74CJ</v>
+        <v>HWPQA280084J88AO</v>
       </c>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>WO9403554U</v>
+        <v>RG569796N</v>
       </c>
       <c r="B40" t="s">
         <v>1561</v>
@@ -22752,13 +22752,13 @@
       </c>
       <c r="I40" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>QYCBR745069O24GX</v>
+        <v>JXOHB143236F62YU</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>FB2060487L</v>
+        <v>FQ9094303J</v>
       </c>
       <c r="B41" t="s">
         <v>1562</v>
@@ -22768,13 +22768,13 @@
       </c>
       <c r="I41" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>ZMMIQ494122O47CR</v>
+        <v>CSOHU851069L83GZ</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>XV6817367B</v>
+        <v>GU841393C</v>
       </c>
       <c r="B42" t="s">
         <v>1563</v>
@@ -22784,13 +22784,13 @@
       </c>
       <c r="I42" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>LCEOD515723L34LN</v>
+        <v>GGUWS370763D10MM</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>LT2588220H</v>
+        <v>CH3185075A</v>
       </c>
       <c r="B43" t="s">
         <v>1564</v>
@@ -22800,13 +22800,13 @@
       </c>
       <c r="I43" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>IXYAD276998W79JH</v>
+        <v>ISTEC72705Y47NI</v>
       </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>ND8133576C</v>
+        <v>FV1093234T</v>
       </c>
       <c r="B44" t="s">
         <v>1565</v>
@@ -22816,13 +22816,13 @@
       </c>
       <c r="I44" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NWPYA629338C97OB</v>
+        <v>TEORP629953D71AT</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>MY4767916M</v>
+        <v>MJ8109115F</v>
       </c>
       <c r="B45" t="s">
         <v>1566</v>
@@ -22832,13 +22832,13 @@
       </c>
       <c r="I45" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>XCOIG767295A19GO</v>
+        <v>ZYUOO463117E80YY</v>
       </c>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>AV8952823R</v>
+        <v>XB9792028G</v>
       </c>
       <c r="B46" t="s">
         <v>1567</v>
@@ -22848,13 +22848,13 @@
       </c>
       <c r="I46" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>RDWVG871311U43DE</v>
+        <v>DDENT938172A19KE</v>
       </c>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>DW9987955B</v>
+        <v>BH9214196R</v>
       </c>
       <c r="B47" t="s">
         <v>1568</v>
@@ -22864,13 +22864,13 @@
       </c>
       <c r="I47" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>AQLCH993790C23DI</v>
+        <v>NZTLI242327R15LA</v>
       </c>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UM121904G</v>
+        <v>XI2920915B</v>
       </c>
       <c r="B48" t="s">
         <v>1569</v>
@@ -22880,13 +22880,13 @@
       </c>
       <c r="I48" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>SVJCX712112B48IO</v>
+        <v>GCSNW154556R88AN</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>ZQ1863548E</v>
+        <v>YZ970229B</v>
       </c>
       <c r="B49" t="s">
         <v>1570</v>
@@ -22896,13 +22896,13 @@
       </c>
       <c r="I49" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>TSDXU275815S11UO</v>
+        <v>KUXSB309547R46CD</v>
       </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>IU973039R</v>
+        <v>CH271225F</v>
       </c>
       <c r="B50" t="s">
         <v>1571</v>
@@ -22912,13 +22912,13 @@
       </c>
       <c r="I50" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>DUIPS798296G47QY</v>
+        <v>SQHOK478320D82GF</v>
       </c>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>VH833982D</v>
+        <v>NS9421595M</v>
       </c>
       <c r="B51" t="s">
         <v>1572</v>
@@ -22928,13 +22928,13 @@
       </c>
       <c r="I51" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>QTVAM903340C13AM</v>
+        <v>SWCYI362265B50CK</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>FU71821R</v>
+        <v>QZ4627062O</v>
       </c>
       <c r="B52" t="s">
         <v>1573</v>
@@ -22944,13 +22944,13 @@
       </c>
       <c r="I52" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>QZQFD561259U60WY</v>
+        <v>LWSTC683601R79EV</v>
       </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>TD6809504T</v>
+        <v>VX3844545A</v>
       </c>
       <c r="B53" t="s">
         <v>1574</v>
@@ -22960,13 +22960,13 @@
       </c>
       <c r="I53" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>MWFWF904691W52BR</v>
+        <v>WQPXY927723D81UC</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>WD9101527P</v>
+        <v>IT1765329A</v>
       </c>
       <c r="B54" t="s">
         <v>1575</v>
@@ -22976,13 +22976,13 @@
       </c>
       <c r="I54" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KJZCZ207729N25EH</v>
+        <v>MWDXW245541H99QX</v>
       </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>JZ5959427A</v>
+        <v>DH458497J</v>
       </c>
       <c r="B55" t="s">
         <v>1576</v>
@@ -22992,13 +22992,13 @@
       </c>
       <c r="I55" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>UEWRA767550X13WO</v>
+        <v>XRYYU49948S49RW</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>BF3380967R</v>
+        <v>GW4167182V</v>
       </c>
       <c r="B56" t="s">
         <v>1577</v>
@@ -23008,13 +23008,13 @@
       </c>
       <c r="I56" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>MDEJD626454V68FH</v>
+        <v>HGYQN542291Y41NZ</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>ZH3336539I</v>
+        <v>RO9114785T</v>
       </c>
       <c r="B57" t="s">
         <v>1578</v>
@@ -23024,13 +23024,13 @@
       </c>
       <c r="I57" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>THGBA144951M31QW</v>
+        <v>OCFUZ172210V33AY</v>
       </c>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>TV8937249O</v>
+        <v>YD637487R</v>
       </c>
       <c r="B58" t="s">
         <v>1579</v>
@@ -23040,13 +23040,13 @@
       </c>
       <c r="I58" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NQTKV583398L43WZ</v>
+        <v>CMDTX351444V54HC</v>
       </c>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>KE2197084E</v>
+        <v>VH6652380G</v>
       </c>
       <c r="B59" t="s">
         <v>1580</v>
@@ -23056,13 +23056,13 @@
       </c>
       <c r="I59" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>NDBGX19278F88HS</v>
+        <v>XSEKZ793087E94QI</v>
       </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>SX2383951A</v>
+        <v>YA3682003T</v>
       </c>
       <c r="B60" t="s">
         <v>1581</v>
@@ -23072,13 +23072,13 @@
       </c>
       <c r="I60" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>FSXFX332521S54JD</v>
+        <v>TTOMH348122W16FR</v>
       </c>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>SP1369639X</v>
+        <v>TF2952161R</v>
       </c>
       <c r="B61" t="s">
         <v>1582</v>
@@ -23088,13 +23088,13 @@
       </c>
       <c r="I61" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>HESAW938306H89LS</v>
+        <v>KLRZC234977Y56PH</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UR2521718A</v>
+        <v>QO6177654Y</v>
       </c>
       <c r="B62" t="s">
         <v>1583</v>
@@ -23104,13 +23104,13 @@
       </c>
       <c r="I62" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>ZTIVT199499R65VP</v>
+        <v>OVLZO156145F22BL</v>
       </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>HT1733975N</v>
+        <v>GQ2920132K</v>
       </c>
       <c r="B63" t="s">
         <v>1584</v>
@@ -23120,13 +23120,13 @@
       </c>
       <c r="I63" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>KKHSW176745W14HD</v>
+        <v>ULCZN64963T81KN</v>
       </c>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>DK9328262D</v>
+        <v>QE9229009P</v>
       </c>
       <c r="B64" t="s">
         <v>1585</v>
@@ -23136,13 +23136,13 @@
       </c>
       <c r="I64" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>WKDNP27436Z90RR</v>
+        <v>YNHTR400031M71SY</v>
       </c>
     </row>
     <row r="65" spans="1:9">
       <c r="A65" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>XL6125226S</v>
+        <v>WI8305403S</v>
       </c>
       <c r="B65" t="s">
         <v>1586</v>
@@ -23152,13 +23152,13 @@
       </c>
       <c r="I65" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>HPKBX422544W3AB</v>
+        <v>AIUUK104227L64JL</v>
       </c>
     </row>
     <row r="66" spans="1:9">
       <c r="A66" s="6" t="str">
         <f t="shared" ref="A66:A129" ca="1" si="3">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,9999999)&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>FU805558B</v>
+        <v>ZR4885599L</v>
       </c>
       <c r="B66" t="s">
         <v>1587</v>
@@ -23168,13 +23168,13 @@
       </c>
       <c r="I66" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>FNDOE629890P67BL</v>
+        <v>QTOTX717742J40MB</v>
       </c>
     </row>
     <row r="67" spans="1:9">
       <c r="A67" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>XW4206449U</v>
+        <v>EK9990209T</v>
       </c>
       <c r="B67" t="s">
         <v>1588</v>
@@ -23184,13 +23184,13 @@
       </c>
       <c r="I67" t="str">
         <f t="shared" ref="I67:I130" ca="1" si="4">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,999999)&amp;CHAR(RANDBETWEEN(65,90))&amp;(RANDBETWEEN(1,99))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>UKZRF234658V41MQ</v>
+        <v>IJETY497372J63SH</v>
       </c>
     </row>
     <row r="68" spans="1:9">
       <c r="A68" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>HJ3467969J</v>
+        <v>WF4916192M</v>
       </c>
       <c r="B68" t="s">
         <v>1589</v>
@@ -23200,13 +23200,13 @@
       </c>
       <c r="I68" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>QNEOB471894R84VX</v>
+        <v>SDGVP43732T87TT</v>
       </c>
     </row>
     <row r="69" spans="1:9">
       <c r="A69" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>RI3481869V</v>
+        <v>II134613F</v>
       </c>
       <c r="B69" t="s">
         <v>1590</v>
@@ -23216,13 +23216,13 @@
       </c>
       <c r="I69" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>BKJQZ591542W43HL</v>
+        <v>JQXVP684191U49TU</v>
       </c>
     </row>
     <row r="70" spans="1:9">
       <c r="A70" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>BH9004029W</v>
+        <v>FF3352379C</v>
       </c>
       <c r="B70" t="s">
         <v>1591</v>
@@ -23232,13 +23232,13 @@
       </c>
       <c r="I70" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>ZGEPA113299W41GN</v>
+        <v>POVYD288603M57KA</v>
       </c>
     </row>
     <row r="71" spans="1:9">
       <c r="A71" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>CT9876362U</v>
+        <v>EB1922026F</v>
       </c>
       <c r="B71" t="s">
         <v>1592</v>
@@ -23248,13 +23248,13 @@
       </c>
       <c r="I71" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>YWRCY182239J12IZ</v>
+        <v>ODKOR202419E7TB</v>
       </c>
     </row>
     <row r="72" spans="1:9">
       <c r="A72" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>TU1690633R</v>
+        <v>TI7492749H</v>
       </c>
       <c r="B72" t="s">
         <v>1593</v>
@@ -23264,13 +23264,13 @@
       </c>
       <c r="I72" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>QCEML663428E3FP</v>
+        <v>WYOLA546339Y9CT</v>
       </c>
     </row>
     <row r="73" spans="1:9">
       <c r="A73" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>ZK3199302F</v>
+        <v>KB8886539E</v>
       </c>
       <c r="B73" t="s">
         <v>1594</v>
@@ -23280,13 +23280,13 @@
       </c>
       <c r="I73" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>PGZOT461698O73FT</v>
+        <v>QDVLA107326N6VW</v>
       </c>
     </row>
     <row r="74" spans="1:9">
       <c r="A74" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>GU5751557P</v>
+        <v>BH3351056B</v>
       </c>
       <c r="B74" t="s">
         <v>1595</v>
@@ -23296,13 +23296,13 @@
       </c>
       <c r="I74" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>DWZPF673223D31HJ</v>
+        <v>KVGWK133670H69TS</v>
       </c>
     </row>
     <row r="75" spans="1:9">
       <c r="A75" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>HO7522228C</v>
+        <v>YM5255365Y</v>
       </c>
       <c r="B75" t="s">
         <v>1596</v>
@@ -23312,13 +23312,13 @@
       </c>
       <c r="I75" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>YZRJP850573T50PW</v>
+        <v>VGLUY694625D97OF</v>
       </c>
     </row>
     <row r="76" spans="1:9">
       <c r="A76" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>YR4265141E</v>
+        <v>LD4039238C</v>
       </c>
       <c r="B76" t="s">
         <v>1597</v>
@@ -23328,13 +23328,13 @@
       </c>
       <c r="I76" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>RDHKU168419T82UU</v>
+        <v>RUBQG359170A67ZM</v>
       </c>
     </row>
     <row r="77" spans="1:9">
       <c r="A77" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>AY127720C</v>
+        <v>EO9896915O</v>
       </c>
       <c r="B77" t="s">
         <v>1598</v>
@@ -23344,13 +23344,13 @@
       </c>
       <c r="I77" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>NZUPE835398N24ER</v>
+        <v>LISFG499136V47DM</v>
       </c>
     </row>
     <row r="78" spans="1:9">
       <c r="A78" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UE9741631T</v>
+        <v>HO6163579R</v>
       </c>
       <c r="B78" t="s">
         <v>1599</v>
@@ -23360,13 +23360,13 @@
       </c>
       <c r="I78" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>BKUXW135421R92RA</v>
+        <v>IATIA754784K84YE</v>
       </c>
     </row>
     <row r="79" spans="1:9">
       <c r="A79" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>DX3537023W</v>
+        <v>TH8052563D</v>
       </c>
       <c r="B79" t="s">
         <v>1600</v>
@@ -23376,13 +23376,13 @@
       </c>
       <c r="I79" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>BTOAM276459R37CS</v>
+        <v>KYVZW568015U70YO</v>
       </c>
     </row>
     <row r="80" spans="1:9">
       <c r="A80" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>VG4968A</v>
+        <v>UH8769956N</v>
       </c>
       <c r="B80" t="s">
         <v>1601</v>
@@ -23392,13 +23392,13 @@
       </c>
       <c r="I80" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>RQLGJ901528U67LX</v>
+        <v>FHKLV706619K30RG</v>
       </c>
     </row>
     <row r="81" spans="1:9">
       <c r="A81" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>WF4095871L</v>
+        <v>ME5401262W</v>
       </c>
       <c r="B81" t="s">
         <v>1602</v>
@@ -23408,13 +23408,13 @@
       </c>
       <c r="I81" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>LZRBE575077Q15BO</v>
+        <v>QLYKH410177U73DU</v>
       </c>
     </row>
     <row r="82" spans="1:9">
       <c r="A82" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UW6062704G</v>
+        <v>QA3266283F</v>
       </c>
       <c r="B82" t="s">
         <v>1603</v>
@@ -23424,13 +23424,13 @@
       </c>
       <c r="I82" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>PQYTS408390B94TR</v>
+        <v>ZYNRP291792A41MQ</v>
       </c>
     </row>
     <row r="83" spans="1:9">
       <c r="A83" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>KY3047445K</v>
+        <v>HW958574O</v>
       </c>
       <c r="B83" t="s">
         <v>1604</v>
@@ -23440,13 +23440,13 @@
       </c>
       <c r="I83" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>YMUZG827153Z84WR</v>
+        <v>CLKYN697911C47SH</v>
       </c>
     </row>
     <row r="84" spans="1:9">
       <c r="A84" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>TZ4296337Z</v>
+        <v>QL7311979G</v>
       </c>
       <c r="B84" t="s">
         <v>1605</v>
@@ -23456,13 +23456,13 @@
       </c>
       <c r="I84" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>HISLD662310C2EH</v>
+        <v>DARAT576668O14XS</v>
       </c>
     </row>
     <row r="85" spans="1:9">
       <c r="A85" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UX9419536X</v>
+        <v>VV6379821J</v>
       </c>
       <c r="B85" t="s">
         <v>1606</v>
@@ -23472,13 +23472,13 @@
       </c>
       <c r="I85" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>IKZYW537173E63QX</v>
+        <v>FBHTV592844P62UL</v>
       </c>
     </row>
     <row r="86" spans="1:9">
       <c r="A86" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>QZ5532385T</v>
+        <v>JL5781311C</v>
       </c>
       <c r="B86" t="s">
         <v>1607</v>
@@ -23488,13 +23488,13 @@
       </c>
       <c r="I86" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>XKZOO956359M10IZ</v>
+        <v>OMOYG447708A65ZL</v>
       </c>
     </row>
     <row r="87" spans="1:9">
       <c r="A87" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>MH8808751N</v>
+        <v>HM3746414S</v>
       </c>
       <c r="B87" t="s">
         <v>1608</v>
@@ -23504,13 +23504,13 @@
       </c>
       <c r="I87" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>ZPRSK206396N22EQ</v>
+        <v>QFOJL79131T73IE</v>
       </c>
     </row>
     <row r="88" spans="1:9">
       <c r="A88" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UD1347269K</v>
+        <v>BN9489078R</v>
       </c>
       <c r="B88" t="s">
         <v>1609</v>
@@ -23520,13 +23520,13 @@
       </c>
       <c r="I88" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>ZXSVE682768H66DU</v>
+        <v>XKYHW530012C19SX</v>
       </c>
     </row>
     <row r="89" spans="1:9">
       <c r="A89" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>KH7201873K</v>
+        <v>GP7911716R</v>
       </c>
       <c r="B89" t="s">
         <v>1610</v>
@@ -23536,13 +23536,13 @@
       </c>
       <c r="I89" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>YJFCS1868C5VS</v>
+        <v>XTJEC17709I17YU</v>
       </c>
     </row>
     <row r="90" spans="1:9">
       <c r="A90" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>CX831816D</v>
+        <v>SK1601738J</v>
       </c>
       <c r="B90" t="s">
         <v>1611</v>
@@ -23552,13 +23552,13 @@
       </c>
       <c r="I90" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>UITWN788729C96HC</v>
+        <v>MSIYZ527324W63QL</v>
       </c>
     </row>
     <row r="91" spans="1:9">
       <c r="A91" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>SX6381245U</v>
+        <v>JQ2169645N</v>
       </c>
       <c r="B91" t="s">
         <v>1612</v>
@@ -23568,13 +23568,13 @@
       </c>
       <c r="I91" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>WMUMM717174C55EX</v>
+        <v>QGYBM699406X20EN</v>
       </c>
     </row>
     <row r="92" spans="1:9">
       <c r="A92" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>ZM2542034H</v>
+        <v>YU1188518U</v>
       </c>
       <c r="B92" t="s">
         <v>1613</v>
@@ -23584,13 +23584,13 @@
       </c>
       <c r="I92" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>NTHGY340151M68YV</v>
+        <v>DSUKH75200Q79MS</v>
       </c>
     </row>
     <row r="93" spans="1:9">
       <c r="A93" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>GA2599836Z</v>
+        <v>VR7428191B</v>
       </c>
       <c r="B93" t="s">
         <v>1614</v>
@@ -23600,13 +23600,13 @@
       </c>
       <c r="I93" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>MYMLM980228I38WY</v>
+        <v>VRTXZ793368J5CP</v>
       </c>
     </row>
     <row r="94" spans="1:9">
       <c r="A94" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>WV7622694J</v>
+        <v>VM2329488O</v>
       </c>
       <c r="B94" t="s">
         <v>1615</v>
@@ -23616,13 +23616,13 @@
       </c>
       <c r="I94" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>CIYID86726P87WL</v>
+        <v>ZJSFP987077A36FV</v>
       </c>
     </row>
     <row r="95" spans="1:9">
       <c r="A95" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>OC7432887O</v>
+        <v>IJ9377593D</v>
       </c>
       <c r="B95" t="s">
         <v>1616</v>
@@ -23632,13 +23632,13 @@
       </c>
       <c r="I95" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>AVDUG143062D99WH</v>
+        <v>JDODY919881K11AS</v>
       </c>
     </row>
     <row r="96" spans="1:9">
       <c r="A96" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>RQ7025519Z</v>
+        <v>JH2405292L</v>
       </c>
       <c r="B96" t="s">
         <v>1617</v>
@@ -23648,13 +23648,13 @@
       </c>
       <c r="I96" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>PMLRF821255J78GD</v>
+        <v>CKYFL124445D31BY</v>
       </c>
     </row>
     <row r="97" spans="1:9">
       <c r="A97" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>YI2427848P</v>
+        <v>NC6624488Z</v>
       </c>
       <c r="B97" t="s">
         <v>1618</v>
@@ -23664,13 +23664,13 @@
       </c>
       <c r="I97" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>WJTEK788307N3JK</v>
+        <v>BEHPV497289U64VX</v>
       </c>
     </row>
     <row r="98" spans="1:9">
       <c r="A98" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>IR5092041N</v>
+        <v>NN8571209U</v>
       </c>
       <c r="B98" t="s">
         <v>1619</v>
@@ -23680,13 +23680,13 @@
       </c>
       <c r="I98" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>SPDHR158368A64PK</v>
+        <v>YGXBO875094D62MG</v>
       </c>
     </row>
     <row r="99" spans="1:9">
       <c r="A99" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>RV8764704H</v>
+        <v>XX788875D</v>
       </c>
       <c r="B99" t="s">
         <v>1620</v>
@@ -23696,13 +23696,13 @@
       </c>
       <c r="I99" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>WYRQA276183Y24ML</v>
+        <v>JINDZ238405W19WS</v>
       </c>
     </row>
     <row r="100" spans="1:9">
       <c r="A100" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>LQ1869867E</v>
+        <v>EB674172Y</v>
       </c>
       <c r="B100" t="s">
         <v>1621</v>
@@ -23712,13 +23712,13 @@
       </c>
       <c r="I100" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>UJPOU760687E94XT</v>
+        <v>KPHQF598122D20YO</v>
       </c>
     </row>
     <row r="101" spans="1:9">
       <c r="A101" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>MS4295528M</v>
+        <v>YH7180003Y</v>
       </c>
       <c r="B101" t="s">
         <v>1622</v>
@@ -23728,13 +23728,13 @@
       </c>
       <c r="I101" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>QULGL129856P45US</v>
+        <v>AKRRK298969V84BX</v>
       </c>
     </row>
     <row r="102" spans="1:9">
       <c r="A102" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>AL787582U</v>
+        <v>YE6976817E</v>
       </c>
       <c r="B102" t="s">
         <v>1623</v>
@@ -23744,13 +23744,13 @@
       </c>
       <c r="I102" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>WODTI347107D57FH</v>
+        <v>MJPIQ761870T75TR</v>
       </c>
     </row>
     <row r="103" spans="1:9">
       <c r="A103" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>LI4226178R</v>
+        <v>GQ8886837Z</v>
       </c>
       <c r="B103" t="s">
         <v>1624</v>
@@ -23760,13 +23760,13 @@
       </c>
       <c r="I103" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>SHABA307114R2LH</v>
+        <v>MXPFD84302I91SY</v>
       </c>
     </row>
     <row r="104" spans="1:9">
       <c r="A104" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>CW605673O</v>
+        <v>RM7422576D</v>
       </c>
       <c r="B104" t="s">
         <v>1625</v>
@@ -23776,13 +23776,13 @@
       </c>
       <c r="I104" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>PZCQT811096X55EH</v>
+        <v>CRHWU755012F72VW</v>
       </c>
     </row>
     <row r="105" spans="1:9">
       <c r="A105" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>LB9737913S</v>
+        <v>EK1215876F</v>
       </c>
       <c r="B105" t="s">
         <v>1626</v>
@@ -23792,13 +23792,13 @@
       </c>
       <c r="I105" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>LGPYW262291O67QE</v>
+        <v>TGVJL425903C39SL</v>
       </c>
     </row>
     <row r="106" spans="1:9">
       <c r="A106" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>VJ61737U</v>
+        <v>JA5712739I</v>
       </c>
       <c r="B106" t="s">
         <v>1627</v>
@@ -23808,13 +23808,13 @@
       </c>
       <c r="I106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>XLUSP356357G28MK</v>
+        <v>LUVUR201848R5DS</v>
       </c>
     </row>
     <row r="107" spans="1:9">
       <c r="A107" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>ZP2994134X</v>
+        <v>VF354535B</v>
       </c>
       <c r="B107" t="s">
         <v>1628</v>
@@ -23824,13 +23824,13 @@
       </c>
       <c r="I107" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>UVLBE731473Y95PP</v>
+        <v>ZIDOO964219D93EL</v>
       </c>
     </row>
     <row r="108" spans="1:9">
       <c r="A108" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>SQ4127323S</v>
+        <v>JL269710Y</v>
       </c>
       <c r="B108" t="s">
         <v>1629</v>
@@ -23840,13 +23840,13 @@
       </c>
       <c r="I108" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>DODVB660362V8HM</v>
+        <v>EKMSM215449G7BD</v>
       </c>
     </row>
     <row r="109" spans="1:9">
       <c r="A109" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>AJ1952942Z</v>
+        <v>SH7213422O</v>
       </c>
       <c r="B109" t="s">
         <v>1630</v>
@@ -23856,13 +23856,13 @@
       </c>
       <c r="I109" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>GTGPD130305I22EE</v>
+        <v>SLLKL367410I69YN</v>
       </c>
     </row>
     <row r="110" spans="1:9">
       <c r="A110" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>BV1995546O</v>
+        <v>ZW9134754O</v>
       </c>
       <c r="B110" t="s">
         <v>1631</v>
@@ -23872,13 +23872,13 @@
       </c>
       <c r="I110" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>FCOWO806563A32GH</v>
+        <v>BLLKF351779A57JI</v>
       </c>
     </row>
     <row r="111" spans="1:9">
       <c r="A111" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>TP573761D</v>
+        <v>PM6057760I</v>
       </c>
       <c r="B111" t="s">
         <v>1632</v>
@@ -23888,13 +23888,13 @@
       </c>
       <c r="I111" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>KZZPD824788W53MO</v>
+        <v>IXORH430685G8CZ</v>
       </c>
     </row>
     <row r="112" spans="1:9">
       <c r="A112" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>JN1117574D</v>
+        <v>CA294355U</v>
       </c>
       <c r="B112" t="s">
         <v>1633</v>
@@ -23904,13 +23904,13 @@
       </c>
       <c r="I112" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>WNUGL331074C23XE</v>
+        <v>KKELW35224F89LL</v>
       </c>
     </row>
     <row r="113" spans="1:9">
       <c r="A113" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>ME9174323G</v>
+        <v>ZQ1889576O</v>
       </c>
       <c r="B113" t="s">
         <v>1634</v>
@@ -23920,13 +23920,13 @@
       </c>
       <c r="I113" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>WAYYD772454A64AC</v>
+        <v>GBLTY243501V76PN</v>
       </c>
     </row>
     <row r="114" spans="1:9">
       <c r="A114" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>LY836035J</v>
+        <v>KO4293284P</v>
       </c>
       <c r="B114" t="s">
         <v>1635</v>
@@ -23936,13 +23936,13 @@
       </c>
       <c r="I114" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>OJNKL720744S32LE</v>
+        <v>DYHRO666589X36XT</v>
       </c>
     </row>
     <row r="115" spans="1:9">
       <c r="A115" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>QR6462394N</v>
+        <v>LD2339461V</v>
       </c>
       <c r="B115" t="s">
         <v>1636</v>
@@ -23952,13 +23952,13 @@
       </c>
       <c r="I115" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>OBREU373386F79RT</v>
+        <v>LROBR764460L50SB</v>
       </c>
     </row>
     <row r="116" spans="1:9">
       <c r="A116" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>QE1718440K</v>
+        <v>ZB6622522G</v>
       </c>
       <c r="B116" t="s">
         <v>1637</v>
@@ -23968,13 +23968,13 @@
       </c>
       <c r="I116" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>RTRXQ772218U26FI</v>
+        <v>SZRFL110433P98LU</v>
       </c>
     </row>
     <row r="117" spans="1:9">
       <c r="A117" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>AH7080886C</v>
+        <v>BG7632601F</v>
       </c>
       <c r="B117" t="s">
         <v>1638</v>
@@ -23984,13 +23984,13 @@
       </c>
       <c r="I117" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>QGHJS480320W97BZ</v>
+        <v>BNMQT481757G76SV</v>
       </c>
     </row>
     <row r="118" spans="1:9">
       <c r="A118" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>IR8378486U</v>
+        <v>PS7819610O</v>
       </c>
       <c r="B118" t="s">
         <v>1639</v>
@@ -24000,13 +24000,13 @@
       </c>
       <c r="I118" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>NMNVE752692I51KG</v>
+        <v>QQBUD681579A42KD</v>
       </c>
     </row>
     <row r="119" spans="1:9">
       <c r="A119" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>KO9743218Y</v>
+        <v>SW9224766D</v>
       </c>
       <c r="B119" t="s">
         <v>1640</v>
@@ -24016,13 +24016,13 @@
       </c>
       <c r="I119" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>MHBZM663694P84OJ</v>
+        <v>REVOZ861650I37TU</v>
       </c>
     </row>
     <row r="120" spans="1:9">
       <c r="A120" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>TP4568917H</v>
+        <v>UP444219B</v>
       </c>
       <c r="B120" t="s">
         <v>1641</v>
@@ -24032,13 +24032,13 @@
       </c>
       <c r="I120" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>ODZII9489U40GV</v>
+        <v>WIDQB772182U30WI</v>
       </c>
     </row>
     <row r="121" spans="1:9">
       <c r="A121" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>XX345810H</v>
+        <v>QU4597037S</v>
       </c>
       <c r="B121" t="s">
         <v>1642</v>
@@ -24048,13 +24048,13 @@
       </c>
       <c r="I121" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>WMIUI919525R44SH</v>
+        <v>UPCWE835959S55TH</v>
       </c>
     </row>
     <row r="122" spans="1:9">
       <c r="A122" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>HO5385515F</v>
+        <v>XC8722810T</v>
       </c>
       <c r="B122" t="s">
         <v>1643</v>
@@ -24064,13 +24064,13 @@
       </c>
       <c r="I122" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>TQLLO230548Z10HH</v>
+        <v>ZBOWQ913145N62TZ</v>
       </c>
     </row>
     <row r="123" spans="1:9">
       <c r="A123" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>YL429091Y</v>
+        <v>XD499265Z</v>
       </c>
       <c r="B123" t="s">
         <v>1644</v>
@@ -24080,13 +24080,13 @@
       </c>
       <c r="I123" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>STXXO75123Q69DP</v>
+        <v>KTOZN455133R60JX</v>
       </c>
     </row>
     <row r="124" spans="1:9">
       <c r="A124" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>OF6742848T</v>
+        <v>ZB7272121X</v>
       </c>
       <c r="B124" t="s">
         <v>1645</v>
@@ -24096,13 +24096,13 @@
       </c>
       <c r="I124" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>LOIDN523601E43CS</v>
+        <v>BVBAO853416L64TR</v>
       </c>
     </row>
     <row r="125" spans="1:9">
       <c r="A125" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>AK5365056G</v>
+        <v>MP6811626N</v>
       </c>
       <c r="B125" t="s">
         <v>1646</v>
@@ -24112,13 +24112,13 @@
       </c>
       <c r="I125" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>PUOIA422488T83ZQ</v>
+        <v>ACAHU985072Z59YG</v>
       </c>
     </row>
     <row r="126" spans="1:9">
       <c r="A126" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>FJ2290446X</v>
+        <v>VS2173742A</v>
       </c>
       <c r="B126" t="s">
         <v>1647</v>
@@ -24128,13 +24128,13 @@
       </c>
       <c r="I126" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>VRMGI211670C80FL</v>
+        <v>URGVH305768D54OZ</v>
       </c>
     </row>
     <row r="127" spans="1:9">
       <c r="A127" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UK4463996T</v>
+        <v>QQ546015V</v>
       </c>
       <c r="B127" t="s">
         <v>1648</v>
@@ -24144,13 +24144,13 @@
       </c>
       <c r="I127" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>OKDNS103176Q75QL</v>
+        <v>PVAKQ555902C6KS</v>
       </c>
     </row>
     <row r="128" spans="1:9">
       <c r="A128" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>HD4152463Y</v>
+        <v>CZ3983062T</v>
       </c>
       <c r="B128" t="s">
         <v>1649</v>
@@ -24160,13 +24160,13 @@
       </c>
       <c r="I128" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>GFMZM311044N31IU</v>
+        <v>PVLUW736633W75ZD</v>
       </c>
     </row>
     <row r="129" spans="1:9">
       <c r="A129" s="6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>BR2693664W</v>
+        <v>FJ2910867R</v>
       </c>
       <c r="B129" t="s">
         <v>1650</v>
@@ -24176,13 +24176,13 @@
       </c>
       <c r="I129" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>JQPTR454532I14BX</v>
+        <v>ADAIX679266R71DY</v>
       </c>
     </row>
     <row r="130" spans="1:9">
       <c r="A130" s="6" t="str">
         <f t="shared" ref="A130:A193" ca="1" si="5">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,9999999)&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>YJ1996120E</v>
+        <v>EO2107989A</v>
       </c>
       <c r="B130" t="s">
         <v>1651</v>
@@ -24192,13 +24192,13 @@
       </c>
       <c r="I130" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>ZNTCJ846346O97XS</v>
+        <v>QKURW701390Y31ND</v>
       </c>
     </row>
     <row r="131" spans="1:9">
       <c r="A131" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>WC471801X</v>
+        <v>EV4551705L</v>
       </c>
       <c r="B131" t="s">
         <v>1652</v>
@@ -24208,13 +24208,13 @@
       </c>
       <c r="I131" t="str">
         <f t="shared" ref="I131:I194" ca="1" si="6">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,999999)&amp;CHAR(RANDBETWEEN(65,90))&amp;(RANDBETWEEN(1,99))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>OTGGH217468E77ZW</v>
+        <v>JOITU392514B89BA</v>
       </c>
     </row>
     <row r="132" spans="1:9">
       <c r="A132" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>GQ295815F</v>
+        <v>DP3048703N</v>
       </c>
       <c r="B132" t="s">
         <v>1653</v>
@@ -24224,13 +24224,13 @@
       </c>
       <c r="I132" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>PJYYW676223Z50UI</v>
+        <v>HRNUC298756W61WK</v>
       </c>
     </row>
     <row r="133" spans="1:9">
       <c r="A133" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>FF1797825G</v>
+        <v>QK4799918E</v>
       </c>
       <c r="B133" t="s">
         <v>1654</v>
@@ -24240,13 +24240,13 @@
       </c>
       <c r="I133" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>AWFJB334723L38JD</v>
+        <v>POQPR536917O64FQ</v>
       </c>
     </row>
     <row r="134" spans="1:9">
       <c r="A134" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>IG4913061V</v>
+        <v>IK2579212U</v>
       </c>
       <c r="B134" t="s">
         <v>1655</v>
@@ -24256,13 +24256,13 @@
       </c>
       <c r="I134" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>CCHRS967021D63RZ</v>
+        <v>RQUBX410090W1KB</v>
       </c>
     </row>
     <row r="135" spans="1:9">
       <c r="A135" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>KE2022875I</v>
+        <v>XN2597773M</v>
       </c>
       <c r="B135" t="s">
         <v>1656</v>
@@ -24272,13 +24272,13 @@
       </c>
       <c r="I135" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>UZMUP729509G64KR</v>
+        <v>UIOAX485173D53YJ</v>
       </c>
     </row>
     <row r="136" spans="1:9">
       <c r="A136" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>PK5976850L</v>
+        <v>YG90836J</v>
       </c>
       <c r="B136" t="s">
         <v>1657</v>
@@ -24288,13 +24288,13 @@
       </c>
       <c r="I136" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>RZZVS687157Y68UL</v>
+        <v>UKTCZ158385P26ET</v>
       </c>
     </row>
     <row r="137" spans="1:9">
       <c r="A137" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>EW401050F</v>
+        <v>ZY1287164U</v>
       </c>
       <c r="B137" t="s">
         <v>1658</v>
@@ -24304,13 +24304,13 @@
       </c>
       <c r="I137" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>IVUYI782058M91AI</v>
+        <v>SKFVM956440P85EO</v>
       </c>
     </row>
     <row r="138" spans="1:9">
       <c r="A138" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>LV6318762O</v>
+        <v>YD3193395B</v>
       </c>
       <c r="B138" t="s">
         <v>1659</v>
@@ -24320,13 +24320,13 @@
       </c>
       <c r="I138" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>TPFUR150575Z4PZ</v>
+        <v>LEETU120125S57PQ</v>
       </c>
     </row>
     <row r="139" spans="1:9">
       <c r="A139" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>VK4390449M</v>
+        <v>TS1588393G</v>
       </c>
       <c r="B139" t="s">
         <v>1660</v>
@@ -24336,13 +24336,13 @@
       </c>
       <c r="I139" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>CBSDA625606R50AL</v>
+        <v>QRVUX373543K82XI</v>
       </c>
     </row>
     <row r="140" spans="1:9">
       <c r="A140" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>NW4754589T</v>
+        <v>JA4317645P</v>
       </c>
       <c r="B140" t="s">
         <v>1661</v>
@@ -24352,13 +24352,13 @@
       </c>
       <c r="I140" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>RPZAE892507N29PL</v>
+        <v>JEHTU456168J57JY</v>
       </c>
     </row>
     <row r="141" spans="1:9">
       <c r="A141" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>RO4815903Y</v>
+        <v>PX1229051V</v>
       </c>
       <c r="B141" t="s">
         <v>1662</v>
@@ -24368,13 +24368,13 @@
       </c>
       <c r="I141" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>SUXOB97752M21BV</v>
+        <v>NCJZR747619M26MK</v>
       </c>
     </row>
     <row r="142" spans="1:9">
       <c r="A142" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>ST1845047U</v>
+        <v>HY4975890Z</v>
       </c>
       <c r="B142" t="s">
         <v>1663</v>
@@ -24384,13 +24384,13 @@
       </c>
       <c r="I142" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>HBBWS142558P15TW</v>
+        <v>NKXWF509005Q23YT</v>
       </c>
     </row>
     <row r="143" spans="1:9">
       <c r="A143" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>GA5706771S</v>
+        <v>TX9363802Q</v>
       </c>
       <c r="B143" t="s">
         <v>1664</v>
@@ -24400,13 +24400,13 @@
       </c>
       <c r="I143" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>WVQKP373090W81TU</v>
+        <v>BUEUJ8632U22OE</v>
       </c>
     </row>
     <row r="144" spans="1:9">
       <c r="A144" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>VF372942R</v>
+        <v>DE8350964E</v>
       </c>
       <c r="B144" t="s">
         <v>1665</v>
@@ -24416,13 +24416,13 @@
       </c>
       <c r="I144" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>BUTQT989119L3IB</v>
+        <v>BHCZA754782O42BK</v>
       </c>
     </row>
     <row r="145" spans="1:12">
       <c r="A145" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>UB1036058W</v>
+        <v>FJ9178749P</v>
       </c>
       <c r="B145" t="s">
         <v>1666</v>
@@ -24432,13 +24432,13 @@
       </c>
       <c r="I145" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>SGWMA312536S30MU</v>
+        <v>YHGEQ790726P97OL</v>
       </c>
     </row>
     <row r="146" spans="1:12">
       <c r="A146" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>DW6762077Z</v>
+        <v>TG4590507Q</v>
       </c>
       <c r="B146" t="s">
         <v>1667</v>
@@ -24448,13 +24448,13 @@
       </c>
       <c r="I146" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>DWUWS438815L73TA</v>
+        <v>ZFUSX356606J83CF</v>
       </c>
     </row>
     <row r="147" spans="1:12">
       <c r="A147" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>AM4903020J</v>
+        <v>TF8089007M</v>
       </c>
       <c r="B147" t="s">
         <v>1668</v>
@@ -24464,13 +24464,13 @@
       </c>
       <c r="I147" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>QDDEO413444U23TY</v>
+        <v>CYYPM603774C48XW</v>
       </c>
     </row>
     <row r="148" spans="1:12">
       <c r="A148" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>CH6742505B</v>
+        <v>XR3180719O</v>
       </c>
       <c r="B148" t="s">
         <v>1669</v>
@@ -24480,13 +24480,13 @@
       </c>
       <c r="I148" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>NSBFZ947159X5GI</v>
+        <v>UBMMU401178V66KO</v>
       </c>
     </row>
     <row r="149" spans="1:12">
       <c r="A149" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>KJ71344Z</v>
+        <v>WL8202502U</v>
       </c>
       <c r="B149" t="s">
         <v>1670</v>
@@ -24496,13 +24496,13 @@
       </c>
       <c r="I149" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>FRDFZ882051U56WR</v>
+        <v>XVVCU124865K24VL</v>
       </c>
     </row>
     <row r="150" spans="1:12">
       <c r="A150" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>MQ3256089R</v>
+        <v>TG2269419C</v>
       </c>
       <c r="B150" t="s">
         <v>1671</v>
@@ -24512,13 +24512,13 @@
       </c>
       <c r="I150" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>UTQKW195567W67LX</v>
+        <v>TBYHG468001T93IB</v>
       </c>
     </row>
     <row r="151" spans="1:12">
       <c r="A151" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>ML9909333B</v>
+        <v>MP1062593J</v>
       </c>
       <c r="B151" t="s">
         <v>1672</v>
@@ -24528,13 +24528,13 @@
       </c>
       <c r="I151" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>UEKEB166453V78JI</v>
+        <v>YWFJE357812R42JJ</v>
       </c>
     </row>
     <row r="152" spans="1:12">
       <c r="A152" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>DL4937517M</v>
+        <v>XC3048968C</v>
       </c>
       <c r="B152" t="s">
         <v>1673</v>
@@ -24544,7 +24544,7 @@
       </c>
       <c r="I152" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>ZZQAX183130S41XA</v>
+        <v>XGJOG100904S28ZP</v>
       </c>
       <c r="K152" s="28" t="e">
         <f t="shared" ref="K152" si="7">RIGHT(J152, LEN(J152)-1)</f>
@@ -24558,7 +24558,7 @@
     <row r="153" spans="1:12">
       <c r="A153" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>MV7716475A</v>
+        <v>AP544379Z</v>
       </c>
       <c r="B153" t="s">
         <v>1674</v>
@@ -24568,13 +24568,13 @@
       </c>
       <c r="I153" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>TPTYX337930A14WE</v>
+        <v>STOVI468529X94DH</v>
       </c>
     </row>
     <row r="154" spans="1:12">
       <c r="A154" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>CY849766P</v>
+        <v>BP4884264S</v>
       </c>
       <c r="B154" t="s">
         <v>1675</v>
@@ -24584,13 +24584,13 @@
       </c>
       <c r="I154" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>ALZLB272680V36ID</v>
+        <v>ERQOP583331C98IW</v>
       </c>
     </row>
     <row r="155" spans="1:12">
       <c r="A155" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>JI6793157I</v>
+        <v>QB9727115X</v>
       </c>
       <c r="B155" t="s">
         <v>1676</v>
@@ -24600,13 +24600,13 @@
       </c>
       <c r="I155" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>VRTDT325561O74ZN</v>
+        <v>MPLTC839205F2WU</v>
       </c>
     </row>
     <row r="156" spans="1:12">
       <c r="A156" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>HN7755953S</v>
+        <v>DD7015595K</v>
       </c>
       <c r="B156" t="s">
         <v>1677</v>
@@ -24616,13 +24616,13 @@
       </c>
       <c r="I156" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>JTBZE472482Y40GF</v>
+        <v>TARCA412543J57QE</v>
       </c>
     </row>
     <row r="157" spans="1:12">
       <c r="A157" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>KR9143626I</v>
+        <v>FL3755712D</v>
       </c>
       <c r="B157" t="s">
         <v>1678</v>
@@ -24632,13 +24632,13 @@
       </c>
       <c r="I157" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LDPOR876654W65DX</v>
+        <v>IZGQK519393S58DZ</v>
       </c>
     </row>
     <row r="158" spans="1:12">
       <c r="A158" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>NC8411176B</v>
+        <v>VU4247392T</v>
       </c>
       <c r="B158" t="s">
         <v>1679</v>
@@ -24648,13 +24648,13 @@
       </c>
       <c r="I158" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>ARGVB850248F72JY</v>
+        <v>JOXGZ211147H84WN</v>
       </c>
     </row>
     <row r="159" spans="1:12">
       <c r="A159" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>UX2864461J</v>
+        <v>XV2538753J</v>
       </c>
       <c r="B159" t="s">
         <v>1680</v>
@@ -24664,13 +24664,13 @@
       </c>
       <c r="I159" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>QMNDG709856R11DM</v>
+        <v>JTTWF804460F10AP</v>
       </c>
     </row>
     <row r="160" spans="1:12">
       <c r="A160" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>YV9556978Z</v>
+        <v>FI5460839O</v>
       </c>
       <c r="B160" t="s">
         <v>1681</v>
@@ -24680,13 +24680,13 @@
       </c>
       <c r="I160" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>QZSJB552915H73AS</v>
+        <v>JAHVI686742R60PU</v>
       </c>
     </row>
     <row r="161" spans="1:9">
       <c r="A161" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>JZ3348191E</v>
+        <v>ME3477188J</v>
       </c>
       <c r="B161" t="s">
         <v>1682</v>
@@ -24696,13 +24696,13 @@
       </c>
       <c r="I161" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>KOIRT645720A34FW</v>
+        <v>PWTAE870079P40VX</v>
       </c>
     </row>
     <row r="162" spans="1:9">
       <c r="A162" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>YT4751442Q</v>
+        <v>MO801633S</v>
       </c>
       <c r="B162" t="s">
         <v>1683</v>
@@ -24712,13 +24712,13 @@
       </c>
       <c r="I162" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>VJHBJ877750C77JU</v>
+        <v>PNZPZ309543E49GI</v>
       </c>
     </row>
     <row r="163" spans="1:9">
       <c r="A163" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>QV9335353O</v>
+        <v>MD1814748O</v>
       </c>
       <c r="B163" t="s">
         <v>1684</v>
@@ -24728,13 +24728,13 @@
       </c>
       <c r="I163" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LSUQI742935R90JR</v>
+        <v>OSMDK605262Z91WX</v>
       </c>
     </row>
     <row r="164" spans="1:9">
       <c r="A164" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>YR39512K</v>
+        <v>YY434950E</v>
       </c>
       <c r="B164" t="s">
         <v>1685</v>
@@ -24744,13 +24744,13 @@
       </c>
       <c r="I164" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>JWVHV222624N35NB</v>
+        <v>JDXJF515107B95NJ</v>
       </c>
     </row>
     <row r="165" spans="1:9">
       <c r="A165" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>LH3928469I</v>
+        <v>GG7392995T</v>
       </c>
       <c r="B165" t="s">
         <v>1686</v>
@@ -24760,13 +24760,13 @@
       </c>
       <c r="I165" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>PRRVP596109W58QO</v>
+        <v>HFEYB693215D19OJ</v>
       </c>
     </row>
     <row r="166" spans="1:9">
       <c r="A166" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>IP475060J</v>
+        <v>HY6963843J</v>
       </c>
       <c r="B166" t="s">
         <v>1687</v>
@@ -24776,13 +24776,13 @@
       </c>
       <c r="I166" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>KIXYP290761J59RY</v>
+        <v>CIBWR537613V18HH</v>
       </c>
     </row>
     <row r="167" spans="1:9">
       <c r="A167" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>IZ7501512F</v>
+        <v>YK4071880V</v>
       </c>
       <c r="B167" t="s">
         <v>1688</v>
@@ -24792,13 +24792,13 @@
       </c>
       <c r="I167" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>URTPR223090S30LY</v>
+        <v>IGCDN360573H86NZ</v>
       </c>
     </row>
     <row r="168" spans="1:9">
       <c r="A168" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>QT6831510X</v>
+        <v>PR881970I</v>
       </c>
       <c r="B168" t="s">
         <v>1689</v>
@@ -24808,13 +24808,13 @@
       </c>
       <c r="I168" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>PIRMT281354A10UU</v>
+        <v>UZHDO472953M93NZ</v>
       </c>
     </row>
     <row r="169" spans="1:9">
       <c r="A169" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>SZ2020922W</v>
+        <v>FM4218610G</v>
       </c>
       <c r="B169" t="s">
         <v>1690</v>
@@ -24824,13 +24824,13 @@
       </c>
       <c r="I169" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>YVCME782811O29HP</v>
+        <v>LINBL248986J4XF</v>
       </c>
     </row>
     <row r="170" spans="1:9">
       <c r="A170" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>QB1257552O</v>
+        <v>QZ3830730B</v>
       </c>
       <c r="B170" t="s">
         <v>1691</v>
@@ -24840,13 +24840,13 @@
       </c>
       <c r="I170" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>TVACX221157Y62AP</v>
+        <v>JAGMQ298441F97CL</v>
       </c>
     </row>
     <row r="171" spans="1:9">
       <c r="A171" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>LI2376345U</v>
+        <v>CV3085578Y</v>
       </c>
       <c r="B171" t="s">
         <v>1692</v>
@@ -24856,13 +24856,13 @@
       </c>
       <c r="I171" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>PRNIB127583X13FN</v>
+        <v>EMKPZ125577A80LH</v>
       </c>
     </row>
     <row r="172" spans="1:9">
       <c r="A172" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>OV9973914K</v>
+        <v>FW4043399T</v>
       </c>
       <c r="B172" t="s">
         <v>1693</v>
@@ -24872,13 +24872,13 @@
       </c>
       <c r="I172" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>WQCTA341782G87TP</v>
+        <v>ZWFIH76933Z4EQ</v>
       </c>
     </row>
     <row r="173" spans="1:9">
       <c r="A173" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>WT4298069S</v>
+        <v>GK9619386C</v>
       </c>
       <c r="B173" t="s">
         <v>1694</v>
@@ -24888,13 +24888,13 @@
       </c>
       <c r="I173" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>WAHRC27648B71XZ</v>
+        <v>IFNQN119917M80EN</v>
       </c>
     </row>
     <row r="174" spans="1:9">
       <c r="A174" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>VG6168320F</v>
+        <v>DM1866525H</v>
       </c>
       <c r="B174" t="s">
         <v>1695</v>
@@ -24904,13 +24904,13 @@
       </c>
       <c r="I174" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>JEWFS355043J62GU</v>
+        <v>WCHWY728635I82IO</v>
       </c>
     </row>
     <row r="175" spans="1:9">
       <c r="A175" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>NK3432611O</v>
+        <v>VI2556249Y</v>
       </c>
       <c r="B175" t="s">
         <v>1696</v>
@@ -24920,13 +24920,13 @@
       </c>
       <c r="I175" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>MSETL933709J88QG</v>
+        <v>FTPSI696417L10WC</v>
       </c>
     </row>
     <row r="176" spans="1:9">
       <c r="A176" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>EX1921839Q</v>
+        <v>KR317623K</v>
       </c>
       <c r="B176" t="s">
         <v>1697</v>
@@ -24936,13 +24936,13 @@
       </c>
       <c r="I176" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>AQSVP213375T79XU</v>
+        <v>WIEEF162702J97FG</v>
       </c>
     </row>
     <row r="177" spans="1:9">
       <c r="A177" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>GY2997642D</v>
+        <v>FA8916161E</v>
       </c>
       <c r="B177" t="s">
         <v>1698</v>
@@ -24952,13 +24952,13 @@
       </c>
       <c r="I177" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>ESCKD123625L71RR</v>
+        <v>YBHLV152610K67PE</v>
       </c>
     </row>
     <row r="178" spans="1:9">
       <c r="A178" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>BO4059730V</v>
+        <v>WQ8218353V</v>
       </c>
       <c r="B178" t="s">
         <v>1699</v>
@@ -24968,13 +24968,13 @@
       </c>
       <c r="I178" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>KPDOF471258X15ZZ</v>
+        <v>ELRXB186274R52QT</v>
       </c>
     </row>
     <row r="179" spans="1:9">
       <c r="A179" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>DA906877G</v>
+        <v>GA372013M</v>
       </c>
       <c r="B179" t="s">
         <v>1700</v>
@@ -24984,13 +24984,13 @@
       </c>
       <c r="I179" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>QCSFQ441539W11HM</v>
+        <v>PFEAR117429N45DB</v>
       </c>
     </row>
     <row r="180" spans="1:9">
       <c r="A180" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>FR1618941U</v>
+        <v>RP9973188C</v>
       </c>
       <c r="B180" t="s">
         <v>1701</v>
@@ -25000,13 +25000,13 @@
       </c>
       <c r="I180" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>PFYLV57644U90BY</v>
+        <v>MSDLN790494H36JA</v>
       </c>
     </row>
     <row r="181" spans="1:9">
       <c r="A181" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>YB5431863P</v>
+        <v>SQ9086660Y</v>
       </c>
       <c r="B181" t="s">
         <v>1702</v>
@@ -25016,13 +25016,13 @@
       </c>
       <c r="I181" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>BBAFQ706563F35AZ</v>
+        <v>NSSAS549359M8EL</v>
       </c>
     </row>
     <row r="182" spans="1:9">
       <c r="A182" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>YQ7396946U</v>
+        <v>WF2284029U</v>
       </c>
       <c r="B182" t="s">
         <v>1703</v>
@@ -25032,13 +25032,13 @@
       </c>
       <c r="I182" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>HAHBO412881A89WF</v>
+        <v>WATXR95701T61CW</v>
       </c>
     </row>
     <row r="183" spans="1:9">
       <c r="A183" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>LR8297583Q</v>
+        <v>AX373903F</v>
       </c>
       <c r="B183" t="s">
         <v>1704</v>
@@ -25048,13 +25048,13 @@
       </c>
       <c r="I183" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>PMHBA108714B68MA</v>
+        <v>LXQRC58374A77KD</v>
       </c>
     </row>
     <row r="184" spans="1:9">
       <c r="A184" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>SS8894115P</v>
+        <v>LD3225419C</v>
       </c>
       <c r="B184" t="s">
         <v>1705</v>
@@ -25064,13 +25064,13 @@
       </c>
       <c r="I184" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>RYLOK58425T42NY</v>
+        <v>IGWZG676202B43WJ</v>
       </c>
     </row>
     <row r="185" spans="1:9">
       <c r="A185" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>PS7584831T</v>
+        <v>SW1419297J</v>
       </c>
       <c r="B185" t="s">
         <v>1706</v>
@@ -25080,13 +25080,13 @@
       </c>
       <c r="I185" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>GCYDM980740M48VU</v>
+        <v>HMHXV233392D22SD</v>
       </c>
     </row>
     <row r="186" spans="1:9">
       <c r="A186" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>BU22158M</v>
+        <v>SM1259847A</v>
       </c>
       <c r="B186" t="s">
         <v>1707</v>
@@ -25096,13 +25096,13 @@
       </c>
       <c r="I186" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>KKAZA425070I29NI</v>
+        <v>GZFYL546373B19GK</v>
       </c>
     </row>
     <row r="187" spans="1:9">
       <c r="A187" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>PC7618068K</v>
+        <v>VQ7924434K</v>
       </c>
       <c r="B187" t="s">
         <v>1708</v>
@@ -25112,13 +25112,13 @@
       </c>
       <c r="I187" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>ZHWQZ150488W19MO</v>
+        <v>NKWRY639897Q95EV</v>
       </c>
     </row>
     <row r="188" spans="1:9">
       <c r="A188" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>JN2989662I</v>
+        <v>QX5925328Z</v>
       </c>
       <c r="B188" t="s">
         <v>1709</v>
@@ -25128,13 +25128,13 @@
       </c>
       <c r="I188" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LBEOF201362W62DD</v>
+        <v>DMLBR123021H58SW</v>
       </c>
     </row>
     <row r="189" spans="1:9">
       <c r="A189" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>HV6372500S</v>
+        <v>RY7752716F</v>
       </c>
       <c r="B189" t="s">
         <v>1710</v>
@@ -25144,13 +25144,13 @@
       </c>
       <c r="I189" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>MCFMU66253M88TG</v>
+        <v>CPTVE485946X37PS</v>
       </c>
     </row>
     <row r="190" spans="1:9">
       <c r="A190" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>WG24901K</v>
+        <v>YH2181577T</v>
       </c>
       <c r="B190" t="s">
         <v>1711</v>
@@ -25160,13 +25160,13 @@
       </c>
       <c r="I190" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>MHCUJ688047M36CU</v>
+        <v>SOUJR942977G62DA</v>
       </c>
     </row>
     <row r="191" spans="1:9">
       <c r="A191" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>GK7891302K</v>
+        <v>XZ6774166C</v>
       </c>
       <c r="B191" t="s">
         <v>1712</v>
@@ -25176,13 +25176,13 @@
       </c>
       <c r="I191" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>KNNHB211040G41SA</v>
+        <v>NKIND828530A40TU</v>
       </c>
     </row>
     <row r="192" spans="1:9">
       <c r="A192" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>ZQ6652586E</v>
+        <v>HG2940932X</v>
       </c>
       <c r="B192" t="s">
         <v>1713</v>
@@ -25192,13 +25192,13 @@
       </c>
       <c r="I192" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>PGXPG565079U56PB</v>
+        <v>GGPGF3126A48LS</v>
       </c>
     </row>
     <row r="193" spans="1:9">
       <c r="A193" s="6" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>HJ2029108V</v>
+        <v>XS2394283F</v>
       </c>
       <c r="B193" t="s">
         <v>1714</v>
@@ -25208,13 +25208,13 @@
       </c>
       <c r="I193" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>LRUML878771O27BX</v>
+        <v>EZIXS804714D78SY</v>
       </c>
     </row>
     <row r="194" spans="1:9">
       <c r="A194" s="6" t="str">
         <f t="shared" ref="A194:A257" ca="1" si="8">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,9999999)&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>EP7552716D</v>
+        <v>RE3526950I</v>
       </c>
       <c r="B194" t="s">
         <v>1715</v>
@@ -25224,13 +25224,13 @@
       </c>
       <c r="I194" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>NQIMO26129J62YM</v>
+        <v>CCWGB620570X78IU</v>
       </c>
     </row>
     <row r="195" spans="1:9">
       <c r="A195" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>UJ1973167Z</v>
+        <v>DI6377627F</v>
       </c>
       <c r="B195" t="s">
         <v>1716</v>
@@ -25240,13 +25240,13 @@
       </c>
       <c r="I195" t="str">
         <f t="shared" ref="I195:I250" ca="1" si="9">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,999999)&amp;CHAR(RANDBETWEEN(65,90))&amp;(RANDBETWEEN(1,99))&amp;CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>TGVHJ885853H73UM</v>
+        <v>XLMBB215826U9RH</v>
       </c>
     </row>
     <row r="196" spans="1:9">
       <c r="A196" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>EI4336711J</v>
+        <v>QP6317620F</v>
       </c>
       <c r="B196" t="s">
         <v>1717</v>
@@ -25256,13 +25256,13 @@
       </c>
       <c r="I196" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>GGKKA905597H37VM</v>
+        <v>OMZGG77942D86TE</v>
       </c>
     </row>
     <row r="197" spans="1:9">
       <c r="A197" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>KW4038349U</v>
+        <v>UI1503871E</v>
       </c>
       <c r="B197" t="s">
         <v>1718</v>
@@ -25272,13 +25272,13 @@
       </c>
       <c r="I197" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>ISXQS59871H17XO</v>
+        <v>CLRWF618171C53MX</v>
       </c>
     </row>
     <row r="198" spans="1:9">
       <c r="A198" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>MJ8229443F</v>
+        <v>BC4290286V</v>
       </c>
       <c r="B198" t="s">
         <v>1719</v>
@@ -25288,13 +25288,13 @@
       </c>
       <c r="I198" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>XEWSZ653008M90WO</v>
+        <v>BGEDA4233L15ZB</v>
       </c>
     </row>
     <row r="199" spans="1:9">
       <c r="A199" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>AB9893787Q</v>
+        <v>MX11039R</v>
       </c>
       <c r="B199" t="s">
         <v>1720</v>
@@ -25304,13 +25304,13 @@
       </c>
       <c r="I199" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>EETNJ89281S8DP</v>
+        <v>DOGEK522305J76UK</v>
       </c>
     </row>
     <row r="200" spans="1:9">
       <c r="A200" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>XR1908418U</v>
+        <v>CW3646236F</v>
       </c>
       <c r="B200" t="s">
         <v>1721</v>
@@ -25320,13 +25320,13 @@
       </c>
       <c r="I200" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>FBECK254111Y95JI</v>
+        <v>HNTBL786990J13HG</v>
       </c>
     </row>
     <row r="201" spans="1:9">
       <c r="A201" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>QU8168893L</v>
+        <v>TE3332275D</v>
       </c>
       <c r="B201" t="s">
         <v>1722</v>
@@ -25336,13 +25336,13 @@
       </c>
       <c r="I201" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>COVOO692771T95XM</v>
+        <v>QUJUM292363Q64MD</v>
       </c>
     </row>
     <row r="202" spans="1:9">
       <c r="A202" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>CZ1333171E</v>
+        <v>QY4612218I</v>
       </c>
       <c r="B202" t="s">
         <v>1723</v>
@@ -25352,13 +25352,13 @@
       </c>
       <c r="I202" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>KLHBI775268G5JU</v>
+        <v>RUSWW878327E40QJ</v>
       </c>
     </row>
     <row r="203" spans="1:9">
       <c r="A203" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>KF8155426J</v>
+        <v>MS1577731X</v>
       </c>
       <c r="B203" t="s">
         <v>1724</v>
@@ -25368,13 +25368,13 @@
       </c>
       <c r="I203" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>SPREA494178F41HN</v>
+        <v>KQSXJ817937D5XI</v>
       </c>
     </row>
     <row r="204" spans="1:9">
       <c r="A204" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>PD7402708D</v>
+        <v>GW1068550B</v>
       </c>
       <c r="B204" t="s">
         <v>1725</v>
@@ -25384,13 +25384,13 @@
       </c>
       <c r="I204" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>SKCUR96962P35QM</v>
+        <v>RRNAY36486N97NR</v>
       </c>
     </row>
     <row r="205" spans="1:9">
       <c r="A205" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>MV2315284I</v>
+        <v>GH2377456S</v>
       </c>
       <c r="B205" t="s">
         <v>1726</v>
@@ -25400,13 +25400,13 @@
       </c>
       <c r="I205" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>QDAGR821028J66EM</v>
+        <v>IJABB607488T64IN</v>
       </c>
     </row>
     <row r="206" spans="1:9">
       <c r="A206" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>XP8858406H</v>
+        <v>MH9931615O</v>
       </c>
       <c r="B206" t="s">
         <v>1727</v>
@@ -25416,13 +25416,13 @@
       </c>
       <c r="I206" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>IJGSU461034J22RK</v>
+        <v>DYKAB742576V35JE</v>
       </c>
     </row>
     <row r="207" spans="1:9">
       <c r="A207" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>MT7069206X</v>
+        <v>JH7299994U</v>
       </c>
       <c r="B207" t="s">
         <v>1728</v>
@@ -25432,13 +25432,13 @@
       </c>
       <c r="I207" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>JBLVU225680J48IQ</v>
+        <v>OEMFW35569P16VO</v>
       </c>
     </row>
     <row r="208" spans="1:9">
       <c r="A208" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>RI654128O</v>
+        <v>HN9422431B</v>
       </c>
       <c r="B208" t="s">
         <v>1729</v>
@@ -25448,13 +25448,13 @@
       </c>
       <c r="I208" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>BPPTG613954W37RA</v>
+        <v>IDOFB410717N14TE</v>
       </c>
     </row>
     <row r="209" spans="1:9">
       <c r="A209" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>EX6070930V</v>
+        <v>KK7287736C</v>
       </c>
       <c r="B209" t="s">
         <v>1730</v>
@@ -25464,13 +25464,13 @@
       </c>
       <c r="I209" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>SJOME528911Z48RB</v>
+        <v>QYAZP136568N14CS</v>
       </c>
     </row>
     <row r="210" spans="1:9">
       <c r="A210" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>BH5669105W</v>
+        <v>UH8296762K</v>
       </c>
       <c r="B210" t="s">
         <v>1731</v>
@@ -25480,13 +25480,13 @@
       </c>
       <c r="I210" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>HOVKJ862977Z92FQ</v>
+        <v>JUSCC892534W61WF</v>
       </c>
     </row>
     <row r="211" spans="1:9">
       <c r="A211" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>NK5242121P</v>
+        <v>PR8173888B</v>
       </c>
       <c r="B211" t="s">
         <v>1732</v>
@@ -25496,13 +25496,13 @@
       </c>
       <c r="I211" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>MUNQO616191U60YF</v>
+        <v>QBULI57412Z83PK</v>
       </c>
     </row>
     <row r="212" spans="1:9">
       <c r="A212" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>AE2680486L</v>
+        <v>JO9935177E</v>
       </c>
       <c r="B212" t="s">
         <v>1733</v>
@@ -25512,13 +25512,13 @@
       </c>
       <c r="I212" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>SBZOC25893G51WV</v>
+        <v>PXJWE901129F31RB</v>
       </c>
     </row>
     <row r="213" spans="1:9">
       <c r="A213" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>UH2821158E</v>
+        <v>OO2091069Z</v>
       </c>
       <c r="B213" t="s">
         <v>1734</v>
@@ -25528,13 +25528,13 @@
       </c>
       <c r="I213" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>BGFXW441023Q50TH</v>
+        <v>KOQZH745159B72GU</v>
       </c>
     </row>
     <row r="214" spans="1:9">
       <c r="A214" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>UC2574966D</v>
+        <v>DA8714282K</v>
       </c>
       <c r="B214" t="s">
         <v>1735</v>
@@ -25544,13 +25544,13 @@
       </c>
       <c r="I214" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>NCIZX789337D24BL</v>
+        <v>DTGJR523067L60WT</v>
       </c>
     </row>
     <row r="215" spans="1:9">
       <c r="A215" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>KY703476T</v>
+        <v>IG4795992O</v>
       </c>
       <c r="B215" t="s">
         <v>1736</v>
@@ -25560,13 +25560,13 @@
       </c>
       <c r="I215" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>FRBKK756911B61EQ</v>
+        <v>FHXNG835452R32PV</v>
       </c>
     </row>
     <row r="216" spans="1:9">
       <c r="A216" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>SW8778144W</v>
+        <v>NK422128V</v>
       </c>
       <c r="B216" t="s">
         <v>1737</v>
@@ -25576,13 +25576,13 @@
       </c>
       <c r="I216" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>RILZT909885M25HP</v>
+        <v>RXEDC846089P59ZQ</v>
       </c>
     </row>
     <row r="217" spans="1:9">
       <c r="A217" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>KF1205512W</v>
+        <v>JN4128938X</v>
       </c>
       <c r="B217" t="s">
         <v>1738</v>
@@ -25592,13 +25592,13 @@
       </c>
       <c r="I217" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>GRGAJ140723B44GF</v>
+        <v>RNZIE347171I39CY</v>
       </c>
     </row>
     <row r="218" spans="1:9">
       <c r="A218" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>LU1031761P</v>
+        <v>PU5510715Q</v>
       </c>
       <c r="B218" t="s">
         <v>1739</v>
@@ -25608,13 +25608,13 @@
       </c>
       <c r="I218" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>SMCIG989796R47PG</v>
+        <v>JTMEY329244A12AP</v>
       </c>
     </row>
     <row r="219" spans="1:9">
       <c r="A219" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>IJ6770731G</v>
+        <v>CG6750174Y</v>
       </c>
       <c r="B219" t="s">
         <v>1740</v>
@@ -25624,13 +25624,13 @@
       </c>
       <c r="I219" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>DTFTB966697R51FL</v>
+        <v>YSGUM412450P56NY</v>
       </c>
     </row>
     <row r="220" spans="1:9">
       <c r="A220" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>NR5342731V</v>
+        <v>VH5754064X</v>
       </c>
       <c r="B220" t="s">
         <v>1741</v>
@@ -25640,13 +25640,13 @@
       </c>
       <c r="I220" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>WYVSM604645N36JH</v>
+        <v>QXJAK892414L79FD</v>
       </c>
     </row>
     <row r="221" spans="1:9">
       <c r="A221" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>OW2341668E</v>
+        <v>ZM7437271I</v>
       </c>
       <c r="B221" t="s">
         <v>1742</v>
@@ -25656,13 +25656,13 @@
       </c>
       <c r="I221" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>QPNHI273157O35PP</v>
+        <v>BMSQV403310T82GS</v>
       </c>
     </row>
     <row r="222" spans="1:9">
       <c r="A222" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>JT1190786M</v>
+        <v>OH5155544G</v>
       </c>
       <c r="B222" t="s">
         <v>1743</v>
@@ -25672,13 +25672,13 @@
       </c>
       <c r="I222" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>YEKKM483227X84ZL</v>
+        <v>MEJKU600501T38CG</v>
       </c>
     </row>
     <row r="223" spans="1:9">
       <c r="A223" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>ZV5392790D</v>
+        <v>RH5881279W</v>
       </c>
       <c r="B223" t="s">
         <v>1744</v>
@@ -25688,13 +25688,13 @@
       </c>
       <c r="I223" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>VSULT903695H38EI</v>
+        <v>NHHCC300991B54PE</v>
       </c>
     </row>
     <row r="224" spans="1:9">
       <c r="A224" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>LV5734640D</v>
+        <v>EX8183707X</v>
       </c>
       <c r="B224" t="s">
         <v>1745</v>
@@ -25704,13 +25704,13 @@
       </c>
       <c r="I224" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>HNWIC553082V85HX</v>
+        <v>APJAC646775L26KF</v>
       </c>
     </row>
     <row r="225" spans="1:9">
       <c r="A225" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>QI5369840J</v>
+        <v>MQ2089940X</v>
       </c>
       <c r="B225" t="s">
         <v>1746</v>
@@ -25720,13 +25720,13 @@
       </c>
       <c r="I225" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>ZSWDQ991397G74QN</v>
+        <v>ICMWJ355B32PK</v>
       </c>
     </row>
     <row r="226" spans="1:9">
       <c r="A226" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>PX4288531U</v>
+        <v>EI4035455Z</v>
       </c>
       <c r="B226" t="s">
         <v>1747</v>
@@ -25736,13 +25736,13 @@
       </c>
       <c r="I226" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>FLWGW66920X30GA</v>
+        <v>KJKOQ274282W20DG</v>
       </c>
     </row>
     <row r="227" spans="1:9">
       <c r="A227" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>IL6346578I</v>
+        <v>QB5544028Q</v>
       </c>
       <c r="B227" t="s">
         <v>1748</v>
@@ -25752,13 +25752,13 @@
       </c>
       <c r="I227" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>OOLWI498904I45TK</v>
+        <v>VLCNR606887S61GD</v>
       </c>
     </row>
     <row r="228" spans="1:9">
       <c r="A228" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>JJ9733120F</v>
+        <v>QG7564084Q</v>
       </c>
       <c r="B228" t="s">
         <v>1749</v>
@@ -25768,13 +25768,13 @@
       </c>
       <c r="I228" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>UMWBU910780I67NX</v>
+        <v>APHUQ964622E58UT</v>
       </c>
     </row>
     <row r="229" spans="1:9">
       <c r="A229" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>GE9430770B</v>
+        <v>UA9300430E</v>
       </c>
       <c r="B229" t="s">
         <v>1750</v>
@@ -25784,13 +25784,13 @@
       </c>
       <c r="I229" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>HUHGX754760K36XF</v>
+        <v>UWTYB829156Z30MW</v>
       </c>
     </row>
     <row r="230" spans="1:9">
       <c r="A230" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>HT7760807K</v>
+        <v>QV1813426S</v>
       </c>
       <c r="B230" t="s">
         <v>1751</v>
@@ -25800,13 +25800,13 @@
       </c>
       <c r="I230" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>DCNLQ965150T3KO</v>
+        <v>DVRNF905808C52RR</v>
       </c>
     </row>
     <row r="231" spans="1:9">
       <c r="A231" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>NA9613223O</v>
+        <v>LM335013Z</v>
       </c>
       <c r="B231" t="s">
         <v>1752</v>
@@ -25816,13 +25816,13 @@
       </c>
       <c r="I231" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>HXUYM700484O35GR</v>
+        <v>QKNOF743355H97WT</v>
       </c>
     </row>
     <row r="232" spans="1:9">
       <c r="A232" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>WT7192130L</v>
+        <v>ZH4407322N</v>
       </c>
       <c r="B232" t="s">
         <v>1753</v>
@@ -25832,13 +25832,13 @@
       </c>
       <c r="I232" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>WIDJI100141S91OC</v>
+        <v>LYSDP908920A86QS</v>
       </c>
     </row>
     <row r="233" spans="1:9">
       <c r="A233" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>KN6201321G</v>
+        <v>QF760972A</v>
       </c>
       <c r="B233" t="s">
         <v>1754</v>
@@ -25848,13 +25848,13 @@
       </c>
       <c r="I233" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>PHBHK931033P69ZO</v>
+        <v>KAWGD729671W67YL</v>
       </c>
     </row>
     <row r="234" spans="1:9">
       <c r="A234" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>VI4181059A</v>
+        <v>ON5985096Q</v>
       </c>
       <c r="B234" t="s">
         <v>1755</v>
@@ -25864,13 +25864,13 @@
       </c>
       <c r="I234" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>CQIKT377697I81HD</v>
+        <v>HRWAV606023Z77EP</v>
       </c>
     </row>
     <row r="235" spans="1:9">
       <c r="A235" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>VP9719793Q</v>
+        <v>ES516045D</v>
       </c>
       <c r="B235" t="s">
         <v>1756</v>
@@ -25880,13 +25880,13 @@
       </c>
       <c r="I235" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>JTAPB310652V83WF</v>
+        <v>DVRFK683558F28UE</v>
       </c>
     </row>
     <row r="236" spans="1:9">
       <c r="A236" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>XJ6322813K</v>
+        <v>HJ1595002I</v>
       </c>
       <c r="B236" t="s">
         <v>1757</v>
@@ -25896,13 +25896,13 @@
       </c>
       <c r="I236" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>VIXQH494235I61CY</v>
+        <v>NMNXP564834C59HY</v>
       </c>
     </row>
     <row r="237" spans="1:9">
       <c r="A237" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>HM8306987O</v>
+        <v>VA7184050I</v>
       </c>
       <c r="B237" t="s">
         <v>1758</v>
@@ -25912,13 +25912,13 @@
       </c>
       <c r="I237" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>CQNHK922801W66YD</v>
+        <v>YEUHA257933U33PQ</v>
       </c>
     </row>
     <row r="238" spans="1:9">
       <c r="A238" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>ET7801797K</v>
+        <v>GX4378655W</v>
       </c>
       <c r="B238" t="s">
         <v>1759</v>
@@ -25928,13 +25928,13 @@
       </c>
       <c r="I238" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>RYUEF654243G85OP</v>
+        <v>KTBJW418634V78NG</v>
       </c>
     </row>
     <row r="239" spans="1:9">
       <c r="A239" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>RL9452606L</v>
+        <v>AL1185558P</v>
       </c>
       <c r="B239" t="s">
         <v>1760</v>
@@ -25944,13 +25944,13 @@
       </c>
       <c r="I239" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>MTTIP822358Q40QJ</v>
+        <v>UVQBW808640S74NF</v>
       </c>
     </row>
     <row r="240" spans="1:9">
       <c r="A240" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>FO9729572F</v>
+        <v>WB5995864Q</v>
       </c>
       <c r="B240" t="s">
         <v>1761</v>
@@ -25960,13 +25960,13 @@
       </c>
       <c r="I240" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>FUPXT705944N63GI</v>
+        <v>QFNIG893763C67BP</v>
       </c>
     </row>
     <row r="241" spans="1:9">
       <c r="A241" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>ZX9530406O</v>
+        <v>NC9742082S</v>
       </c>
       <c r="B241" t="s">
         <v>1762</v>
@@ -25976,13 +25976,13 @@
       </c>
       <c r="I241" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>JUQYA984074B87IY</v>
+        <v>SQBJG71267V78KR</v>
       </c>
     </row>
     <row r="242" spans="1:9">
       <c r="A242" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>GH2543272B</v>
+        <v>EJ3232646Q</v>
       </c>
       <c r="B242" t="s">
         <v>1763</v>
@@ -25992,13 +25992,13 @@
       </c>
       <c r="I242" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>ATXRI349142D96UV</v>
+        <v>UGPAE645047T88FC</v>
       </c>
     </row>
     <row r="243" spans="1:9">
       <c r="A243" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>RE5159908O</v>
+        <v>FQ6050175K</v>
       </c>
       <c r="B243" t="s">
         <v>1764</v>
@@ -26008,104 +26008,104 @@
       </c>
       <c r="I243" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>MFFMZ787522X97EA</v>
+        <v>PMMYN785767E61LV</v>
       </c>
     </row>
     <row r="244" spans="1:9">
       <c r="A244" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>BA8829094L</v>
+        <v>YX9997032Y</v>
       </c>
       <c r="B244" t="s">
         <v>1765</v>
       </c>
       <c r="I244" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>PLIYA745539Z36SL</v>
+        <v>LCKHY74202E64RY</v>
       </c>
     </row>
     <row r="245" spans="1:9">
       <c r="A245" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>YB9527716A</v>
+        <v>KE6965912Z</v>
       </c>
       <c r="B245" t="s">
         <v>1766</v>
       </c>
       <c r="I245" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>VGQKW307370X16YA</v>
+        <v>TUJKD257304V9UM</v>
       </c>
     </row>
     <row r="246" spans="1:9">
       <c r="A246" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>SK8645580N</v>
+        <v>QO2169760P</v>
       </c>
       <c r="B246" t="s">
         <v>1767</v>
       </c>
       <c r="I246" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>PZQBE267421N30TA</v>
+        <v>SBMGZ760013F18IM</v>
       </c>
     </row>
     <row r="247" spans="1:9">
       <c r="A247" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>YL7268550D</v>
+        <v>RF3097295A</v>
       </c>
       <c r="B247" t="s">
         <v>1768</v>
       </c>
       <c r="I247" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>CAHOH851344A6PD</v>
+        <v>CYOMK905366L52DX</v>
       </c>
     </row>
     <row r="248" spans="1:9">
       <c r="A248" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>EP9334854F</v>
+        <v>OV5365781X</v>
       </c>
       <c r="B248" t="s">
         <v>1769</v>
       </c>
       <c r="I248" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>ALJRC269148L71VT</v>
+        <v>JOVFV767493O56MI</v>
       </c>
     </row>
     <row r="249" spans="1:9">
       <c r="A249" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>TA9504255R</v>
+        <v>BV2045696V</v>
       </c>
       <c r="B249" t="s">
         <v>1770</v>
       </c>
       <c r="I249" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>IRPDU673538Y71WS</v>
+        <v>FBRWO258170Z12GS</v>
       </c>
     </row>
     <row r="250" spans="1:9">
       <c r="A250" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>JG3331763W</v>
+        <v>QV6789226X</v>
       </c>
       <c r="B250" t="s">
         <v>1771</v>
       </c>
       <c r="I250" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>XHURA606180C19KY</v>
+        <v>ZDSFV380685U63BZ</v>
       </c>
     </row>
     <row r="251" spans="1:9">
       <c r="A251" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>JH9683030R</v>
+        <v>MZ8089793V</v>
       </c>
       <c r="B251" t="s">
         <v>1772</v>
@@ -26114,7 +26114,7 @@
     <row r="252" spans="1:9">
       <c r="A252" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>IP5032269J</v>
+        <v>HJ5278814B</v>
       </c>
       <c r="B252" t="s">
         <v>1773</v>
@@ -26123,7 +26123,7 @@
     <row r="253" spans="1:9">
       <c r="A253" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>UN9134160B</v>
+        <v>FP1948131U</v>
       </c>
       <c r="B253" t="s">
         <v>1774</v>
@@ -26132,7 +26132,7 @@
     <row r="254" spans="1:9">
       <c r="A254" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>WR5217109H</v>
+        <v>SV8393968W</v>
       </c>
       <c r="B254" t="s">
         <v>1775</v>
@@ -26141,7 +26141,7 @@
     <row r="255" spans="1:9">
       <c r="A255" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>GE4919812U</v>
+        <v>IC9077045O</v>
       </c>
       <c r="B255" t="s">
         <v>1776</v>
@@ -26150,7 +26150,7 @@
     <row r="256" spans="1:9">
       <c r="A256" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>SN550655A</v>
+        <v>HK8899921Y</v>
       </c>
       <c r="B256" t="s">
         <v>1777</v>
@@ -26159,7 +26159,7 @@
     <row r="257" spans="1:2">
       <c r="A257" s="6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>JG3719253S</v>
+        <v>YN9546919T</v>
       </c>
       <c r="B257" t="s">
         <v>1778</v>
@@ -26168,7 +26168,7 @@
     <row r="258" spans="1:2">
       <c r="A258" s="6" t="str">
         <f t="shared" ref="A258:A300" ca="1" si="10">CHAR(RANDBETWEEN(65,90))&amp;CHAR(RANDBETWEEN(65,90))&amp;RANDBETWEEN(0,9999999)&amp;CHAR(RANDBETWEEN(65,90))</f>
-        <v>JC355010I</v>
+        <v>QX5941539I</v>
       </c>
       <c r="B258" t="s">
         <v>1779</v>
@@ -26177,7 +26177,7 @@
     <row r="259" spans="1:2">
       <c r="A259" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>HO132417T</v>
+        <v>TL803790S</v>
       </c>
       <c r="B259" t="s">
         <v>1780</v>
@@ -26186,7 +26186,7 @@
     <row r="260" spans="1:2">
       <c r="A260" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>UN8541913N</v>
+        <v>QT9417815E</v>
       </c>
       <c r="B260" t="s">
         <v>1781</v>
@@ -26195,7 +26195,7 @@
     <row r="261" spans="1:2">
       <c r="A261" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>UC893381W</v>
+        <v>BP1852307P</v>
       </c>
       <c r="B261" t="s">
         <v>1782</v>
@@ -26204,7 +26204,7 @@
     <row r="262" spans="1:2">
       <c r="A262" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>XP7168311C</v>
+        <v>UW9941269E</v>
       </c>
       <c r="B262" t="s">
         <v>1783</v>
@@ -26213,7 +26213,7 @@
     <row r="263" spans="1:2">
       <c r="A263" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>SE3323080T</v>
+        <v>BS6904317G</v>
       </c>
       <c r="B263" t="s">
         <v>1784</v>
@@ -26222,7 +26222,7 @@
     <row r="264" spans="1:2">
       <c r="A264" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>NC2035111G</v>
+        <v>TX9817483U</v>
       </c>
       <c r="B264" t="s">
         <v>1785</v>
@@ -26231,7 +26231,7 @@
     <row r="265" spans="1:2">
       <c r="A265" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>NA893557E</v>
+        <v>FV1269241O</v>
       </c>
       <c r="B265" t="s">
         <v>1786</v>
@@ -26240,7 +26240,7 @@
     <row r="266" spans="1:2">
       <c r="A266" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>WM3587023R</v>
+        <v>AL8997837L</v>
       </c>
       <c r="B266" t="s">
         <v>1787</v>
@@ -26249,7 +26249,7 @@
     <row r="267" spans="1:2">
       <c r="A267" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>QN4992779G</v>
+        <v>LD2784293O</v>
       </c>
       <c r="B267" t="s">
         <v>1788</v>
@@ -26258,7 +26258,7 @@
     <row r="268" spans="1:2">
       <c r="A268" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>AQ3732638H</v>
+        <v>IB2704663N</v>
       </c>
       <c r="B268" t="s">
         <v>1789</v>
@@ -26267,7 +26267,7 @@
     <row r="269" spans="1:2">
       <c r="A269" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>YH3692895T</v>
+        <v>CZ3918242D</v>
       </c>
       <c r="B269" t="s">
         <v>1790</v>
@@ -26276,7 +26276,7 @@
     <row r="270" spans="1:2">
       <c r="A270" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>BC8512083Y</v>
+        <v>DI5649755V</v>
       </c>
       <c r="B270" t="s">
         <v>1791</v>
@@ -26285,7 +26285,7 @@
     <row r="271" spans="1:2">
       <c r="A271" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>QR7182884V</v>
+        <v>IP2279185W</v>
       </c>
       <c r="B271" t="s">
         <v>1792</v>
@@ -26294,7 +26294,7 @@
     <row r="272" spans="1:2">
       <c r="A272" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>RG7051218C</v>
+        <v>FE4861986X</v>
       </c>
       <c r="B272" t="s">
         <v>1793</v>
@@ -26303,7 +26303,7 @@
     <row r="273" spans="1:2">
       <c r="A273" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>XL7451926Z</v>
+        <v>ZB3638764Z</v>
       </c>
       <c r="B273" t="s">
         <v>1794</v>
@@ -26312,7 +26312,7 @@
     <row r="274" spans="1:2">
       <c r="A274" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>KB4581908M</v>
+        <v>WX1817805T</v>
       </c>
       <c r="B274" t="s">
         <v>1795</v>
@@ -26321,7 +26321,7 @@
     <row r="275" spans="1:2">
       <c r="A275" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>GH1200811J</v>
+        <v>LJ9359094V</v>
       </c>
       <c r="B275" t="s">
         <v>1796</v>
@@ -26330,7 +26330,7 @@
     <row r="276" spans="1:2">
       <c r="A276" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>PD8340210S</v>
+        <v>HM668113O</v>
       </c>
       <c r="B276" t="s">
         <v>1797</v>
@@ -26339,7 +26339,7 @@
     <row r="277" spans="1:2">
       <c r="A277" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>NQ221841S</v>
+        <v>UO2634769T</v>
       </c>
       <c r="B277" t="s">
         <v>1798</v>
@@ -26348,7 +26348,7 @@
     <row r="278" spans="1:2">
       <c r="A278" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>TY7271317H</v>
+        <v>RL5851297Y</v>
       </c>
       <c r="B278" t="s">
         <v>1799</v>
@@ -26357,7 +26357,7 @@
     <row r="279" spans="1:2">
       <c r="A279" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>US5246442S</v>
+        <v>GU4921873E</v>
       </c>
       <c r="B279" t="s">
         <v>1800</v>
@@ -26366,7 +26366,7 @@
     <row r="280" spans="1:2">
       <c r="A280" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>LU3804553H</v>
+        <v>HI3036605J</v>
       </c>
       <c r="B280" t="s">
         <v>1801</v>
@@ -26375,7 +26375,7 @@
     <row r="281" spans="1:2">
       <c r="A281" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>TE9077424V</v>
+        <v>DL7787482Z</v>
       </c>
       <c r="B281" t="s">
         <v>1802</v>
@@ -26384,7 +26384,7 @@
     <row r="282" spans="1:2">
       <c r="A282" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>ZF6944213E</v>
+        <v>CK3760563C</v>
       </c>
       <c r="B282" t="s">
         <v>1803</v>
@@ -26393,7 +26393,7 @@
     <row r="283" spans="1:2">
       <c r="A283" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>VS4650423S</v>
+        <v>ID600832H</v>
       </c>
       <c r="B283" t="s">
         <v>1804</v>
@@ -26402,7 +26402,7 @@
     <row r="284" spans="1:2">
       <c r="A284" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>XC9686143L</v>
+        <v>JQ5580111R</v>
       </c>
       <c r="B284" t="s">
         <v>1805</v>
@@ -26411,7 +26411,7 @@
     <row r="285" spans="1:2">
       <c r="A285" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>FG4457432X</v>
+        <v>YF195254L</v>
       </c>
       <c r="B285" t="s">
         <v>1806</v>
@@ -26420,7 +26420,7 @@
     <row r="286" spans="1:2">
       <c r="A286" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>YG2146221Q</v>
+        <v>KU621056N</v>
       </c>
       <c r="B286" t="s">
         <v>1807</v>
@@ -26429,7 +26429,7 @@
     <row r="287" spans="1:2">
       <c r="A287" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>XT3482908S</v>
+        <v>LN3007795W</v>
       </c>
       <c r="B287" t="s">
         <v>1808</v>
@@ -26438,7 +26438,7 @@
     <row r="288" spans="1:2">
       <c r="A288" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>XV5608166G</v>
+        <v>UI7614632P</v>
       </c>
       <c r="B288" t="s">
         <v>1809</v>
@@ -26447,7 +26447,7 @@
     <row r="289" spans="1:2">
       <c r="A289" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>NS156311A</v>
+        <v>AE7322548X</v>
       </c>
       <c r="B289" t="s">
         <v>1810</v>
@@ -26456,7 +26456,7 @@
     <row r="290" spans="1:2">
       <c r="A290" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>AH5619178C</v>
+        <v>WK3806646A</v>
       </c>
       <c r="B290" t="s">
         <v>1811</v>
@@ -26465,7 +26465,7 @@
     <row r="291" spans="1:2">
       <c r="A291" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>CX8391109U</v>
+        <v>VV2596370F</v>
       </c>
       <c r="B291" t="s">
         <v>1812</v>
@@ -26474,7 +26474,7 @@
     <row r="292" spans="1:2">
       <c r="A292" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>WP6248009X</v>
+        <v>KC1787832B</v>
       </c>
       <c r="B292" t="s">
         <v>1813</v>
@@ -26483,7 +26483,7 @@
     <row r="293" spans="1:2">
       <c r="A293" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>TX5345499V</v>
+        <v>NL5712295L</v>
       </c>
       <c r="B293" t="s">
         <v>1814</v>
@@ -26492,7 +26492,7 @@
     <row r="294" spans="1:2">
       <c r="A294" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>BY77834B</v>
+        <v>QM481708B</v>
       </c>
       <c r="B294" t="s">
         <v>1815</v>
@@ -26501,7 +26501,7 @@
     <row r="295" spans="1:2">
       <c r="A295" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>HZ2737182L</v>
+        <v>JI877412N</v>
       </c>
       <c r="B295" t="s">
         <v>1816</v>
@@ -26510,7 +26510,7 @@
     <row r="296" spans="1:2">
       <c r="A296" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>LY4531354X</v>
+        <v>EX8862713D</v>
       </c>
       <c r="B296" t="s">
         <v>1817</v>
@@ -26519,7 +26519,7 @@
     <row r="297" spans="1:2">
       <c r="A297" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>HM1468722F</v>
+        <v>YC8205839X</v>
       </c>
       <c r="B297" t="s">
         <v>1818</v>
@@ -26528,7 +26528,7 @@
     <row r="298" spans="1:2">
       <c r="A298" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>LC4804452A</v>
+        <v>TP136756X</v>
       </c>
       <c r="B298" t="s">
         <v>1819</v>
@@ -26537,7 +26537,7 @@
     <row r="299" spans="1:2">
       <c r="A299" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>VJ6411709P</v>
+        <v>SY2489799E</v>
       </c>
       <c r="B299" t="s">
         <v>1820</v>
@@ -26546,7 +26546,7 @@
     <row r="300" spans="1:2">
       <c r="A300" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>DM506571F</v>
+        <v>GU1283503C</v>
       </c>
       <c r="B300" t="s">
         <v>1821</v>

</xml_diff>